<commit_message>
Runthrough 2 - Collecting PNG and XLSX Files Updated
</commit_message>
<xml_diff>
--- a/climate_tracker/policy_actions.xlsx
+++ b/climate_tracker/policy_actions.xlsx
@@ -17,14 +17,13 @@
     <sheet name="Argentina’s average share of e" sheetId="8" r:id="rId8"/>
     <sheet name="Waste" sheetId="9" r:id="rId9"/>
     <sheet name="Methane" sheetId="10" r:id="rId10"/>
-    <sheet name="Power" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="148">
   <si>
     <t>country_name</t>
   </si>
@@ -35,171 +34,171 @@
     <t>Argentina</t>
   </si>
   <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Türkiye</t>
+  </si>
+  <si>
+    <t>UAE</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
     <t>Germany</t>
   </si>
   <si>
+    <t>EU</t>
+  </si>
+  <si>
     <t>India</t>
   </si>
   <si>
     <t>Indonesia</t>
   </si>
   <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>EU</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>Saudi Arabia</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>South Africa</t>
-  </si>
-  <si>
-    <t>Switzerland</t>
-  </si>
-  <si>
-    <t>Türkiye</t>
-  </si>
-  <si>
-    <t>UAE</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>Japan</t>
   </si>
   <si>
     <t>We rate Argentina’s policies and actions as “Critically insufficient” when compared with modelled domestic emissions pathways . This rating indicates that Argentina’s climate policies reflect minimal to no action and are not at all consistent with the Paris Agreement’s 1.5°C temperature limit. Argentina’s policies and action rating compared to modelled domestic pathways is now lower than in our previous assessment due to an update in our projections for the agriculture sector. Newer projections expect higher agricultural and livestock production by 2030, leading to ~2% higher emissions under current policies. Argentina’s policies and action also remain inadequate to achieve its NDC target, let alone be 1.5°C compatible. The CAT estimates that under current policies Argentina will miss its target by 54 MtCO 2 e. To be 1.5°C compatible, Argentina’s policies and action projections should be at least 175 MtCO 2 e lower in 2030.</t>
   </si>
   <si>
+    <t>Australia’s current policies are rated as “Insufficient” against modelled domestic pathways. The CAT’s policies and action scenarios are based on the Australian Government’s emissions projections, last released in November 2023, and policies which have been subsequently implemented. The introduction of new measures to tackle transport emissions were not sufficient to improve the rating. The government’s 82% renewable electricity target remains an announced rather than current policies in our assessment as it is not enshrined in law and progress towards the target is lagging. With current policies, Australia will fall short of its 2030 target. The “Insufficient” rating indicates that Australia’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow Australia’s approach, warming would reach over 2°C and up to 3°C. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
+  </si>
+  <si>
+    <t>The CAT rates Brazil’s policies and action as “Insufficient”. Brazil’s emissions (excluding emissions from the forestry and land sector) have steadily increased over the past decades but are expected to essentially plateau under current policies, growing only slightly until 2030. Yet, Brazil needs to cut its emissions this decade to meet its 2030 target and for 1.5°C compatibility. The “Insufficient” rating indicates that Brazil’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow Brazil’s approach, warming would reach over 2°C and up to 3°C. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
+  </si>
+  <si>
+    <t>Canada’s emissions are finally starting to trend downwards as the government continues to implement its climate policy agenda, but there remains a significant gap between current policies and Canada’s NDC target. Implementing planned policies will contribute significantly to closing that gap, but further action is needed. Our rating of Canada’s policies and action has improved to “Insufficient”, with the latest emissions projections showing significantly lower expected emissions for 2030. That said, it is still far from 1.5°C compatibility on a global least cost basis. If all countries were to follow Canada’s approach, warming could reach over 2°C and up to 3°C. If Canada can successfully implement all of the measures it has planned, it would go a long way to closing this ambition gap.</t>
+  </si>
+  <si>
+    <t>Chile’s current policies are almost sufficient when rated against modelled domestic pathways. The “Almost sufficient” rating indicates that Chile’s climate policies and action in 2030 are not yet consistent with the 1.5°C temperature limit but could be, with moderate improvements. If all countries were to follow Chile’s approach, warming could be held below—but not well below—2°C. Chile’s upper end of its current policy projections sits in the “Insufficient” range, meaning a lack of implementation of mitigation policies and increased natural gas consumption from retrofitting coal plants could result in a worse rating for Chile. Our 1.5°C modelled domestic pathway is based on global least-cost mitigation and defines the minimum level of emission reductions needed at home to be 1.5°C compatible. It should be taken as the floor, and not ceiling, for domestic ambition. According to our assessment, emissions under Chile’s currently implemented policies would reach 100–108 MtCO 2 e (excl. LULUCF) by 2030 (6–13% below 2021 levels). The CAT estimates that Chile reached peak emissions in 2021, ahead of the 2025 target in its NDC. However, this emissions level is still insufficient to reach both the conditional and unconditional 2030 NDC targets (88–95 MtCO 2 e), let alone be on a 1.5°C trajectory. Chile will need to implement additional policies in order to be 1.5°C compatible. Since our previous assessment, Chile has continued to shut down coal plants according to its phase-out plan. Over 1.2 GW of coal capacity from 11 plants has been retired since 2019 and an additional nine units have committed to retire or convert to natural gas between 2024 and 2025. While considered a “transition fuel” by the Chilean government, gas is still a fossil fuel that needs to be phased out – therefore, Chile must be careful when repurposing the plants to avoid the risk of carbon lock-in and stranded assets. Recent scientific literature highlights that there is no room for investment in new oil, gas, and coal activities if global warming is to be limited to 1.5°C (Green et al. , 2024). While there were discussions in August 2022 around bringing forward the coal phase-out year to 2030, it has not been mentioned in the Second Phase of the Energy Transition strategy released in 2023 (Ministerio de Energía, 2022a). An early coal phase-out, where electricity generation is replaced by renewable sources rather than fossil gas, could significantly impact Chile’s current policies pathway and bring it considerably closer to a 1.5°C trajectory. The transport sector makes up a significant share of Chile’s total GHG emissions, especially as its energy consumption continues to increase. The Electromobility Strategy, Energy Efficiency Law, and ban on ICE cars by 2035 are key policies expected to accelerate the low-carbon transportation transition, but Chile’s EV sales have yet to exceed 1%. More could be done to encourage EV uptake and decrease energy demand, for instance, by reforming diesel fuel subsidies and a incentivising a modal shift in transportation. Maintaining the LULUCF sink is an important component of Chile’s climate targets, which is threatened by the increased frequency and severity of wildfires related to climate change. While Chile has ambitious commitments for reforestation and sustainable forest management in its NDC, the pace of implementation has been far too slow, and stronger policies to support reforestation and forest management are needed. At the same time, Chile should avoid relying on LULUCF sinks for its targets and prioritise cutting emissions in other sectors. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
+  </si>
+  <si>
+    <t>China's suite of sectoral 14th FYPs set out a range of mitigation measures to prepare the country for a post-coal transition and the country is on track to meet its energy sector targets. Fossil fuel dependence will continue but renewables are also being deployed at a rapid pace: it remains uncertain whether the acceleration of renewables will be sufficient to meet the growth in energy demand and reduce dependence on coal and gas at the same time. China’s emissions under current policies are projected to peak before 2025. In our conservative scenario (CPP max), we assume China's energy-related CO₂ emissions will plateau at their peak level for around five years, given the absence of emission reduction targets after peaking (this could potentially change with more ambitious new NDC targets scheduled for 2025). CPP max suggests that China risks failing to meet its domestic target of reducing carbon intensity by 18% by 2025 from the 2020 level, as highlighted by other analyses (CREA and GEM, 2024b; Myllyvirta, 2024b). In our optimistic current policy scenario (CPP min) however, the pace of renewable integration ramps up even faster to add more than 300 GW annually. In this case, renewables will be able to meet growing energy demand and electrification while also substantially displacing coal and replacing the need for fossil gas in end-use sectors. China’s GHG emissions begin the first stages of structural decline as the country shifts from controlling energy to controlling carbon, although more action is needed to reach its carbon neutrality by 2060 target. After updating our projections to incorporate the latest policy developments and analysis, we project GHG emissions levels to between 13.8 to 14.6 GtCO₂e in 2030. China’s current policies scenario projections are rated as “Insufficient” when compared to their fair-share contribution to climate change mitigation. The “Insufficient” rating indicates that China’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow China’s approach, warming would reach over 2°C and up to 3°C. China is expected to implement additional policies with its own resources but will also need international support to implement policies in line with full decarbonisation. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
+  </si>
+  <si>
+    <t>NOTE: This update does not conduct a new rating of the UK’s climate targets, as the new government only entered power in July 2024. Instead, it describes the context inherited by the new government and highlights key areas for improvement. We will respond to any major announcements and provide an updated rating for the UK in 2025. We rate the UK’s current policies until 2030 as “Insufficient”, when compared to modelled domestic pathways. The new government needs to take rapid action to develop and implement climate policies to reduce emissions. Our 1.5°C modelled domestic pathway is based on global least-cost mitigation and defines the minimum level of emissions reductions needed at home to be 1.5°C compatible. It should be taken as the floor, and not ceiling, for domestic ambition. The UK’s stalled progress in climate policy development over recent years means that, without immediate and rapid change, the UK can no longer be considered a leader in global climate action. The “Insufficient” rating indicates that the UK’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow the UK’s approach, warming would reach over 2°C and up to 3°C. The new government has strongly indicated that it intends to address this policy shortfall, introducing new funding and delivery mechanisms to close the gap. The CAT will be tracking these policy developments and provide an updated assessment of the progress made in 2025. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
+  </si>
+  <si>
+    <t>We rate Saudi Arabia’s policies and actions against modelled domestic pathways as “Critically Insufficient” . This rating indicates that Saudi Arabia’s policies and action in 2030 reflect minimal to no action and are not at all consistent with limiting warming to 1.5°C. If all countries were to follow Saudi Arabia’s approach, warming would exceed 4°C. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
+  </si>
+  <si>
+    <t>Singapore’s current policies are “Insufficient” when compared to modelled domestic pathways. The “Insufficient” rating indicates that Singapore’s policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow Singapore’s approach, warming would reach over 2°C and up to 3°C. While CAT modelled domestic pathways do not reflect Singapore’s particularly low domestic RE potential, these pathways do reflect the rapid decarbonisation in the Southeast Asian region that Singapore should follow, if not lead. Given its context, Singapore can play an even larger role in driving regional decarbonisation and energy collaboration.</t>
+  </si>
+  <si>
+    <t>We rate South Africa’s current policies and actions as “Insufficient”. The “Insufficient” rating indicates that South Africa’s climate policies and action in 2030 need substantial improvements to be consistent with the Paris Agreement’s 1.5°C temperature limit. If all countries were to follow South Africa’s approach, warming would reach over 2°C and up to 3°C. Under these current policies, South Africa will not achieve the necessary emissions reductions needed to meet its NDC target range for 2030. Despite a range of measures passed in July 2022, the energy crisis has persisted in South Africa with load-shedding reaching record highs. Additional measures are being taken to reform the power sector, including the government taking over some of Eskom’s debt, and procurement processes for renewables and controversial fossil gas generation capacity are ongoing. The Just Energy Transition Investment Plan (JET IP), presented in November 2022, indicates the power sector will receive the bulk of the USD 8.5bn investment package from donor countries. However, the Governments of South Africa and the donor countries have expressed concerns that the plans under the agreement to retire coal plants may be delayed amid the energy crisis. An updated IRP is expected this year but has already faced delays. However, this has not stopped the private sector from investing in renewables – the country hit a new solar investment record in 2023, importing over USD 650m in solar cells, panels and modules in the first half of 2023, up from USD 345m in all of 2022. The pending IRP update could build on this momentum from the private sector to accelerate renewables. To take advantage of increasing domestic and international demand for renewable and storage technologies, the government released the South African Renewable Energy Masterplan (SAREM) for public comment in July 2023. The plan aims to develop industrial value chains for these technologies within South Africa to drive development and create jobs. If considering South Africa’s planned but not yet implemented policies, our rating of policies and actions would go up to “1.5°C compatible”. The stringent implementation of proposed economy-wide and sector-specific policy measures would enable South Africa to achieve at least the top end of its NDC range, failling within the current range.</t>
+  </si>
+  <si>
+    <t>Switzerland’s efforts to tackle climate change are heading in the right direction again, since passing the new Federal Act on a Secure Electricity Supply with Renewable Energies in June 2024. Under current policies, Switzerland is projected to achieve even its not specified, estimated domestic target of a 30% to 33% reduction below 1990 levels. The CAT rates Switzerland’s current policies as “Almost sufficient” when compared to modelled domestic pathways. The “Almost sufficient” rating indicates that Switzerland’s climate policies and action in 2030 are not yet consistent with limiting warming to 1.5°C. If all countries were to follow Switzerland’s approach, warming could be held at – but not below – 2°C. Further information on how the CAT rates countries (against modelled pathways and fair share) can be found here .</t>
+  </si>
+  <si>
+    <t>We rate Türkiye’s current policies and action as “Highly insufficient” when compared to its fair share contribution as this metric is more favourable than the modelled domestic pathways. The “Highly insufficient” rating indicates that Türkiye’s policies and action in 2030 lead to rising, rather than falling, emissions and are not at all consistent with limiting warming to 1.5°C. If all countries were to follow Türkiye’s approach, warming could reach over 3°C and up to 4°C. The CAT estimates that Türkiye’s emissions will be between 537-634 MtCO 2 e in 2030 (excluding LULUCF) under current policies and action. Türkiye is on track to achieve its updated NDC target based on our emissions estimate for 2030 under current policies. Türkiye’s policies and action rating has changed from “Critically insufficient” in the previous rating to “Highly insufficient”. The rating change is due to an update in methodology of the quantification of the current policies and action range. Previously, our method for quantifying the current policy pathway relied heavily on the ‘With Measures’ (WM) scenario developed by Türkiye for its 2015 INDC with a historic base year of 2012. Türkiye has not updated its WEM scenario since then and states that it does not reflect the current state of its policy landscape (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2023). We have therefore chosen to update our methodology. For a full explanation of our assumptions behind the current policy pathway, please see the ‘ Assumptions ’ tab. Türkiye needs to focus on adopting further policies and action to stop its emissions growth and start reducing emissions towards decarbonisation.</t>
+  </si>
+  <si>
+    <t>The CAT rates the UAE’s policies and actions as “Insufficient” when compared with modelled domestic emissions pathways. The “Insufficient” rating indicates that the UAE’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow the UAE’s approach, warming would reach over 2°C and up to 3°C. The UAE’s policies and action rating has improved compared to our previous assessment for two reasons. First, the UAE’s newly published current policy scenarios (included in its LTS) lead to 17% lower emissions by 2030. This scenario includes a sectoral breakdown and detailed information at the measure level. This is a significant improvement compared to our previous current policy scenarios which were based only on the implementation of the Energy Strategy 2050. Second, the UAE’s 5 th National Communication to the UNFCCC also includes updated inventory data, which is 15% lower than our previous estimates, mainly due to differences in industrial process emissions and fugitive emissions. These also impact the absolute value estimated for the UAE’s 2030 emissions under current policies. The UAE’s LTS, published in 2024, includes targets and current policy projections for all major sectors of the economy, and detail both existing and planned measures to achieve them. While this is a significant step in transparency, it also shows that the UAE plans to rely heavily on carbon capture and storage (CCS) technologies especially after 2030 and towards its 2050 target, which undermines the credibility of its climate policies and targets.</t>
+  </si>
+  <si>
+    <t>According to our analysis, the US will need to implement additional policies to reach its targets. We project GHG emissions will reach between 4.6–5.4 GtCO 2 e in 2030 (excluding emissions from land use, land use change and forestry, or LULUCF). This is equivalent to 29%–39% reduction from 2005 levels (excl. LULUCF), which is insufficient to meet the NDC target (45%–50% excl. LULUCF). The Inflation Reduction Act (IRA), passed in 2022, represents a significant milestone in US climate policy. While its full impact is still unfolding due to the nature of its 10-year implementation plan, the first years have shown real promise. The IRA is mobilising historic investments in clean energy, driving clean projects, creating jobs, and attracting private sector funding. EPA standards for the power and transport sectors, passed in 2024, provide two further milestones in important policy areas. However, to achieve its domestic emissions reductions target—let alone to reach a 1.5°C-compatible emissions level—the government needs to complement its recent advancements with further sector-specific policies and a shift away from fossil fuels. The projected emissions trajectory range is wider in this update than previously, due to the incorporation of new analyses that better highlight the uncertainties related to the IRA's implementation. While the middle of the policy projections' range falls into the “Insufficient” category, its lower end, representing a positive outlook on the government’s current policies, falls into the “Almost sufficient” range. The “Insufficient” rating indicates that the US’ climate policies and action in 2030 need substantial improvements to be consistent with the 1.5°C temperature limit. If all countries were to follow the US approach, warming would reach over 2°C and up to 3°C. The Biden Administration has set the goal to decarbonise the power sector by 2035, which is consistent with a Paris Agreement pathway . Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
+  </si>
+  <si>
     <t>Germany’s current policies are “almost sufficient” when compared to modelled domestic pathways. With implemented policies, Germany’s 2030 target is in danger and it will not achieve its long-term targets. The “Almost sufficient” rating indicates that Germany’s climate policies and action in 2030 are not yet consistent with limiting warming to 1.5°C but could be, with moderate improvements. If all countries were to follow Germany’s approach, warming could be held at—but not well below—2°C . Further information on how the CAT rates countries (against modelled pathways and fair share) can be found here .</t>
   </si>
   <si>
+    <t>The CAT rates the EU’s current policies and actions against modelled domestic pathways as “Insufficient”. The “Insufficient” rating indicates that the EU’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow the EU’s approach, warming would reach over 2°C and up to 3°C. With its current policies in place, the EU’s emissions will reach between 2,470 and 2,755 MtCO 2 e (excluding LULUCF) in 2030. This current policies pathway does not set it on track to meet its existing 2030 NDC target of 2,307 MtCO 2 e (excluding LULUCF) by 2030. This represents 3–9% ambition gap. For more details on our projections, see the Assumptions tab. To be 1.5°C compatible, current policies would need to reach at least 1,815 MtCO 2 e (excluding LULUCF) by 2030. Our 1.5°C modelled domestic pathway is based on global least-cost mitigation and defines the minimum level of emission reductions needed domestically to be 1.5°C compatible. It should be taken as the floor, and not ceiling, for domestic ambition. Our planned policies projections of 2,370–2,400 MtCO 2 e (excluding LULUCF) reflects the EU’s 2030 indicative renewable energy goal (of a further 2.5%, totalling 45%) as well as policy proposals that have been announced but remain to be adopted, most notably is the Energy Taxation Directive. If the EU adhered to the full list of planned policies, then it would be close to achieving its 2030 NDC target, missing the mark by 1–2%. The full spectrum of policies proposed and adopted under the Fit-for-55 and REPowerEU legislative packages have been effective in improving projected emission reductions by 2030, though some of the regulations are yet to come into effect. Despite the enormous regulatory exercise that the EU has been pursuing, many gaps still remain, with loopholes and lax enforcement mechanisms in the policy design. Additional action is required to address these issues, including: Further information on how the CAT rates countries (against modelled pathways and fair share) can be found here .</t>
+  </si>
+  <si>
     <t>CAT rates India’s current policies and action as “Insufficient” when compared to its fair share contribution. The “Insufficient” rating indicates that India’s climate policies and action in 2030 need substantial improvements to be consistent with the 1.5°C temperature limit. If all countries were to follow India’s approach, warming would reach over 2°C and up to 3°C. India will need to implement some additional policies with its own resources to make a fair contribution to addressing climate change but will also need international support to implement all the policies necessary for 1.5°C compatibility. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
   </si>
   <si>
     <t>The CAT rates Indonesia’s policies and actions “Critically Insufficient when compared to their fair share contribution to climate change mitigation. The “Critically insufficient” rating indicates that Indonesia’s policies and action in 2030 currently reflect minimal to no action and are not at all consistent with limiting warming to 1.5°C. If all countries were to follow Indonesia’s approach, warming would exceed 4°C. In the 2023 assessment, current policy projections increased by around 300 MtCO 2 e in 2030 compared to the previous 2022 assessment, driven by a huge increase in 2022 emissions and quantification of emissions from Indonesia’s off-grid coal power pipeline. This figure remains unchanged in this update, as no quantitative adjustments were made in this round. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
   </si>
   <si>
-    <t>Australia’s current policies are rated as “Insufficient” against modelled domestic pathways. The CAT’s policies and action scenarios are based on the Australian Government’s emissions projections, last released in November 2023, and policies which have been subsequently implemented. The introduction of new measures to tackle transport emissions were not sufficient to improve the rating. The government’s 82% renewable electricity target remains an announced rather than current policies in our assessment as it is not enshrined in law and progress towards the target is lagging. With current policies, Australia will fall short of its 2030 target. The “Insufficient” rating indicates that Australia’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow Australia’s approach, warming would reach over 2°C and up to 3°C. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
-  </si>
-  <si>
-    <t>The CAT rates Brazil’s policies and action as “Insufficient”. Brazil’s emissions (excluding emissions from the forestry and land sector) have steadily increased over the past decades but are expected to essentially plateau under current policies, growing only slightly until 2030. Yet, Brazil needs to cut its emissions this decade to meet its 2030 target and for 1.5°C compatibility. The “Insufficient” rating indicates that Brazil’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow Brazil’s approach, warming would reach over 2°C and up to 3°C. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
-  </si>
-  <si>
-    <t>Canada’s emissions are finally starting to trend downwards as the government continues to implement its climate policy agenda, but there remains a significant gap between current policies and Canada’s NDC target. Implementing planned policies will contribute significantly to closing that gap, but further action is needed. Our rating of Canada’s policies and action has improved to “Insufficient”, with the latest emissions projections showing significantly lower expected emissions for 2030. That said, it is still far from 1.5°C compatibility on a global least cost basis. If all countries were to follow Canada’s approach, warming could reach over 2°C and up to 3°C. If Canada can successfully implement all of the measures it has planned, it would go a long way to closing this ambition gap.</t>
-  </si>
-  <si>
-    <t>Chile’s current policies are almost sufficient when rated against modelled domestic pathways. The “Almost sufficient” rating indicates that Chile’s climate policies and action in 2030 are not yet consistent with the 1.5°C temperature limit but could be, with moderate improvements. If all countries were to follow Chile’s approach, warming could be held below—but not well below—2°C. Chile’s upper end of its current policy projections sits in the “Insufficient” range, meaning a lack of implementation of mitigation policies and increased natural gas consumption from retrofitting coal plants could result in a worse rating for Chile. Our 1.5°C modelled domestic pathway is based on global least-cost mitigation and defines the minimum level of emission reductions needed at home to be 1.5°C compatible. It should be taken as the floor, and not ceiling, for domestic ambition. According to our assessment, emissions under Chile’s currently implemented policies would reach 100–108 MtCO 2 e (excl. LULUCF) by 2030 (6–13% below 2021 levels). The CAT estimates that Chile reached peak emissions in 2021, ahead of the 2025 target in its NDC. However, this emissions level is still insufficient to reach both the conditional and unconditional 2030 NDC targets (88–95 MtCO 2 e), let alone be on a 1.5°C trajectory. Chile will need to implement additional policies in order to be 1.5°C compatible. Since our previous assessment, Chile has continued to shut down coal plants according to its phase-out plan. Over 1.2 GW of coal capacity from 11 plants has been retired since 2019 and an additional nine units have committed to retire or convert to natural gas between 2024 and 2025. While considered a “transition fuel” by the Chilean government, gas is still a fossil fuel that needs to be phased out – therefore, Chile must be careful when repurposing the plants to avoid the risk of carbon lock-in and stranded assets. Recent scientific literature highlights that there is no room for investment in new oil, gas, and coal activities if global warming is to be limited to 1.5°C (Green et al. , 2024). While there were discussions in August 2022 around bringing forward the coal phase-out year to 2030, it has not been mentioned in the Second Phase of the Energy Transition strategy released in 2023 (Ministerio de Energía, 2022a). An early coal phase-out, where electricity generation is replaced by renewable sources rather than fossil gas, could significantly impact Chile’s current policies pathway and bring it considerably closer to a 1.5°C trajectory. The transport sector makes up a significant share of Chile’s total GHG emissions, especially as its energy consumption continues to increase. The Electromobility Strategy, Energy Efficiency Law, and ban on ICE cars by 2035 are key policies expected to accelerate the low-carbon transportation transition, but Chile’s EV sales have yet to exceed 1%. More could be done to encourage EV uptake and decrease energy demand, for instance, by reforming diesel fuel subsidies and a incentivising a modal shift in transportation. Maintaining the LULUCF sink is an important component of Chile’s climate targets, which is threatened by the increased frequency and severity of wildfires related to climate change. While Chile has ambitious commitments for reforestation and sustainable forest management in its NDC, the pace of implementation has been far too slow, and stronger policies to support reforestation and forest management are needed. At the same time, Chile should avoid relying on LULUCF sinks for its targets and prioritise cutting emissions in other sectors. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
-  </si>
-  <si>
-    <t>China's suite of sectoral 14th FYPs set out a range of mitigation measures to prepare the country for a post-coal transition and the country is on track to meet its energy sector targets. Fossil fuel dependence will continue but renewables are also being deployed at a rapid pace: it remains uncertain whether the acceleration of renewables will be sufficient to meet the growth in energy demand and reduce dependence on coal and gas at the same time. China’s emissions under current policies are projected to peak before 2025. In our conservative scenario (CPP max), we assume China's energy-related CO₂ emissions will plateau at their peak level for around five years, given the absence of emission reduction targets after peaking (this could potentially change with more ambitious new NDC targets scheduled for 2025). CPP max suggests that China risks failing to meet its domestic target of reducing carbon intensity by 18% by 2025 from the 2020 level, as highlighted by other analyses (CREA and GEM, 2024b; Myllyvirta, 2024b). In our optimistic current policy scenario (CPP min) however, the pace of renewable integration ramps up even faster to add more than 300 GW annually. In this case, renewables will be able to meet growing energy demand and electrification while also substantially displacing coal and replacing the need for fossil gas in end-use sectors. China’s GHG emissions begin the first stages of structural decline as the country shifts from controlling energy to controlling carbon, although more action is needed to reach its carbon neutrality by 2060 target. After updating our projections to incorporate the latest policy developments and analysis, we project GHG emissions levels to between 13.8 to 14.6 GtCO₂e in 2030. China’s current policies scenario projections are rated as “Insufficient” when compared to their fair-share contribution to climate change mitigation. The “Insufficient” rating indicates that China’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow China’s approach, warming would reach over 2°C and up to 3°C. China is expected to implement additional policies with its own resources but will also need international support to implement policies in line with full decarbonisation. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
-  </si>
-  <si>
-    <t>The CAT rates the EU’s current policies and actions against modelled domestic pathways as “Insufficient”. The “Insufficient” rating indicates that the EU’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow the EU’s approach, warming would reach over 2°C and up to 3°C. With its current policies in place, the EU’s emissions will reach between 2,470 and 2,755 MtCO 2 e (excluding LULUCF) in 2030. This current policies pathway does not set it on track to meet its existing 2030 NDC target of 2,307 MtCO 2 e (excluding LULUCF) by 2030. This represents 3–9% ambition gap. For more details on our projections, see the Assumptions tab. To be 1.5°C compatible, current policies would need to reach at least 1,815 MtCO 2 e (excluding LULUCF) by 2030. Our 1.5°C modelled domestic pathway is based on global least-cost mitigation and defines the minimum level of emission reductions needed domestically to be 1.5°C compatible. It should be taken as the floor, and not ceiling, for domestic ambition. Our planned policies projections of 2,370–2,400 MtCO 2 e (excluding LULUCF) reflects the EU’s 2030 indicative renewable energy goal (of a further 2.5%, totalling 45%) as well as policy proposals that have been announced but remain to be adopted, most notably is the Energy Taxation Directive. If the EU adhered to the full list of planned policies, then it would be close to achieving its 2030 NDC target, missing the mark by 1–2%. The full spectrum of policies proposed and adopted under the Fit-for-55 and REPowerEU legislative packages have been effective in improving projected emission reductions by 2030, though some of the regulations are yet to come into effect. Despite the enormous regulatory exercise that the EU has been pursuing, many gaps still remain, with loopholes and lax enforcement mechanisms in the policy design. Additional action is required to address these issues, including: Further information on how the CAT rates countries (against modelled pathways and fair share) can be found here .</t>
-  </si>
-  <si>
-    <t>NOTE: This update does not conduct a new rating of the UK’s climate targets, as the new government only entered power in July 2024. Instead, it describes the context inherited by the new government and highlights key areas for improvement. We will respond to any major announcements and provide an updated rating for the UK in 2025. We rate the UK’s current policies until 2030 as “Insufficient”, when compared to modelled domestic pathways. The new government needs to take rapid action to develop and implement climate policies to reduce emissions. Our 1.5°C modelled domestic pathway is based on global least-cost mitigation and defines the minimum level of emissions reductions needed at home to be 1.5°C compatible. It should be taken as the floor, and not ceiling, for domestic ambition. The UK’s stalled progress in climate policy development over recent years means that, without immediate and rapid change, the UK can no longer be considered a leader in global climate action. The “Insufficient” rating indicates that the UK’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow the UK’s approach, warming would reach over 2°C and up to 3°C. The new government has strongly indicated that it intends to address this policy shortfall, introducing new funding and delivery mechanisms to close the gap. The CAT will be tracking these policy developments and provide an updated assessment of the progress made in 2025. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
-  </si>
-  <si>
-    <t>We rate Saudi Arabia’s policies and actions against modelled domestic pathways as “Critically Insufficient” . This rating indicates that Saudi Arabia’s policies and action in 2030 reflect minimal to no action and are not at all consistent with limiting warming to 1.5°C. If all countries were to follow Saudi Arabia’s approach, warming would exceed 4°C. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
-  </si>
-  <si>
-    <t>Singapore’s current policies are “Insufficient” when compared to modelled domestic pathways. The “Insufficient” rating indicates that Singapore’s policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow Singapore’s approach, warming would reach over 2°C and up to 3°C. While CAT modelled domestic pathways do not reflect Singapore’s particularly low domestic RE potential, these pathways do reflect the rapid decarbonisation in the Southeast Asian region that Singapore should follow, if not lead. Given its context, Singapore can play an even larger role in driving regional decarbonisation and energy collaboration.</t>
-  </si>
-  <si>
-    <t>We rate South Africa’s current policies and actions as “Insufficient”. The “Insufficient” rating indicates that South Africa’s climate policies and action in 2030 need substantial improvements to be consistent with the Paris Agreement’s 1.5°C temperature limit. If all countries were to follow South Africa’s approach, warming would reach over 2°C and up to 3°C. Under these current policies, South Africa will not achieve the necessary emissions reductions needed to meet its NDC target range for 2030. Despite a range of measures passed in July 2022, the energy crisis has persisted in South Africa with load-shedding reaching record highs. Additional measures are being taken to reform the power sector, including the government taking over some of Eskom’s debt, and procurement processes for renewables and controversial fossil gas generation capacity are ongoing. The Just Energy Transition Investment Plan (JET IP), presented in November 2022, indicates the power sector will receive the bulk of the USD 8.5bn investment package from donor countries. However, the Governments of South Africa and the donor countries have expressed concerns that the plans under the agreement to retire coal plants may be delayed amid the energy crisis. An updated IRP is expected this year but has already faced delays. However, this has not stopped the private sector from investing in renewables – the country hit a new solar investment record in 2023, importing over USD 650m in solar cells, panels and modules in the first half of 2023, up from USD 345m in all of 2022. The pending IRP update could build on this momentum from the private sector to accelerate renewables. To take advantage of increasing domestic and international demand for renewable and storage technologies, the government released the South African Renewable Energy Masterplan (SAREM) for public comment in July 2023. The plan aims to develop industrial value chains for these technologies within South Africa to drive development and create jobs. If considering South Africa’s planned but not yet implemented policies, our rating of policies and actions would go up to “1.5°C compatible”. The stringent implementation of proposed economy-wide and sector-specific policy measures would enable South Africa to achieve at least the top end of its NDC range, failling within the current range.</t>
-  </si>
-  <si>
-    <t>Switzerland’s efforts to tackle climate change are heading in the right direction again, since passing the new Federal Act on a Secure Electricity Supply with Renewable Energies in June 2024. Under current policies, Switzerland is projected to achieve even its not specified, estimated domestic target of a 30% to 33% reduction below 1990 levels. The CAT rates Switzerland’s current policies as “Almost sufficient” when compared to modelled domestic pathways. The “Almost sufficient” rating indicates that Switzerland’s climate policies and action in 2030 are not yet consistent with limiting warming to 1.5°C. If all countries were to follow Switzerland’s approach, warming could be held at – but not below – 2°C. Further information on how the CAT rates countries (against modelled pathways and fair share) can be found here .</t>
-  </si>
-  <si>
-    <t>We rate Türkiye’s current policies and action as “Highly insufficient” when compared to its fair share contribution as this metric is more favourable than the modelled domestic pathways. The “Highly insufficient” rating indicates that Türkiye’s policies and action in 2030 lead to rising, rather than falling, emissions and are not at all consistent with limiting warming to 1.5°C. If all countries were to follow Türkiye’s approach, warming could reach over 3°C and up to 4°C. The CAT estimates that Türkiye’s emissions will be between 537-634 MtCO 2 e in 2030 (excluding LULUCF) under current policies and action. Türkiye is on track to achieve its updated NDC target based on our emissions estimate for 2030 under current policies. Türkiye’s policies and action rating has changed from “Critically insufficient” in the previous rating to “Highly insufficient”. The rating change is due to an update in methodology of the quantification of the current policies and action range. Previously, our method for quantifying the current policy pathway relied heavily on the ‘With Measures’ (WM) scenario developed by Türkiye for its 2015 INDC with a historic base year of 2012. Türkiye has not updated its WEM scenario since then and states that it does not reflect the current state of its policy landscape (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2023). We have therefore chosen to update our methodology. For a full explanation of our assumptions behind the current policy pathway, please see the ‘ Assumptions ’ tab. Türkiye needs to focus on adopting further policies and action to stop its emissions growth and start reducing emissions towards decarbonisation.</t>
-  </si>
-  <si>
-    <t>The CAT rates the UAE’s policies and actions as “Insufficient” when compared with modelled domestic emissions pathways. The “Insufficient” rating indicates that the UAE’s climate policies and action in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow the UAE’s approach, warming would reach over 2°C and up to 3°C. The UAE’s policies and action rating has improved compared to our previous assessment for two reasons. First, the UAE’s newly published current policy scenarios (included in its LTS) lead to 17% lower emissions by 2030. This scenario includes a sectoral breakdown and detailed information at the measure level. This is a significant improvement compared to our previous current policy scenarios which were based only on the implementation of the Energy Strategy 2050. Second, the UAE’s 5 th National Communication to the UNFCCC also includes updated inventory data, which is 15% lower than our previous estimates, mainly due to differences in industrial process emissions and fugitive emissions. These also impact the absolute value estimated for the UAE’s 2030 emissions under current policies. The UAE’s LTS, published in 2024, includes targets and current policy projections for all major sectors of the economy, and detail both existing and planned measures to achieve them. While this is a significant step in transparency, it also shows that the UAE plans to rely heavily on carbon capture and storage (CCS) technologies especially after 2030 and towards its 2050 target, which undermines the credibility of its climate policies and targets.</t>
-  </si>
-  <si>
-    <t>According to our analysis, the US will need to implement additional policies to reach its targets. We project GHG emissions will reach between 4.6–5.4 GtCO 2 e in 2030 (excluding emissions from land use, land use change and forestry, or LULUCF). This is equivalent to 29%–39% reduction from 2005 levels (excl. LULUCF), which is insufficient to meet the NDC target (45%–50% excl. LULUCF). The Inflation Reduction Act (IRA), passed in 2022, represents a significant milestone in US climate policy. While its full impact is still unfolding due to the nature of its 10-year implementation plan, the first years have shown real promise. The IRA is mobilising historic investments in clean energy, driving clean projects, creating jobs, and attracting private sector funding. EPA standards for the power and transport sectors, passed in 2024, provide two further milestones in important policy areas. However, to achieve its domestic emissions reductions target—let alone to reach a 1.5°C-compatible emissions level—the government needs to complement its recent advancements with further sector-specific policies and a shift away from fossil fuels. The projected emissions trajectory range is wider in this update than previously, due to the incorporation of new analyses that better highlight the uncertainties related to the IRA's implementation. While the middle of the policy projections' range falls into the “Insufficient” category, its lower end, representing a positive outlook on the government’s current policies, falls into the “Almost sufficient” range. The “Insufficient” rating indicates that the US’ climate policies and action in 2030 need substantial improvements to be consistent with the 1.5°C temperature limit. If all countries were to follow the US approach, warming would reach over 2°C and up to 3°C. The Biden Administration has set the goal to decarbonise the power sector by 2035, which is consistent with a Paris Agreement pathway . Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
-  </si>
-  <si>
     <t>The CAT rates Japan’s policies and action against modelled domestic pathways as “Insufficient”. This rating indicates that Japan’s policies and actions in 2030 need substantial improvements to be consistent with limiting warming to 1.5°C. If all countries were to follow Japan’s approach, warming would reach over 2°C and up to 3°C. Further information on how the CAT rates countries (against modelled domestic pathways and fair share) can be found here .</t>
   </si>
   <si>
     <t>Under current policies, total emissions (excluding LULUCF) are still projected to grow significantly after 2022, namely by about 15% above 2022 levels by 2030, reaching about 405 MtCO 2 in 2030 (excl. LULUCF). In 2022, emissions in Argentina rebounded above 2019 levels after a sharp drop in 2020 due to COVID-19. This puts Argentina’s emissions projections under current policies at approximately 15% above its 2030 target. Our analysis of current policies is based on projections developed by the National University of Central Buenos Aires (UNICEN) (Blanco &amp; Keesler, 2022; Keesler &amp; Blanco, 2024). These projections include relevant policy developments up to 2022. Later developments, such as the power sector reforms, power subsidies reform and large fossil fuel investments proposed by the current government could have a significant impact on how emissions develop in the next few years, but are not yet reflected in our current emissions projections. According to UNICEN’s modelling results, if Argentina were to implement additional policies to scale-up low carbon energy sources and reduce energy demand, it could almost reach its NDC target (Blanco &amp; Keesler, 2022). This would require, reaching a carbon-free power grid by 2050, reaching 100% EV sales by 2050, and increasing energy efficiency. However, to be consistent with limiting warming to 1.5°C, Argentina would also need to speed up the achievement of those measures, plus develop more ambitious policies, especially to stop deforestation, and reduce livestock-related emissions. UNICEN also models a carbon neutrality scenario for Argentina’s AFOLU sector. This scenario shows the sector could become carbon neutral by 2050 by increasing the GHG efficiency of livestock production by 10%, reducing synthetic fertiliser use by 90%, increasing the collection of crop residues by 25%, reducing grasslands and forests burning by 90%, reducing deforestation by 90%, and increasing both commercial forestry and forest restoration. Critically, this scenario also includes the reduction of livestock for domestic consumption ‘following the trends of the latest years in domestic consumption’ (Keesler &amp; Blanco, 2024). Argentina’s energy sector is its biggest source of GHG emissions, reaching 174 MtCO 2 eq in 2020 (54% of the total). Total energy supply increased 81% between 1990 and 2021, and fossil fuels still account for around 89%, mostly gas (50%) and oil (36%). President Milei’s administration, which took office in December 2023, has substantially restructured Argentina’s national government, with a focus on reducing the size of the public administration, and cutting expenditure. In this process, the former Ministry of Environment has been reduced to the sub-secretary level, under the Secretary of Sport, Tourism and Environment (EcoNews Global, 2023). During his presidential campaign, President Milei stated he does not believe in man-made climate change and that his government would not support climate policies, including threats to leave the Paris Agreement (Colombo, 2023). More recently, his administration stated that Argentina will not be leaving the Paris Agreement, but the outlook looks bleak on increasing or even maintaining climate ambition in Argentina for the next four years (Spring, 2023). The new government plans to continue developing the Vaca Muerta fossil gas fields, as well as the fossil gas pipeline and the LNG terminal, both planned by the previous administration. To support these large investments, the government set out an incentive package called RIGI or Incentive Regime for Large Investments (KPMG, 2024). In January 2023, the government started negotiating contracts with oil and fossil gas producers at Vaca Muerta to ensure the future pipeline will work at capacity (Government of Argentina, 2022e). In June 2023, the fossil gas pipeline was finished ahead of schedule and began operations. It is expected to carry 11 mm3/d during 2023, and to reach 22 mm3/d in 2024, which represents around 15% of the country’s current consumption (Diamante, 2023). This has the potential to prevent Argentina from meeting its climate targets through higher upstream energy emissions as well as the lock-in effects of fossil fuel infrastructure. In July 2024, a compressor plant was installed to increase the carrying capacity of the pipeline by 5 m3/d, and a second section of the pipeline is still under construction (Government of Argentina, 2024d). During the second half of 2023 the Argentinian government produced three strategic climate policies: the National Strategy for International Climate Financing 2023, the National Strategy for the Use of Carbon Markets 2023 and the National Strategy for Sustainable Finance, 2023 (ENFS) (Banco Central de la República Argentina, 2023; Government of Argentina, 2023d; MECON, 2023). However, these are so far only high-level documents meant to structure future work on designing climate finance roadmaps and possibly a cap-and-trade system in the Argentinian power and industry sectors. It remains uncertain whether these policies will be designed and implemented by the Milei administration. In December 2022, the government published its new National Climate Change Mitigation and Adaptation Plan until 2030 (Government of Argentina, 2022d). This strategy was published shortly after Argentina submitted its Long-term Strategy to the UNFCCC, and reiterates both Argentina’s NDC and LTS targets, as well as expanding on many of the measures presented in Argentina’s Fourth BUR earlier in 2022. So far, the strategy seems to still be in place, but whether its implementation will continue during Milei’s administration is uncertain. The strategy includes detailed information on Argentina’s climate measures and targets covering all major sectors. Some highlights of this strategy include targets for the decarbonisation of the transport sector, incentives to increase energy efficiency in buildings, and measures to reduce food loss and waste. This strategy, however, does not include any new renewable energy targets or measures, and it does not include any significant measures to reduce emissions from the AFOLU sector, especially from livestock.</t>
   </si>
   <si>
+    <t>Although the government introduced several new policies towards the end of 2023 and throughout 2024, mostly in the power, transport and industry sectors, they were accompanied by continued support for both coal and fossil gas production for many decades to come. The ongoing revisions of historical and projected LULUCF estimates puts the government closer to meeting its emissions reduction targets without making meaningful emissions reductions across the economy. Australia’s policies and action are projected to achieve emission reductions between 17% and 21% below 2005 levels by 2030, excluding LULUCF. Under current policies, Australia’s total GHG emissions excluding LULUCF are projected to fall to 438 MtCO 2 e (446 MtCO 2 e in AR5 GWPs) by 2030. When also taking announced policies into account, emissions excluding LULUCF would fall to 417 MtCO 2 e by 2030 (424 MtCO 2 e in AR5 GWPs) by 2030. Slow progress towards 82% renewable energy The Capacity Investment Scheme, expanded in November 2023, is the government’s main instrument to bridge the currently significant gap to the 82% renewable electricity target (DCCEEW, 2023b; Open Electricity, 2024a, 2024b). This expanded CIS aims to deliver 32 GW of new clean energy capacity by 2030, comprised of 23 GW of variable renewable capacity and 9 GW of dispatchable capacity, such as battery storage. While not legislated, the 82% target is assumed in the government’s emission projections to apply to the nation’s four main grids (NEM, WEM, DKIS, NWIS), but not to other minor grids or off-grid generation. Under the government’s baseline projections, which excludes the expanded CIS, the share of renewables in Australia’s on-grid generation would reach 72% by 2030, largely due to solar and wind energy deployment (DCCEEW, 2023b). As of June 2024, renewables penetration of the National Electricity Market, Australia’s largest grid, stood at 38% (Open Electricity, 2024a). Although it is too early to assess the impact of the expanded CIS, Australia’s power sector cannot yet be considered on-track to meet its 82% renewable electricity target, nor is it on a 1.5°C-compatible trajectory. Investment in large-scale renewable generation stalled in 2023, with just AUD 1.5bn committed to new projects, substantially down from 6.5bn in 2022 (Clean Energy Council, 2024). The rollout of renewables in Australia continues to be obstructed by slow planning and environmental approval processes, higher costs, and tighter markets for equipment and labour. Coal power still accounted for nearly half of Australia’s total generation in 2023, while fossil gas accounted for 18% (DCCEEW, 2024a). There is no explicit emissions reduction policy for the electricity sector, nor a federal-level coal and fossil gas phase-out plan and timeline. Green industry In 2024, the government has unveiled new energy-related policy documents for the post-fossil fuel exports era. The ‘Future Made in Australia’ plan announced in 2024, allocates AUD 22.7bn (USD 14.9bn) over 10 years to attract investment in key industries and realise Australia’s potential to become a “renewable energy superpower” (Australian Government, 2024). The scheme is targeted at renewable hydrogen, green metals, low carbon liquid fuels, critical minerals processing, and clean energy manufacturing including battery and solar panel supply chains. The plan does not include support for fossil fuels. The government’s updated National Hydrogen Strategy, released in 2024, sets targets for both production and export of hydrogen (DCCEEW, 2024c). The strategy specifically targets renewable-based hydrogen, which is an improvement on the 2019 strategy which also encompassed fossil fuel-derived hydrogen. No end in sight to fossil fuels Nevertheless, the government has also reaffirmed its commitment to fossil fuel production and exports. In some of the most impactful decisions made by the Albanese government, the government approved three coal mine extensions in September 2024, allowing them to continue operating for another 30–40 years (ABC News, 2024d; The Guardian, 2024). These decisions will result in well over an additional billion tonnes of CO 2 being emitted to the atmosphere, on top of the four previous coal mining approvals issued in 2023 (The Australia Institute, 2024b). Australia remains a massive exporter of fossil fuels and, in 2023, was the world’s second-largest exporter of coal and third-largest exporter of liquefied natural gas (LNG) (Energy Institute, 2024). The government’s Future Gas Strategy, released in May 2024, doubles down on the role of gas in Australia’s domestic energy sector and exports to 2050 and beyond (DISR, 2024a). The strategy reinforces the government’s ongoing commitment to development of new fossil gas supply and continued LNG exports. The Safeguard Mechanism is the Australian government’s central policy for reducing industrial emissions by imposing declining baselines on large industrial facilities. In 2023, the 219 facilities covered by the mechanism emitted 139 MtCO 2 e (26% of Australia’s total emissions excluding LULUCF) (Clean Energy Regulator, 2024; DCCEEW, 2024i). The mechanism allows for unlimited use of offsets to meet declining baselines, creating uncertainty about actual emissions reductions that will be achieved and the effectiveness of the scheme. Alone the emissions from existing and committed LNG projects and all committed coal projects, which make up around half of Safeguard Mechanism facilities, would leave no room for other industries in the scheme, who would find themselves having to make additional steeper cuts to keep to the government’s set 100 MtCO2e limit ( Climate Analytics, 2023 ). The transport sector is projected to become the greatest source of emissions in by 2030, as power sector emissions decline (DCCEEW, 2023b). The government’s long-awaited New Vehicle Efficiency Standard (NVES) was introduced in 2024 and will apply to new cars sold from 2025 onward, making Australia one of the last developed countries to adopt such standards (DITRDCA, 2024). The standard sets emissions intensity targets imposed on suppliers across the fleet of vehicles they sell each year. The New Vehicle Efficiency Standard and the National Electric Vehicle Strategy, released in 2023, do not set a strategy or targets for public transport, cargo and modal shift, leaving a gap in the government’s transport sector policies.</t>
+  </si>
+  <si>
+    <t>In October 2022, Luiz Inácio Lula da Silva was elected president of Brazil for the third time, defeating former president Jair Bolsonaro. He assumed the presidency in January 2023, quickly moving away from the previous administration’s policies and reconstructing the country’s environmental policy which had suffered from budget cuts and policy rollbacks (Nature, 2023). Some positive policy developments can already be highlighted, including: Following the resubmission of its NDC in October 2023, the Inter-ministerial Council on Climate Change began reviewing the National Climate Change Policy (PNMC), which will now include sectoral mitigation and adaptation strategies covering the period up to 2035 as well as indicative sectoral targets for 2030 and 2035, a process that could take up to two years (Talanoa, 2023). Recent studies reported deforestation rates falling in response to political action (BBC, 2024; Global Forest Watch, 2024). A 36% drop in primary forest losses in Brazil in 2023 compared to 2022 levels was celebrated as an example of the effects of re-establishing law enforcement in the forestry sector. However, deforestation remains higher than in the early 2010s, with negative trends in some regions like the Cerrado where deforestation actually increased by 6% in 2023 (BBC, 2024; Nature, 2023) Brazil's presidency of the G20 summit in 2024 and hosting of COP30 in 2025 highlight its renewed engagement with the international community on environmental issues, signalling its commitment to shaping international climate policy. This is particularly relevant as 2025 will be the year when countries are mandated to submit updated and more ambitious 2035 climate targets under the Paris Agreement. The development of new policies such as the Ecological Transformation Plan (PTE) to promote sustainable development while reducing Brazil’s overall environmental footprint, and which includes energy transition as one of its six pillars of action (Government of Brazil, 2023d; Talanoa, 2023). However, there are still important and inconsistent elements in the new policy development that raise concerns about the prioritisation of sustainability and environmental goals within Brazil's infrastructure agenda, which cast serious doubt on the government's commitment to ecological transformation and transition away from fossil fuels (Nature, 2023), in particular: Brazil’s Novo PAC (a new USD 350bn growth acceleration programme designed to stimulate private and public investments in infrastructure, development and environmental projects) which assigned around USD 110bn (just over 30%) of its budget to “energy transition and security” while earmarking 63% of its budget for the oil and fossil gas industries, mainly for the production and development of these fossil fuels (Government of Brazil, 2023c, 2023e). The actions outlined under the energy transition pillar of the PTE focus mostly on reducing transport emissions by electrification or low-carbon fuels and further development of wind and solar energy; without concrete targets related to a transition away from fossil fuels. Brazil is yet to put forward a timeline for phasing out fossil fuels and questions remain as to how it will achieve an energy transition in a just and equitable way (Nature, 2023). Our calculations show Brazil’s total emissions (excluding LULUCF) will reach between 1,162 MtCO 2 e and 1,197 MtCO 2 e in 2030 under current policies, almost 25% above 2005 levels. Brazil is not on track to reach neither its 2025 target nor its 2030. To peak and then rapidly decrease emissions, as required in order to limit warming to 1.5°C, Brazil will need to sustain and strengthen policy implementation and accelerate mitigation action in all sectors— including a reversal of present plans to expand fossil fuel energy sources.</t>
+  </si>
+  <si>
+    <t>The speed and scale of Canada’s climate policy implementation does not match the urgency of the climate crisis and much more work is needed. Emissions in 2030 are projected to be 603 MtCO 2 e (excl. LULUCF contributions) or 20% below 2005 levels, lower than our last update, due to continued policy implementation, but a far cry from the 377–495 MtCO 2 e level Canada needs to reach to meet its updated NDC target. In March 2022, Canada released its latest climate change plan, building on earlier strategies released in 2016 and 2020 (Environment and Climate Change Canada, 2020a, 2022a; Government of Canada, 2016b). The measures outlined in the plan are not yet sufficient to ensure Canada meets its NDC target, nor have all been implemented yet. It came on the heels of a damning report in November 2021 by Canada’s Commissioner of the Environment and Sustainable Development outlining 30 years of the government’s failure to meet its targets and reduce greenhouse gas emissions (Commissioner of the Environment and Sustainable Development, 2021; Office of the Auditor General of Canada, 2021). Canada is developing additional policies which are captured in our planned policies scenario. Of the major initiatives (regulations for clean electricity, post-2026 LDV model year standards, oil and gas methane target, and landfill gas), only the EV sales mandate has been implemented since the government released its 2023 projections. Our current policy projection is based on these projections and modified to include the impact of the EV sales target. The step-up in climate action over the last four years was driven by a vulnerable minority Liberal Party government, enabled through support from the New Democratic Party. This progress risks being dialled back after the next elections, set for 2025, if the Conservatives were to come to power. They have already promised to ‘Axe the tax’, i.e. abolish the carbon pricing system. In preparation, the government has designated almost half of the CAD 15 billion (USD 11bn) in the Canada Growth Fund to be spent on Contracts for Difference or similar offtake agreements to ensure stability to investors in the coming months (Environment and Climate Change Canada, 2023a) Carbon pricing Mandatory carbon pricing has been in effect across Canada since 2019 (Government of Canada, 2018a). The legislation enacting the carbon pricing scheme, the Greenhouse Gas Pollution Pricing Act , was found to be constitutional by the country’s top court in March 2021 after three provinces challenged it (Supreme Court of Canada, 2021). A second challenge from the province of Manitoba was also dismissed by the Federal Court in October 2021. Under the scheme, all Canadian provinces and territories must have a cap-and-trade system or carbon tax in place. Jurisdictions without such systems or taxes will fall under the federal backstop. The federal system has two components: a regulatory charge on fossil fuels and an output-based pricing system (OBPS), which applies to major emitting industrial facilities. The federal government will review its carbon pricing benchmark in 2026. The initial carbon price of CAD 20/tCO 2 e was set in 2019 and increased by CAD 10 per year, reaching CAD 50/tCO 2 e in 2022. In its latest climate plan, the government stated it will increase the carbon price by another CAD 15 per year for the 2023–2030 period, reaching CAD 170/tCO 2 e in 2030 (around USD 125) (Environment and Climate Change Canada, 2020a; Government of Canada, 2021k). While the carbon price is heading in the right direction, it is still below the USD 170–290 (2015$) needed to be compatible with 1.5°C (Boehm et al., 2023). A 2022 audit of the scheme found the government had taken steps to address some of the scheme’s weaknesses, but that requirements for large emitters were poor and could be strengthened (Commissioner of the Environment and Sustainable Development, 2022a; Office of the Auditor General of Canada, 2022a). National GHG Offset System In June 2022, the federal government established a GHG Offset system for activities not covered by carbon pricing (Government of Canada, 2022e). Credits generated under the system can be used to reduce the compliance costs of industrial facilities covered by the OBPS. At present, the system only covers landfill methane recovery and refrigeration systems, but protocols are being prepared for forest management, livestock feed management, enhanced soil carbon, manure methane emissions and direct air carbon dioxide capture and sequestration (Government of Canada, 2022c). The ministry is also looking into ways to remove barriers and enhance participation in the system by Indigenous peoples (Government of Canada, 2022f).</t>
+  </si>
+  <si>
+    <t>Between 2010 and 2022, Chile’s emissions increased by 27%, from 88 MtCO 2 e to 112 MtCO 2 e, excluding LULUCF. When considering Chile’s current policies, we estimate that Chile’s emissions already peaked in 2021 at a level of 115 MtCO 2 e. According to our assessment, Chile’s emissions levels in 2030 under current policies will be between 100–108 MtCO 2 e/year (excl. LULUCF). Our analysis suggests that Chile will not meet its conditional nor unconditional NDC targets in 2030 under current policies, or be 1.5° compatible. Compared to our previous assessment, emissions under current policies have increased due to higher historical emissions than previously projected, a stronger rebound after COVID, and changes to the current policy assumptions. Chile’s key climate policies include the Energy Efficiency Law (Law 21.305/2021), a legal framework aiming to reduce energy consumption across the power, transport, buildings, and industry sectors. It also includes the coal phase-out, where all of Chile’s coal-fired units (28) are expected to retire or be retrofitted by 2040. An earlier coal phase-out could have a sizable impact on Chile’s current policy trajectory, but only if the coal capacity is replaced with generation from renewable energy sources. The CAT estimates that choosing to retrofit coal plants with gas could lead to at least 3 MtCO 2 e fewer in emission reductions in the short-term compared to retiring coal-fired units and using renewable electricity sources, and can lead to carbon lock-in risks and stranded assets. The Electromobility Strategy guides climate policy in the transport sector and sets out an action plan to electrify 100% of the urban public transport vehicle fleet by 2050 and ban the sale of new cars with combustion engines in 2035. Chile has also introduced a carbon tax (Law 20.780/2014), although its price is likely too low to result in emissions reductions. In June 2022, Chile passed the Framework Law on Climate Change (21455) (Congreso Nacional de Chile, 2022). It includes the 2050 GHG neutrality target and recognises the NDC target, making them legally binding. As a result, Chile now has a legal framework that assigns responsibilities and strengthens the legal and institutional basis for implementing climate change mitigation and adaptation policies across all sectors, and is moving towards a low emissions economy. It also presents a paradigm shift in Chile’s environmental policy, as climate action is now not only the responsibility of the environment ministry but is spread across 17 national ministries, as well as regional governments and municipalities, and even includes the private sector. While most of the important regulations outlined in the Framework Law on Climate Change have come into force, Chile has been delayed in implementing two new regulations and modifying two existing regulations (Peña, 2024). The regulation on its Article 6 framework is heading into its consultation stage, but there has been no movement on its related law outlining the requirements and verification method around the GHG emissions reduction or absorption certificates. The law also mandates the relevant ministries to develop sectoral mitigation plans by 2024, but no plans have yet been released (CR2 and Centro de Derecho Ambiental, 2024). Since our previous assessment, there have been no major changes to Chile’s climate policies. New laws to promote renewable energy and address critical barriers like a lack of transmission lines, such as the Law on Energy Storage and Electromobility and the Energy Transition Law, have been in the legislative process for a couple of years now. Chile has nevertheless made progress in that time, publishing new sectoral strategies to guide its short-term climate plans such as the Initial Agenda for the Second Phase of the Energy Transition, the Ministry of Energy’s Decarbonisation Plan, the Roadmap for the Advancement of Electromobility, as well as the Green Hydrogen Action Plan 2023-2030. Chile is on track with its 2040 coal phase-out plan, meeting its goal of retiring 11 plants by 2024, and has even accelerated its implementation. Nine of the remaining coal-fired units have currently committed to being retired or retrofitted between 2024 and 2025, although it is unclear whether the retirement or reconversion will be timely. However, the eight remaining coal plants have yet to make a firm commitment: it is still possible for them to continue operating until 2040. While there were some discussions in 2022 on adopting an even earlier, more ambitious phase-out date of 2030, this has not been mentioned in a while. To bring its current policies considerably closer to a 1.5°C trajectory, Chile could update its national commitment to phase out coal-fired power by 2030.</t>
+  </si>
+  <si>
+    <t>China’s current policies scenario projections have been updated to reach GHG emission levels (excl. LULUCF) of 13.8 to 14.6 GtCO₂e/yr in 2030 – roughly 29% higher than 2010 levels. The 14th FYPs aims to cut energy intensity by 13.5% and emissions intensity by 18% by 2025 from 2020 levels (Xinhua News Agency, 2021). However, progress from 2020-23 was minimal, with only a 2% drop in energy intensity and a 4.6% drop in emission intensity (Myllyvirta, 2024b). To ensure the achievement of its 14th FYP targets, the State Council sets its 2024 targets to reduce the energy intensity and emission intensity by 2.5% and 3.9% respectively (The State Council of the People’s Republic of China, 2024). China’s CO₂ emissions in the second quarter of 2024 dropped for the first time since the country reopened from its “zero-Covid” lockdowns in December 2022 (Myllyvirta, 2024a). This reduction was mainly driven by a surge in clean energy additions, reversing the growth of fossil fuel power. Despite cautious and conservative government reactions, it suggests that China’s CO₂ emissions may have already peaked in 2023. If not, they are likely to peak well before 2025, five years ahead of the 2030 target (Bloomberg News, 2024b). China achieved its 1,200 GW wind and solar capacity target six years ahead of schedule, reaching 1,206 GW in July 2024, with forecasts predicting 1,310 GW by year-end. (Bloomberg News, 2024d; CEC, 2024) China's reliance on fossil fuel consumption is a key factor driving global emissions. Despite having the world’s largest coal power pipeline, China reduced its coal plant permits by 83% in the first half of 2024, allowing only 9 GW, after permitting over 100 GW of coal power annually in 2022 and 2023 (CREA and GEM, 2024a; GEM et al. , 2024). This drop in new coal approvals doesn’t necessarily indicate an early coal peaking, as addressing the coal power projects permitted during the 2022-23 surge remains a significant challenge for China if it wants to peak emissions and avoid a costly coal lock-in. The government has introduced a "low carbon transformation" action plan. This plan aims to reduce emissions from existing coal plants through biomass co-firing, green ammonia co-firing, and CCUS technologies from 2025 to 2027 (NDRC and NEA, 2024a). While shifting away from coal is essential for achieving a 1.5-compatible power system, reducing emissions from coal plants that will remain in use for some time through technical improvements is still sensible. This approach will further raise the cost of coal-fired power, thus promoting renewable energy, especially as nearly half of China’s coal-fired power generators are operating at a loss even before accounting for costly new measures (Myllyvirta, 2024a). The draft of the Energy Law of the People's Republic of China was opened for public consultation at the Standing Committee of the National People's Congress (NPC) meeting on April 26, 2024. This will be China's first comprehensive law with a fundamental and overarching role in the energy sector, integrating various stand-alone energy laws and regulations, such as the Electricity Law, the Coal Law, the Energy Conservation Law, and the Renewable Energy Law. The Energy Law could be formally introduced within 2024 (Dai, 2024). Article 20 of Chapter 3 of the draft law explicitly supports the priority development of renewable energy, the rational development and clean, efficient use of fossil energy, and the orderly promotion of replacing fossil energy with non-fossil energy, as well as replacing high-carbon energy with low-carbon energy (NDRC and NEA, 2024b). Launched in 2021, China’s Emissions Trading Scheme (ETS) covers over 2,000 companies in the power sector, 40% of China’s total carbon emissions, and recorded over 24.9 billion yuan (USD 3.4bn) in total transactions in 2023. The ETS has thus far had minimal impact on CO₂ emission reduction, primarily due to a generous supply of allowances and the absence of a stringent emissions cap. New regulations on ETS management published in February 2024 significantly increased the punishment for non-compliance, data fraud and market manipulation behaviours (IKI, 2024). In July, China published new rules for public consultations, prohibiting participants in the Emissions Trading System (ETS) from borrowing allowances from future years and more strictly limiting the carrying over of unused permits from previous years (MEE, 2024). Beyond the power sector, China plans to expand its ETS to seven other high-emitting sectors covered by the European Union Carbon Border Adjustment Mechanism (CBAM) regulations. (Tan, 2022). China's industry sector is targeting electrification and efficiency improvements to meet demand and reduce reliance on fossil fuels. Steel, cement, and aluminium are the main drivers of emissions in the industry sector; all the subsectors have aligned with the economy-wide carbon peaking timeline before 2030 (MIIT of China, NDRC and MEE, 2022). The Special Action Plan for Energy Conservation and Emission Reduction in the Iron and Steel Industry, issued in June 2024, aims to reduce comprehensive energy consumption per tonne of steel by over 2% by the end of 2025 compared to 2023 levels (NDRC et al. , 2024).The national ETS has also announced to expand to include steel, cement, and aluminium by the end of 2024 (ChinaNews, 2024). The government is also taking decisive action to control capacity and production in the steel and cement sectors to address overcapacity and reduce emissions. As of August 23, 2024, all new steel plant permits have been indefinitely suspended, following an earlier policy of granting permits only for electric-powered steelmaking plants (MIIT of China, 2024). Carbon capture, utilisation and storage (CCUS) and the development of hydrogen solutions are on the radar of policymakers in China's harder-to-abate sectors for decarbonisation, although CCUS doesn’t lead to complete decarbonisation. The new "low carbon transformation" action plan for coal power plants highlights CCUS technologies as a key method for reducing emissions from existing coal plants from 2025 to 2027 (NDRC and NEA, 2024a). As the world's largest producer of hydrogen, China published its national hydrogen strategy and is targeting modest production of 100,000–200,000 tonnes of renewable-based hydrogen by 2025, which could reach 100 million tonnes by 2060 (Yao, 2022). To transition to a low-carbon transport sector, the government has spent decades prioritising new energy vehicles (NEVs) sales, including battery electric vehicles (BEVs), plug-in hybrid vehicles (PHEVs), and fuel cell electric vehicles (FCEVs). China dominates the global electric vehicle (EV) industry, having produced more than half of the EVs worldwide in 2023. This dominance is driving global EV development and intensifying pressure on European and North American companies to improve competence. In response, the EU, the US, and Canada have imposed additional tariffs on Chinese-made EVs to counter China's market and price advantages (Song et al. , 2024). China's domestic NEV market share reportedly exceeded 30% in 2023 (already exceeding the 20% target in 2025) despite ending NEV subsidies for producers in 2022; the government aims for a 40% market share by 2030 (Government of China, 2021; Xinhua News Agency, 2024). China has also been prioritising improving accessibility and electrification of its public transport systems, with the expansion of national high-speed rail and local electric public transport systems prominent in its COVID economic stimulus packages and latest FYPs. The government aims to expand its massive high-speed rail network from the current 45,000 km to approximately 70,000 km by 2035. It has also launched a pilot program for cities to procure around two million electric public vehicles before 2035 (O. Wang, 2022; CGTN, 2023). While China's real estate market is in a downturn, and investment in new construction projects is expected to slow down, the stock of projects under construction and the growing demand for higher living standards will still present challenges in terms of energy consumption and emissions in the building sector. To address this, the Chinese government has outlined targets in its 14th Five-Year Plan (FYP) for Building Energy Efficiency and Green Building and Implementation Plan for Carbon Peaking in Urban and Rural Construction (MoHURD of China, 2022; MoHURD of China and NDRC, 2022). The plan sets energy consumption caps in building operations, increases the energy efficiency of new buildings, and sets indicators for renovating existing buildings with efficiency measures and constructing ultra-low or zero-energy consumption buildings. The plans also contain indicators for increasing solar and geothermal applications to new buildings, raising the proportion of energy from renewable electricity, and reducing emissions intensity and energy intensity in residential and commercial buildings. China has increased efforts to expand its forestry and grasslands, in part due to their role in achieving the country’s carbon peaking and carbon neutrality targets. The government has implemented various domestic forest conservation and afforestation policies, and in the 14th FYP, it has set a target to plant 36,000 km2 of new forest annually until 2025 to increase the country’s forest coverage (NGFA of China, 2021). Internationally, China has increased its forestry pledge and signed the Glasgow Declaration on Forest and Land Use and separate joint agreements with the EU and the US on reducing deforestation. China is engaged in domestic discussions to include methane in its 2035 NDC updates. The long-awaited Methane Action Plan was published in November 2023 (State Council of China, 2023a), setting basic directions to control methane emissions across sectors as well as emphasising the establishment of a methane MRV system. However, the action plan does not specify any quantitative emission reduction targets or commitments. China finally ratified and started enforcing the Kigali Amendment in 2022 (Rudd, 2021). China reported that it halted new production capacity of five of the 11 HFCs it produces (covering 75% of total HFC production) two years ahead of the freeze requirements of the Amendment (McKenna, 2022). According to our analysis, China would reduce emissions by a modest ~50 MtCO₂e/year by 2030 under the Kigali Amendment’s phase-out schedule, although reductions could increase to almost 300 MtCO₂e/year by 2045.</t>
+  </si>
+  <si>
+    <t>The new government has inherited a challenging policy context. The final years of the previous government were marked by chronic delays to key delivery mechanisms, rollbacks to other essential climate polices, and a clear lack of commitment to reducing emissions at the pace and scale needed to align with the Paris Agreement’s long-term temperature goal. As a result, in July 2024, only 24–32% of the emissions cuts needed to reach the UK’s climate targets were covered by credible policy (CCC, 2024). The new government has highlighted that it wants to address this situation and close the implementation gap. It has already made a start on this, with some hopeful first signs including: In the power sector, where the government has set a target to achieve clean power by 2030. A decarbonised power sector by 2030 is a herculean endeavour, but would help unlock emissions cuts in other sectors, as clean electricity powers buildings, transport and industry. It would also demonstrate the viability of a clean power sector and rapid transition at scale, which could catalyse increased ambition in other countries and enable the UK to act as a global leader on power sector decarbonisation. To support this goal, the government has already lifted the de facto ban on onshore wind (DESNZ, 2024c) and secured record renewables capacity in the first auction after expanding the budget for renewables (DESNZ, 2024a, 2024d). In the buildings sector, the government has committed to double funding for energy efficiency improvements (Seddon, 2024), has signalled a willingness to enforce minimum efficiency standards in rental properties (DESNZ, 2024b) (a policy that was removed by the previous government), and has announced guidance on the next tranche of funding for retrofitting. However, this will not be enough to close the implementation gap. Much more will be needed, including: Ramping up renewables. The government’s commitment to clean power needs to be backed by a laser-focus on delivery. The latest renewable auction delivered record levels of renewables, including 5 GW of offshore wind. But this is still not enough to achieve clean power by 2030 – more needs to be done. Grids and storage will also be key to the power sector transition. Accelerating electrification. Removing policy costs from electricity bills would help incentivise industrial electrification and ensure that heat pumps truly cut consumer bills. Specific policies to incentive industrial electrification are also needed, and planning barriers to heat pumps and electric vehicle charging points need to be removed. Reversing recent rollbacks . The previous government exempted 20% of houses from the fossil-fuelled boiler ban, and delayed the ban on petrol and diesel vehicle sales to 2035. These policy rollbacks should be reversed.</t>
+  </si>
+  <si>
+    <t>Saudi Arabia has done little to decarbonise its economy. We expect its emissions to rise to 800–830 MtCO 2 e in 2030, a 15–­19% increase from 2021 levels. It remains difficult to assess whether Saudi Arabia’s current policies reach its NDC target, given the significant uncertainties around its target (see details in the Assumptions section ). Saudi Arabia’s energy sector remains dominated by fossil fuels, which represented almost 100% of the total energy supply in 2022 (IEA, 2023b). The Saudi government expects the overall demand for energy, including for oil and fossil gas, to continue increasing until 2030 and beyond (KAPSARC, 2021). Saudi Arabia’s “Vision 2030” aims to diversify its economy beyond oil, which accounted for around two thirds of total budget revenues in 2022. However, the government clearly has no intention to phase out fossil fuels. Saudi Arabia is betting on carbon capture and storage (CCS) technologies as a smokescreen to continue expanding oil and gas production. While Aramco abandoned its plan to increase oil production capacity to 13 million barrels per day (mb/d) by 2027, this decision appears largely driven by strategic considerations rather than a commitment to phase out fossil fuels. This reversal reflects changes in the global oil market, including slowing demand growth and increased production from non-OPEC countries, particularly the U.S. Even if Saudi Arabia were to reach its 50% target for renewable energy in the electricity mix, we project that emissions would still rise to 730–770 MtCO 2 e by 2030. Despite its vast solar energy potential, Saudi Arabia has only installed about 2.7 GW of renewable energy capacity as of 2023, generating around 1% of total electricity (IRENA, 2024b). Carbon crediting schemes In 2022, Saudi Arabia’s sovereign wealth fund, the Public Investment Fund (PIF), and the Saudi Stock Exchange Tadawul set up a voluntary carbon market in the Middle East and North Africa. The first auction in November 2022 offered one million tonnes of carbon credits (Bloomberg, 2022). Saudi Arabia has also announced the launch of a domestic carbon crediting scheme in early 2024, which will purportedly enable companies to offset their emissions by buying credits compliant with Article 6 of the Paris Agreement. The scheme appears to be voluntary, project-based and covers all sectors (Carbon-Pulse, 2023; Kingdom of Saudi Arabia, 2024). Despite the apparent focus on companies procuring credits, Saudi Arabia also appears to plan on using the credits to meet parts of its national climate pledge, including its 2060 net zero target. Based on the information published as of November 2024, it is unclear how this could work in practice in a manner that avoids both a company and the government from claiming rights to the same emission reductions ("double counting") – an outcome that would undermine the integrity of the credits, and potentially lead to an overall rise in emissions. The establishment of a voluntary carbon market in Saudi Arabia should complement and not serve to distract from - or displace - critically-needed domestic mitigation efforts. Information on how the Kingdom intends to use its carbon crediting scheme remains unclear or lacks details, and presents major risks that it will seek to use carbon credits with questionable integrity as a smokescreen to justify continuing its trajectory of maintaining high levels of domestic emissions. For more information on the role of voluntary carbon markets under the Paris Agreement and their associated risks, see Fearnehough et al. 2020 .</t>
+  </si>
+  <si>
+    <t>According to our current policy emissions pathway, Singapore’s GHG emissions dipped in 2020 due to the economic impact of COVID-19 and will steadily rise in the coming years, reaching 56-57 MtCO 2 e in 2030. Although Singapore’s emissions continue to grow, we project that emissions will be lower in 2030 than its latest NDC target, making a compelling argument for Singapore to raise its level of ambition in its forthcoming NDC. A more ambitious target would demonstrate the government’s commitment to contributing its fair share to global climate change mitigation. A Future Energy Fund, with an initial reserve of SGD 5bn, was announced in the 2024 budget and aims to support Singapore’s transition to cleaner fuels (CNA, 2024). As part of this announcement, Singapore’s Deputy Prime Minister, Lawrence Wong, highlighted both Singapore’s strategy to import low carbon electricity as well as its National Hydrogen Strategy, released in 2022. Singapore has an opportunity to take regional leadership in the green hydrogen space by becoming a regional hub of storage, trading, and transportation of green hydrogen for other Asian countries (Somani, 2022). The government introduced a carbon tax in 2019, initially set at SDG 5/tCO 2 e (USD 4/tCO 2 e). The carbon tax was increased to SGD 25/tCO 2 e (USD 19/tCO 2 e) from 2024 and will be increased to SGD 45/tCO 2 e by 2026-2027, with a target of reaching SGD 50-80/tCO 2 e (USD 38-60/tCO 2 e) by 2030 (National Climate Change Secretariat, 2024a; World Bank, 2023a). The tax currently applies to around 50 facilities in in the manufacturing, power, waste and water sector, and covers 80% of Singapore’s total GHG emissions (National Climate Change Secretariat, 2024a). In 2023, the government released an eligibility list for international carbon credits, which companies are permitted to use to offset up to 5% of the carbon tax liability (National Environment Agency, 2023). Despite the fivefold increase in 2024, Singapore’s carbon price is still significantly lower than those in Europe and Canada (The World Bank, 2024). The IPCC Working Group III indicates that under 1.5°C pathways, the marginal abatement cost of carbon in 2030 is about USD 220/tCO 2 in 2015 terms or USD 281/tCO 2 in 2023 terms (IPCC, 2022; World Bank, 2023b). This is 5-7 times higher than Singapore’s intended 2030 carbon price, which equates to USD 38-60/tCO 2 in 2023 terms. Although, pricing carbon needs to be understood in terms of national context, there is a large difference between Singapore’s price and the IPCC 1.5°C pathway range. A carbon tax can encourage more renewable energy in place of fossil fuel energy through changes in relative prices. However, a higher carbon price would need to be implemented earlier, to shift incentives enough to set emissions on a downward trajectory, compatible with the Paris Agreement (Carbon Market Watch, 2017; Warren, 2014). Singapore’s mitigation strategy is based on three areas: increasing energy and carbon efficiency, reducing carbon emissions in power generation, and developing low-carbon technology (Ministry of the Environment and Water Resources, 2016). Improving energy efficiency across the economy is the backbone of Singapore’s mitigation strategy. In its latest National Climate Action Plan (Ministry of the Environment and Water Resources, 2016), the government listed a number of policies to improve energy efficiency across all sectors, including an Energy Conservation Act, Green Mark Certification and Energy Labelling schemes, and home appliances Energy Performance Standards, among others. The Government has implemented a target of 80% of buildings to be certified green buildings by 2030. As of 2022, 55% of buildings have met this standard (Building and Construction Authority, 2023).</t>
+  </si>
+  <si>
+    <t>The CAT estimates South Africa’s emissions under current policies are on track to reach 462–502 MtCO 2 e excluding LULUCF by 2030, equivalent to 7–14% below 2010 levels excluding LULUCF. Under these current policy projections, South Africa’s emission levels in 2030 will be above the upper bound of the updated NDC target range for the same year (around 25–65 MtCO 2 e higher). The range of our latest projections have decreased slightly compared to our previous projection from September 2022. This is due to a slight revision of historical data using the latest government reported inventory data for 2007 to 2020 and updated estimates of 2021 from PRIMAP (see ‘Assumptions’ section ) (DFFE, 2023; Gütschow &amp; Pflüger, 2023). We further estimate that emission levels could decrease to as low as 404 MtCO 2 e excluding LULUCF by 2030 if South Africa were to implement its planned policies, including the expansion plans for the renewable electricity procurement, the accelerated switch to low-carbon mode of transport, energy efficiency measures, and the carbon tax. Under these planned policies projections, South Africa would reach the upper bound of its 2030 NDC target range. These findings emphasise the emissions reduction potential of a stringent implementation of proposed economy-wide and sector-specific policy measures. Recovery response to the COVID-19 pandemic The COVID-19 pandemic has exacerbated South Africa’s health, social and economic challenges. After an economic downturn of 6% of GDP in 2020, the International Monetary Fund reported a recovery of 5% of GDP in 2021 (IMF, 2023b). Economic recovery was dampened in 2022 due to the global fallout of Russia’s invasion of Ukraine, more frequent and prolonged power outages and severe floods (IMF, 2023a). The CAT estimates a drop in emissions in 2020 of 6% below 2019 levels due to a drastic slowdown of domestic economic activity and international trade. The CAT estimates a 1% uptick in emissions between 2020 and 2021. The South African government introduced several support programmes in direct response to the immediate COVID-19 crisis and released a ‘Economic Reconstruction and Recovery Plan’ in October 2020 (Government of South Africa, 2021a; IMF, 2020). The plan comprised a range of both low-carbon and high-carbon recovery measures. High-carbon measures included the procurement of emergency electricity capacity in a technology-neutral auction, several measures to promote mining operations without specific conditions for low-carbon operations, and promotion of its liquefied petroleum gas (LPG) infrastructure. Low-carbon measures included further support for energy efficiency retrofits and promotion of low-carbon urban public transport. A tracking tool published in 2021 indicates the South African government has spent only around 3% of all recovery spending totalling USD 2.5bn on deliberately low-carbon measures (Global Recovery Observatory, 2021). South Africa’s response to the COVID-19 pandemic overall stands in contrast to domestic and international calls for a ‘green’ and low-carbon economic recovery (Climate Action Tracker, 2020; IEA/IMF, 2020). Recent developments on cross-sectoral policies In October 2023, South Africa’s National Assembly approved the Climate Change Bill, which would still need approval from the National Council of Provinces and the President (Centre for Environmental Rights, 2023; Republic of South Arica, 2023). The draft Climate Change Bill was originally released in June 2018 for public consultation and only formally introduced to Parliament in February 2022 (Government of South Africa, 2021c, 2022a). If passed, the Bill would be a significant step forward for South Africa, making its NDC legally binding. Under the legislation, the Minister responsible for Environmental Affairs together with the Ministerial Committee on Climate Change established by the Bill would have to set sectoral emission targets for each GHG emitting sector in line with the national emission target every five years and carbon budgets would be allocated to significant GHG emitting companies. Carbon budgets would put a cap on emissions and make it mandatory for companies to constrain their emissions. However, the Bill has been criticized for relying on intended measures by the National Treasury to levy fees for those who emit in excess of their set carbon budgets, allowing emitters to “pay to pollute” (Centre for Environmental Rights, 2023). South Africa adopted a carbon tax in February 2019 covering fossil fuel combustion emissions, industrial processes and product use emissions, and fugitive emissions such as those from coal mining (Climate Home News, 2019; Reuters, 2019). The tax was implemented in June 2019 (KPMG, 2019). Recent analysis indicates that the carbon tax currently does not effectively contribute to emission reductions given the low levy in comparison with other carbon prices, generous basic allowance and other available exemptions such as the use of offset credits (Szabo, 2021). A basic tax-free threshold for around 60% of emissions and additional allowances for specific sectors would result in tax exemptions for up to 95% of emissions during the first phase originally planned to go until 2022. While the full carbon tax rate is proposed to be R120/tCO 2 e (US$ 8/tCO 2 e), after exemptions, the effective tax rate is expected to be between R6–48/tCO 2 e (US$ 0.4–3/tCO 2 e) (KPMG, 2019). While the South African government adjusted the carbon tax rate before exemptions slightly upward to R144 (US$9 /tCO 2 e) as of January 2022, the first phase of the carbon tax roll-out will be continued until 2025 (KPMG, 2022; Steenkamp, 2022). The government further plans to reach a carbon price of US$ 30/tCO 2 e by 2030 and US$ 120/tCO 2 e by 2050. The Carbon Tax implementation will be accompanied by a package of tax incentives and revenue recycling measures to minimise the impact of the first phase of the policy (up to 2022) on the price of electricity and energy intensive sectors including mining, iron and steel (EY, 2017, 2018). In June 2022, the Presidential Climate Commission released its framework for a Just Transition in South Africa after extensive stakeholder consultations (Presidential Climate Commission, 2022). The framework aims to inform policy making at the nexus of climate and development issues in South Africa to enable deep, just, and transformational shifts. International partnership to support just transition in the energy sector At COP26, South Africa, France, Germany, UK, USA and the EU made a political declaration to establish a long-term partnership to support South Africa’s pathway to low-emissions and climate resilient development. The partners resolved to mobilise an initial USD 8.5bn in grants, concessional loans, guarantees, private investments, and technical support in the first five-year period between 2023-2027 to accelerate the decarbonisation of South Africa’s electricity system to achieve the most ambitious NDC target, support a just transition that protects vulnerable workers and communities, and support green industrialisation, including green hydrogen and low-carbon transport technologies (Farand, 2021; Government of South Africa, 2021d). The South African Just Energy Transition Partnership (JETP) builds on a country-led, donor-supported process by the South African government, putting a distinct focus on a just transition, including retraining and supporting coal workers. In November 2022, the Government of South Africa presented the Just Energy Transition Investment Plan (JET IP) for 2023 to 2027 (The Presidency of South Africa, 2022). The vast majority of the USD 8.5bn is planned for the electricity sector (USD 7.7bn), with USD 6.9bn going to electricity infrastructure. The JET IP indicates transmission and distribution infrastructure will be prioritised to enable the uptake of renewables and leverage large-scale private sector investment in renewables. Outside the electricity sector, USD 200m is tagged for “new energy vehicles” (NEVs), with a focus on battery electric vehicles, and USD 700 m will go to green hydrogen. The JET IP estimates the total financing needs of the low-carbon transition at USD 98.7bn. A more comprehensive implementation plan is expected to be launched in November 2023. However, uncertainty remains on the timeline for coal plant retirements amid the energy crisis, and many have raised concerns on the implementation of promised retraining for impacted coal workers (Civillini, 2023; Molelekwa, 2023). There is also concern that the plan could add to South Africa’s already significant debt burden, with only about 4% of the USD 8.5 bn provided as grants (Civillini, 2023; The Presidency of South Africa, 2022).</t>
+  </si>
+  <si>
+    <t>Switzerland’s emissions decreased from 45 MtCO 2 e in 2021 to 41 MtCO 2 e in 2022, 25% below 1990 levels. The decrease from 2021 to 2022 was mainly driven by a lower demand for gas and heating fuel in the building sector due to the warmer than average winter and subsequently lower need for space heating. The new Federal Act on a Secure Electricity Supply with Renewable Energies (Bundesgesetz Über Eine Sichere Stromversorgung Mit Erneuerbaren Energien, 2024), approved in a June 2024 referendum, greatly impacts emissions projections under current policies, potentially leading to emissions levels as low as 28 MtCO 2 e (excluding LULUCF) by 2030. This projected reduction is equivalent to almost 50% reduction below 1990 levels (excluding LULUCF). Switzerland would therefore meet its estimated domestic target of a 30% to 33% reduction in emissions below 1990 levels under current policies and would get very close to meeting its overall NDC of a 50% reduction below 1990 levels through even without the use of carbon credits from international mechanisms. CO 2 Act The CO2 Act is the key policy addressing emission reductions in Switzerland. To implement the Paris Agreement in Swiss legislation, an amendment of the CO 2 Act (known as Total Revision) was drafted to make the 2030 NDC target legally binding (Schweizer Parlament, 2020). However, the Act was rejected in a public referendum in 2021, forcing Switzerland to extend its expired and unambitious CO 2 Act to 2024 and start a process of drafting a new amendment. A new amendment of the CO 2 Act (known as CO 2 Succession Act) was subsequently presented and accepted by parliament in March 2024. This version, however, includes substantially weaker provisions than the original, and all draft versions appear to have decreased in ambition in every round; i.e. there is no longer a clear domestic emissions reduction target, and all bans were removed from the original text. Besides the 2030 target, the Act includes measures across various sectors including buildings, transport, industry, and aviation. It also covers climate adaptation support, support for companies exposed to the emissions trading system, and cleaner energy technologies like biogas and renewable fuels (Bundesgesetz Über Die Reduktion Der CO 2 -Emissionen (CO 2 -Gesetz), 2024). As this piece of legislation is still open for public consultation and amendments, and will only come into effect in 2025, it is not yet included in current policy calculations. Climate Protection Act On 18 June 2023, the Swiss people accepted another important piece of legislation in a public referendum, the Federal Act on Climate Protection Objectives, Innovation and Enhancement of Energy Security (the Climate Protection Act). It enshrines the net-zero emissions target for Switzerland by 2050 in law and sets interim and sectoral targets. The Climate Protection Act also promotes innovation by providing support for companies to achieve their net zero target, addresses energy security through a programme that funds the replacement of fossil-fuel and electric resistance heating systems and covers adaptation support. The Act, however, is mainly a framework law, mandating the parliament to work out more concrete objectives and measures to meet the 2040 and 2050 sectoral targets. The Federal Act on a Secure Electricity Supply with Renewable Energies (see below) is set out to address this to some extent. Carbon Levy (CO 2 tax) Switzerland introduced a carbon levy charged on fossil fuels in 2008, which covers ~35% of CO 2 emissions. The fee was repeatedly raised over time, culminating at CHF 120 per tonne of CO 2 (USD 130) in 2022, making it the highest CO 2 levy in Europe (Swiss Broadcasting Corporation, 2021) (Alex Mengden, 2024). The CO 2 Succession Act proposes to avoid many taxes altogether in favour of tax incentives and funding instruments in the transport, buildings, and industry sectors. The emphasis of Swiss climate policy is increasingly focussing on incentives rather than bans and restrictions, in order to avoid more rejection at the ballot, which means it includes some exemptions to the CO 2 levy, including plant operators that commit to reducing emissions by 2040. The majority of the proceeds from the levy are reimbursed to the citizens, or they flow into the (new) buildings programme and the economy. In 2023, the total revenue from the levy was around CHF 1.1 bn (USD 1.3 bn), of which roughly two thirds was redistributed to the population and the rest to the economy (Bundesamt für Umwelt BAFU, 2024a) Emissions Trading Scheme Another cross-sectoral instrument influencing greenhouse gas emissions is Switzerland’s emissions trading scheme (ETS). Companies participating in the ETS are excluded from an obligation to pay the emissions levy. After linking with the EU ETS in 2020, the price of Swiss emissions allowances broadly aligned with the higher EU allowance prices, which will accelerate emission reductions by the emitters responsible for a third of emissions resulting from the combustion of fossil fuels (EEX, 2019; Swiss Federal Audit Office, 2017). In November 2019, the Federal Council expanded the scope of the Swiss ETS to include civil aviation and fossil-thermal power plants (ICAP, 2020). ECHR Ruling In November 2020, a group of senior women in Switzerland filed a case against the Swiss government at the European Court of Human Rights (ECHR), claiming that inadequate climate policies threaten their health and violate their rights to life and private life. The court ruled in April 2024 that Switzerland had failed to protect these rights from climate change impacts and lacked an effective regulatory framework to meet emission targets, marking an unprecedented application of human rights law in climate litigation. Despite this landmark ruling, in June 2024, the Swiss parliament rejected the ECHR's decision, arguing that the country already has an effective climate strategy and the Swiss government subsequently also dismissed the court's findings in August 2024, asserting that its climate policies are adequate and have been bolstered by recent legislation. Environmental groups criticised this dismissal, arguing that Switzerland's plans do not sufficiently address the urgent need to limit global warming to 1.5°C. The CAT echoes these concerns, indicating that while some progress is being made, Switzerland still falls short of meeting the standards set by the ECHR ruling (Domhnall O’Sullivan, 2024; Imogen Foulkes, 2024; Sabin Center for Climate Change Law, 2024).</t>
+  </si>
+  <si>
+    <t>A key feature of Turkish policy planning involves reducing its reliance on fossil fuel imports. In 2022 alone, Türkiye’s net energy trade deficit was USD 81 bn, placing a burden not only on its economy but also leaving it vulnerable to volatile commodity markets and geopolitical shifts (Türkiye Cumhuriyet Merkez Bankası (Central Bank of the Republic of Türkiye), 2023; Ugurtas, 2022). Increasing energy independence is therefore a strategic goal of the Turkish government, with diversification of the energy mix central to government policy. Managing energy demand is a first step to reducing reliance on imported fossil fuels. The energy intensity of Türkiye’s economy is low and decreased by a further 6.2% in 2022 compared to the previous year (Republic of Türkiye Ministry of Energy and Natural Resources, 2024b). However, it is also the fastest growing energy consumer in the OECD (Republic of Türkiye Ministry of Foreign Affairs, 2022). Through its 2030 Energy Efficiency Strategy and Action Plan, Türkiye aims to reduce energy consumption by 16% by investing USD 20 bn in energy efficiency projects (Republic of Türkiye Ministry of Energy and Natural Resources, 2024b). If realised, these investments could allow Türkiye to decouple energy consumption from economic growth and reduce dependence on imported fossil fuels. Türkiye intends to have 120 GW of installed wind and solar capacity by 2035. Along with hydropower and biomass, Türkiye’s installed renewable capacity in 2035 will be 160 GW (Republic of Türkiye Ministry of Energy and Natural Resources, 2024c; Turkish Ministry of Energy and Natural Resources, 2022). Meeting the wind and solar targets will involve bringing at least 7.5–8 GW online every year, significantly more than what was envisioned in Türkiye’s 2022 National Energy Plan. However, implementation will need to shift up a gear, as the country is struggling to meet even its National Energy Plan’s targets due to a slower than planned renewables rollout. For instance, 2023 saw the least wind capacity in 13 years added to the grid. Regularity changes including streamlining the permitting process and improving investment conditions are intended to stimulate private investment in renewable energy projects. Despite the improved commitment to renewables, Türkiye is yet to commit to a phase-out plan for coal or fossil gas, which need to be taken out of the energy mix in the 2030s if Türkiye is to align with the 1.5°C temperature goal (Robins, 2023; Turkish Ministry of Energy and Natural Resources, 2022). Instead, Türkiye plans to become a fossil gas hub and expand coal capacity (Robins, 2023; Turkish Ministry of Energy and Natural Resources, 2022). If Türkiye is serious about its net zero emissions target, then it will need to introduce a plan to phase out fossil fuels. The most significant piece of industrial policy of the last year has been the introduction of an Emissions Trading System (ETS) in line with the EU’s ETS. This will likely be the backbone of emissions reductions in Türkiye’s industry sector and will help mitigate some of the more severe impacts of the EU’s Carbon Border Adjustment Mechanism (CBAM). CBAM will levy a carbon tax on some product groups imported into the EU if they fail to align with EU emissions standards (European Commission, 2024). Ramping up production of Türkiye’s domestically produced electric vehicle (EV), the Togg, and high-speed electric trains forms an important part of Türkiye’s industrial strategy which can support domestic uptake while opening a new revenue stream from exports. Türkiye also plans to invest USD 298 bn up to 2053 in the transport sector. Sectoral targets include increasing the share of rail in passenger transport to 5.31% and to 20.12% in freight transport by 2035, up from 2019 levels of 0.89% and 3.13%, respectively (Republic of Türkiye Ministry of Transport and Infrastructure, 2023).</t>
+  </si>
+  <si>
+    <t>The CAT estimates the UAE’s 2030 emissions under current policies are set, in a best case scenario, to plateau close to 2022 levels, at around 214 MtCO 2 e, or continue to increase to about 259 MtCO 2 e. Under current policies, the UAE is set to miss its latest 2030 emissions reduction target. To meet its 2030 NDC target, the government needs to implement more ambitious policies and reduce its 2030 emissions by a further 15–40%. However, if the UAE implements the planned policies outlined in both its NDC and LTS, it could potentially reach its target. For more information, please see the Assumptions tab. Since 2023, the UAE has published information on many relevant climate policies across all sectors of the economy. Both its NDC from 2023 and its LTS from early 2024 provide details on policies and action, both current and planned, in the power, industry, transport, buildings, agriculture and waste sectors (Government of the UAE, 2023a, 2024b). This is a significant step in transparency, which allows for a better understanding of how the UAE plans to reduce its emissions to meet its NDC and net zero targets. However, it also shows a critical overreliance on carbon capture and storage both in the power and industry sectors, a smokescreen allowing the country to continue expanding its oil and fossil gas production and use while claiming to be on the way to net zero. In recent years, the UAE has announced plans to invest in renewables both at home and abroad, including a USD 100bn commitment together with the United States (Associated Press, 2023). However, in parallel it continues to invest into fossil fuel production. The UAE is planning to significantly increase its oil production in the next years, and is pushing to reach “gas self-sufficiency”, with major investments in offshore gas production. In November 2022, ADNOC announced a USD 150bn investment plan to expand its oil and gas business in the next five years (The Guardian, 2023). As part of this plan, ADNOC awarded contracts worth USD 17bn in October 2023 for the Hail and Ghasha Offshore Development project. This project aims to produce 1.5 billion standard cubic feet per day (bscfd) of gas before the end of the decade (Reuters, 2023). For more details, see the Power sector section below. The developments and the investment going towards new fossil fuel infrastructure are not consistent with limiting global warming to 1.5°C, instead are likely to lock the UAE into a high-emissions trajectory and undermine its transition towards renewable energy. Instead of ramping up its gas production towards self-sufficiency, the UAE should set out an ambitious plan to phase-out its dependency on gas for electricity and switch to renewables, which would reduce prices and price volatility for consumers, and avoid the risk of stranded assets (CAT, 2022).</t>
+  </si>
+  <si>
+    <t>The US will need to implement additional policies to reach its 2030 and long-term targets. After an increase in GHG emissions between 2021 and 2022, emissions started to decline in 2023 (-1.9%) (Rhodium Group, 2024). The government has set a target to reduce emissions by 3.8–4.2 GtCO 2 e/year in 2030. According to our projections, emissions are forecasted to decline at an average of 1.7%–3.9% per year and reach between 4.6–5.4 GtCO 2 e/year by 2030 (29%–39% below 2005 levels; and 19%–31% below 1990), excluding emissions from land use, land use change and forestry (LULUCF). Under these projections, the US would achieve 64%–87% of its emissions reductions target in 2030, indicating a gap of 13%–36% that would need to be filled with new and additional climate policies and action. As it stands, the 2030 target is not 1.5˚C compatible. Reaching a level in line with a global least-cost pathway requires further reductions of 1.4–2.2 GtCO 2 e below the current policy pathway. Compared to CAT projections in August 2023, our range of emission projections includes an updated estimate of the Inflation Reduction Act’s (IRA) impact, as well as estimates of the impact of the US Environmental Protection Agency’s (EPA) 2024 regulations for the power and transport sectors. As a result, the US emissions projections decreased relative to the CAT’s previous projections, while the range, based on existing policies, widened for 2030–2035. The upper bound decreased by 2% and the lower bound decreased by 8%. The reduced, widened range in emission projections highlights the continued effort by the US government to cut emissions, while recognising the high uncertainty of policy outcomes; especially for the government’s flagship climate policies, including the IRA and the Bipartisan Infrastructure Law (BIL). The IRA injects USD 370bn into the US economy over a 10-year period. This infusion takes the form of tax credits, grants, and loans intended to develop and deploy the clean energy technologies and investments that are essential for the economy's decarbonisation (The White House, 2023a). Since the IRA's implementation in 2022, the country has witnessed a significant surge in public and private investment in clean energy projects and infrastructure: between August 2022 and February 2024, investment in announced clean energy projects and infrastructure totalled USD 352bn. Specific highlights include record investment in battery and electric vehicle (EV) manufacturing and in grid and transmission infrastructure (Climate Power, 2024c). Due to these investments, the share of clean energy investments in total investments increased from 3.7% in Q4 of 2022 to 5% in Q4 in 2023, representing a significant uptick in the role that clean energy investments play in the US economy (Rhodium Group; MIT CEEPR;, 2024). Given the scale of public investment, some studies suggest that the IRA could spur USD 3tn in private investments over the coming decade (Goldman Sachs, 2023). The BIL and IRA, alongside the Creating Helpful Incentives to Produce Semiconductors (CHIPS) and Science Act, have set the stage for record private investment in the construction of domestic manufacturing facilities (U.S. Department of the Treasury, 2023b). Before the IRA and CHIPS Act were signed, annual investment in manufacturing construction remained below USD 150bn. Since the acts’ passage, investment surged to an all-time high of USD 223bn by February 2024 (FRED Economic data, 2024; Joint Economic Committee, 2024). Investment in the EV supply chain, especially in battery cell manufacturing and critical mineral production, has increased significantly and accounted for nearly two-thirds of all clean manufacturing investments by the end of 2023 (Rhodium Group; MIT CEEPR;, 2024). As a result of this increase in investment, the US surpassed the EU in battery cell manufacturing capacity in 2023, even though the EU’s capacity was two times larger than the US’ capacity in 2021 (Delgado et al., 2024). These investments contribute to job creation, with estimates showing that the IRA’s provisions have already generated over 270,000 clean energy jobs (Climate Power, 2024b). The act has also contributed to a more just energy transition by targeting disadvantaged communities and rural areas. Many of the announced investments specifically target and aim to contribute to the economic development of these regions and communities (U.S. Department of the Treasury, 2023a). In early 2024, the US expanded its climate policy portfolio through the addition of several EPA policies (U.S. Environmental Protection Agency, 2024i, 2024l). The EPA introduced several standards for gas and coal-fired power plants and updated its vehicle emissions standards. Even though these standards were watered down before their finalisation (see Electricity generation and Transport sections below), they add an important regulatory complement to the incentive-based IRA: by setting yearly emissions levels for technologies, the standards provide important guidance for the private sector. To realise its 2030 and 2035 targets and to align with the Paris Agreement’s 1.5˚C temperature goal, the US has to implement further, more ambitious policies and measures. Additional measures could focus on those sectors in which ambitious action has yet to be taken, such as the building or agriculture sector. At the same time, the government can further strengthen existing policies across all sectors; for example, the government could extend the IRA beyond 2030, introduce coal phase-out targets for 2030, and enhance energy efficiency standards (America Is All In, 2024). Manufacturing capacity could also be strengthened, in particular for wind turbine and heat pump production (IEA, 2024a). Given that the federal government’s jurisdiction is limited some policy areas, state governments can play a significant role. Some states, such as Massachusetts, Michigan, and Minnesota, have recently introduced climate policies that are more ambitious than at the federal level (Joselow &amp; Montalbano, 2023). To advance climate action at the subnational level, state governments can adopt of renewable portfolio standards (RPS) and introduce sales targets for EVs. Despite the IRA’s remarkable measures to support clean energy and address climate change, the IRA includes several concessions to the fossil fuel industry. The concessions are described in the Power section.</t>
+  </si>
+  <si>
     <t>Since it came into power in December 2021, the German government has been significantly accelerating domestic climate policy implementation, but remains deeply divided on the general approach, reflecting the divergent positions of the different coalition parties. We observe that the Green Party is pushing for fast action, e.g. in buildings and for renewables, the Social Democrats and, in particular, the Liberal Party are delaying implementation. All parties support expansion of LNG terminals, which is counterproductive to climate policy. The restructuring of the ministries at the beginning of the current legislature looked as though emphasis was given to climate action: there is now one Ministry of Economic Affairs and Climate, which lifts climate policy up the agenda. The Ministry of Foreign Affairs is now responsible for climate change negotiations, giving it prominence. The Ministries of Transport and Finance in turn have ministers from the Liberal Party, which has a far more lenient approach to climate policy than the Green Party. We conclude from our review of the inventory (UBA, 2024b) and government emissions projections from March 2024 (UBA, 2024c), that the 2030 target is still in danger, even if the official projections claim that it will be met in aggregate. The official projections are very optimistic as they assume that the 80% renewable electricity target is met, CO 2 prices remain high and activity of emission-intensive industry remains low. Recent capacity additions for wind are not at all in line with that goal and CO 2 prices are currently lower than assumed. The government therefore needs to remain active to ensure that its own target is safely met. We also find that the way the government plans to meet the 2030 target (UBA, 2024c) may make it almost impossible to meet the 2045 climate neutrality target for all sectors. The government weakened the climate change law in May 2024, replacing the compliance mechanism around binding sectoral targets with the ability for sectors to compensate for each other, as long as the overall target is met.  Amending the compliance mechanism conceals the fact that the transport and buildings sectors will exceed their 2030 targets. It will be almost impossible for the transport sector to catch up after 2030 unless drastic and disruptive measures are taken, such as extremely high CO 2 prices or driving bans. Compensation by the other sectors is also not possible after 2030, as it will become increasingly difficult for sectors to avoid the last few tonnes of CO 2 . It is also worrying that Germany will miss the legally binding target within the EU effort-sharing scheme, in which transport and buildings are counted together. There is a threat of high payments, as any failure to meet the target must be offset by certificates. Overall, Germany will exceed its target by at least 126 MtCO 2 e, costing German taxpayers, at a roughly estimated price of EUR 100 per certificate, EUR 12bn. The new May 2024 climate law makes the whole government responsible for meeting the targets, rather than individual ministries. However, the previous law had explicitly placed individual ministries as responsible for achieving their sectoral targets, to make them accountable for climate policy in their respective sector. The May 2024 dilution of responsibility reduces the likelihood of Germany meeting its targets. The ministries of buildings and transport failed to submit the emergency programme required by the old climate law and have consequently been brought to court by NGOs. In the coalition contract, the new government decided not to raise the ambition of the mitigation target, but promised the measures adopted in the coalition agreement would overachieve the target (ARD, 2021). Not only does the government still need to meet its 2030 target, it needs to enhance it, as it’s still not 1.5˚C compatible. Germany, along with all governments, have agreed to increase their 2030 action as part of UNFCCC decisions since 2021. The coalition also wanted to introduce a climate check for each new law, but implementation has been slow. In early 2023, the Federal Environment Agency (UBA) tendered a project to consider possible approaches, the research was not completed as of June 2024 and a climate check has not yet been introduced. To cope with Russia’s unlawful invasion of Ukraine and related energy security issues, Germany introduced a set of measures, some of which are counterproductive to climate policy. The government still plans to develop an overcapacity of LNG import infrastructure (Höhne et al., 2023; Marquardt et al., 2023), which risks a lock-in of fossil fuels and brings into question Germany’s long-term ambitions for GHG neutrality. The coalition embarked on making the climate transition socially just, but has so far failed to do so in several areas: a climate dividend (“Klimageld”), to pay back revenues from carbon pricing on a per capita basis, was seeded in the coalition contract but will now probably only be implemented after 2025, under the next government (Deutschlandfunk, 2024). A temporary rebate on VAT for fuels and a compensation mechanism for high gas prices during times of very high energy prices were given without social differentiation. A positive step is that the new heating law differentiates the subsidies for CO 2 -free heating systems by household income.</t>
   </si>
   <si>
+    <t>Economy-wide emissions across the EU have continued to fall since 2019, when the new European government at the time came to power, roughly by 6% from 2019 to 2022 (the last available data point). In June 2024, European Parliament elections were held, and President von der Leyen was re-elected as head of the European Commission. The new work plan for the next Commission has signalled a shift towards framing climate action in the context of decarbonising Europe’s industries, focusing on competitiveness on a global stage and an increasing attention towards developing a new market for carbon removals. In its previous legislative cycle (2019–2024), the European Green Deal which encapsulated the Fit-for-55 package and REPowerEU legislative packages set out a path for the EU to achieve climate neutrality by 2050. Some key policies and regulations introduced and revised include the: Renewable Energy Directive (RED III) Energy Efficiency Directive new EU ETS II covering transport and buildings Carbon Border Adjustment Mechanism Effort Sharing Directive For more detail see the previous assessment from February 2024 here In the past year, the final elements of the Fit-for-55 and REPowerEU packages were finalised and adopted prior to the June elections including the; Gas Regulation and Directive, Methane Regulation, Energy Performance in Buildings Directive and Carbon Removal Certification Framework, which are covered in more details for this assessment. President von der Leyen’s plans to launch a “Clean Industrial Deal” seeking to build upon existing policies to pivot Europe’s industries. The plan focuses on scaling up manufacturing of net-zero emission technologies and investing in skilled workers to satisfy the growing domestic need for net-zero emission technologies, like electric vehicles (EVs) and heat pumps (von der Leyen, 2024a). With this revision to existing industry related policies, the EU aims to become a global competitor with China and the US in the green technology market race. There will be a big push for expanding and improving rail networks and performance, which is a key measure needed to facilitate a modal shift to an alternative less carbon intensive mode of transport compares to airplanes and cars.</t>
+  </si>
+  <si>
     <t>The CAT estimates that India’s emissions will be around 4.0-4.3 GtCO 2 e in 2030 under current policies. India’s climate policy is spread across several policy documents, sector-specific strategies and laws with the National Action Plan for Climate Change (NAPCC) serving as the overarching guidance for these efforts. In 2023 some very important policy documents and laws covering the energy sector emerged, including the National Electricity Plan 2023 (NEP2023), the National Green Hydrogen Mission and the recently amended Energy Conservation Act (Ministry of Law and Justice, 2022; Ministry of New And Renewable Energy, 2023; Ministry of Power, 2022c). These documents and laws play a crucial role in shaping the energy landscape. There has been a steady increase in the deployment of renewable energy in the country, including both utility-scale and rooftop solar. Due to this consistent growth, the share of coal capacity has dropped below 50% for the first time. This milestone reflects the growing shift towards cleaner energy sources, supported by an impressive 83% increase in investment in renewable energy projects during 2023-24. Large-scale renewable energy projects are gathering momentum, with 69 GW of capacity, primarily solar power, currently out for tender—surpassing the government’s target of 50 GW. Meanwhile, rooftop solar installations are on the rise, with a projected addition of 4 GW in fiscal year 2024. This growth is largely driven by favourable policies and financial mechanisms (Economic Times, 2024b). However, this increase in renewable energy capacity is barely able to keep up with the surging demand. As a result, the generation share of renewable energy, including large hydro, remains around 18%, showing no improvement since last year (CEA, 2024a). To further accelerate the transition to renewable energy, the government has initiated viability gap funding (VGF) of approximately USD 893m for offshore wind energy projects, signalling its commitment to diversifying and strengthening the renewable energy mix. Additionally, regional disparity has been observed in renewable energy deployment in the country, where southern states are leading the trend with higher renewable energy potential and a strong state-level policy push (Economic Times, 2024e). This could be a potential risk to a just transition away from coal, as most of the coal mines and thermal power plants are in the central to eastern part of the nation. It has been anticipated that India will see a more than 83% increase in investments in renewable energy projects to around USD 16.5bn in 2024 (Business Standard, 2024b). India’s fossil fuel companies have also started to diversify their investment into the renewable energy sector (Economic Times, 2024c; MERCOM, 2024) . India has not yet committed to phasing out coal power or committing to a future without fossil gas. Last year, the government adopted the National Electricity Plan, which indicated a pause in coal capacity addition, at least in the short run (Ministry of Power, 2023b). However, this is not being realised, as the current capacity under construction exceeds what the plan proposes (Global Energy Monitor, 2024). While the government has abandoned plans to add more gas power to its electricity generation, it has increased the utilisation of existing gas power plants to meet energy demands due to severe heat stress. India is again experiencing extreme summer temperatures in 2024, as in previous years. The peak demand in May reached approximately 246 GW, surpassing last year’s peak of 243 GW. It is projected that India’s peak demand in 2024 will reach 260 GW. Power consumption spiked by 14% in May 2024 compared to the same period in the previous year (CEA, 2024a). To meet this increased energy demand, there has been a steady rise in the domestic production and import of both coal and fossil gas. While this may be necessary for short-term energy demand, it poses significant risks for long-term energy security due to the volatility of global fossil fuel markets, potential supply disruptions, and the environmental and economic consequences of continued reliance on fossil fuel energy sources. India has a new government, led by Prime Minister Narendra Modi, now beginning his third term. This continuity in leadership is anticipated to sustain policy consistency in India's renewable energy sector and maintain momentum in these areas. Under Modi’s administration, there has been a marked decline in subsidies for the oil and gas sectors (IISD, 2024). It is important that similar reductions will be applied to the coal sector. Ministers in Modi's government have repeatedly emphasised that they will not compromise on power for growth, planning an 80 GW addition to coal power capacity by 2031-32 (PIB, 2023). This suggests a potential status quo in policies related to the thermal power sector and domestic coal production.</t>
   </si>
   <si>
     <t>Indonesia, under the new administration of President Prabowo Subianto, is placing a strong emphasis on continuing the economic and infrastructure development of his predecessor, former President Joko Widodo, and self-sufficiency in food, water, and energy. However, this approach raises significant environmental concerns, particularly regarding the future trajectory of energy and climate policy. Recent developments in Indonesia's energy sector highlight the conflict between increasing support for renewables and the continued expansion of fossil fuel capacity, mainly coal. On a positive note, Indonesia signed the Just Energy Transition Partnership (JETP) with the International Partner Group (IPG), with an overall commitment of USD 21.6 bn. The JETP Comprehensive Investment and Policy Plan (CIPP) outlines several key investment focus areas targeting the on-grid power system: peaking emissions by 2030, capping them at 250 MtCO 2 , increasing the share of on-grid renewable power to 44% in 2030, and reaching net-zero by 2050. On the other hand, progress in renewable energy progress has been slow, comprising only 13% of the energy mix in 2023. As a result, the government intends to lower its 2025 renewables target from 23% to 17-19%, which is at odds with the more ambitious JETP goals. Meeting these goals remains challenging due to difficulty attracting large investments, ongoing electricity oversupply issues, and policies that artificially lower coal prices. On the carbon pricing front, Indonesia launched Southeast Asia's first Emissions Trading System (ETS) in 2023, with plans for it to evolve into a hybrid cap-tax-and-trade system by 2025, eventually covering all fossil fuel-based power plants. A carbon tax, delayed until 2025, will start at around USD 2/tCO₂e, with plans to increase the rate and expand coverage to other sectors. The New and Renewable Energy Bill, intended to support renewable energy, has faced repeated delays, partly due to debates over power wheeling provisions. The Bill also includes controversial definitions like “new energy”, which encompasses nuclear and coal-derived products. The country is also considering nuclear power as part of its strategy to achieve net-zero emissions by 2060, although the CAT does not view this as a solution. In the transport sector, Indonesia has policies in place to support biofuels and electric vehicles, but current outcomes fall short of national targets. The biodiesel mandate programme has progressively increased blending levels, reaching 35% (B35) by 2023, with plans to increase to 40% (B40) by 2025 and 50% (B50) by 2029. However, concerns remain about the link between biofuel development and deforestation. Electric vehicle adoption faces barriers such as high local content requirements and insufficient charging infrastructure, despite government incentives and targets. Public transport usage remains low in most Indonesian cities, with the exception of Jakarta. The development of public transport primarily focuses on major cities, with ongoing projects like the expansion of Jakarta Mass Rapid Transit (MRT) system and plans for Light Rail Transit (LRT) in Bali. Bus Rapid Transit (BRT) systems are being developed in six pilot cities, with TransJakarta leading the way in electrifying public transport. However, financing remains a significant barrier to accelerating the electrification of BRT systems and long-haul buses. Deforestation remains a critical issue in Indonesia, with the forestry sector accounting for almost half of the country’s total emissions over the last 20 years, reaching around 1 GtCO 2 e per year. Indonesia aims to reach a net negative 140 MtCO 2 e in GHG emissions by 2030 under its FOLU Net Sink programme. However, given current LULUCF emission trends and policy projections estimated to result in emissions of around 920 MtCO 2 e per year in 2030, it is uncertain how Indonesia will achieve such steep emission reductions within this short timeframe. In the agriculture sector, the food estate programme, launched to enhance food self-sufficiency, has failed to address food security and poses significant environmental and social risks. The conversion of biodiverse habitats threatens endangered species and violates indigenous land rights. The initiatives neglect core issues like food distribution inefficiencies and access to affordable, nutritious food. To improve food resilience, Indonesia should diversify its agriculture to include a wider array of nutritious crops, invest in sustainable practices, and improve its food supply chain and infrastructure. Indonesia has implemented policies to promote energy efficiency in the buildings sector, targeting a 15% reduction in energy consumption by 2025. The government is also progressing green buildings through regulation and certification efforts, with initiatives like the Indonesia Green Affordable Housing Programme aiming to build and retrofit green housing units. Challenges remain, particularly in the residential sector, which accounts for a significant portion of building energy demand and has limited adoption of green building standards. The growing digital economy has also driven demand for green data centres.</t>
   </si>
   <si>
-    <t>Although the government introduced several new policies towards the end of 2023 and throughout 2024, mostly in the power, transport and industry sectors, they were accompanied by continued support for both coal and fossil gas production for many decades to come. The ongoing revisions of historical and projected LULUCF estimates puts the government closer to meeting its emissions reduction targets without making meaningful emissions reductions across the economy. Australia’s policies and action are projected to achieve emission reductions between 17% and 21% below 2005 levels by 2030, excluding LULUCF. Under current policies, Australia’s total GHG emissions excluding LULUCF are projected to fall to 438 MtCO 2 e (446 MtCO 2 e in AR5 GWPs) by 2030. When also taking announced policies into account, emissions excluding LULUCF would fall to 417 MtCO 2 e by 2030 (424 MtCO 2 e in AR5 GWPs) by 2030. Slow progress towards 82% renewable energy The Capacity Investment Scheme, expanded in November 2023, is the government’s main instrument to bridge the currently significant gap to the 82% renewable electricity target (DCCEEW, 2023b; Open Electricity, 2024a, 2024b). This expanded CIS aims to deliver 32 GW of new clean energy capacity by 2030, comprised of 23 GW of variable renewable capacity and 9 GW of dispatchable capacity, such as battery storage. While not legislated, the 82% target is assumed in the government’s emission projections to apply to the nation’s four main grids (NEM, WEM, DKIS, NWIS), but not to other minor grids or off-grid generation. Under the government’s baseline projections, which excludes the expanded CIS, the share of renewables in Australia’s on-grid generation would reach 72% by 2030, largely due to solar and wind energy deployment (DCCEEW, 2023b). As of June 2024, renewables penetration of the National Electricity Market, Australia’s largest grid, stood at 38% (Open Electricity, 2024a). Although it is too early to assess the impact of the expanded CIS, Australia’s power sector cannot yet be considered on-track to meet its 82% renewable electricity target, nor is it on a 1.5°C-compatible trajectory. Investment in large-scale renewable generation stalled in 2023, with just AUD 1.5bn committed to new projects, substantially down from 6.5bn in 2022 (Clean Energy Council, 2024). The rollout of renewables in Australia continues to be obstructed by slow planning and environmental approval processes, higher costs, and tighter markets for equipment and labour. Coal power still accounted for nearly half of Australia’s total generation in 2023, while fossil gas accounted for 18% (DCCEEW, 2024a). There is no explicit emissions reduction policy for the electricity sector, nor a federal-level coal and fossil gas phase-out plan and timeline. Green industry In 2024, the government has unveiled new energy-related policy documents for the post-fossil fuel exports era. The ‘Future Made in Australia’ plan announced in 2024, allocates AUD 22.7bn (USD 14.9bn) over 10 years to attract investment in key industries and realise Australia’s potential to become a “renewable energy superpower” (Australian Government, 2024). The scheme is targeted at renewable hydrogen, green metals, low carbon liquid fuels, critical minerals processing, and clean energy manufacturing including battery and solar panel supply chains. The plan does not include support for fossil fuels. The government’s updated National Hydrogen Strategy, released in 2024, sets targets for both production and export of hydrogen (DCCEEW, 2024c). The strategy specifically targets renewable-based hydrogen, which is an improvement on the 2019 strategy which also encompassed fossil fuel-derived hydrogen. No end in sight to fossil fuels Nevertheless, the government has also reaffirmed its commitment to fossil fuel production and exports. In some of the most impactful decisions made by the Albanese government, the government approved three coal mine extensions in September 2024, allowing them to continue operating for another 30–40 years (ABC News, 2024d; The Guardian, 2024). These decisions will result in well over an additional billion tonnes of CO 2 being emitted to the atmosphere, on top of the four previous coal mining approvals issued in 2023 (The Australia Institute, 2024b). Australia remains a massive exporter of fossil fuels and, in 2023, was the world’s second-largest exporter of coal and third-largest exporter of liquefied natural gas (LNG) (Energy Institute, 2024). The government’s Future Gas Strategy, released in May 2024, doubles down on the role of gas in Australia’s domestic energy sector and exports to 2050 and beyond (DISR, 2024a). The strategy reinforces the government’s ongoing commitment to development of new fossil gas supply and continued LNG exports. The Safeguard Mechanism is the Australian government’s central policy for reducing industrial emissions by imposing declining baselines on large industrial facilities. In 2023, the 219 facilities covered by the mechanism emitted 139 MtCO 2 e (26% of Australia’s total emissions excluding LULUCF) (Clean Energy Regulator, 2024; DCCEEW, 2024i). The mechanism allows for unlimited use of offsets to meet declining baselines, creating uncertainty about actual emissions reductions that will be achieved and the effectiveness of the scheme. Alone the emissions from existing and committed LNG projects and all committed coal projects, which make up around half of Safeguard Mechanism facilities, would leave no room for other industries in the scheme, who would find themselves having to make additional steeper cuts to keep to the government’s set 100 MtCO2e limit ( Climate Analytics, 2023 ). The transport sector is projected to become the greatest source of emissions in by 2030, as power sector emissions decline (DCCEEW, 2023b). The government’s long-awaited New Vehicle Efficiency Standard (NVES) was introduced in 2024 and will apply to new cars sold from 2025 onward, making Australia one of the last developed countries to adopt such standards (DITRDCA, 2024). The standard sets emissions intensity targets imposed on suppliers across the fleet of vehicles they sell each year. The New Vehicle Efficiency Standard and the National Electric Vehicle Strategy, released in 2023, do not set a strategy or targets for public transport, cargo and modal shift, leaving a gap in the government’s transport sector policies.</t>
-  </si>
-  <si>
-    <t>In October 2022, Luiz Inácio Lula da Silva was elected president of Brazil for the third time, defeating former president Jair Bolsonaro. He assumed the presidency in January 2023, quickly moving away from the previous administration’s policies and reconstructing the country’s environmental policy which had suffered from budget cuts and policy rollbacks (Nature, 2023). Some positive policy developments can already be highlighted, including: Following the resubmission of its NDC in October 2023, the Inter-ministerial Council on Climate Change began reviewing the National Climate Change Policy (PNMC), which will now include sectoral mitigation and adaptation strategies covering the period up to 2035 as well as indicative sectoral targets for 2030 and 2035, a process that could take up to two years (Talanoa, 2023). Recent studies reported deforestation rates falling in response to political action (BBC, 2024; Global Forest Watch, 2024). A 36% drop in primary forest losses in Brazil in 2023 compared to 2022 levels was celebrated as an example of the effects of re-establishing law enforcement in the forestry sector. However, deforestation remains higher than in the early 2010s, with negative trends in some regions like the Cerrado where deforestation actually increased by 6% in 2023 (BBC, 2024; Nature, 2023) Brazil's presidency of the G20 summit in 2024 and hosting of COP30 in 2025 highlight its renewed engagement with the international community on environmental issues, signalling its commitment to shaping international climate policy. This is particularly relevant as 2025 will be the year when countries are mandated to submit updated and more ambitious 2035 climate targets under the Paris Agreement. The development of new policies such as the Ecological Transformation Plan (PTE) to promote sustainable development while reducing Brazil’s overall environmental footprint, and which includes energy transition as one of its six pillars of action (Government of Brazil, 2023d; Talanoa, 2023). However, there are still important and inconsistent elements in the new policy development that raise concerns about the prioritisation of sustainability and environmental goals within Brazil's infrastructure agenda, which cast serious doubt on the government's commitment to ecological transformation and transition away from fossil fuels (Nature, 2023), in particular: Brazil’s Novo PAC (a new USD 350bn growth acceleration programme designed to stimulate private and public investments in infrastructure, development and environmental projects) which assigned around USD 110bn (just over 30%) of its budget to “energy transition and security” while earmarking 63% of its budget for the oil and fossil gas industries, mainly for the production and development of these fossil fuels (Government of Brazil, 2023c, 2023e). The actions outlined under the energy transition pillar of the PTE focus mostly on reducing transport emissions by electrification or low-carbon fuels and further development of wind and solar energy; without concrete targets related to a transition away from fossil fuels. Brazil is yet to put forward a timeline for phasing out fossil fuels and questions remain as to how it will achieve an energy transition in a just and equitable way (Nature, 2023). Our calculations show Brazil’s total emissions (excluding LULUCF) will reach between 1,162 MtCO 2 e and 1,197 MtCO 2 e in 2030 under current policies, almost 25% above 2005 levels. Brazil is not on track to reach neither its 2025 target nor its 2030. To peak and then rapidly decrease emissions, as required in order to limit warming to 1.5°C, Brazil will need to sustain and strengthen policy implementation and accelerate mitigation action in all sectors— including a reversal of present plans to expand fossil fuel energy sources.</t>
-  </si>
-  <si>
-    <t>The speed and scale of Canada’s climate policy implementation does not match the urgency of the climate crisis and much more work is needed. Emissions in 2030 are projected to be 603 MtCO 2 e (excl. LULUCF contributions) or 20% below 2005 levels, lower than our last update, due to continued policy implementation, but a far cry from the 377–495 MtCO 2 e level Canada needs to reach to meet its updated NDC target. In March 2022, Canada released its latest climate change plan, building on earlier strategies released in 2016 and 2020 (Environment and Climate Change Canada, 2020a, 2022a; Government of Canada, 2016b). The measures outlined in the plan are not yet sufficient to ensure Canada meets its NDC target, nor have all been implemented yet. It came on the heels of a damning report in November 2021 by Canada’s Commissioner of the Environment and Sustainable Development outlining 30 years of the government’s failure to meet its targets and reduce greenhouse gas emissions (Commissioner of the Environment and Sustainable Development, 2021; Office of the Auditor General of Canada, 2021). Canada is developing additional policies which are captured in our planned policies scenario. Of the major initiatives (regulations for clean electricity, post-2026 LDV model year standards, oil and gas methane target, and landfill gas), only the EV sales mandate has been implemented since the government released its 2023 projections. Our current policy projection is based on these projections and modified to include the impact of the EV sales target. The step-up in climate action over the last four years was driven by a vulnerable minority Liberal Party government, enabled through support from the New Democratic Party. This progress risks being dialled back after the next elections, set for 2025, if the Conservatives were to come to power. They have already promised to ‘Axe the tax’, i.e. abolish the carbon pricing system. In preparation, the government has designated almost half of the CAD 15 billion (USD 11bn) in the Canada Growth Fund to be spent on Contracts for Difference or similar offtake agreements to ensure stability to investors in the coming months (Environment and Climate Change Canada, 2023a) Carbon pricing Mandatory carbon pricing has been in effect across Canada since 2019 (Government of Canada, 2018a). The legislation enacting the carbon pricing scheme, the Greenhouse Gas Pollution Pricing Act , was found to be constitutional by the country’s top court in March 2021 after three provinces challenged it (Supreme Court of Canada, 2021). A second challenge from the province of Manitoba was also dismissed by the Federal Court in October 2021. Under the scheme, all Canadian provinces and territories must have a cap-and-trade system or carbon tax in place. Jurisdictions without such systems or taxes will fall under the federal backstop. The federal system has two components: a regulatory charge on fossil fuels and an output-based pricing system (OBPS), which applies to major emitting industrial facilities. The federal government will review its carbon pricing benchmark in 2026. The initial carbon price of CAD 20/tCO 2 e was set in 2019 and increased by CAD 10 per year, reaching CAD 50/tCO 2 e in 2022. In its latest climate plan, the government stated it will increase the carbon price by another CAD 15 per year for the 2023–2030 period, reaching CAD 170/tCO 2 e in 2030 (around USD 125) (Environment and Climate Change Canada, 2020a; Government of Canada, 2021k). While the carbon price is heading in the right direction, it is still below the USD 170–290 (2015$) needed to be compatible with 1.5°C (Boehm et al., 2023). A 2022 audit of the scheme found the government had taken steps to address some of the scheme’s weaknesses, but that requirements for large emitters were poor and could be strengthened (Commissioner of the Environment and Sustainable Development, 2022a; Office of the Auditor General of Canada, 2022a). National GHG Offset System In June 2022, the federal government established a GHG Offset system for activities not covered by carbon pricing (Government of Canada, 2022e). Credits generated under the system can be used to reduce the compliance costs of industrial facilities covered by the OBPS. At present, the system only covers landfill methane recovery and refrigeration systems, but protocols are being prepared for forest management, livestock feed management, enhanced soil carbon, manure methane emissions and direct air carbon dioxide capture and sequestration (Government of Canada, 2022c). The ministry is also looking into ways to remove barriers and enhance participation in the system by Indigenous peoples (Government of Canada, 2022f).</t>
-  </si>
-  <si>
-    <t>Between 2010 and 2022, Chile’s emissions increased by 27%, from 88 MtCO 2 e to 112 MtCO 2 e, excluding LULUCF. When considering Chile’s current policies, we estimate that Chile’s emissions already peaked in 2021 at a level of 115 MtCO 2 e. According to our assessment, Chile’s emissions levels in 2030 under current policies will be between 100–108 MtCO 2 e/year (excl. LULUCF). Our analysis suggests that Chile will not meet its conditional nor unconditional NDC targets in 2030 under current policies, or be 1.5° compatible. Compared to our previous assessment, emissions under current policies have increased due to higher historical emissions than previously projected, a stronger rebound after COVID, and changes to the current policy assumptions. Chile’s key climate policies include the Energy Efficiency Law (Law 21.305/2021), a legal framework aiming to reduce energy consumption across the power, transport, buildings, and industry sectors. It also includes the coal phase-out, where all of Chile’s coal-fired units (28) are expected to retire or be retrofitted by 2040. An earlier coal phase-out could have a sizable impact on Chile’s current policy trajectory, but only if the coal capacity is replaced with generation from renewable energy sources. The CAT estimates that choosing to retrofit coal plants with gas could lead to at least 3 MtCO 2 e fewer in emission reductions in the short-term compared to retiring coal-fired units and using renewable electricity sources, and can lead to carbon lock-in risks and stranded assets. The Electromobility Strategy guides climate policy in the transport sector and sets out an action plan to electrify 100% of the urban public transport vehicle fleet by 2050 and ban the sale of new cars with combustion engines in 2035. Chile has also introduced a carbon tax (Law 20.780/2014), although its price is likely too low to result in emissions reductions. In June 2022, Chile passed the Framework Law on Climate Change (21455) (Congreso Nacional de Chile, 2022). It includes the 2050 GHG neutrality target and recognises the NDC target, making them legally binding. As a result, Chile now has a legal framework that assigns responsibilities and strengthens the legal and institutional basis for implementing climate change mitigation and adaptation policies across all sectors, and is moving towards a low emissions economy. It also presents a paradigm shift in Chile’s environmental policy, as climate action is now not only the responsibility of the environment ministry but is spread across 17 national ministries, as well as regional governments and municipalities, and even includes the private sector. While most of the important regulations outlined in the Framework Law on Climate Change have come into force, Chile has been delayed in implementing two new regulations and modifying two existing regulations (Peña, 2024). The regulation on its Article 6 framework is heading into its consultation stage, but there has been no movement on its related law outlining the requirements and verification method around the GHG emissions reduction or absorption certificates. The law also mandates the relevant ministries to develop sectoral mitigation plans by 2024, but no plans have yet been released (CR2 and Centro de Derecho Ambiental, 2024). Since our previous assessment, there have been no major changes to Chile’s climate policies. New laws to promote renewable energy and address critical barriers like a lack of transmission lines, such as the Law on Energy Storage and Electromobility and the Energy Transition Law, have been in the legislative process for a couple of years now. Chile has nevertheless made progress in that time, publishing new sectoral strategies to guide its short-term climate plans such as the Initial Agenda for the Second Phase of the Energy Transition, the Ministry of Energy’s Decarbonisation Plan, the Roadmap for the Advancement of Electromobility, as well as the Green Hydrogen Action Plan 2023-2030. Chile is on track with its 2040 coal phase-out plan, meeting its goal of retiring 11 plants by 2024, and has even accelerated its implementation. Nine of the remaining coal-fired units have currently committed to being retired or retrofitted between 2024 and 2025, although it is unclear whether the retirement or reconversion will be timely. However, the eight remaining coal plants have yet to make a firm commitment: it is still possible for them to continue operating until 2040. While there were some discussions in 2022 on adopting an even earlier, more ambitious phase-out date of 2030, this has not been mentioned in a while. To bring its current policies considerably closer to a 1.5°C trajectory, Chile could update its national commitment to phase out coal-fired power by 2030.</t>
-  </si>
-  <si>
-    <t>China’s current policies scenario projections have been updated to reach GHG emission levels (excl. LULUCF) of 13.8 to 14.6 GtCO₂e/yr in 2030 – roughly 29% higher than 2010 levels. The 14th FYPs aims to cut energy intensity by 13.5% and emissions intensity by 18% by 2025 from 2020 levels (Xinhua News Agency, 2021). However, progress from 2020-23 was minimal, with only a 2% drop in energy intensity and a 4.6% drop in emission intensity (Myllyvirta, 2024b). To ensure the achievement of its 14th FYP targets, the State Council sets its 2024 targets to reduce the energy intensity and emission intensity by 2.5% and 3.9% respectively (The State Council of the People’s Republic of China, 2024). China’s CO₂ emissions in the second quarter of 2024 dropped for the first time since the country reopened from its “zero-Covid” lockdowns in December 2022 (Myllyvirta, 2024a). This reduction was mainly driven by a surge in clean energy additions, reversing the growth of fossil fuel power. Despite cautious and conservative government reactions, it suggests that China’s CO₂ emissions may have already peaked in 2023. If not, they are likely to peak well before 2025, five years ahead of the 2030 target (Bloomberg News, 2024b). China achieved its 1,200 GW wind and solar capacity target six years ahead of schedule, reaching 1,206 GW in July 2024, with forecasts predicting 1,310 GW by year-end. (Bloomberg News, 2024d; CEC, 2024) China's reliance on fossil fuel consumption is a key factor driving global emissions. Despite having the world’s largest coal power pipeline, China reduced its coal plant permits by 83% in the first half of 2024, allowing only 9 GW, after permitting over 100 GW of coal power annually in 2022 and 2023 (CREA and GEM, 2024a; GEM et al. , 2024). This drop in new coal approvals doesn’t necessarily indicate an early coal peaking, as addressing the coal power projects permitted during the 2022-23 surge remains a significant challenge for China if it wants to peak emissions and avoid a costly coal lock-in. The government has introduced a "low carbon transformation" action plan. This plan aims to reduce emissions from existing coal plants through biomass co-firing, green ammonia co-firing, and CCUS technologies from 2025 to 2027 (NDRC and NEA, 2024a). While shifting away from coal is essential for achieving a 1.5-compatible power system, reducing emissions from coal plants that will remain in use for some time through technical improvements is still sensible. This approach will further raise the cost of coal-fired power, thus promoting renewable energy, especially as nearly half of China’s coal-fired power generators are operating at a loss even before accounting for costly new measures (Myllyvirta, 2024a). The draft of the Energy Law of the People's Republic of China was opened for public consultation at the Standing Committee of the National People's Congress (NPC) meeting on April 26, 2024. This will be China's first comprehensive law with a fundamental and overarching role in the energy sector, integrating various stand-alone energy laws and regulations, such as the Electricity Law, the Coal Law, the Energy Conservation Law, and the Renewable Energy Law. The Energy Law could be formally introduced within 2024 (Dai, 2024). Article 20 of Chapter 3 of the draft law explicitly supports the priority development of renewable energy, the rational development and clean, efficient use of fossil energy, and the orderly promotion of replacing fossil energy with non-fossil energy, as well as replacing high-carbon energy with low-carbon energy (NDRC and NEA, 2024b). Launched in 2021, China’s Emissions Trading Scheme (ETS) covers over 2,000 companies in the power sector, 40% of China’s total carbon emissions, and recorded over 24.9 billion yuan (USD 3.4bn) in total transactions in 2023. The ETS has thus far had minimal impact on CO₂ emission reduction, primarily due to a generous supply of allowances and the absence of a stringent emissions cap. New regulations on ETS management published in February 2024 significantly increased the punishment for non-compliance, data fraud and market manipulation behaviours (IKI, 2024). In July, China published new rules for public consultations, prohibiting participants in the Emissions Trading System (ETS) from borrowing allowances from future years and more strictly limiting the carrying over of unused permits from previous years (MEE, 2024). Beyond the power sector, China plans to expand its ETS to seven other high-emitting sectors covered by the European Union Carbon Border Adjustment Mechanism (CBAM) regulations. (Tan, 2022). China's industry sector is targeting electrification and efficiency improvements to meet demand and reduce reliance on fossil fuels. Steel, cement, and aluminium are the main drivers of emissions in the industry sector; all the subsectors have aligned with the economy-wide carbon peaking timeline before 2030 (MIIT of China, NDRC and MEE, 2022). The Special Action Plan for Energy Conservation and Emission Reduction in the Iron and Steel Industry, issued in June 2024, aims to reduce comprehensive energy consumption per tonne of steel by over 2% by the end of 2025 compared to 2023 levels (NDRC et al. , 2024).The national ETS has also announced to expand to include steel, cement, and aluminium by the end of 2024 (ChinaNews, 2024). The government is also taking decisive action to control capacity and production in the steel and cement sectors to address overcapacity and reduce emissions. As of August 23, 2024, all new steel plant permits have been indefinitely suspended, following an earlier policy of granting permits only for electric-powered steelmaking plants (MIIT of China, 2024). Carbon capture, utilisation and storage (CCUS) and the development of hydrogen solutions are on the radar of policymakers in China's harder-to-abate sectors for decarbonisation, although CCUS doesn’t lead to complete decarbonisation. The new "low carbon transformation" action plan for coal power plants highlights CCUS technologies as a key method for reducing emissions from existing coal plants from 2025 to 2027 (NDRC and NEA, 2024a). As the world's largest producer of hydrogen, China published its national hydrogen strategy and is targeting modest production of 100,000–200,000 tonnes of renewable-based hydrogen by 2025, which could reach 100 million tonnes by 2060 (Yao, 2022). To transition to a low-carbon transport sector, the government has spent decades prioritising new energy vehicles (NEVs) sales, including battery electric vehicles (BEVs), plug-in hybrid vehicles (PHEVs), and fuel cell electric vehicles (FCEVs). China dominates the global electric vehicle (EV) industry, having produced more than half of the EVs worldwide in 2023. This dominance is driving global EV development and intensifying pressure on European and North American companies to improve competence. In response, the EU, the US, and Canada have imposed additional tariffs on Chinese-made EVs to counter China's market and price advantages (Song et al. , 2024). China's domestic NEV market share reportedly exceeded 30% in 2023 (already exceeding the 20% target in 2025) despite ending NEV subsidies for producers in 2022; the government aims for a 40% market share by 2030 (Government of China, 2021; Xinhua News Agency, 2024). China has also been prioritising improving accessibility and electrification of its public transport systems, with the expansion of national high-speed rail and local electric public transport systems prominent in its COVID economic stimulus packages and latest FYPs. The government aims to expand its massive high-speed rail network from the current 45,000 km to approximately 70,000 km by 2035. It has also launched a pilot program for cities to procure around two million electric public vehicles before 2035 (O. Wang, 2022; CGTN, 2023). While China's real estate market is in a downturn, and investment in new construction projects is expected to slow down, the stock of projects under construction and the growing demand for higher living standards will still present challenges in terms of energy consumption and emissions in the building sector. To address this, the Chinese government has outlined targets in its 14th Five-Year Plan (FYP) for Building Energy Efficiency and Green Building and Implementation Plan for Carbon Peaking in Urban and Rural Construction (MoHURD of China, 2022; MoHURD of China and NDRC, 2022). The plan sets energy consumption caps in building operations, increases the energy efficiency of new buildings, and sets indicators for renovating existing buildings with efficiency measures and constructing ultra-low or zero-energy consumption buildings. The plans also contain indicators for increasing solar and geothermal applications to new buildings, raising the proportion of energy from renewable electricity, and reducing emissions intensity and energy intensity in residential and commercial buildings. China has increased efforts to expand its forestry and grasslands, in part due to their role in achieving the country’s carbon peaking and carbon neutrality targets. The government has implemented various domestic forest conservation and afforestation policies, and in the 14th FYP, it has set a target to plant 36,000 km2 of new forest annually until 2025 to increase the country’s forest coverage (NGFA of China, 2021). Internationally, China has increased its forestry pledge and signed the Glasgow Declaration on Forest and Land Use and separate joint agreements with the EU and the US on reducing deforestation. China is engaged in domestic discussions to include methane in its 2035 NDC updates. The long-awaited Methane Action Plan was published in November 2023 (State Council of China, 2023a), setting basic directions to control methane emissions across sectors as well as emphasising the establishment of a methane MRV system. However, the action plan does not specify any quantitative emission reduction targets or commitments. China finally ratified and started enforcing the Kigali Amendment in 2022 (Rudd, 2021). China reported that it halted new production capacity of five of the 11 HFCs it produces (covering 75% of total HFC production) two years ahead of the freeze requirements of the Amendment (McKenna, 2022). According to our analysis, China would reduce emissions by a modest ~50 MtCO₂e/year by 2030 under the Kigali Amendment’s phase-out schedule, although reductions could increase to almost 300 MtCO₂e/year by 2045.</t>
-  </si>
-  <si>
-    <t>Economy-wide emissions across the EU have continued to fall since 2019, when the new European government at the time came to power, roughly by 6% from 2019 to 2022 (the last available data point). In June 2024, European Parliament elections were held, and President von der Leyen was re-elected as head of the European Commission. The new work plan for the next Commission has signalled a shift towards framing climate action in the context of decarbonising Europe’s industries, focusing on competitiveness on a global stage and an increasing attention towards developing a new market for carbon removals. In its previous legislative cycle (2019–2024), the European Green Deal which encapsulated the Fit-for-55 package and REPowerEU legislative packages set out a path for the EU to achieve climate neutrality by 2050. Some key policies and regulations introduced and revised include the: Renewable Energy Directive (RED III) Energy Efficiency Directive new EU ETS II covering transport and buildings Carbon Border Adjustment Mechanism Effort Sharing Directive For more detail see the previous assessment from February 2024 here In the past year, the final elements of the Fit-for-55 and REPowerEU packages were finalised and adopted prior to the June elections including the; Gas Regulation and Directive, Methane Regulation, Energy Performance in Buildings Directive and Carbon Removal Certification Framework, which are covered in more details for this assessment. President von der Leyen’s plans to launch a “Clean Industrial Deal” seeking to build upon existing policies to pivot Europe’s industries. The plan focuses on scaling up manufacturing of net-zero emission technologies and investing in skilled workers to satisfy the growing domestic need for net-zero emission technologies, like electric vehicles (EVs) and heat pumps (von der Leyen, 2024a). With this revision to existing industry related policies, the EU aims to become a global competitor with China and the US in the green technology market race. There will be a big push for expanding and improving rail networks and performance, which is a key measure needed to facilitate a modal shift to an alternative less carbon intensive mode of transport compares to airplanes and cars.</t>
-  </si>
-  <si>
-    <t>The new government has inherited a challenging policy context. The final years of the previous government were marked by chronic delays to key delivery mechanisms, rollbacks to other essential climate polices, and a clear lack of commitment to reducing emissions at the pace and scale needed to align with the Paris Agreement’s long-term temperature goal. As a result, in July 2024, only 24–32% of the emissions cuts needed to reach the UK’s climate targets were covered by credible policy (CCC, 2024). The new government has highlighted that it wants to address this situation and close the implementation gap. It has already made a start on this, with some hopeful first signs including: In the power sector, where the government has set a target to achieve clean power by 2030. A decarbonised power sector by 2030 is a herculean endeavour, but would help unlock emissions cuts in other sectors, as clean electricity powers buildings, transport and industry. It would also demonstrate the viability of a clean power sector and rapid transition at scale, which could catalyse increased ambition in other countries and enable the UK to act as a global leader on power sector decarbonisation. To support this goal, the government has already lifted the de facto ban on onshore wind (DESNZ, 2024c) and secured record renewables capacity in the first auction after expanding the budget for renewables (DESNZ, 2024a, 2024d). In the buildings sector, the government has committed to double funding for energy efficiency improvements (Seddon, 2024), has signalled a willingness to enforce minimum efficiency standards in rental properties (DESNZ, 2024b) (a policy that was removed by the previous government), and has announced guidance on the next tranche of funding for retrofitting. However, this will not be enough to close the implementation gap. Much more will be needed, including: Ramping up renewables. The government’s commitment to clean power needs to be backed by a laser-focus on delivery. The latest renewable auction delivered record levels of renewables, including 5 GW of offshore wind. But this is still not enough to achieve clean power by 2030 – more needs to be done. Grids and storage will also be key to the power sector transition. Accelerating electrification. Removing policy costs from electricity bills would help incentivise industrial electrification and ensure that heat pumps truly cut consumer bills. Specific policies to incentive industrial electrification are also needed, and planning barriers to heat pumps and electric vehicle charging points need to be removed. Reversing recent rollbacks . The previous government exempted 20% of houses from the fossil-fuelled boiler ban, and delayed the ban on petrol and diesel vehicle sales to 2035. These policy rollbacks should be reversed.</t>
-  </si>
-  <si>
-    <t>Saudi Arabia has done little to decarbonise its economy. We expect its emissions to rise to 800–830 MtCO 2 e in 2030, a 15–­19% increase from 2021 levels. It remains difficult to assess whether Saudi Arabia’s current policies reach its NDC target, given the significant uncertainties around its target (see details in the Assumptions section ). Saudi Arabia’s energy sector remains dominated by fossil fuels, which represented almost 100% of the total energy supply in 2022 (IEA, 2023b). The Saudi government expects the overall demand for energy, including for oil and fossil gas, to continue increasing until 2030 and beyond (KAPSARC, 2021). Saudi Arabia’s “Vision 2030” aims to diversify its economy beyond oil, which accounted for around two thirds of total budget revenues in 2022. However, the government clearly has no intention to phase out fossil fuels. Saudi Arabia is betting on carbon capture and storage (CCS) technologies as a smokescreen to continue expanding oil and gas production. While Aramco abandoned its plan to increase oil production capacity to 13 million barrels per day (mb/d) by 2027, this decision appears largely driven by strategic considerations rather than a commitment to phase out fossil fuels. This reversal reflects changes in the global oil market, including slowing demand growth and increased production from non-OPEC countries, particularly the U.S. Even if Saudi Arabia were to reach its 50% target for renewable energy in the electricity mix, we project that emissions would still rise to 730–770 MtCO 2 e by 2030. Despite its vast solar energy potential, Saudi Arabia has only installed about 2.7 GW of renewable energy capacity as of 2023, generating around 1% of total electricity (IRENA, 2024b). Carbon crediting schemes In 2022, Saudi Arabia’s sovereign wealth fund, the Public Investment Fund (PIF), and the Saudi Stock Exchange Tadawul set up a voluntary carbon market in the Middle East and North Africa. The first auction in November 2022 offered one million tonnes of carbon credits (Bloomberg, 2022). Saudi Arabia has also announced the launch of a domestic carbon crediting scheme in early 2024, which will purportedly enable companies to offset their emissions by buying credits compliant with Article 6 of the Paris Agreement. The scheme appears to be voluntary, project-based and covers all sectors (Carbon-Pulse, 2023; Kingdom of Saudi Arabia, 2024). Despite the apparent focus on companies procuring credits, Saudi Arabia also appears to plan on using the credits to meet parts of its national climate pledge, including its 2060 net zero target. Based on the information published as of November 2024, it is unclear how this could work in practice in a manner that avoids both a company and the government from claiming rights to the same emission reductions ("double counting") – an outcome that would undermine the integrity of the credits, and potentially lead to an overall rise in emissions. The establishment of a voluntary carbon market in Saudi Arabia should complement and not serve to distract from - or displace - critically-needed domestic mitigation efforts. Information on how the Kingdom intends to use its carbon crediting scheme remains unclear or lacks details, and presents major risks that it will seek to use carbon credits with questionable integrity as a smokescreen to justify continuing its trajectory of maintaining high levels of domestic emissions. For more information on the role of voluntary carbon markets under the Paris Agreement and their associated risks, see Fearnehough et al. 2020 .</t>
-  </si>
-  <si>
-    <t>According to our current policy emissions pathway, Singapore’s GHG emissions dipped in 2020 due to the economic impact of COVID-19 and will steadily rise in the coming years, reaching 56-57 MtCO 2 e in 2030. Although Singapore’s emissions continue to grow, we project that emissions will be lower in 2030 than its latest NDC target, making a compelling argument for Singapore to raise its level of ambition in its forthcoming NDC. A more ambitious target would demonstrate the government’s commitment to contributing its fair share to global climate change mitigation. A Future Energy Fund, with an initial reserve of SGD 5bn, was announced in the 2024 budget and aims to support Singapore’s transition to cleaner fuels (CNA, 2024). As part of this announcement, Singapore’s Deputy Prime Minister, Lawrence Wong, highlighted both Singapore’s strategy to import low carbon electricity as well as its National Hydrogen Strategy, released in 2022. Singapore has an opportunity to take regional leadership in the green hydrogen space by becoming a regional hub of storage, trading, and transportation of green hydrogen for other Asian countries (Somani, 2022). The government introduced a carbon tax in 2019, initially set at SDG 5/tCO 2 e (USD 4/tCO 2 e). The carbon tax was increased to SGD 25/tCO 2 e (USD 19/tCO 2 e) from 2024 and will be increased to SGD 45/tCO 2 e by 2026-2027, with a target of reaching SGD 50-80/tCO 2 e (USD 38-60/tCO 2 e) by 2030 (National Climate Change Secretariat, 2024a; World Bank, 2023a). The tax currently applies to around 50 facilities in in the manufacturing, power, waste and water sector, and covers 80% of Singapore’s total GHG emissions (National Climate Change Secretariat, 2024a). In 2023, the government released an eligibility list for international carbon credits, which companies are permitted to use to offset up to 5% of the carbon tax liability (National Environment Agency, 2023). Despite the fivefold increase in 2024, Singapore’s carbon price is still significantly lower than those in Europe and Canada (The World Bank, 2024). The IPCC Working Group III indicates that under 1.5°C pathways, the marginal abatement cost of carbon in 2030 is about USD 220/tCO 2 in 2015 terms or USD 281/tCO 2 in 2023 terms (IPCC, 2022; World Bank, 2023b). This is 5-7 times higher than Singapore’s intended 2030 carbon price, which equates to USD 38-60/tCO 2 in 2023 terms. Although, pricing carbon needs to be understood in terms of national context, there is a large difference between Singapore’s price and the IPCC 1.5°C pathway range. A carbon tax can encourage more renewable energy in place of fossil fuel energy through changes in relative prices. However, a higher carbon price would need to be implemented earlier, to shift incentives enough to set emissions on a downward trajectory, compatible with the Paris Agreement (Carbon Market Watch, 2017; Warren, 2014). Singapore’s mitigation strategy is based on three areas: increasing energy and carbon efficiency, reducing carbon emissions in power generation, and developing low-carbon technology (Ministry of the Environment and Water Resources, 2016). Improving energy efficiency across the economy is the backbone of Singapore’s mitigation strategy. In its latest National Climate Action Plan (Ministry of the Environment and Water Resources, 2016), the government listed a number of policies to improve energy efficiency across all sectors, including an Energy Conservation Act, Green Mark Certification and Energy Labelling schemes, and home appliances Energy Performance Standards, among others. The Government has implemented a target of 80% of buildings to be certified green buildings by 2030. As of 2022, 55% of buildings have met this standard (Building and Construction Authority, 2023).</t>
-  </si>
-  <si>
-    <t>The CAT estimates South Africa’s emissions under current policies are on track to reach 462–502 MtCO 2 e excluding LULUCF by 2030, equivalent to 7–14% below 2010 levels excluding LULUCF. Under these current policy projections, South Africa’s emission levels in 2030 will be above the upper bound of the updated NDC target range for the same year (around 25–65 MtCO 2 e higher). The range of our latest projections have decreased slightly compared to our previous projection from September 2022. This is due to a slight revision of historical data using the latest government reported inventory data for 2007 to 2020 and updated estimates of 2021 from PRIMAP (see ‘Assumptions’ section ) (DFFE, 2023; Gütschow &amp; Pflüger, 2023). We further estimate that emission levels could decrease to as low as 404 MtCO 2 e excluding LULUCF by 2030 if South Africa were to implement its planned policies, including the expansion plans for the renewable electricity procurement, the accelerated switch to low-carbon mode of transport, energy efficiency measures, and the carbon tax. Under these planned policies projections, South Africa would reach the upper bound of its 2030 NDC target range. These findings emphasise the emissions reduction potential of a stringent implementation of proposed economy-wide and sector-specific policy measures. Recovery response to the COVID-19 pandemic The COVID-19 pandemic has exacerbated South Africa’s health, social and economic challenges. After an economic downturn of 6% of GDP in 2020, the International Monetary Fund reported a recovery of 5% of GDP in 2021 (IMF, 2023b). Economic recovery was dampened in 2022 due to the global fallout of Russia’s invasion of Ukraine, more frequent and prolonged power outages and severe floods (IMF, 2023a). The CAT estimates a drop in emissions in 2020 of 6% below 2019 levels due to a drastic slowdown of domestic economic activity and international trade. The CAT estimates a 1% uptick in emissions between 2020 and 2021. The South African government introduced several support programmes in direct response to the immediate COVID-19 crisis and released a ‘Economic Reconstruction and Recovery Plan’ in October 2020 (Government of South Africa, 2021a; IMF, 2020). The plan comprised a range of both low-carbon and high-carbon recovery measures. High-carbon measures included the procurement of emergency electricity capacity in a technology-neutral auction, several measures to promote mining operations without specific conditions for low-carbon operations, and promotion of its liquefied petroleum gas (LPG) infrastructure. Low-carbon measures included further support for energy efficiency retrofits and promotion of low-carbon urban public transport. A tracking tool published in 2021 indicates the South African government has spent only around 3% of all recovery spending totalling USD 2.5bn on deliberately low-carbon measures (Global Recovery Observatory, 2021). South Africa’s response to the COVID-19 pandemic overall stands in contrast to domestic and international calls for a ‘green’ and low-carbon economic recovery (Climate Action Tracker, 2020; IEA/IMF, 2020). Recent developments on cross-sectoral policies In October 2023, South Africa’s National Assembly approved the Climate Change Bill, which would still need approval from the National Council of Provinces and the President (Centre for Environmental Rights, 2023; Republic of South Arica, 2023). The draft Climate Change Bill was originally released in June 2018 for public consultation and only formally introduced to Parliament in February 2022 (Government of South Africa, 2021c, 2022a). If passed, the Bill would be a significant step forward for South Africa, making its NDC legally binding. Under the legislation, the Minister responsible for Environmental Affairs together with the Ministerial Committee on Climate Change established by the Bill would have to set sectoral emission targets for each GHG emitting sector in line with the national emission target every five years and carbon budgets would be allocated to significant GHG emitting companies. Carbon budgets would put a cap on emissions and make it mandatory for companies to constrain their emissions. However, the Bill has been criticized for relying on intended measures by the National Treasury to levy fees for those who emit in excess of their set carbon budgets, allowing emitters to “pay to pollute” (Centre for Environmental Rights, 2023). South Africa adopted a carbon tax in February 2019 covering fossil fuel combustion emissions, industrial processes and product use emissions, and fugitive emissions such as those from coal mining (Climate Home News, 2019; Reuters, 2019). The tax was implemented in June 2019 (KPMG, 2019). Recent analysis indicates that the carbon tax currently does not effectively contribute to emission reductions given the low levy in comparison with other carbon prices, generous basic allowance and other available exemptions such as the use of offset credits (Szabo, 2021). A basic tax-free threshold for around 60% of emissions and additional allowances for specific sectors would result in tax exemptions for up to 95% of emissions during the first phase originally planned to go until 2022. While the full carbon tax rate is proposed to be R120/tCO 2 e (US$ 8/tCO 2 e), after exemptions, the effective tax rate is expected to be between R6–48/tCO 2 e (US$ 0.4–3/tCO 2 e) (KPMG, 2019). While the South African government adjusted the carbon tax rate before exemptions slightly upward to R144 (US$9 /tCO 2 e) as of January 2022, the first phase of the carbon tax roll-out will be continued until 2025 (KPMG, 2022; Steenkamp, 2022). The government further plans to reach a carbon price of US$ 30/tCO 2 e by 2030 and US$ 120/tCO 2 e by 2050. The Carbon Tax implementation will be accompanied by a package of tax incentives and revenue recycling measures to minimise the impact of the first phase of the policy (up to 2022) on the price of electricity and energy intensive sectors including mining, iron and steel (EY, 2017, 2018). In June 2022, the Presidential Climate Commission released its framework for a Just Transition in South Africa after extensive stakeholder consultations (Presidential Climate Commission, 2022). The framework aims to inform policy making at the nexus of climate and development issues in South Africa to enable deep, just, and transformational shifts. International partnership to support just transition in the energy sector At COP26, South Africa, France, Germany, UK, USA and the EU made a political declaration to establish a long-term partnership to support South Africa’s pathway to low-emissions and climate resilient development. The partners resolved to mobilise an initial USD 8.5bn in grants, concessional loans, guarantees, private investments, and technical support in the first five-year period between 2023-2027 to accelerate the decarbonisation of South Africa’s electricity system to achieve the most ambitious NDC target, support a just transition that protects vulnerable workers and communities, and support green industrialisation, including green hydrogen and low-carbon transport technologies (Farand, 2021; Government of South Africa, 2021d). The South African Just Energy Transition Partnership (JETP) builds on a country-led, donor-supported process by the South African government, putting a distinct focus on a just transition, including retraining and supporting coal workers. In November 2022, the Government of South Africa presented the Just Energy Transition Investment Plan (JET IP) for 2023 to 2027 (The Presidency of South Africa, 2022). The vast majority of the USD 8.5bn is planned for the electricity sector (USD 7.7bn), with USD 6.9bn going to electricity infrastructure. The JET IP indicates transmission and distribution infrastructure will be prioritised to enable the uptake of renewables and leverage large-scale private sector investment in renewables. Outside the electricity sector, USD 200m is tagged for “new energy vehicles” (NEVs), with a focus on battery electric vehicles, and USD 700 m will go to green hydrogen. The JET IP estimates the total financing needs of the low-carbon transition at USD 98.7bn. A more comprehensive implementation plan is expected to be launched in November 2023. However, uncertainty remains on the timeline for coal plant retirements amid the energy crisis, and many have raised concerns on the implementation of promised retraining for impacted coal workers (Civillini, 2023; Molelekwa, 2023). There is also concern that the plan could add to South Africa’s already significant debt burden, with only about 4% of the USD 8.5 bn provided as grants (Civillini, 2023; The Presidency of South Africa, 2022).</t>
-  </si>
-  <si>
-    <t>Switzerland’s emissions decreased from 45 MtCO 2 e in 2021 to 41 MtCO 2 e in 2022, 25% below 1990 levels. The decrease from 2021 to 2022 was mainly driven by a lower demand for gas and heating fuel in the building sector due to the warmer than average winter and subsequently lower need for space heating. The new Federal Act on a Secure Electricity Supply with Renewable Energies (Bundesgesetz Über Eine Sichere Stromversorgung Mit Erneuerbaren Energien, 2024), approved in a June 2024 referendum, greatly impacts emissions projections under current policies, potentially leading to emissions levels as low as 28 MtCO 2 e (excluding LULUCF) by 2030. This projected reduction is equivalent to almost 50% reduction below 1990 levels (excluding LULUCF). Switzerland would therefore meet its estimated domestic target of a 30% to 33% reduction in emissions below 1990 levels under current policies and would get very close to meeting its overall NDC of a 50% reduction below 1990 levels through even without the use of carbon credits from international mechanisms. CO 2 Act The CO2 Act is the key policy addressing emission reductions in Switzerland. To implement the Paris Agreement in Swiss legislation, an amendment of the CO 2 Act (known as Total Revision) was drafted to make the 2030 NDC target legally binding (Schweizer Parlament, 2020). However, the Act was rejected in a public referendum in 2021, forcing Switzerland to extend its expired and unambitious CO 2 Act to 2024 and start a process of drafting a new amendment. A new amendment of the CO 2 Act (known as CO 2 Succession Act) was subsequently presented and accepted by parliament in March 2024. This version, however, includes substantially weaker provisions than the original, and all draft versions appear to have decreased in ambition in every round; i.e. there is no longer a clear domestic emissions reduction target, and all bans were removed from the original text. Besides the 2030 target, the Act includes measures across various sectors including buildings, transport, industry, and aviation. It also covers climate adaptation support, support for companies exposed to the emissions trading system, and cleaner energy technologies like biogas and renewable fuels (Bundesgesetz Über Die Reduktion Der CO 2 -Emissionen (CO 2 -Gesetz), 2024). As this piece of legislation is still open for public consultation and amendments, and will only come into effect in 2025, it is not yet included in current policy calculations. Climate Protection Act On 18 June 2023, the Swiss people accepted another important piece of legislation in a public referendum, the Federal Act on Climate Protection Objectives, Innovation and Enhancement of Energy Security (the Climate Protection Act). It enshrines the net-zero emissions target for Switzerland by 2050 in law and sets interim and sectoral targets. The Climate Protection Act also promotes innovation by providing support for companies to achieve their net zero target, addresses energy security through a programme that funds the replacement of fossil-fuel and electric resistance heating systems and covers adaptation support. The Act, however, is mainly a framework law, mandating the parliament to work out more concrete objectives and measures to meet the 2040 and 2050 sectoral targets. The Federal Act on a Secure Electricity Supply with Renewable Energies (see below) is set out to address this to some extent. Carbon Levy (CO 2 tax) Switzerland introduced a carbon levy charged on fossil fuels in 2008, which covers ~35% of CO 2 emissions. The fee was repeatedly raised over time, culminating at CHF 120 per tonne of CO 2 (USD 130) in 2022, making it the highest CO 2 levy in Europe (Swiss Broadcasting Corporation, 2021) (Alex Mengden, 2024). The CO 2 Succession Act proposes to avoid many taxes altogether in favour of tax incentives and funding instruments in the transport, buildings, and industry sectors. The emphasis of Swiss climate policy is increasingly focussing on incentives rather than bans and restrictions, in order to avoid more rejection at the ballot, which means it includes some exemptions to the CO 2 levy, including plant operators that commit to reducing emissions by 2040. The majority of the proceeds from the levy are reimbursed to the citizens, or they flow into the (new) buildings programme and the economy. In 2023, the total revenue from the levy was around CHF 1.1 bn (USD 1.3 bn), of which roughly two thirds was redistributed to the population and the rest to the economy (Bundesamt für Umwelt BAFU, 2024a) Emissions Trading Scheme Another cross-sectoral instrument influencing greenhouse gas emissions is Switzerland’s emissions trading scheme (ETS). Companies participating in the ETS are excluded from an obligation to pay the emissions levy. After linking with the EU ETS in 2020, the price of Swiss emissions allowances broadly aligned with the higher EU allowance prices, which will accelerate emission reductions by the emitters responsible for a third of emissions resulting from the combustion of fossil fuels (EEX, 2019; Swiss Federal Audit Office, 2017). In November 2019, the Federal Council expanded the scope of the Swiss ETS to include civil aviation and fossil-thermal power plants (ICAP, 2020). ECHR Ruling In November 2020, a group of senior women in Switzerland filed a case against the Swiss government at the European Court of Human Rights (ECHR), claiming that inadequate climate policies threaten their health and violate their rights to life and private life. The court ruled in April 2024 that Switzerland had failed to protect these rights from climate change impacts and lacked an effective regulatory framework to meet emission targets, marking an unprecedented application of human rights law in climate litigation. Despite this landmark ruling, in June 2024, the Swiss parliament rejected the ECHR's decision, arguing that the country already has an effective climate strategy and the Swiss government subsequently also dismissed the court's findings in August 2024, asserting that its climate policies are adequate and have been bolstered by recent legislation. Environmental groups criticised this dismissal, arguing that Switzerland's plans do not sufficiently address the urgent need to limit global warming to 1.5°C. The CAT echoes these concerns, indicating that while some progress is being made, Switzerland still falls short of meeting the standards set by the ECHR ruling (Domhnall O’Sullivan, 2024; Imogen Foulkes, 2024; Sabin Center for Climate Change Law, 2024).</t>
-  </si>
-  <si>
-    <t>A key feature of Turkish policy planning involves reducing its reliance on fossil fuel imports. In 2022 alone, Türkiye’s net energy trade deficit was USD 81 bn, placing a burden not only on its economy but also leaving it vulnerable to volatile commodity markets and geopolitical shifts (Türkiye Cumhuriyet Merkez Bankası (Central Bank of the Republic of Türkiye), 2023; Ugurtas, 2022). Increasing energy independence is therefore a strategic goal of the Turkish government, with diversification of the energy mix central to government policy. Managing energy demand is a first step to reducing reliance on imported fossil fuels. The energy intensity of Türkiye’s economy is low and decreased by a further 6.2% in 2022 compared to the previous year (Republic of Türkiye Ministry of Energy and Natural Resources, 2024b). However, it is also the fastest growing energy consumer in the OECD (Republic of Türkiye Ministry of Foreign Affairs, 2022). Through its 2030 Energy Efficiency Strategy and Action Plan, Türkiye aims to reduce energy consumption by 16% by investing USD 20 bn in energy efficiency projects (Republic of Türkiye Ministry of Energy and Natural Resources, 2024b). If realised, these investments could allow Türkiye to decouple energy consumption from economic growth and reduce dependence on imported fossil fuels. Türkiye intends to have 120 GW of installed wind and solar capacity by 2035. Along with hydropower and biomass, Türkiye’s installed renewable capacity in 2035 will be 160 GW (Republic of Türkiye Ministry of Energy and Natural Resources, 2024c; Turkish Ministry of Energy and Natural Resources, 2022). Meeting the wind and solar targets will involve bringing at least 7.5–8 GW online every year, significantly more than what was envisioned in Türkiye’s 2022 National Energy Plan. However, implementation will need to shift up a gear, as the country is struggling to meet even its National Energy Plan’s targets due to a slower than planned renewables rollout. For instance, 2023 saw the least wind capacity in 13 years added to the grid. Regularity changes including streamlining the permitting process and improving investment conditions are intended to stimulate private investment in renewable energy projects. Despite the improved commitment to renewables, Türkiye is yet to commit to a phase-out plan for coal or fossil gas, which need to be taken out of the energy mix in the 2030s if Türkiye is to align with the 1.5°C temperature goal (Robins, 2023; Turkish Ministry of Energy and Natural Resources, 2022). Instead, Türkiye plans to become a fossil gas hub and expand coal capacity (Robins, 2023; Turkish Ministry of Energy and Natural Resources, 2022). If Türkiye is serious about its net zero emissions target, then it will need to introduce a plan to phase out fossil fuels. The most significant piece of industrial policy of the last year has been the introduction of an Emissions Trading System (ETS) in line with the EU’s ETS. This will likely be the backbone of emissions reductions in Türkiye’s industry sector and will help mitigate some of the more severe impacts of the EU’s Carbon Border Adjustment Mechanism (CBAM). CBAM will levy a carbon tax on some product groups imported into the EU if they fail to align with EU emissions standards (European Commission, 2024). Ramping up production of Türkiye’s domestically produced electric vehicle (EV), the Togg, and high-speed electric trains forms an important part of Türkiye’s industrial strategy which can support domestic uptake while opening a new revenue stream from exports. Türkiye also plans to invest USD 298 bn up to 2053 in the transport sector. Sectoral targets include increasing the share of rail in passenger transport to 5.31% and to 20.12% in freight transport by 2035, up from 2019 levels of 0.89% and 3.13%, respectively (Republic of Türkiye Ministry of Transport and Infrastructure, 2023).</t>
-  </si>
-  <si>
-    <t>The CAT estimates the UAE’s 2030 emissions under current policies are set, in a best case scenario, to plateau close to 2022 levels, at around 214 MtCO 2 e, or continue to increase to about 259 MtCO 2 e. Under current policies, the UAE is set to miss its latest 2030 emissions reduction target. To meet its 2030 NDC target, the government needs to implement more ambitious policies and reduce its 2030 emissions by a further 15–40%. However, if the UAE implements the planned policies outlined in both its NDC and LTS, it could potentially reach its target. For more information, please see the Assumptions tab. Since 2023, the UAE has published information on many relevant climate policies across all sectors of the economy. Both its NDC from 2023 and its LTS from early 2024 provide details on policies and action, both current and planned, in the power, industry, transport, buildings, agriculture and waste sectors (Government of the UAE, 2023a, 2024b). This is a significant step in transparency, which allows for a better understanding of how the UAE plans to reduce its emissions to meet its NDC and net zero targets. However, it also shows a critical overreliance on carbon capture and storage both in the power and industry sectors, a smokescreen allowing the country to continue expanding its oil and fossil gas production and use while claiming to be on the way to net zero. In recent years, the UAE has announced plans to invest in renewables both at home and abroad, including a USD 100bn commitment together with the United States (Associated Press, 2023). However, in parallel it continues to invest into fossil fuel production. The UAE is planning to significantly increase its oil production in the next years, and is pushing to reach “gas self-sufficiency”, with major investments in offshore gas production. In November 2022, ADNOC announced a USD 150bn investment plan to expand its oil and gas business in the next five years (The Guardian, 2023). As part of this plan, ADNOC awarded contracts worth USD 17bn in October 2023 for the Hail and Ghasha Offshore Development project. This project aims to produce 1.5 billion standard cubic feet per day (bscfd) of gas before the end of the decade (Reuters, 2023). For more details, see the Power sector section below. The developments and the investment going towards new fossil fuel infrastructure are not consistent with limiting global warming to 1.5°C, instead are likely to lock the UAE into a high-emissions trajectory and undermine its transition towards renewable energy. Instead of ramping up its gas production towards self-sufficiency, the UAE should set out an ambitious plan to phase-out its dependency on gas for electricity and switch to renewables, which would reduce prices and price volatility for consumers, and avoid the risk of stranded assets (CAT, 2022).</t>
-  </si>
-  <si>
-    <t>The US will need to implement additional policies to reach its 2030 and long-term targets. After an increase in GHG emissions between 2021 and 2022, emissions started to decline in 2023 (-1.9%) (Rhodium Group, 2024). The government has set a target to reduce emissions by 3.8–4.2 GtCO 2 e/year in 2030. According to our projections, emissions are forecasted to decline at an average of 1.7%–3.9% per year and reach between 4.6–5.4 GtCO 2 e/year by 2030 (29%–39% below 2005 levels; and 19%–31% below 1990), excluding emissions from land use, land use change and forestry (LULUCF). Under these projections, the US would achieve 64%–87% of its emissions reductions target in 2030, indicating a gap of 13%–36% that would need to be filled with new and additional climate policies and action. As it stands, the 2030 target is not 1.5˚C compatible. Reaching a level in line with a global least-cost pathway requires further reductions of 1.4–2.2 GtCO 2 e below the current policy pathway. Compared to CAT projections in August 2023, our range of emission projections includes an updated estimate of the Inflation Reduction Act’s (IRA) impact, as well as estimates of the impact of the US Environmental Protection Agency’s (EPA) 2024 regulations for the power and transport sectors. As a result, the US emissions projections decreased relative to the CAT’s previous projections, while the range, based on existing policies, widened for 2030–2035. The upper bound decreased by 2% and the lower bound decreased by 8%. The reduced, widened range in emission projections highlights the continued effort by the US government to cut emissions, while recognising the high uncertainty of policy outcomes; especially for the government’s flagship climate policies, including the IRA and the Bipartisan Infrastructure Law (BIL). The IRA injects USD 370bn into the US economy over a 10-year period. This infusion takes the form of tax credits, grants, and loans intended to develop and deploy the clean energy technologies and investments that are essential for the economy's decarbonisation (The White House, 2023a). Since the IRA's implementation in 2022, the country has witnessed a significant surge in public and private investment in clean energy projects and infrastructure: between August 2022 and February 2024, investment in announced clean energy projects and infrastructure totalled USD 352bn. Specific highlights include record investment in battery and electric vehicle (EV) manufacturing and in grid and transmission infrastructure (Climate Power, 2024c). Due to these investments, the share of clean energy investments in total investments increased from 3.7% in Q4 of 2022 to 5% in Q4 in 2023, representing a significant uptick in the role that clean energy investments play in the US economy (Rhodium Group; MIT CEEPR;, 2024). Given the scale of public investment, some studies suggest that the IRA could spur USD 3tn in private investments over the coming decade (Goldman Sachs, 2023). The BIL and IRA, alongside the Creating Helpful Incentives to Produce Semiconductors (CHIPS) and Science Act, have set the stage for record private investment in the construction of domestic manufacturing facilities (U.S. Department of the Treasury, 2023b). Before the IRA and CHIPS Act were signed, annual investment in manufacturing construction remained below USD 150bn. Since the acts’ passage, investment surged to an all-time high of USD 223bn by February 2024 (FRED Economic data, 2024; Joint Economic Committee, 2024). Investment in the EV supply chain, especially in battery cell manufacturing and critical mineral production, has increased significantly and accounted for nearly two-thirds of all clean manufacturing investments by the end of 2023 (Rhodium Group; MIT CEEPR;, 2024). As a result of this increase in investment, the US surpassed the EU in battery cell manufacturing capacity in 2023, even though the EU’s capacity was two times larger than the US’ capacity in 2021 (Delgado et al., 2024). These investments contribute to job creation, with estimates showing that the IRA’s provisions have already generated over 270,000 clean energy jobs (Climate Power, 2024b). The act has also contributed to a more just energy transition by targeting disadvantaged communities and rural areas. Many of the announced investments specifically target and aim to contribute to the economic development of these regions and communities (U.S. Department of the Treasury, 2023a). In early 2024, the US expanded its climate policy portfolio through the addition of several EPA policies (U.S. Environmental Protection Agency, 2024i, 2024l). The EPA introduced several standards for gas and coal-fired power plants and updated its vehicle emissions standards. Even though these standards were watered down before their finalisation (see Electricity generation and Transport sections below), they add an important regulatory complement to the incentive-based IRA: by setting yearly emissions levels for technologies, the standards provide important guidance for the private sector. To realise its 2030 and 2035 targets and to align with the Paris Agreement’s 1.5˚C temperature goal, the US has to implement further, more ambitious policies and measures. Additional measures could focus on those sectors in which ambitious action has yet to be taken, such as the building or agriculture sector. At the same time, the government can further strengthen existing policies across all sectors; for example, the government could extend the IRA beyond 2030, introduce coal phase-out targets for 2030, and enhance energy efficiency standards (America Is All In, 2024). Manufacturing capacity could also be strengthened, in particular for wind turbine and heat pump production (IEA, 2024a). Given that the federal government’s jurisdiction is limited some policy areas, state governments can play a significant role. Some states, such as Massachusetts, Michigan, and Minnesota, have recently introduced climate policies that are more ambitious than at the federal level (Joselow &amp; Montalbano, 2023). To advance climate action at the subnational level, state governments can adopt of renewable portfolio standards (RPS) and introduce sales targets for EVs. Despite the IRA’s remarkable measures to support clean energy and address climate change, the IRA includes several concessions to the fossil fuel industry. The concessions are described in the Power section.</t>
-  </si>
-  <si>
     <t>The CAT estimates that Japan’s implemented policies will lead to emission levels of 31% to 38% below 2013 levels in 2030, falling short of its latest NDC target of a 42% reduction below 2013 levels, both excluding LULUCF. Without additional measures, Japan will likely miss its NDC target, as well as the 60% reduction below 2013 levels target, the only one we estimate to be 1.5°C-compatible . In 2023, the government adopted the Green Transformation (GX) Basic Policy, a set of initiatives that aims to generate approximately JPY150 tn (approx. USD 1 tn) of public-private investment over the next 10 years (METI, 2023e). This new strategy seeks to ramp up decarbonisation efforts in key industrial sectors through the GX League, a voluntary group of industries who individually set their own decarbonisation targets to be in line with the national reduction targets and participate in an emissions trading scheme to achieve them (i.e. 46% emissions reduction in 2030 below 2013 levels and achieving carbon neutrality by 2050) (CAS, 2022; METI, 2022a). As of March 2024, 747 companies which collectively account for 50% of CO 2 emissions (including indirect emissions from electricity use in households) have joined the group (METI, 2024a). In 2024, as part of the GX basic policy, the Japanese government issued the world’s first sovereign transition bonds called the Japan Climate Transition Bonds. The first tranche was auctioned in February 2024. However, the GX Basic Policy places more emphasis on economic growth and energy security, than on prioritising ambitious decarbonisation efforts. In fact, the new strategy does not provide any emissions reduction targets for 2030 or 2050. While it finally lays out a blueprint for the introduction of a carbon pricing scheme, there are concerns that the system envisioned by the government will not be effective in reducing Japan’s emissions. It remains unclear whether the emissions trading scheme currently being considered for 2026 will still be based on voluntary participation (InfluenceMap, 2023; METI, 2023d). On top of that, the carbon levy, which will only be implemented in 2028, is expected to be set at a low level (Renewable Energy Institute, 2023d). There are also concerns that the GX Basic Policy will keep Japan wedded to coal, as it puts a strong emphasis on the need to develop CCS technologies, and ammonia and hydrogen co-firing, as tools to curb emissions in coal fired power plants. These technologies are all distractions from the need for Japan to phase out coal-fired power by 2030 at the latest. Studies show that Japan could achieve between 80-90% of clean electricity share by 2035, thereby reducing its dependence on fossil fuel and bolstering its energy security (Renewable Energy Institute, 2024; Shirashi et al, 2023). In a significant policy shift, Japan unveiled plans to build new generation nuclear reactors, as part of the GX Basic Policy. Despite this policy reversal, the first turn toward nuclear power since the Fukushima disaster, many regulatory and political hurdles remain, and it is unlikely that the new reactors will be operational before 2035-2040. One policy expected to contribute to significant additional reductions, though its effects would only take place in the long-term, is the revision of building standards by which all new houses and buildings will need to comply with upgraded energy efficiency standards from 2025 (MLIT, 2022). This is a significant step forward as the emissions from the buildings sector increased by 34% in 2020 above 1990 levels while Japan currently aims to achieve 28% emissions reduction in 2030 below 1990 levels. (GIO, 2022; Government of Japan, 2021b). To also support decarbonising existing houses and buildings, several measures have been introduced including financial support for house renovations to improve energy efficiency as well as promoting the use of renewable energy in buildings (MLIT, 2022). Japan aims to achieve on stock average net-zero energy consumption for newly constructed buildings (ZEBs) and houses (ZEHs) by 2030 as well as all buildings and houses by 2050 (MLIT, 2022). Additionally, the Tokyo Metropolitan Government has mandated majority of new buildings and houses to install solar panels from 2025 (The Japan Times, 2022b) The table below illustrates the fuel mix in the power sector in 2022, and the different assumptions for our projections, in comparison to the IEA World Energy Outlook (WEO) 2023 (IEA, 2023) (See Assumptions tab for details). Table 1: Electricity mix in Japan: 2022 historical data and 2030 projections</t>
   </si>
   <si>
@@ -209,231 +208,231 @@
     <t>In 2022, emissions from industry, including industrial processes, oil and fossil gas production and excluding indirect emissions from power consumption in industry, reached 48.4 MtCO 2 e in Argentina, or 14% of total GHG emissions (Government of Argentina, 2024a). In 2022, industry represented 22% of total energy demand (IEA, 2023). The biggest subsectors by production value are food and beverage manufacturing (31%), construction (14%) and the manufacturing of chemical substances and products (12%). The industrial sector is also the biggest consumer of fossil gas after thermoelectric generation plants. However, most process-related emissions stem from steel and cement production (Government of Argentina, 2023a). The government seeks to promote energy management systems for industrial companies. In 2018, the Ministry of Energy passed Provision 3/2018, which establishes that companies benefitting from reduced electricity prices under Resolution 1-E/2017 have to implement the ISO norm 50001 on energy management systems, including the development of an energy management action plan, energy performance targets and indicators to monitor progress (Ministry of Energy and Mining, 2018). In its 2022 climate strategy, the government reinstates its existing plans and measures for reducing energy consumption in businesses (Government of Argentina, 2022d). Oil and fossil gas Argentina continues to develop its oil and gas sector, mostly focusing on increasing production in the Vaca Muerta shale fields, as well as investing in transport and export infrastructure. In 2024 both oil and fossil gas production continued to increase compared to previous years, with large contributions from Vaca Muerta. In the first half of 2024, gas production increased 5% compared to the same period in the previous year, reaching 25,000 million cubic meters. Oil production also continues to increase, reaching 692 thousand barrels per day in May 2024 (an 8.8% increase compared to 2023), with Vaca Muerta accounting for almost 70% of the total (Ambito, 2024b, 2024a). Major ongoing developments in the oil and fossil gas industry include: The construction of a new segment of the Nestor Kirchner fossil gas pipeline (Iden, 2023; Redacción Central, 2020) The construction of a compressor plant in Tratayén, which increased the carrying capacity of the existing Nestor Kirchner fossil gas pipeline by 50% (Government of Argentina, 2024d) Development plans for the Vaca Muerta south fields (Ciruzzi, 2024) Plans to develop an LNG port in Rio Negro (LNGPrime, 2024) Agreement with Golar LNG and Pan American Energy to deploy a 2.45 mt/year Floating Liquified Natural Gas plant in Argentina to channel exports from Vaca Muerta (Enerdata, 2024) Offshore exploration activities off the coast of Buenos Aires failing to find fossil fuels, with some players withdrawing among decreasing interest (Terzaghi, 2024) These developments will most likely impact total emissions in the country through increases in fugitive emissions, as well as creating lock-in of fossil infrastructure and disincentives for a deeper transformation of the energy sector. An increased dependence on internationally-traded goods can increase Argentina’s vulnerability to external shocks. The increased production of fossil fuels could also lead to higher energy consumption. As part of its push towards domestic oil and fossil gas production, the government also plans to set out measures to reduce flaring and leakage, but so far as not provided any specific measures or targets (Government of Argentina, 2022d). Over the period 2012-2022, flaring has doubled from 600 MM3 to 1200 MM3 (GFMR, 2023). Hydrogen Argentina has begun setting out plans to produce green hydrogen, both with the aim of domestic use and exports. In 2023, it set out its National Strategy for the Development of a Hydrogen Economy. This strategy sets out targets to produce 5 mt/y of “low emissions hydrogen”, which will require 30 GW of electrolysis capacity, and 55 GW of renewable electricity generation capacity by 2030. Roughly 80% of all production is expected to be exported (Government of Argentina, 2023c). In 2022, it was announced that Australian firm Fortescue will invest USD 8.4bn in the Argentinian province of Rio Negro to develop green hydrogen. The first phase of the project will generate 650 MW and include a wind farm and a port for transportation. It will initially be destined for export, but capacity can be expanded to 8 GW in future phases, enabling the dedication of some production for the domestic market. This project fits into a provincial plan to produce 2.2 Mt by 2030 (Garcia Pastormerlo, 2021). In its 2022 climate strategy, the government also included plans to prepare a National Hydrogen Strategy with more clear milestones for Argentina’s domestic hydrogen industry (Government of Argentina, 2022d). In 2023, the EU also announced plans to finance the development of green hydrogen in Argentina. The original plan to invest EUR 200 million to develop green hydrogen for export to Europe is now under discussion with the current administration, who pledged to present new legislation this year to streamline processes related to hydrogen production, certification and export (Collins, 2024).</t>
   </si>
   <si>
+    <t>Australia’s industrial sector, including industrial energy use, industrial process emissions and fugitive emissions, accounted for 30% of Australia’s total emissions excluding LULUCF in 2023 (DCCEEW, 2023b). The government announced the ‘Future Made in Australia’ plan in the 2024–25 budget, allocating AUD 22.7bn (USD 14.9bn) over 10 years to attract investment in key industries and realise Australia’s potential to become a “renewable energy superpower” (Australian Government, 2024). Priority industries identified under the scheme include renewable hydrogen, green metals, low carbon liquid fuels, critical minerals processing, and clean energy manufacturing including battery and solar panel supply chains. Australia is a major exporter of both coal and LNG. Emissions from coal and LNG use at the final export destination are not accounted for in the national greenhouse gas inventory. Australia exports more than double its domestic emissions from its coal, fossil gas and oil exports (Climate Action Tracker, 2023b; Climate Analytics, 2024a). Coal mining Australia is the world's largest exporter of metallurgical coal, accounting for around half of all exports, and the second-largest exporter of thermal coal (DISR, 2024b). In 2023, Australia was the second-largest coal exporter overall and the fifth-largest coal producer (Energy Institute, 2024). Despite a projected decline in domestic coal power, coal production and exports are forecast to remain stable, at odds with the global efforts towards decarbonisation. Close to 90% of produced coal was exported in 2023 (DCCEEW, 2024a). The government projects that run-of-mine coal production will increase by 9% from 559 Mt in 2023 to 612 Mt in 2027, before falling to 488 Mt by 2035 (DCCEEW, 2024h). Sustained or even increasing levels of coal production are clearly inconsistent with the goals of the Paris Agreement (IEA, 2023d). 1.5°C-compatible pathways would see coal production fall 78% below 2020 levels by 2030 (SEI et al., 2023). Government approval of coal mine projects remains a contentious issue in Australia. In September 2024, the Environment Minister gave the green light for three NSW mines to extend their operations for another 30–40 years: the Narrabri Underground Mine Stage 3 expansion, the Ravensworth Underground Mine, and the Mount Pleasant project (ABC News, 2024d; The Guardian, 2024). Combined, these three projects are expected to result in additional emissions of 1.36 GtCO 2 e (The Australia Institute, 2024b). These approvals are in addition to the four coal mining projects approved in 2023: the Isaac River and Ensham mines in Queensland, and the Narrabri Underground and Mount Pleasant mines in NSW. As of December 2023, there were 53 coal projects in the development pipeline, of which ten were already committed (DISR, 2023). While many of the proposed coal projects are still speculative, Australia has the highest number of proposed coal mine projects among OECD nations (Global Energy Monitor, 2023). Fugitive emissions from coal mining are discussed below in the Methane section. Oil &amp; gas production Australia was the world's third-largest exporter of liquefied natural gas (LNG) in 2023, after being the largest exporter in 2021 (Energy Institute, 2024). Around 80% of fossil gas production goes towards LNG production for export, including LNG plant own consumption (DCCEEW, 2023a). The Federal government released its Future Gas Strategy in May 2024 which sets out the government’s ongoing commitment to development of new fossil gas supply and continued LNG exports as a “reliable and trusted trade and investment partner” (DISR, 2024a). The strategy embeds the role of fossil gas in Australia’s domestic energy sector and exports to 2050 and beyond, and (wrongly) claims that fossil gas is needed for the global energy transition. This is despite the inclusion of the IEA’s Net Zero Emissions scenario in the analysis, which clearly calls for a rapid decline in global gas demand (IEA, 2023d). As is the case for coal, Australia still does not have a gas phase-out strategy and timeline. The government projects that LNG production and export will be sustained at current levels until at least 2035, with 82 Mt expected in 2035 – the same as in 2023 levels (DCCEEW, 2024h). These projected exports account for several large-scale projects sanctioned across 2021 and 2022. The Barossa backfill to Santos’ Darwin LNG is expected to commence in 2025. Woodside’s massive Scarborough development and linked Pluto LNG plant expansion is expected to start up in 2026. Backfill to Shell’s Prelude FLNG facility from the Crux field is expected to come online in 2027. Both Crux and Barossa are carbon-intensive fields with a high percentage of reservoir CO 2 (DCCEEW, 2022b). The government’s LNG projections also assumed that Woodside’s Browse project would startup in 2030, but the project appears to have stalled with the state Environment Protection Agency deeming the project “unacceptable” (ABC News, 2024b). The biggest uncertainty for future gas production in Australia is Tamboran Resources’ plan to frack the Beetaloo basin in the Northern Territory (NT) and export the gas via a new 6.6 Mtpa LNG plant to be built in the Middle Arm Precinct in Darwin. This could eventually be expanded to 20 Mtpa. Far from achieving net zero domestic lifecycle emissions, as recommended by the NT government’s Pepper Inquiry, emissions from Beetaloo and Middle Arm development have been found to be severely underestimated, and the potential to offset its emissions are greatly exaggerated: it would generate more emissions than the 2030 emissions reduction goal under the Safeguard Mechanism regulations, and require international offsets currently banned under that legislation (Climate Analytics, 2023). The Middle Arm development was the subject of a recent federal Senate Inquiry into the environmental impact of the development and the federal government’s AUD 1.5bn commitment for the project, which failed to reach a unanimous set of recommendations (ABC News, 2024c). Despite being presented as a sustainable precinct, the industrial project could include fossil gas-generated hydrogen (“blue” hydrogen) production, minerals processing, and petrochemical processing, in addition to the current and planned LNG facilities (ABC News, 2024c). Fossil gas companies are also exploring opportunities to frack the Canning Basin, in Western Australia (ABC News, 2023b; Climate Analytics, 2024b). The oil and gas industry continues to benefit from significant government support, which included AUD 14.5bn in spending and tax breaks in 2023–24 (The Australia Institute, 2024a). The largest component of this total is the Fuel Tax Credit Scheme at AUD 9.6bn which subsidises fossil fuel consumption. In 2023, the government revised the Petroleum Resource Rent Tax (PRRT) to introduce a cap on the use of deductions by LNG producers to no more than 90% of their assessable income. To date, no Australian LNG project has paid any PRRT (Minister for Finance, 2023). These subsidies support the fossil fuel industry and its exports, despite the need for a global phase-out. CCS Carbon capture and storage (CCS) is being proposed as a solution to mitigate reservoir CO 2 from gas fields which historically has been vented directly to the atmosphere. This is the case at Chevron’s Gorgon plant, Australia’s only operating CCS project, and at Santos’ Moomba CCS project, which is under construction and scheduled to commence operation in 2024. However, implementing CCS for reservoir CO 2 does nothing to mitigate fugitive methane emissions that occur throughout the gas lifecycle, and therefore would mitigate only a portion of the greenhouse gas emissions associated with fossil fuel production. Nevertheless, CCS projects continue to be pursued by gas producers with government backing. Chevon’s CCS facilities at its Gorgon LNG plant have consistently underperformed and fallen short of sequestering the 80% of reservoir CO 2 as required by the project’s state environmental approvals. Despite having an announced annual capture capacity of 4 MtCO 2 /year, Gorgon CCS has sequestered just 10 MtCO 2 in total over the five years to August 2024 (ABC News, 2023a; Chevron, 2021, 2024). Santos is also planning the Bayu-Undan CCS project to enable the development of the Barossa field offshore near Darwin. The project would involve capturing CO 2 from the carbon-intensive Barossa field, transporting it via Darwin by pipeline, and then sequestering in the depleted Bayu-Undan field in the Timor Sea, off the coast of Timor-L'este. The government’s 2023 sea dumping legislation paves the way for the project to proceed (ABC News, 2023c). The Bayu-Undan CCS project has a design capacity of up to 10 MtCO 2 /year and is one of two projects proposed as part of the Middle Arm development, with the other being INPEX’s Bonaparte project (Northern Territory Government, 2024). The government is counting on CCS as its predominant strategy to reduce fugitive emissions under the Safeguard Mechanism. The government estimates that by 2030, CCS will capture 1 MtCO 2 e (AR5 values) from LNG facilities, in addition to CO 2 captured at Gorgon, and 1.5 MtCO 2 e from domestic gas production at Moomba (DCCEEW, 2023b). The government projects that CCS at LNG plants will scale up to 4 MtCO 2 e by 2035. However, given the experience at Gorgon, it is doubtful whether any of these projects will achieve their design capture rate. Hydrogen The government released an updated National Hydrogen Strategy in 2024 (DCCEEW, 2024c). Under the strategy the government has set baseline and stretch targets for renewable hydrogen production of 0.5–1.5 million tonnes per year by 2030 and 15–30 million tonnes per year by 2050. The government is also targeting exports of green hydrogen (or equivalent derivatives) of 0.2 million tonnes by 2030, and a stretch target of 1.2 million tonnes. The 2024 National Hydrogen Strategy specifically prioritises renewable hydrogen production in comparison to the 2019 National Hydrogen Strategy which defined ‘clean’ hydrogen as hydrogen produced via electrolysis with renewable energy or hydrogen derived from fossil fuels with greater than 90% carbon capture. The proposed Guarantee of Origin Scheme would measure and verify the emissions intensity of produced hydrogen. The Hydrogen Production Tax Incentive, a component of the Future Made in Australia policy package, will provide an incentive of AUD 2/kg renewable hydrogen for up to 10 years of production for projects that reach final investment decision by 2030. The AUD 4bn Hydrogen Headstart program, introduced in 2023, provides funding support to selected large-scale renewable hydrogen projects to cover the current gap between production cost and market prices (DCCEEW, 2024c). As of October 2024, there were 14 pilot-scale hydrogen projects operating in Australia with all except two producing renewable hydrogen (CSIRO, 2024). Safeguard Mechanism The Safeguard Mechanism is the Australian government’s central policy for reducing industrial emissions. It has been in place since 2016 and was substantially reformed in 2023. The Safeguard Mechanism applies to large industrial facilities emitting more than 100 KtCO 2 e per year and imposes declining limits on facility net emissions or ‘baselines’. The power sector is treated separately from industrial facilities. Under the reformed SGM, baselines will decline by 4.9% each year to 2030 (DCCEEW, 2024k). To comply with declining baselines, facilities must either cut their emissions, acquire Australian Carbon Credit Units (ACCUs), or purchase newly introduced Safeguard Mechanism Credits (SMCs). The reform allows for unlimited use of offsets to meet declining baselines. Past 2030, baselines decline rate will be determined in five-year blocks to align with the 2050 net zero target (DCCEEW, 2023b). The design of the mechanism assumes significant new fossil fuel projects to come online, such as new carbon-intensive gas fields and coal mines (Clean Energy Regulator, 2023b; Department of Climate Change, 2023e; Reputex, 2023). The reform mandates new shale gas projects must have net zero scope-1 emissions, i.e. domestic emissions occurring during fossil gas production, and that new gas fields will be given a zero baseline for reservoir CO 2 (DCCEEW, 2024k). The effectiveness of the mechanism depends on the extent to which existing and new facilities covered under the mechanism rely on offsets to meet their baselines. In 2023, 219 facilities were covered by the SGM accounting for gross emissions of 138.7 MtCO 2 e (Clean Energy Regulator, 2024), which was approximately 26% of Australia’s total emissions excluding LULUCF (DCCEEW, 2024i). The same facilities also surrendered 1.2 million ACCUs in 2023, meaning that SGM facilities collectively offset 1.2 MtCO 2 e to meet their baselines in preference to making direct on-site emissions reductions. The reformed SGM aims to reduce net SGM facility emissions from 138 MtCO 2 e in 2022 to around 100 Mt in 2030 (AR5 values). The government projects that gross emissions from SGM facilities will reduce from 138 MtCO 2 e in 2022 to 121 MtCO 2 e in 2030, and that net emissions (i.e. accounting for offsets), would fall to 93 MtCO 2 e in 2030. This reduction implies that less than half of the abatement to 2030 will result from on-site emissions cuts.</t>
+  </si>
+  <si>
+    <t>Oil and gas production At over a third of total emissions, oil and gas production represents Canada’s largest source of emissions (Environment and Climate Change Canada, 2024). While the sector’s emissions dropped in 2020 due to the pandemic, they are projected to reach again 2019 levels under current policies by 2030 as production is projected to increase. Canada’s exported emissions from oil and gas are continuing to rise, surpassing its total domestic GHG emissions, and sitting at about 939 MtCO 2 in 2022 (Bernstien, 2024). This comes at a time when the IEA has called for no new investments in oil, gas and coal if we are to stay below the 1.5°C limit of the Paris Agreement. The government seems incapable of kicking its oil and gas addiction. It has promised to set a cap on emissions for the sector, and believes this can be achieved while increasing production. Regulations for the cap are being consulted on in 2024 and are due to be finalised in 2025. They are not yet modelled in our projections. The government is also planning to strengthen methane emission regulations in the sector (see the Methane section below) (Government of Canada, 2023b). In April 2022, the government approved an offshore oil and gas megaproject, Bay du Nord (Impact Assessment Agency of Canada, 2022a). The project is required to be net zero from 2050 onwards, but production could continue until 2058 (Impact Assessment Agency of Canada, 2021, 2022a). The environment and energy ministers disagree over whether this will be the last development of its kind in Canada (CBC News, 2022). Whether the project will actually proceed is unclear: the company delayed the project by three years amidst concerns over high costs, and challenges to the environmental and economic assessments continue (Canada, 2023; Federal Court of Canada, 2023; Nickel, 2023; Sierra Club, 2024). The costs of current oil and gas expansion projects continue to rise. The Trans Mountain oil pipeline expansion, due to start operation in 2024 (Calgary Herald, 2023; Trans Mountain Corporation, 2022), is now expected to cost seven times more than when the government first purchased the pipeline (CAD 5.4 bn) (Lindsay, 2021; Williams, 2023). In June 2022, a budget watchdog concluded that it was not viable and would cost the government around CAD 600 million in net losses (Thurton, 2022). Others have estimated that losses will be much higher (The Energy Mix, 2022; Williams, 2023). Costs associated with the pipeline for the country’s first LNG export terminal, on the country’s west coast, are also soaring (Jang, 2022; Simmons, 2022). While this pipeline is not government-owned, there are questions as to whether it will be able to recoup all of the subsidies provided (Simmons, 2022). The LNG project will only begin exporting fossil gas to Asia in 2025–2026. Meanwhile, a new anti-greenwashing regulation is causing oil and gas industry associations to scrub their websites of unsubstantiated CCS claims (Noakes, 2024). Net-Zero Producers Forum Canada is part of the ‘Net Zero Producers Forum’, along with other oil and gas majors: Norway, Qatar, Saudi Arabia, the UAE and the US (Natural Resources Canada, 2021a; U.S. Department of Energy, 2021). The forum’s stated aim is to develop ‘pragmatic net zero emission strategies’, including reducing methane emissions and supporting the use of CCS, but it does not tackle the core issue of phasing down production. Beyond holding its first Ministerial meeting and establishing a working group in March 2022, there is little evidence of concrete action more than a year after its formation. Meanwhile, investors and international oil companies continue to exit Canada’s tar sands (Morgan, 2020; Reuters, 2021; The Canadian Press, 2020; Total, 2020; Tuttle, 2022). Beyond Oil and Gas Alliance (BOGA) The province of Quebec is a member of BOGA, but Canada as a whole is not. In April 2022, Quebec passed a law banning any further production and mandated that existing drill sites be shut down within three years (Government of Quebec, 2022). The move is largely symbolic as the province is not a producer of oil and gas (Canada Energy Regulator, 2022). Coal mining In 2021, the government committed to banning thermal coal exports from and through Canada by 2030 (Liberal Party of Canada, 2021b; Prime Minister of Canada, 2021b). The reference to ‘through Canada’ is important, as many American west coast miners export their coal through Canada due to resistance to developing the export infrastructure in their own country (Institute for Energy Economics and Financial Analysis, 2021; Kuykendall, 2021). While establishing the ban is in the trade minister’s mandate letter , he has not yet taken action to implement it (Global Affairs Canada, 2022; Prime Minister of Canada, 2021a). On the contrary, Canadian coal exports soared in 2023, causing the opposition party to call the government to task on this issue (The Canadian Press, 2024a, 2024b). Canada had been criticised for its hypocritical stance on coal mining, and for not subjecting a thermal coal mine expansion to a federal impact assessment, notwithstanding its position in the Powering Past Coal Alliance (Rabson, 2020). In June 2021, Canada clarified its policy position on thermal coal mining, finding that any new mines or expansions of existing mines would likely cause unacceptable environmental effects (Government of Canada, 2021i). One coal mining expansion project is still attempting to get approval, with environmental groups fighting the government's decision to lift the requirement for an environmental impact assessment (Ecojustice, 2023; Impact Assessment Agency of Canada, 2022b).</t>
+  </si>
+  <si>
+    <t>Chile is the world’s leading copper exporter, and the mining and industry sector is Chile’s largest consumer of final energy, accounting for 36% of energy consumption in 2021 and approximately 17% of total GHG emissions (IEA, 2024a). In 2021, 44% of mining electricity consumption came from renewable sources, and it is estimated that it will reach 62% in 2025. Chile has established several targets to minimise emissions from the mining and industry sector in its energy strategy (PEN). They include: an emissions reduction target of 70% of direct GHG emissions from fuel use in the industry and mining sector by 2050 below 2018 levels, an improvement of energy intensity of large energy consumers by at least 25% in 2050 below 2021, a requirement that at least 90% of energy for heating and cooling in industry must come from sustainable sources by 2050, a goal of 100,000 new energy jobs by 2030, direct and indirect, from sustainable energy projects in new energy-related industries, and a requirement that 100% of medium and large companies in Chile must implement effective and monitorable energy efficiency and/or renewable energy measures. These measures are also featured in Chile’s LTS (Gobierno de Chile, 2021; Ministerio de Energía, 2022c). Mining companies themselves play an important role in meeting these targets. The Chilean Copper Commission (COCHILCO) has carried out surveys and compiled data on GHG emissions and energy consumption, the Green Mining Roundtable was launched in 2019, and the Chilean Economic Development Agency (CORFO) has supported the deployment of hydrogen vehicles for mining (Ministerio de Energía, 2020a). The deployment of green hydrogen and its derivatives in the mining sector is a key component of Chile’s Green Hydrogen Strategy and Action Plan (Gobierno de Chile, 2024). The National Mining Policy 2050, developed by the Ministry of Mining, was approved in early 2023, and includes several objectives related to GHG emissions and environmental considerations. Notably, it includes a target to reduce emissions from large mining operations by at least 50% by 2030, and to become a carbon-neutral industry by 2040. It also outlines a zero-emissions fleet plan to be released by 2025 and implemented by 2030, as well as an objective for 90% of electricity contracts to come from renewable sources by 2030 and 100% by 2050 (Gobierno de Chile, 2023a). Along with being responsible for the monitoring and implementation of the above, the Ministry of Mining is also directed to establish GHG emissions targets for scope 1, 2, and 3 that comply with the 2030 target. Among the provisions of the new Energy Efficiency Law approved in early 2021 is the promotion of energy management in the country's largest consumers. These include all large companies with consumption over 50 Tcal per year (210 TJ/yr), cumulatively accounting for more than one third of the country’s consumed energy. These so-called consumers with energy management capacity have to implement an energy management system that covers at least 80% of their emissions and will additionally have to prepare an annual public report on several performance indicators, including energy consumption and energy intensity (Ministerio de Energía, 2021d; Ministerio de Hacienda: Oficina de Partes, 2021)</t>
+  </si>
+  <si>
+    <t>Industry is the largest energy-consuming sector in China, accounting for 58–59% of the country’s final consumption in 2022 (IEA, 2023b). Half of the direct energy consumed in the sector currently comes from coal and fossil gas, although combined shares of the fossil fuels are expected to plateau in the next decade as China targets increasing electrification and efficiency to meet expected demand (IEA, 2023b). Steel and cement output for real estate and infrastructure construction are the main drivers of industry emissions and the primary cause of China’s dip in emissions in 2022.Given the sector’s gargantuan energy consumption, decarbonisation of major industrial subsectors is critical—and central—to achieving national climate and energy targets. The government’s new industry peaking implementation plan has aligned the entire sector’s CO₂ emissions peaking timeline with China’s 2030 NDC target, while the 14th FYP for Green Industry Development has matched the economy-wide energy and emission intensity reduction targets (MIIT of China, 2021; MIIT of China, NDRC and MEE, 2022). China has set its carbon peaking targets for steel, cement, and aluminium for the year 2030, despite prior discussions regarding the feasibility of reaching these peaks by 2025. The delayed emission peaking timelines are to allow the sectors breathing space amidst energy and supply chain security concerns and to consolidate a less ambitious target that could be reached by all companies in a bid to tackle other industry concerns such as overcapacity and pollution (Guoping and Zou, 2022; Lin, 2022). China also set interim objectives for 2025, including reducing the energy intensity of steel production by 2% and recycling 320 million tonnes of scrap steel, as well as reducing the energy intensity of cement production by 3% (from 2020 levels) (Bloomberg, 2021; EEO, 2021; China Dialogue, 2022; MIIT of China, 2022; MoHURD of China and NDRC, 2022). To achieve a 1.5°C-compatible steel industry, China must retire its emissions-intensive Blast Furnace-Basic Oxygen Furnace (BF-BOF) route and cease building new coal-based steel plants. The resulting capacity gap should be filled through increased scrap recycling and green hydrogen-based direct iron reduction (DRI), with ironmaking prioritizing the use of electric arc furnaces (EAF) powered by clean energy (Climate Action Tracker, 2024). The Special Action Plan for Energy Conservation and Emission Reduction in the Iron and Steel Industry, issued in June 2024, aims to reduce energy consumption per unit of product by more than 1% for the BF-BOF and by more than 2% for EAF by 2025 compared to 2023 levels (NDRC et al. , 2024). The government is taking decisive steps to transition the steel sector to low-carbon production and address overcapacity by indefinitely suspending all new steel plant permits as of August 23, 2024. Earlier in the year, permits were only granted for EAF steelmaking plants (MIIT of China, 2024). By cutting steel output and increasing scrap-based steel production through EAFs, China could reduce CO₂ emissions from the steel industry by 200 Mt by 2025—equivalent to the EU's annual emissions from steelmaking (CREA, 2024). Key emitting sectors, such as cement, steel, and aluminium are likely to be the first targeted in the scope expansion of the country’s ETS (Wang, 2021; Wulandari, 2022). While the inclusion of these sectors was already in the pipeline, the approval of Carbon Border Adjustment Mechanism (CBAM) regulations by Europe (to be officially launched in 2026) has added a sense of urgency. To cover sectors eligible under the CBAM phase 1, cement, aluminium and iron and steel, China announced plans to expand its national ETS to include these industries by the end of 2024 (ChinaNews, 2024).. The MoU between the Chinese and German governments in June 2023 highlighted the focus on industrial emission reduction, especially in the cement, steel, chemical, and pulp and paper industries (German and Chinese Governments, 2023). To fully decarbonise China’s harder-to-abate sectors, the development of CCUS and hydrogen solutions have become priority strategy areas. CCUS will be a critical technology to help China drastically reduce emissions towards carbon neutrality in the long-term and has received increasing national attention in the last two decades, with objectives now focusing mainly on large-scale project demonstrations. As of 2021, CCUS was highlighted in the last three FYPs, the Ministry of Ecology and Environment (MEE) has encouraged provinces to pilot and demonstrate CCUS projects, and 29 provinces have already issued policies and plans related to the technology. China has commissioned three projects in 2023 and now has a project pipeline with the potential to capture around 10 MtCO₂/year (IEA, 2023a). However, the efficacy of CCS has yet to be fully realised in any CCUS project anywhere in the world, with budget blowouts and failure to reach announced sequestration rates (IEEFA, 2022). China published its national hydrogen strategy (2021–2035) in 2022, confirming the technology’s key role in China’s future energy system and mitigation efforts. While hydrogen is mainly produced from coal and gas, the plan targets a modest production of 100,000–200,000 tonnes of renewable-based hydrogen with renewable sources by 2025: this would constitute less than 1% of its production (Yao, 2022). The China Hydrogen Alliance estimates this could reach 100 Mt by 2060, accounting for 20 percent of the country’s final energy consumption (Nakano, 2022). The application of hydrogen in steelmaking decarbonisation has commenced, though it remains largely in the R&amp;D phase. An Italian firm specialising in sustainable metal production has partnered with China's leading steel manufacturers, Hesteel Group and Sinosteel, to establish DRI plants powered by hydrogen-enriched fossil gas, with a combined production capacity of 1.6 Mtpa (Tenova, 2020, 2022, 2024). F-gases China ratified and started enforcing the Kigali Amendment in 2022 (Rudd, 2021). China reported that it halted the new production capacity of five of the 11 HFCs it produces (covering 75% of total HFC production) two years ahead of the freeze requirements (McKenna, 2022). According to our analysis, China would reduce emissions by a modest ~50 MtCO₂e/year by 2030 under the Kigali Amendment’s phase-out schedule, although reductions could increase to almost 300 MtCO₂e/year by 2045.</t>
+  </si>
+  <si>
+    <t>The UK’s Industrial Decarbonisation Strategy introduced by the previous government (UK Government, 2021a) aims to reduce industrial emissions by two-thirds below 2018 levels in 2035 and 90% by 2050. While emissions fell 3% in 2022 to 63 MtCO 2 e, they will need to fall much faster, by around 8% per year, to achieve the government’s climate targets (CCC, 2023a). The strategy has a three-pronged approach: switching to low carbon fuels, efficiency gains, and carbon capture and storage (CCS). While some action is beginning to occur on fuel-switching, in particular in the electrification of steel, there remain significant gaps in the policies supporting resource efficiency in the industrial sector (CCC, 2024). Fuel switching In 2023, over 50% of industrial final energy was provided directly by fossil fuels (DESNZ, 2024c). This will need to be reduced substantially on the path to net zero. Two key options are the use of hydrogen, and direct electrification. The Industrial Decarbonisation Strategy sets a target of 50 TWh of fossil fuels to be replaced by low-carbon alternatives by 2035 in the manufacturing sector (UK Government, 2021a). This is roughly a third of industrial fossil consumption in 2022. To support this target, the previous government introduced the Industrial Decarbonisation and Hydrogen Revenue Support (IDHRS) scheme. This is similar to the CfD scheme in the power sector, providing financial support to cover the additional cost of low-carbon hydrogen production. GBP 140m was allocated to support fuel-switching over 2023–2024. This provides a business model to support industrial fuel-switching to hydrogen and is a positive step. There is also a GBP 240m Net Zero Hydrogen Fund (DESNZ, 2023). While these funds are to be welcomed, they are much smaller than the scale of funds being offered in Europe to support hydrogen deployment (Abnett, 2023). Industrial electrification has taken a step forwards in the UK, with the agreement of a deal to transform the Tata steelworks from a coal-fired blast furnace to an electric arc furnace producing recycled steel (H. Thomas &amp; Browne, 2024). In November 2023, a similar decision was announced for the remaining blast furnaces operated by British Steel, although the planned switch date of 2025 may be set back due to grid connection delays (Gill, 2024). This marks a transition away from coal in steelmaking which will reduce emissions. However, there has not yet been sufficient planning on how to ensure a just transition which preserves jobs in local communities dependent on steelmaking. This is a critical gap that must be addressed. There is also a need to drive industrial electrification in a more systematic way, with electricity prices still too high when compared to fossil gas (CCC, 2024). Carbon capture and storage The previous government set an aim of delivering 6 MtCO 2 /yr of industrial CCS by 2030, and 9 MtCO 2 /yr by 2035. This represents around 17% of total abatement in the industrial sector by 2035 (CCC, 2023a). The new government has continued this commitment to CCS, pledging GBP 22 bn of funding to drive CCS projects over the next 25 years (UK Government, 2024). Relying too heavily on CCS to deliver emissions reductions in the industrial sector could be risky, as the majority of previous CCS projects have ended in failure (Abdulla et al., 2020). In many sectors, the role and value of CCS is also being eroded as the cost of renewables declines (Grant, Hawkes, Napp, et al., 2021). CCS should be prioritised for applications where there are few alternatives, such as cement production (E3G, 2023). Fossil fuel supply Achieving the UK’s climate targets will require strong and sustained reductions in oil and gas production, as well as improvements to the emissions intensity of any remaining extraction. Oil and gas demand will need to fall around 30% by 2030 to achieve the UK’s NDC (CCC, 2020). The CCC also suggested that the emissions associated with oil and gas extraction should fall 68% by 2030, through electrification of processes and addressing fugitive emissions (CCC, 2020). The previous UK government moved in the opposite direction, continuing to support new oil and gas extraction in the North Sea, approving the Abigail, Jackdaw and Talbot fields (Oil and Gas Authority, 2023; A. Thomas, 2022; Tidman, 2022). New licensing rounds were held annually (UK Government, 2023a). The incoming government has set a new direction, committing to end licensing for new oil and gas fields (Lempriere, 2024). This is a good start and should be welcomed. However, it does not address the substantial pipeline of projects which have already received exploration licenses and are either waiting for development consent or are already in production. There are thirteen such projects awaiting approval (Dunne, 2024). The new government could strengthen its position on oil and gas by publicly committing to not approve this remaining pipeline of projects, and also set out a clear path to phasing out oil and gas production in the UK in line with the Paris Agreement goals, for example joining the Beyond Oil and Gas Alliance (BOGA).</t>
+  </si>
+  <si>
+    <t>Oil production Oil extraction has been the backbone of the Saudi economy for decades. Saudi Arabia is the world’s second largest oil producer after the United States and is OPEC’s leading oil producer (BP, 2023). It produced approximately 12% of the world’s oil in 2022 and held 17% of proven oil reserves. While the government has taken small steps to diversify the economy, Saudi Arabia remains highly dependent on hydrocarbon revenue. In 2022, Saudi Arabia reported USD 362bn in total crude oil export revenues and an additional USD 45bn in refined petroleum export revenues: several orders of magnitude higher than the oil export revenues from any other country (OEC, 2024). Oil is Saudi’s most exported commodity, accounting for 75% of the total value of exports in 2021 (OPEC, 2023). Over the past two decades oil rents, which are the difference between crude oil market prices and production costs, have consistently contributed at least 20% of Saudi’s annual GDP (World Bank, 2021). This close dependency between Saudi’s GDP growth and the oil market puts the sustainable growth of Saudi’s economy at risk. Recent geopolitical conflicts have once more shown the vulnerability of the global oil market to exogenous shocks. Saudi Arabia does not plan to end investment in new oil production, which is required to hold global warming to 1.5°C (IEA, 2023a). While Aramco recently abandoned its plan to increase oil production capacity to 13 million barrels per day (mb/d) by 2027, this decision appears largely driven by strategic considerations rather than a commitment to phase out fossil fuels. This reversal reflects changes in the global oil market, including slowing demand growth and increased production from non-OPEC countries, particularly the U.S ( FT, 2024 ). The government’s current diversification plans include no scenario with a decline in global oil consumption in the coming decades, which is required to meet the objectives of the Paris Agreement and reach net zero CO 2 emissions by mid-century (IEA, 2023a; IPCC, 2018). Both the “business-as-usual” and the “2030 renewable energy target” scenarios outlined in KAPSARC’s Energy Policy Solutions project hydrocarbon exports to significantly increase until 2050 (KAPSARC, 2021). At COP28, Saudi Aramco signed the Oil and Gas Decarbonisation Charter (OGDC), a new initiative which aims to “accelerate climate action” in the fossil fuel sector. However, the OGDC only addresses a fraction of relevant emissions from oil and gas production. Although most emissions come from fuel combustion, the initiative solely focuses on reducing emissions within the operations of oil and gas companies, such as in drilling and refining processes. Without a commitment to reducing the extraction and burning of fossil fuels, the charter fails to tackle the main driver of climate change. So far, none of the signatories have agreed to cut fossil fuel production. Carbon capture and storage Saudi Arabia is betting on carbon capture and storage (CCS) technologies to reach its climate goals while sustaining its fossil fuel production and exports. As of 2024, it only had one operational CCS plant—which is used for enhanced oil recovery (EOR), rather than reducing emissions from fossil fuels (Global CCS Institute, 2023). The government has a target to capture and store 44 million tonnes of CO 2 annually by 2035. To this end, Saudi Arabia is in the process of building a CCS hub at the industrial complex of Jubail, which it plans to capture CO 2 from fossil gas plants. The hub is expected to be operational from 2027 and the plans are to capture up to nine million tonnes of CO 2 per year from three Aramco fossil gas plants (The CCUS hub, 2023). But given the track record of CCS technology so far, these planned capture rates are questionable. CCS technologies are not commercially viable, nor are they proven at scale, despite large public subsidies for research and development globally. Relying on CCS to the extent Saudi Arabia is planning diverts attention and resources away from cost-effective mitigation options. The use of CCS should be limited to industrial applications where there are fewer options to reduce process emissions—not to reduce emissions from the electricity sector where there are cost-effective mitigation alternatives, not least because CCS does not remove 100% of emissions from power plants. Saudi Arabia is promoting the concept of a Circular Carbon Economy (CCE) to reduce emissions from oil and gas production (Luomi et al., 2021). This, however, only addresses a fraction of relevant emissions as most emissions come from fuel combustion rather than oil and gas extraction and processing. Saudi Arabia’s CCE plans largely rely on the development and deployment of CSS technologies (Kingdom of Saudi Arabia, 2022).</t>
+  </si>
+  <si>
+    <t>In 2021, Singapore’s industrial sector accounted for 44.4% of its primary emissions, plus 16.6% of secondary emissions from electricity use (National Climate Change Secretariat, 2024). Singapore´s mitigation strategy for the industry sector is based on increasing energy and carbon efficiency. The main policies are the Energy Conservation Act from 2013, which mandates monitoring and reporting energy usage and GHG emissions for large energy users; the Energy Efficiency Fund (E2F), which provided grants and tax incentives for energy efficiency investments in industrial processes; and the Energy Efficiency National Partnership Programme (EENP), which is a learning network for companies in the industrial sector to learn about energy efficiency ideas, technologies, practices, and standards (National Environment Agency, 2020). In 2017, the Energy Conservation Act (ECA) was enhanced, requiring, from 2018 onwards, the energy users it covers to have their monitoring plans verified by an independent third party and appoint a GHG manager (National Environment Agency, 2017). From 2021 onwards, these companies must establish a structured energy management system, and periodically assess energy efficiency opportunities at existing industrial facilities. In 2018, minimum energy performance standards were introduced to phase out the least efficient industrial electric motors and expanded to other common industrial equipment and systems thereafter (National Environment Agency, 2018). In the context of Singapore’s 2018 Climate Action Year, over 450 organisations, including industrial manufacturers, made voluntary commitments to improve their carbon footprint or increase awareness on climate change-related issues, such as upgrading existing equipment (e.g. chillers, lightings, appliances) with more energy efficient models, or starting recycling and waste management programmes. Given the voluntary nature of the pledges, and the lack of information to translate these targets into emission reduction targets, we have not included these in our current policy projections. The Sustainable Jurong Island report, which outlines targets and aspirations to decarbonise Singapore’s Energy &amp; Chemical (E&amp;C) hub, is targeting 2 Mt of carbon capture, utilisation and storage (CCUS) by 2030. (Singapore Economic Development Board, 2021) In December 2023 the government signed an agreement with ExxonMobil and Shell to "coordinate the planning and development of a CCS project, capable of capturing and permanently storing at least 2.5 million tons of CO2 a year, by 2030." Storage sites have not yet been selected and no details were included regarding capture facilities or transport infrastructure (Singapore Economic Development Board, 2024). Given the early phase of the consortium development and the track record of CCS across the world to date, including high costs and protracted development times, this is an ambitious target. Other developments on Jurong Island include a 285 MWh battery energy storage system, which surpasses Singapore’s target of 200 MWh energy storage by 2025, and Singapore’s first hydrogen-ready power plant, which will be operational by 2026 and is designed to operate initially on 30% hydrogen gas. A tender to install solar PV on 60 hectares of interim vacant land and the rooftops of five buildings on Jurong Island has also been initiated as part of the SolarRoof and SolarLand programs, following an initial pilot on 3.9 hectares of land (Energy Market Authority, 2023b).</t>
+  </si>
+  <si>
+    <t>Policy and planning documents for the South African industry sector generally address sustainable industrial economic development but barely mention mitigation targets for the industry sector or concrete measures for implementation. The post-2015 draft National Energy Efficiency Strategy proposes industrial sector targets for energy efficiency in 2030; however, there is no indication of implementation. (Department of Energy, 2016). Energy use from the mining and quarrying sector amounted to 185 PJ in 2015 (IEA, 2017). The South African government intends to achieve these targets through implementing several proposed measures such as the National Cleaner Production Centre South Africa (NCPC-SA) that promotes energy efficiency measures, its associated Industrial Energy Efficiency Project (IEE) implemented between 2011–2021 that promoted energy management systems, or the Green Fund South Africa that financially supports green technology research and implementation. However, these measures may only induce small emissions reduction impacts. South Africa is also aiming to develop value chains for renewable energy and storage technologies through the South African Renewable Energy Masterplan (SAREM), released for public comment in July 2023 (The dtic, 2023). The plan particularly aims to take advantage of increasing domestic and international demand for these technologies to drive industrial development and create jobs as part of the just transition. There are no signs of policy-driven emissions reductions in the near future for emissions-intensive subsectors such as steel production and mining, though there has been some interest in hydrogen. The Hydrogen Society Roadmap (2021) and draft Green Hydrogen Commercialisation Strategy (2020) highlight the potential role of and steps to develop green hydrogen for use in steel production, industrial mining, mineral beneficiation, manufacturing, logistics, and other sectors (DSI, 2021; The dtic, 2022). The South African Steel and Metal Fabrication Master Plan 1.0 (2021) mentions hydrogen, along other measures, in consideration of greening the industry (The dtic, 2021). For hydrogen to decarbonise the industry sector, it must be produced using renewable energy. Analysis by the Climate Action Tracker indicates that the steel industry’s emissions intensity would need to be reduced by about 30% in 2030 and by about 90%-100% by 2050 to be compatible with the Paris Agreement.</t>
+  </si>
+  <si>
+    <t>Emissions from manufacturing industries, construction and industrial processes and product use (IPPU), accounted for 23% of Switzerland’s CO 2 emissions in 2022. These levels are almost equal to those in 1990 (Bundesamt für Umwelt BAFU, 2024b). With Switzerland's new Climate Protection Act that passed a referendum in 2023, Switzerland now has emissions reductions targets for the industry sector to reduce emissions by 50% by 2040 and by 90% by 2050 below 1990 levels (Bundesgesetz Über Die Ziele Im Klimaschutz, Die Innovation Und Die Stärkung Der Energiesicherheit (KlG), 2023). Most GHG emission reduction policies and measures affecting Switzerland’s industry sector are implemented under the CO 2 Act and cover CO 2 emissions from fossil fuel use. These include the CO 2 levy on heating and process fuels, the Swiss ETS, and the negotiated reduction commitments. A number of key non-CO 2 emissions are not covered under the Act, and have been targeted separately. For example, a number of provisions relating to substances stable in the atmosphere cover all F-gases and are expected to result in a reduction of roughly 1.1 MtCO 2 e in emissions of such gases in 2020 (Schweizerische Eidgenossenschaft, 2020c). Similar to the EU, Switzerland also uses an ETS to lower emissions from large, energy-intensive entities. The Swiss ETS is much smaller than the European ETS, not only because of the smaller market but also due to the fact that the emissions generated by 54 companies in the power, cement, pharmaceutical, refinery, paper, district heating, and steel sectors covered by the scheme represent only 10% of the country’s emissions. Emissions from the sector were capped in 2013 at 5.63 MtCO 2 , and required to reduce by 1.74% per year in order to reach a target of 4.91 MtCO 2 in 2020 (13% reduction on 2013 levels) (Mission of Switzerland to the European Union, 2017). From 2021, the annual required rate of reduction rose to 2.2% of the 2010 baseline, which applies until 2030 (Federal Office of the Environment, 2020).</t>
+  </si>
+  <si>
+    <t>Türkiye’s industry sector accounts for 25% of total emissions (excl. LULUCF) (Republic of Türkiye Ministry of Energy and Natural Resources, 2023). This share is split between industrial processes (13%) and energy use (12%). The manufacturing industry alone represents over a fifth of Turkish GDP (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024a), so decoupling economic growth from emissions will be critical to Turkish industry on the path to net zero. Cement, iron and steel production account for the majority of process-related emissions (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024a). These industries will be negatively impacted by the EU’s Carbon Adjustment Border Mechanism (CBAM), which will be fully introduced in 2026 (European Commission, 2024). CBAM places a carbon price on goods imported into the EU. Given that the EU represents an important trading partner for Türkiye, decarbonising the industrial sector will be essential to maintaining industrial competitiveness. Türkiye has announced the launch of an Emissions Trading System (ETS) largely modelled on the EU’s ETS (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024a). This is a market mechanism which caps how much GHGs a company can emit, with the cap gradually declining over time. The pilot phase of Türkiye’s ETS will begin in October 2024, with full implementation planned for two years later, in October 2026 (Barut &amp; Kesikli, 2024). Critically, the ETS will also be applied to the shipping sector. By setting a carbon price on emissions from ships entering and exiting Turkish ports, Turkish policy is aligned with EU policy, thus closing potential loopholes which shipping companies could use to avoid carbon prices (Safety4Sea, 2024). The ETS is a central pillar of Türkiye’s climate legislation, and the government has been clear in communicating specific details about the policy (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024b), more so due to its trade implications than climate. Developing clear policies with actionable targets and measures are critical for ministries to successfully reduce emissions. The government’s drafting and communication of the ETS can therefore be followed when developing future climate policies.</t>
+  </si>
+  <si>
+    <t>The industry sector, including oil and gas production, is the largest source of emissions in the UAE, accounting for 46% of the country’s total emissions, or 103 MtCO 2 e. This includes emissions from industrial processes as well as indirect emissions from power and heat generation (Government of the UAE, 2024b). The UAE’s LTS includes a target to reduce industry emissions by 5% below 2019 levels by 2030, and 93% by 2050, while its current policy projections estimate these emissions will rise by 18% above 2019 levels by 2030. The UAE has a series of policies to reduce emissions from its industry sector, mostly focusing on increasing efficiency through adoption of best practices. To reach its target, the UAE plans to adopt a series of policies such as a cap and trade system, contracts for difference, regulated transport and storage for CCS, updated blended cement regulations, updated building codes, hydrogen production incentives and others (Government of the UAE, 2024b). On April 2024, the UAE also ratified the Kigali amendment, committing to reducing HFCs consumption by 87% by 2047 compared to its average consumption in 2024-2026 (IIR, 2024). The UAE plans to reduce its industry emissions through different means. Around 20% of the reductions towards its net zero target will come from fuel substitution and process switches in key industries such as steel and cement (Government of the UAE, 2024b). For example, the UAE’s LTS mentions the switch to concentrated solar power for heat for industrial processes and switching from blast furnaces to hydrogen-powered direct reduced iron processes for steel. However, a large share of the emissions reductions (32%) is expected to come directly from the deployment of CCS and from the decarbonisation of the power sector which will also heavily rely on CCS. Such overreliance on a technology that has not yet been proven at scale can seriously hinder the UAE’s progress towards transitioning its industry sector and can serve as a smokescreen to continue expanding fossil fuel production (Government of the UAE, 2024b). Oil &amp; gas production The UAE is the world’s seventh largest oil producer and 14th largest gas producer (US EIA, 2023a). It is also one of the world’s largest oil exporters. The UAE’s exported emissions from oil and gas are about 2.5 times larger than its domestic emissions (see graph below) (Climate Action Tracker, 2023c). In 2022, oil production reached 4.2 million barrels per day, an increase of 12% compared to the previous year, and surpassed pre-pandemic levels (US EIA, 2023b). Following an OPEC+ decision in October 2022 (Deepthi Nair, 2022), to cut production by twomillion barrels per day (mbpd) in an effort to keep oil prices up the UAE announced it would cut over 140,000 barrels per day from May 2023 until the end of the year (Gulf Today, 2023). However, the government also recently announced it was bringing forward its oil production capacity of five mbpd target (up from 3.8 mbpd currently), from 2030 to 2025, signalling its intent to ramp up production in the short term (Di Paola, 2022). The UAE is also developing oil and gas offshore exploration and production. This is part of its efforts to reach “gas self-sufficiency” (ICLG, 2022). In February 2022, the first offshore fields were discovered, which are estimated to contain between 43 and 57 billion cubic metres of gas (AFP, 2022). During 2022, Abu Dhabi National Oil Company (ADNOC) Drilling was awarded almost USD 6bn in contracts to “maximise value from Abu Dhabi’s offshore oil and gas resources” (World-Energy, 2022). In October 2023, ADNOC awarded contracts worth USD 17 bn for the Hail and Ghasha Offshore Development project. This project aims to produce 1.5 billion standard cubic feet per day (bscfd) of gas before the end of the decade (Reuters, 2023). This is part of a USD 150bn ADNOC plan to increase production of oil and gas. According to the IEA, the development of new fossil fuel infrastructure beyond what was already committed in 2021 is incompatible with reaching net zero by 2050 (IEA, 2021). The UAE’s plans to further develop and invest in new fossil fuel infrastructure are inconsistent with limiting global warming to 1.5°C. These plans are also likely to lock the UAE into a high-emissions trajectory and undermine its transition to renewable energy. Instead of ramping up its gas production towards self-sufficiency, the UAE should set out an ambitious plan to phase-out its dependency on gas for electricity and avoid the risk of stranded assets (CAT, 2022). In October 2023, ADNOC announced plans to double its CCS target from 5 to 10 MtCO 2 e removed annually by 2030 as part of its decarbonisation plan (Energy Voice, 2023). In a sustainable 1.5°C pathway, CCS with fossil fuels does not play a relevant role in energy sector decarbonisation, as renewable energy is much cheaper and has a much lower environmental footprint. The use of CCS needs be limited to industrial applications where it is proven there are no other options to reduce process emissions. Hydrogen During COP26, the UAE unveiled its “Hydrogen Leadership Roadmap”, a strategy aimed at developing the domestic production of green and blue hydrogen aimed at export markets in Asia and Europe. The roadmap already includes seven projects which are either completed or underway (including blue ammonia production). The overarching target of the strategy is to reach a 25% market share in key markets such as India, Japan, Germany and others (H2 World News, 2021). According to the UAE’s 2023 NDC update, several projects are already under way to support the country’s hydrogen ambitions, and a new Hydrogen Strategy is being prepared (Government of the UAE, 2023a). In its updated Energy Strategy 2050, the UAE also includes a target to produce 1.4 Mt of hydrogen annually by 2031. The UAE’s LTS includes additional information on its hydrogen development plans, including production targets of 7.3 Mt by 2040 and 14.9 Mt by 2050. Around half of the hydrogen is expected to come from fossil fuels with CCS (blue hydrogen), with the majority of the second half being green hydrogen and a small share coming from nuclear power (pink hydrogen) (Government of the UAE, 2024b).</t>
+  </si>
+  <si>
+    <t>Direct GHG emissions from industry accounted for 23% of total US emissions in 2023, making it the third largest contributor to US GHG emissions after the transport and electricity sectors. In 2020, emissions from the industrial sector decreased by 6% due the COVID-19 pandemic. In 2021, sectoral emissions increased by 1% as a result of the economy’s recovery. In 2022, emissions remained stable, indicating that the sector’s emissions have not reached pre-pandemic levels again (U.S. Environmental Protection Agency, 2024n). Industrial emissions have remained largely stable over the past decade, even as the US economy has transitioned from a manufacturing to a service-based economy and as industrial processes have experienced efficiency improvements and shifted to less emissions-intensive fuels (U.S. Environmental Protection Agency, 2024n). Under current policies, emissions from the industrial sector are projected to remain stable or minimally decrease as a result of the counteracting forces of renewed growth in domestic manufacturing and strengthen decarbonisation policies under the Inflation Reduction Act (IRA) (King, Kolus, et al., 2024; U.S. Environmental Protection Agency, 2023d). The IRA funds several measures to decarbonise the industrial sector. The act provides USD 5.8bn in funding for the new Advanced Industrial Facilities Deployment Program. In 2024, this programme selected, and began awarding financing to, projects in emissions-intensive industrial facilities (e.g. iron, steel, concrete sectors). The DOE estimates that the programme will reduce 14 MtCO 2 annually (Office of Clean Energy Demonstrations, 2024). The IRA also expands tax credits for carbon capture, utilisation, and sequestration (CCUS) technology, building on the Bipartisan Infrastructure Law’s (BIL) investments in CCUS demonstrations and industrial applications (The White House, 2023b; U.S. Department of Energy, 2022d). Estimates suggest that measures under the IRA for industrial CCUS might reduce up to 240MtCO 2 e/year (U.S. Environmental Protection Agency, 2023d). The IRA includes the Advanced Energy Project Credit, which provides tax credits for industrial and manufacturing facilities that invest in certain clean energy technologies. Eligible facilities either must re-tool with equipment designed to reduce GHG emissions by at least 20%, re-equip, expand, or establish measures for producing and recycling clean energy equipment, or process, refine, and recycle critical materials (The White House, 2023b). A total of USD 10bn in tax credits was allocated in a first round. A second round in 2024 aims to allocate an additional USD 6bn (IRS, 2024; U.S. Department of Energy, 2024g). The US implemented a diverse patchwork of financial incentives to support the research and development of technologies that are key for industrial decarbonisation. However, the government has not introduced instruments to facilitate the commercialisation of many of the technologies needed in hard-to-abate industrial subsectors (System Change Lab, 2024). Unlike the EU, the US has not developed a national emissions trading scheme, which, if designed correctly, could help expediate the commercialisation of key technologies. The challenging economics of many technologies in the industrial sector, such as green hydrogen and CCUS, require clear, robust incentive schemes to de-risk and attract investment (Department of Energy, 2024). Individual products, such as clean and/or green steel, might otherwise still find niche market applications (e.g. via government procurement), but will likely not be sufficiently commercialised to enable a full sector decarbonisation. In March 2023, the US Environmental Protection Agency (EPA) finalised its Good Neighbour Plan, which requires industrial facilities and power plants in 23 states to cut NOx emissions to prevent pollution across state lines. By 2026, the EPA plans to set enforceable NOx emissions control requirements, which will primarily reduce emissions from harmful air pollutants and also reduce CO 2 emissions by 16 MtCO 2 e/year (U.S. Environmental Protection Agency, 2023e). F-gases In December 2020, the US Congress enacted legislation under the American Innovation and Manufacturing (AIM) Act to tackle hydrofluorocarbon emissions (HFC). The act directs the EPA to phase down the production and imports of HFCs by 85% until 2036. It is expected to reduce emissions by 4.7 GtCO 2 e by 2050 via sector-based requirements to transition to non-HFC-emitting alternatives and next-generation technologies (U.S. Environmental Protection Agency, 2021b). In 2024, the US met its HFC phase-down target of reducing HFCs by 40% below 2020 levels (Haroldsen, 2024). The IRA provides an additional USD 38.5m to the EPA to implement the AIM Act (The White House, 2023b). We incorporate the IRA's effects on reducing non-CO 2 emissions into our current policy projections through a review of studies that quantify this impact (see Assumptions section). Hydrogen Hydrogen plays a central role in the Biden Administration’s roadmap for decarbonising hard-to-abate industrial processes and replacing fossil fuel-based feedstock with cleaner alternatives. The IRA established the Hydrogen Production Tax Credit to incentivise domestic production of clean hydrogen and to meet the Biden Administration’s Hydrogen Shot target, which aims to reduce the cost of clean hydrogen by 80% to USD 1 per kilogram through 2030 (The White House, 2023b). Recently, the credit has received criticism for its requirements to minimise emissions from hydrogen production, which certain actors argue are too costly (Pontecorvo, 2024).</t>
+  </si>
+  <si>
     <t>The industry sector in Germany emitted 155 MtCO 2 e in 2023 and accounted for approximately one fifth of Germany’s total emissions (UBA, 2024d). Around 80% of the sector’s total emissions in 2023 came from steel, petrochemical, cement, and chemical production (Kędzierski, 2024). The sector's emissions declined rapidly in the 1990s. Since the 2000s, this decline slowed, with fluctuations mostly driven by economic factors rather than by climate policy. Since 2022 and continuing through 2023, many industries have decreased production because of high energy prices, especially for fossil gas. As a result, emissions have fallen by approximately 15% since 2021 and have overachieved the sector’s emission reductions target for 2023 by 17 MtCO 2 e. Based on the UBA’s forecast, the sector is projected to continue emitting at a level below its annual emission targets until 2027. The UBA acknowledges that the current high energy prices have contributed to lower sectoral emissions and that the price level is likely temporary. The UBA projects that, starting in 2027, the industry sector will overshoot its yearly targets and, ultimately, exceed the climate change law’s 2030 sectoral target by 4 MtCO 2 e. The potential impact of improved energy efficiency measures and other structural changes that would reduce emissions in the long term is minimal (Expertenrat für Klimafragen, 2023). To achieve the 2030 target and get on a pathway towards climate neutrality, the industrial sector needs to reduce fossil energy consumption much faster and electrify processes at much greater speed (ibid). As a reaction to the dual COVID and energy crises, governments of large economies, such as the US and China, have implemented programmes to improve the competitiveness of their domestic industries on the global market. Germany, where export industries are central to the economy, seems under pressure to follow suit, and has previously - and continues to - support its energy intensive industry though a range of exemptions and subsidies. State support for the sector includes exempting industry from the renewable energy levy, reducing the electricity tax rate, reserving free allocations in the EU ETS, and introducing “Carbon Contracts for Difference” (CCfDs) in 2024. The EU ETS, which covers large industrial installations, showed new record CO 2 prices in 2023, breaching EUR 100t/CO 2 in February, 2023 (Twidale et al. , 2023). However, prices have since collapsed: in February 2024, the price had fallen to approximately EUR 52/tCO 2 (Tamellini, 2024). In April, 2024, the ETS price hovered around EUR 70t/CO 2 ; a price level significantly lower than the official projections assume. Even with the previously high allowance prices, the effect of the additional costs for emissions-intensive processes was minor, as a substantial number of allowances for industry were still available for free. The number of free allowances is set to decrease over the next decade. The 2038 target for achieving net-zero under the EU ETS provides a strong signal for industry to decarbonise more rapidly. In the short term, there is a risk that industrial players will not invest in low-carbon solutions, as these technologies are still new and relatively expensive, even if they already pay off in the long-term. To incentivise investments in low-carbon technologies, the government initiated the first round of bidding for CCfDs in March, 2024 (Moulson, 2024). CCfDs guarantee a certain fixed price for low-carbon industrial products and processes that are not yet price competitive. The programme aims at augmenting the uptake of low-carbon technologies in particularly energy-intensive industries, such as the chemical, steel, cement, paper and glass production industries (Kędzierski, 2024). The CCfDs’ first round of bidding makes EUR 4bn available for innovative industrial projects that achieve a 60% emission reduction in three years and a 90% reduction in 15 years, relative to when employing conventional technologies. A second bidding round, worth EUR 19bn, is planned for the end of 2024 (BMWK, 2023b). In theory, this policy lowers the risk, therefore enabling industry to make significant investments in emerging low emission technologies that may substantially reduce the sector’s emissions. However, it remains unclear for how long the federal budget will be able to support such a high-cost intervention. The recent fluctuations in the EU ETS prices further complicate the potential for CCfDs to function as intended (Kędzierski, 2024). Electrification is key to decarbonising the industry sector: a central challenge is the relatively high electricity price in Germany. To alleviate the financial burden of the high price, in November 2023, the government reduced the electricity tax for the industry sector, lowering it from 1.537ct/kWh to the EU’s minimum rate of 0.05ct/kWh (Bundesregierung, 2023). The government has guaranteed this reduced rate through 2025 and, depending on the federal budget, may extend the reduction through 2028. Beyond moderating tax rates in the short term, the Ministry of Economy and Climate Change, in a 2023 working paper on electricity prices for energy-intensive installations, suggests using CCfDs and publicly-guaranteed power purchase agreements for industries with renewable energy producers to facilitate industry access to “cheap green electricity” in the long term (BMWK, 2023g). The government's challenge is to ensure a stable economy in the short term, while transitioning to a zero-carbon industrial sector - in a just manner - in the long term. A robust regulatory framework that supports a long-term vision of transitioning and decarbonising the sector may alleviate bureaucratic challenges, and targeted efforts to address the shortage of skilled workers should be considered to complement subsidies.</t>
   </si>
   <si>
+    <t>The EU’s industrial emissions, both energy related and from industrial processes, accounted for about 24% of its total GHG emissions in 2021 (Climate Analytics, 2024; UNFCCC, 2023). Industrial emissions have been falling on average about 2.3% per year but this is not fast enough and the EU’s industry will need to accelerate this 1.3 times faster than its current trend to reach 1.5°C compatibility (European Climate Neutrality Observatory, 2024b). The EU has not signed the Beyond Oil and Gas (BOGA) declaration but eight of its member states have. Six member states — Denmark, France, Ireland, Portugal, Spain and Sweden — are core members of the Alliance and have committed to ending oil and fossil gas exploration and development (Beyond Oil and Gas Alliance, 2021). To decarbonise its industries, the EU introduced indicative targets in the revised Renewable Energy Directive (EU 2023/2413) for the share of renewables in industry. Article 22 requires the industry sectors in member states to increase the share of renewable energy by an average annual rate of 1.6% between 2021 and 2030. This annual 1.6% indicative benchmark was watered down by the Commission from the initial 1.9% growth rate it estimated it would need to deliver on the REPowerEU objectives (European Commission, 2022a). The revised Renewable Energy Directive also requires that only 42% of incorporated hydrogen be derived from renewable energy by 2030 and 60% by 2035. This means that the industry will use a mix of renewable and fossil fuel derived hydrogen. This design will allow industries to start their shift to hydrogen but access cheaper fossil fuel derived hydrogen until the green hydrogen is available at scale and affordably. The EU does not have any provisions to fully eliminate fossil fuel derived hydrogen from industry beyond 2035, which risks the long-term dependence on fossil derived hydrogen. Green hydrogen The Commission’s Hydrogen Strategy sets out that installed capacity of electrolysers in the EU should reach 40 GW by 2030, resulting in the production of up to 10 million tonnes of green hydrogen, complemented with similar capacity installed in neighbouring countries (European Commission, 2020). The EU hydrogen policy framework has several key gaps hindering market development and does not go far enough to address issues such as high-cost entry barriers and uncertainties. At present, renewable hydrogen is also much more expensive than fossil fuel-based hydrogen. Financial support is fragmented, with a shortage of targeted funds necessary to meet the 2030 REPowerEU goals. Additionally, the EU lacks a clear definition for low-carbon hydrogen, and is only expected to develop a methodology by 2025 as part of the Delegated Act of the revised Gas Regulation. Developing a net zero technology Industry To tackle replacing industrial technology with cleaner alternatives, the EU has been developing a nexus of polices to facilitate the growth of (1) net zero technology industry and (2) industrial carbon removals, encapsulated by the: Net Zero Industry Act (NZIA) (EU) 2024/1735, and more broadly the Green Industrial Plan Industrial Carbon Management Strategy Carbon Removal Certification Framework (proposal) 2040 climate targets (proposal) In June 2024, the Net Zero Industry Act entered into force (European Parliament &amp; European Council, 2024c). It focuses on 19 net zero technologies. It also includes the objective of developing annual injection capacity for carbon capture and storage of 50 MtCO 2 e by 2030 that should be used to mitigate residual emissions. These capacities should be developed by oil and fossil gas companies proportionally to their current oil and gas production levels. The NZIA will be crucial to operationalising the direction set by the Industrial Carbon Management Strategy (ICMS) (European Commission, 2024d). The ICMS lays out how it plans to scale up industrial carbon removals to deliver the EU’s climate neutrality objective, most notably from bioenergy with carbon capture and storage (BECCs) and direct air carbon capture (DACC). It sets out a target to reach 50 MtCO 2 e in carbon removals annually by 2030. The ICMS is strongly linked to the proposed 2040 targets, which are yet to be adopted. In its impact assessment the Commission envisions it would need about 75 MtCO 2 e of industrial carbon removals from BECCs and DACCs by 2040. Additionally, the Commission will create policy options and support mechanisms for industrial carbon removals, including considerations on whether and how to integrate them into the EU Emissions Trading System (ETS) but this is not expected until the planned revision of the ETS in 2026 (EPG, 2024). In April 2024, the political agreement was reached on the Carbon Removal Certification Framework (CRCF) but is still to be adopted (Carbon Gap, 2024a; European Commission, 2022b). The CRCF seeks to establish a framework to certify the emission removals from carbon farming, carbon storage in products and industrial carbon removals (from technologies like Direct Air Carbon Capture and storage (DACCS) and bioenergy with carbon capture and storage (BECCs). The CRCF is the mechanism to deliver on the goals of the ICMS and lays out the role the CDR will play. The CRCF gives the Commission the ability to assess options for CDR and CCS targets. The CRCF is riddled with concerning elements that could go against climate action. The regulation lacks a distinction between emission reductions and removal, potentially allowing removals to offset emissions that should be reduced. It also risks offsetting and greenwashing through the permitting of sales of carbon credits as offsets in voluntary carbon markets, especially if large emitters are allowed to buy these credits. The 2040 climate target communication keeps the role of CCS in the power sector vague under the proposed 2040 targets. This is worrying as the application of CCS to certain sectors is left open to interpretation. The incoming Commission has the opportunity during the subsequent expansion of the Industrial Carbon Management Strategy and Clean Industry Deal to clearly commit to no CCS in the power sector. Carbon Capture and Storage (CCS) refers to technologies which use engineered methods to capture CO 2 from a source and store it geologically. CCS can be applied to a range of different CO 2 sources in different sectors. CCS technologies are neither commercially viable nor proven at scale, despite large public subsidies for research and development globally. Heavily relying on unproven CCS for power generation simply prolongs the use of fossil fuels, diverting attention and resources away from the necessary and urgent switch to renewable energy generation that drives down actual emissions. The use of CCS should be limited to industrial applications where there are fewer options to reduce process emissions—not to reduce emissions from the electricity sector where renewables are cost-effective mitigation alternatives, not least because CCS doesn't remove 100% of emissions from power plants.</t>
+  </si>
+  <si>
     <t>In 2022, industrial process emissions accounted for 9% of total emissions (excl. LULUCF); they have been increasing since 1990 at an annual rate of 4% (Gütschow &amp; Pflüger, 2023). India's industrial sector accounts for the largest share of total primary energy demand, at 38% in 2021, growing at an annual rate of 5% over the last 10 years. 1.5°C compatible pathways show the share of electricity in the industrial energy mix increasing between 30-31% by 2030 compared to 2019 (Climate Analytics, 2021). Electrification of industry is essential to decrease the use of fossil gas and limit the need for green hydrogen, which requires various conversion steps, leading to a much lower efficiency in the process compared to using renewable electricity directly. India needs international support to achieve this. However, high industrial electricity prices in India often act as a barrier to the adoption of technologies that could enable the electrification of industries (IEA, 2020b). Energy efficiency The Indian government amended the 2001 Energy Conservation Act in late 2022 (having last made revisions to the law in 2010). The Act regulates energy consumption by equipment, appliances, buildings and industries. The major amendments include: An obligation to use non-fossil sources of energy for industry, transport, buildings Carbon trading Energy conservation code for buildings, both commercial and residential Standards for vehicles and vessels Allotment of regulatory powers of State Electricity Regulatory Commissions Changes in the governing council of the Bureau of Energy Efficiency The Act mandates the use of non-fossil fuel sources for industries such as mining, steel, cement, textile, chemicals and petrochemicals. The amendments also allow industries to buy renewable energy directly from the producers enabling renewable energy producers price certainty. The main instrument to increase energy efficiency in India’s industry is the Perform, Achieve and Trade (PAT) Mechanism, which has been in place since 2012 and is implemented under the 'National Mission on Enhanced Energy Efficiency’. It covers 13 energy intensive sectors and nearly 25% of the energy use. The first cycle of the PAT scheme resulted in savings of 5.6 GWh and 31 MtCO 2 e between 2012 and 2015 (BEE, 2018). The second cycle of PAT (2016-17 to 2018-19) resulted in total savings of approximately 61.34 MtCO 2 e emissions, resulting in savings of INR 800 bn. Industry is the biggest consumer of fossil gas in India where, apart from being used for energy purposes, it is used as a feedstock for manufacturing fertiliser and petrochemicals. Green hydrogen is going to play an important role in decarbonisation of these industries (Ministry of Petroleum and Natural Gas, 2023). While fossil gas only accounted for 5% of industrial final energy consumption in 2020, the current policies scenario, based on IEA STEPS, shows a four-fold increase in gas use by 2050, reaching 10% of industrial final energy consumption, this is an improvement from previous assessment of 13% (IEA, 2022, 2023c). Early suggestions of a mandatory green hydrogen purchase obligation have been silenced given the apparent cost-competitiveness of domestically produced green hydrogen with grey hydrogen made from imported LNG, the latter getting more expensive due to global market volatility (Verma, 2021). This has been met with resistance from the hydrogen industry which argues that mandates are essential for investor confidence to drive scale-up (The Hindu BusinessLine, 2023). Micro, Small and Medium Enterprises (MSMEs) contribute around 30% of India’s Gross Domestic Product (GDP), 40% of its exports and 20-25% of its heavy industry energy consumption (IEEFA, 2023e). The Bureau of Energy Efficiency (BEE) has organised several initiatives to address awareness and to provide training and capacity building for implementing energy efficiency measures in MSMEs. MSMEs are struggling to secure financing for decarbonisation efforts. This is particularly concerning as MSMEs have the potential for significant emission reductions as they currently rely on outdated technologies and are not covered by existing climate policies. In the budget for 2024, the government has extended financial support to MSMEs for shifting to cleaner energy and implementing energy efficiency measures (Climate Group, 2024). The Indian government plans to launch a pilot carbon market mechanism for MSMEs and the waste sector (Ministry of Power, 2022a). During the stakeholder consultation on the framework of India's proposed carbon market, there has been a proposal to allow the voluntary participation of MSMEs (Global, 2023). India has signed a Memorandum of Understanding (MoU) with the Growth Triangle Joint Business Council created by Indonesia, Thailand, and Malaysia to encourage private investments in MSMEs for the adoption of energy efficiency measures (The Financial Express, 2023). Green hydrogen In India, the push towards green hydrogen is increasingly driven by its vast industrial sector, industries such as steel and fertiliser production are pivotal. India launched its National Green Hydrogen Mission in 2021 (Ministry of Power, 2022b). In January 2023, the mission was updated, with a focus on the development and deployment of green hydrogen with an investment support of USD 2.3 bn by the government, which includes production-linked incentives for the manufacturing of electrolysers and production of green hydrogen (Ministry of New And Renewable Energy, 2023). With this plan, India expects to reach 5 MTPA per annum of green hydrogen capacity by 2030. (The Economic Times, 2023a). The World Bank recently approved a USD 1.5 bn loan to accelerate green hydrogen in India. India aims to become a major exporter of green hydrogen and wants to capture about 10% of the global green hydrogen market by 2030 (Ministry of New And Renewable Energy, 2023). It has already signed an MoU with Singapore to export green hydrogen from 2025 (The Economic Times, 2022). The government has been engaging with key international markets, such as Europe and Japan, to explore opportunities for collaboration and to identify potential export markets for green hydrogen (DownToEarth, 2023b; European Investment Bank, 2023). However, green hydrogen is a nascent technology in India and its commercial viability largely depends on the reduction of electrolyser costs and the availability of round-the-clock renewable energy (IEEFA, 2023c). The government has started auctions under a production-linked incentive programme for electrolyser manufacturing (Reuters, 2023f). Oil India Limited (OIL) recently commissioned India's first 99% pure green hydrogen plant in Jorhat. NTPC has also initiated green hydrogen blending operations in Surat's Piped Natural Gas (PNG) network, starting from a 5% blending to scale up to 20% (Energyworld, 2024). Several Indian and international companies are investing in green hydrogen production to meet India's hydrogen production and export targets. Adani New Industries and TotalEnergies will invest USD 49 bn in green hydrogen over the next decade. L&amp;T, Indian Oil, ReNew Power, and NTPCL are also working on various projects related to green hydrogen production and fuel cells (Telematic Wire, 2023). It is expected that the support from the government and these investments may lead to a decrease in production costs in the coming years. Additional support comes from a 25-year waiver of the inter-state transmission charge for green hydrogen projects. It previously applied to projects set up before 2025, and has now been extended to for hydrogen manufacturing plants commissioned before 2031 (Reuters, 2023b). India’s largest oil refiner, Indian Oil Corporation, estimates that these policy measures will help to reduce the cost of green hydrogen production by 40-50% (Business Standard, 2022). The mandate for green hydrogen purchase has been brought back under consideration for the fertiliser and refinery industries, previously shelved because with the increased price of LNG, the cost of green hydrogen became competitive with grey hydrogen (Hydrogeninsight, 2023). According to an assessment by NITI Aayog, the adoption of green hydrogen (produced domestically) has a cumulative mitigation potential of 3.6 GtCO 2 by 2050 compared to the use of grey hydrogen (Raj et al., 2022). As a sign of increasing policy support for green hydrogen, at the sub-national level, many Indian states have also started to developing policies for green hydrogen hubs (IEEFA, 2023h). Carbon markets India amended its Energy Conservation Act in December 2022, laying the groundwork for a potential domestic carbon market. The Amendment Act includes provisions for the establishment of a carbon market through the introduction of a 'Carbon Credit Trading Scheme' (CCTS) by the Central Government. The Bureau of Energy Efficiency (BEE) has released draft rules for a compliance carbon market based on GHG emissions intensity rather than an absolute cap. The draft outlines compliance mechanisms, emissions intensity trajectories, verification processes, and carbon credit issuance, with specific provisions for entities exceeding or failing to meet targets (Enertdata, 2023). The pilot carbon market, which will likely include four heavy industries -petrochemicals, iron and steel, cement and pulp and paper- is anticipated to become operational from April 2025 (Reuters, 2023d). These heavy industries, which previously had energy efficiency targets under the PAT scheme, seems to have had lax targets, resulting in an over-supply and under-pricing of energy saving certificates (ESCerts). The new rules are intending to take cautious approach in setting a transparent and right target. Carbon capture and storage India is considering CCUS as an emissions reduction strategy to achieve deep decarbonisation in hard-to-abate sectors and to allow it to continue to use its coal resources (Press Information Bureau, 2022a). Major Indian companies are exploring and implementing CCUS technologies to curb their carbon footprint. This includes partnerships with global technology firms (ONGC, 2024). Several pilot projects and initiatives are underway, supported by both government and private sector investments (Economic Times, 2024c). The commercialisation of CCUS in India by 2050 is essentially unlikely without significant R&amp;D incentives as well as international financial support. However, India has acknowledged, in its LT-LEDS, that CCUS is not a viable technology option for retrofitting existing thermal power plants as it is not cost-effective for India (Government of India, 2022a).</t>
   </si>
   <si>
     <t>In 2022, industry accounted for 42% of national energy demand, reaching an estimated 430 MtCO₂e (MEMR, 2023b). The sector saw a huge increase in energy demand, fuelled by the growth of the domestic iron, steel and metallurgy sector, which accounted for almost 60% of coal demand in 2022 (MEMR, 2023b). A large share of the demand is from smelters for the rapidly expanding nickel industry that aims to support the development of Indonesia’s battery supply chain. Indonesia is the world's largest producer of nickel, and as such, will play a key role in the global energy transition. Recognising the need to address industrial emissions, Indonesia aims to reduce emissions from industrial processes by up to 9 MtCO₂e and from industrial waste by up to 28 MtCO₂e by 2030 in its ENDC. Close collaboration among key ministries, including the Ministry of Industry, the Ministry of Energy and Mineral Resources, and the Ministry of Environment and Forestry, would be crucial to implement effective emission reduction measures. Progress has been made in some areas. The cement industry, for example, has reduced its carbon emissions intensity by nearly 13% between 2010 and 2022, dropping from 725 kgCO₂ to 631.7 kgCO₂ per tonne of cement produced. This achievement is the result of using alternative fuels like biomass and waste materials instead of coal, as well as improvements in energy efficiency. The industry's Thermal Substitution Rate, which measures the proportion of energy from alternative fuels, increased to 7.8% in 2022 and is expected to reach 19.82% by 2030 (IESR, 2023a, 2024). The iron and steel industry, however, faces greater challenges. It emits approximately 3.07 tonnes of CO₂ equivalent per tonne of steel, more than twice the global average of 1.41 tonnes. This high emission rate is largely due to outdated, coal-intensive production methods like blast oxygen furnaces. Transitioning to electric arc furnaces, which use electricity and can incorporate renewable energy, could significantly reduce emissions. Currently, electric arc furnaces represent 36% of production capacity, while blast oxygen furnaces account for 64%. Shifting toward electric arc technology and integrating renewable energy sources are essential steps for the industry to reduce its carbon footprint (IESR, 2023a, 2024). The ammonia industry presents significant opportunities for low-carbon transition. Indonesia is one of the world's largest ammonia producers, generating about 7.2 million tonnes annually, primarily for fertiliser production. There is growing interest in "green ammonia," produced using renewable energy. However, production costs are currently high, approximately USD 730 per tonne for green ammonia compared to USD 470 per tonne for conventional methods. Efforts are underway to improve energy efficiency and adopt cleaner technologies, such as utilising renewable energy sources and implementing carbon capture and storage (CCS) (IESR, 2023a, 2024). Encouragingly, several initiatives aim to promote cleaner industrial processes. Green industrial zones are being developed through programmes like the Global Eco-Industrial Parks Programme (GEIPP) Indonesia in Bekasi and Medan, funded by the Swiss government. And as of November 2023, at least 22 low-carbon ammonia projects have been identified in Indonesia, utilising renewable energy sources like hydropower and geothermal energy. Companies like Pupuk Indonesia, which accounts for over 85% of national ammonia production, are investing in low-carbon technologies with goals to reduce CO₂ emissions by 4.8 MtCO₂e by 2030 and 20 MtCO₂e by 2050 (IESR, 2023a, 2024). Despite these positive developments, significant challenges remain. The reliance on coal is a major barrier to reducing emissions, and transitioning to renewable energy sources requires substantial investment and infrastructure development. Technological modernisation is essential, but industries need support to upgrade equipment and adopt new processes. Effective government policies, incentives, and enforcement are critical to drive this transformation (IESR, 2023a, 2024). Industrial and fossil-based power emissions contribute to poor air quality, with Jakarta ranked as one of the most polluted cities globally in 2023 (Jong, 2023), highlighting the urgency of addressing industrial pollution for public health. The Ministry of Industry has been recently tasked with investigating and controlling industrial emissions (Ministry of Industry, 2023). Measures include periodic checks of company reports in the National Industrial Information System (SIINas) and conducting audits to ensure compliance with national regulations.</t>
   </si>
   <si>
-    <t>Australia’s industrial sector, including industrial energy use, industrial process emissions and fugitive emissions, accounted for 30% of Australia’s total emissions excluding LULUCF in 2023 (DCCEEW, 2023b). The government announced the ‘Future Made in Australia’ plan in the 2024–25 budget, allocating AUD 22.7bn (USD 14.9bn) over 10 years to attract investment in key industries and realise Australia’s potential to become a “renewable energy superpower” (Australian Government, 2024). Priority industries identified under the scheme include renewable hydrogen, green metals, low carbon liquid fuels, critical minerals processing, and clean energy manufacturing including battery and solar panel supply chains. Australia is a major exporter of both coal and LNG. Emissions from coal and LNG use at the final export destination are not accounted for in the national greenhouse gas inventory. Australia exports more than double its domestic emissions from its coal, fossil gas and oil exports (Climate Action Tracker, 2023b; Climate Analytics, 2024a). Coal mining Australia is the world's largest exporter of metallurgical coal, accounting for around half of all exports, and the second-largest exporter of thermal coal (DISR, 2024b). In 2023, Australia was the second-largest coal exporter overall and the fifth-largest coal producer (Energy Institute, 2024). Despite a projected decline in domestic coal power, coal production and exports are forecast to remain stable, at odds with the global efforts towards decarbonisation. Close to 90% of produced coal was exported in 2023 (DCCEEW, 2024a). The government projects that run-of-mine coal production will increase by 9% from 559 Mt in 2023 to 612 Mt in 2027, before falling to 488 Mt by 2035 (DCCEEW, 2024h). Sustained or even increasing levels of coal production are clearly inconsistent with the goals of the Paris Agreement (IEA, 2023d). 1.5°C-compatible pathways would see coal production fall 78% below 2020 levels by 2030 (SEI et al., 2023). Government approval of coal mine projects remains a contentious issue in Australia. In September 2024, the Environment Minister gave the green light for three NSW mines to extend their operations for another 30–40 years: the Narrabri Underground Mine Stage 3 expansion, the Ravensworth Underground Mine, and the Mount Pleasant project (ABC News, 2024d; The Guardian, 2024). Combined, these three projects are expected to result in additional emissions of 1.36 GtCO 2 e (The Australia Institute, 2024b). These approvals are in addition to the four coal mining projects approved in 2023: the Isaac River and Ensham mines in Queensland, and the Narrabri Underground and Mount Pleasant mines in NSW. As of December 2023, there were 53 coal projects in the development pipeline, of which ten were already committed (DISR, 2023). While many of the proposed coal projects are still speculative, Australia has the highest number of proposed coal mine projects among OECD nations (Global Energy Monitor, 2023). Fugitive emissions from coal mining are discussed below in the Methane section. Oil &amp; gas production Australia was the world's third-largest exporter of liquefied natural gas (LNG) in 2023, after being the largest exporter in 2021 (Energy Institute, 2024). Around 80% of fossil gas production goes towards LNG production for export, including LNG plant own consumption (DCCEEW, 2023a). The Federal government released its Future Gas Strategy in May 2024 which sets out the government’s ongoing commitment to development of new fossil gas supply and continued LNG exports as a “reliable and trusted trade and investment partner” (DISR, 2024a). The strategy embeds the role of fossil gas in Australia’s domestic energy sector and exports to 2050 and beyond, and (wrongly) claims that fossil gas is needed for the global energy transition. This is despite the inclusion of the IEA’s Net Zero Emissions scenario in the analysis, which clearly calls for a rapid decline in global gas demand (IEA, 2023d). As is the case for coal, Australia still does not have a gas phase-out strategy and timeline. The government projects that LNG production and export will be sustained at current levels until at least 2035, with 82 Mt expected in 2035 – the same as in 2023 levels (DCCEEW, 2024h). These projected exports account for several large-scale projects sanctioned across 2021 and 2022. The Barossa backfill to Santos’ Darwin LNG is expected to commence in 2025. Woodside’s massive Scarborough development and linked Pluto LNG plant expansion is expected to start up in 2026. Backfill to Shell’s Prelude FLNG facility from the Crux field is expected to come online in 2027. Both Crux and Barossa are carbon-intensive fields with a high percentage of reservoir CO 2 (DCCEEW, 2022b). The government’s LNG projections also assumed that Woodside’s Browse project would startup in 2030, but the project appears to have stalled with the state Environment Protection Agency deeming the project “unacceptable” (ABC News, 2024b). The biggest uncertainty for future gas production in Australia is Tamboran Resources’ plan to frack the Beetaloo basin in the Northern Territory (NT) and export the gas via a new 6.6 Mtpa LNG plant to be built in the Middle Arm Precinct in Darwin. This could eventually be expanded to 20 Mtpa. Far from achieving net zero domestic lifecycle emissions, as recommended by the NT government’s Pepper Inquiry, emissions from Beetaloo and Middle Arm development have been found to be severely underestimated, and the potential to offset its emissions are greatly exaggerated: it would generate more emissions than the 2030 emissions reduction goal under the Safeguard Mechanism regulations, and require international offsets currently banned under that legislation (Climate Analytics, 2023). The Middle Arm development was the subject of a recent federal Senate Inquiry into the environmental impact of the development and the federal government’s AUD 1.5bn commitment for the project, which failed to reach a unanimous set of recommendations (ABC News, 2024c). Despite being presented as a sustainable precinct, the industrial project could include fossil gas-generated hydrogen (“blue” hydrogen) production, minerals processing, and petrochemical processing, in addition to the current and planned LNG facilities (ABC News, 2024c). Fossil gas companies are also exploring opportunities to frack the Canning Basin, in Western Australia (ABC News, 2023b; Climate Analytics, 2024b). The oil and gas industry continues to benefit from significant government support, which included AUD 14.5bn in spending and tax breaks in 2023–24 (The Australia Institute, 2024a). The largest component of this total is the Fuel Tax Credit Scheme at AUD 9.6bn which subsidises fossil fuel consumption. In 2023, the government revised the Petroleum Resource Rent Tax (PRRT) to introduce a cap on the use of deductions by LNG producers to no more than 90% of their assessable income. To date, no Australian LNG project has paid any PRRT (Minister for Finance, 2023). These subsidies support the fossil fuel industry and its exports, despite the need for a global phase-out. CCS Carbon capture and storage (CCS) is being proposed as a solution to mitigate reservoir CO 2 from gas fields which historically has been vented directly to the atmosphere. This is the case at Chevron’s Gorgon plant, Australia’s only operating CCS project, and at Santos’ Moomba CCS project, which is under construction and scheduled to commence operation in 2024. However, implementing CCS for reservoir CO 2 does nothing to mitigate fugitive methane emissions that occur throughout the gas lifecycle, and therefore would mitigate only a portion of the greenhouse gas emissions associated with fossil fuel production. Nevertheless, CCS projects continue to be pursued by gas producers with government backing. Chevon’s CCS facilities at its Gorgon LNG plant have consistently underperformed and fallen short of sequestering the 80% of reservoir CO 2 as required by the project’s state environmental approvals. Despite having an announced annual capture capacity of 4 MtCO 2 /year, Gorgon CCS has sequestered just 10 MtCO 2 in total over the five years to August 2024 (ABC News, 2023a; Chevron, 2021, 2024). Santos is also planning the Bayu-Undan CCS project to enable the development of the Barossa field offshore near Darwin. The project would involve capturing CO 2 from the carbon-intensive Barossa field, transporting it via Darwin by pipeline, and then sequestering in the depleted Bayu-Undan field in the Timor Sea, off the coast of Timor-L'este. The government’s 2023 sea dumping legislation paves the way for the project to proceed (ABC News, 2023c). The Bayu-Undan CCS project has a design capacity of up to 10 MtCO 2 /year and is one of two projects proposed as part of the Middle Arm development, with the other being INPEX’s Bonaparte project (Northern Territory Government, 2024). The government is counting on CCS as its predominant strategy to reduce fugitive emissions under the Safeguard Mechanism. The government estimates that by 2030, CCS will capture 1 MtCO 2 e (AR5 values) from LNG facilities, in addition to CO 2 captured at Gorgon, and 1.5 MtCO 2 e from domestic gas production at Moomba (DCCEEW, 2023b). The government projects that CCS at LNG plants will scale up to 4 MtCO 2 e by 2035. However, given the experience at Gorgon, it is doubtful whether any of these projects will achieve their design capture rate. Hydrogen The government released an updated National Hydrogen Strategy in 2024 (DCCEEW, 2024c). Under the strategy the government has set baseline and stretch targets for renewable hydrogen production of 0.5–1.5 million tonnes per year by 2030 and 15–30 million tonnes per year by 2050. The government is also targeting exports of green hydrogen (or equivalent derivatives) of 0.2 million tonnes by 2030, and a stretch target of 1.2 million tonnes. The 2024 National Hydrogen Strategy specifically prioritises renewable hydrogen production in comparison to the 2019 National Hydrogen Strategy which defined ‘clean’ hydrogen as hydrogen produced via electrolysis with renewable energy or hydrogen derived from fossil fuels with greater than 90% carbon capture. The proposed Guarantee of Origin Scheme would measure and verify the emissions intensity of produced hydrogen. The Hydrogen Production Tax Incentive, a component of the Future Made in Australia policy package, will provide an incentive of AUD 2/kg renewable hydrogen for up to 10 years of production for projects that reach final investment decision by 2030. The AUD 4bn Hydrogen Headstart program, introduced in 2023, provides funding support to selected large-scale renewable hydrogen projects to cover the current gap between production cost and market prices (DCCEEW, 2024c). As of October 2024, there were 14 pilot-scale hydrogen projects operating in Australia with all except two producing renewable hydrogen (CSIRO, 2024). Safeguard Mechanism The Safeguard Mechanism is the Australian government’s central policy for reducing industrial emissions. It has been in place since 2016 and was substantially reformed in 2023. The Safeguard Mechanism applies to large industrial facilities emitting more than 100 KtCO 2 e per year and imposes declining limits on facility net emissions or ‘baselines’. The power sector is treated separately from industrial facilities. Under the reformed SGM, baselines will decline by 4.9% each year to 2030 (DCCEEW, 2024k). To comply with declining baselines, facilities must either cut their emissions, acquire Australian Carbon Credit Units (ACCUs), or purchase newly introduced Safeguard Mechanism Credits (SMCs). The reform allows for unlimited use of offsets to meet declining baselines. Past 2030, baselines decline rate will be determined in five-year blocks to align with the 2050 net zero target (DCCEEW, 2023b). The design of the mechanism assumes significant new fossil fuel projects to come online, such as new carbon-intensive gas fields and coal mines (Clean Energy Regulator, 2023b; Department of Climate Change, 2023e; Reputex, 2023). The reform mandates new shale gas projects must have net zero scope-1 emissions, i.e. domestic emissions occurring during fossil gas production, and that new gas fields will be given a zero baseline for reservoir CO 2 (DCCEEW, 2024k). The effectiveness of the mechanism depends on the extent to which existing and new facilities covered under the mechanism rely on offsets to meet their baselines. In 2023, 219 facilities were covered by the SGM accounting for gross emissions of 138.7 MtCO 2 e (Clean Energy Regulator, 2024), which was approximately 26% of Australia’s total emissions excluding LULUCF (DCCEEW, 2024i). The same facilities also surrendered 1.2 million ACCUs in 2023, meaning that SGM facilities collectively offset 1.2 MtCO 2 e to meet their baselines in preference to making direct on-site emissions reductions. The reformed SGM aims to reduce net SGM facility emissions from 138 MtCO 2 e in 2022 to around 100 Mt in 2030 (AR5 values). The government projects that gross emissions from SGM facilities will reduce from 138 MtCO 2 e in 2022 to 121 MtCO 2 e in 2030, and that net emissions (i.e. accounting for offsets), would fall to 93 MtCO 2 e in 2030. This reduction implies that less than half of the abatement to 2030 will result from on-site emissions cuts.</t>
-  </si>
-  <si>
-    <t>Oil and gas production At over a third of total emissions, oil and gas production represents Canada’s largest source of emissions (Environment and Climate Change Canada, 2024). While the sector’s emissions dropped in 2020 due to the pandemic, they are projected to reach again 2019 levels under current policies by 2030 as production is projected to increase. Canada’s exported emissions from oil and gas are continuing to rise, surpassing its total domestic GHG emissions, and sitting at about 939 MtCO 2 in 2022 (Bernstien, 2024). This comes at a time when the IEA has called for no new investments in oil, gas and coal if we are to stay below the 1.5°C limit of the Paris Agreement. The government seems incapable of kicking its oil and gas addiction. It has promised to set a cap on emissions for the sector, and believes this can be achieved while increasing production. Regulations for the cap are being consulted on in 2024 and are due to be finalised in 2025. They are not yet modelled in our projections. The government is also planning to strengthen methane emission regulations in the sector (see the Methane section below) (Government of Canada, 2023b). In April 2022, the government approved an offshore oil and gas megaproject, Bay du Nord (Impact Assessment Agency of Canada, 2022a). The project is required to be net zero from 2050 onwards, but production could continue until 2058 (Impact Assessment Agency of Canada, 2021, 2022a). The environment and energy ministers disagree over whether this will be the last development of its kind in Canada (CBC News, 2022). Whether the project will actually proceed is unclear: the company delayed the project by three years amidst concerns over high costs, and challenges to the environmental and economic assessments continue (Canada, 2023; Federal Court of Canada, 2023; Nickel, 2023; Sierra Club, 2024). The costs of current oil and gas expansion projects continue to rise. The Trans Mountain oil pipeline expansion, due to start operation in 2024 (Calgary Herald, 2023; Trans Mountain Corporation, 2022), is now expected to cost seven times more than when the government first purchased the pipeline (CAD 5.4 bn) (Lindsay, 2021; Williams, 2023). In June 2022, a budget watchdog concluded that it was not viable and would cost the government around CAD 600 million in net losses (Thurton, 2022). Others have estimated that losses will be much higher (The Energy Mix, 2022; Williams, 2023). Costs associated with the pipeline for the country’s first LNG export terminal, on the country’s west coast, are also soaring (Jang, 2022; Simmons, 2022). While this pipeline is not government-owned, there are questions as to whether it will be able to recoup all of the subsidies provided (Simmons, 2022). The LNG project will only begin exporting fossil gas to Asia in 2025–2026. Meanwhile, a new anti-greenwashing regulation is causing oil and gas industry associations to scrub their websites of unsubstantiated CCS claims (Noakes, 2024). Net-Zero Producers Forum Canada is part of the ‘Net Zero Producers Forum’, along with other oil and gas majors: Norway, Qatar, Saudi Arabia, the UAE and the US (Natural Resources Canada, 2021a; U.S. Department of Energy, 2021). The forum’s stated aim is to develop ‘pragmatic net zero emission strategies’, including reducing methane emissions and supporting the use of CCS, but it does not tackle the core issue of phasing down production. Beyond holding its first Ministerial meeting and establishing a working group in March 2022, there is little evidence of concrete action more than a year after its formation. Meanwhile, investors and international oil companies continue to exit Canada’s tar sands (Morgan, 2020; Reuters, 2021; The Canadian Press, 2020; Total, 2020; Tuttle, 2022). Beyond Oil and Gas Alliance (BOGA) The province of Quebec is a member of BOGA, but Canada as a whole is not. In April 2022, Quebec passed a law banning any further production and mandated that existing drill sites be shut down within three years (Government of Quebec, 2022). The move is largely symbolic as the province is not a producer of oil and gas (Canada Energy Regulator, 2022). Coal mining In 2021, the government committed to banning thermal coal exports from and through Canada by 2030 (Liberal Party of Canada, 2021b; Prime Minister of Canada, 2021b). The reference to ‘through Canada’ is important, as many American west coast miners export their coal through Canada due to resistance to developing the export infrastructure in their own country (Institute for Energy Economics and Financial Analysis, 2021; Kuykendall, 2021). While establishing the ban is in the trade minister’s mandate letter , he has not yet taken action to implement it (Global Affairs Canada, 2022; Prime Minister of Canada, 2021a). On the contrary, Canadian coal exports soared in 2023, causing the opposition party to call the government to task on this issue (The Canadian Press, 2024a, 2024b). Canada had been criticised for its hypocritical stance on coal mining, and for not subjecting a thermal coal mine expansion to a federal impact assessment, notwithstanding its position in the Powering Past Coal Alliance (Rabson, 2020). In June 2021, Canada clarified its policy position on thermal coal mining, finding that any new mines or expansions of existing mines would likely cause unacceptable environmental effects (Government of Canada, 2021i). One coal mining expansion project is still attempting to get approval, with environmental groups fighting the government's decision to lift the requirement for an environmental impact assessment (Ecojustice, 2023; Impact Assessment Agency of Canada, 2022b).</t>
-  </si>
-  <si>
-    <t>Chile is the world’s leading copper exporter, and the mining and industry sector is Chile’s largest consumer of final energy, accounting for 36% of energy consumption in 2021 and approximately 17% of total GHG emissions (IEA, 2024a). In 2021, 44% of mining electricity consumption came from renewable sources, and it is estimated that it will reach 62% in 2025. Chile has established several targets to minimise emissions from the mining and industry sector in its energy strategy (PEN). They include: an emissions reduction target of 70% of direct GHG emissions from fuel use in the industry and mining sector by 2050 below 2018 levels, an improvement of energy intensity of large energy consumers by at least 25% in 2050 below 2021, a requirement that at least 90% of energy for heating and cooling in industry must come from sustainable sources by 2050, a goal of 100,000 new energy jobs by 2030, direct and indirect, from sustainable energy projects in new energy-related industries, and a requirement that 100% of medium and large companies in Chile must implement effective and monitorable energy efficiency and/or renewable energy measures. These measures are also featured in Chile’s LTS (Gobierno de Chile, 2021; Ministerio de Energía, 2022c). Mining companies themselves play an important role in meeting these targets. The Chilean Copper Commission (COCHILCO) has carried out surveys and compiled data on GHG emissions and energy consumption, the Green Mining Roundtable was launched in 2019, and the Chilean Economic Development Agency (CORFO) has supported the deployment of hydrogen vehicles for mining (Ministerio de Energía, 2020a). The deployment of green hydrogen and its derivatives in the mining sector is a key component of Chile’s Green Hydrogen Strategy and Action Plan (Gobierno de Chile, 2024). The National Mining Policy 2050, developed by the Ministry of Mining, was approved in early 2023, and includes several objectives related to GHG emissions and environmental considerations. Notably, it includes a target to reduce emissions from large mining operations by at least 50% by 2030, and to become a carbon-neutral industry by 2040. It also outlines a zero-emissions fleet plan to be released by 2025 and implemented by 2030, as well as an objective for 90% of electricity contracts to come from renewable sources by 2030 and 100% by 2050 (Gobierno de Chile, 2023a). Along with being responsible for the monitoring and implementation of the above, the Ministry of Mining is also directed to establish GHG emissions targets for scope 1, 2, and 3 that comply with the 2030 target. Among the provisions of the new Energy Efficiency Law approved in early 2021 is the promotion of energy management in the country's largest consumers. These include all large companies with consumption over 50 Tcal per year (210 TJ/yr), cumulatively accounting for more than one third of the country’s consumed energy. These so-called consumers with energy management capacity have to implement an energy management system that covers at least 80% of their emissions and will additionally have to prepare an annual public report on several performance indicators, including energy consumption and energy intensity (Ministerio de Energía, 2021d; Ministerio de Hacienda: Oficina de Partes, 2021)</t>
-  </si>
-  <si>
-    <t>Industry is the largest energy-consuming sector in China, accounting for 58–59% of the country’s final consumption in 2022 (IEA, 2023b). Half of the direct energy consumed in the sector currently comes from coal and fossil gas, although combined shares of the fossil fuels are expected to plateau in the next decade as China targets increasing electrification and efficiency to meet expected demand (IEA, 2023b). Steel and cement output for real estate and infrastructure construction are the main drivers of industry emissions and the primary cause of China’s dip in emissions in 2022.Given the sector’s gargantuan energy consumption, decarbonisation of major industrial subsectors is critical—and central—to achieving national climate and energy targets. The government’s new industry peaking implementation plan has aligned the entire sector’s CO₂ emissions peaking timeline with China’s 2030 NDC target, while the 14th FYP for Green Industry Development has matched the economy-wide energy and emission intensity reduction targets (MIIT of China, 2021; MIIT of China, NDRC and MEE, 2022). China has set its carbon peaking targets for steel, cement, and aluminium for the year 2030, despite prior discussions regarding the feasibility of reaching these peaks by 2025. The delayed emission peaking timelines are to allow the sectors breathing space amidst energy and supply chain security concerns and to consolidate a less ambitious target that could be reached by all companies in a bid to tackle other industry concerns such as overcapacity and pollution (Guoping and Zou, 2022; Lin, 2022). China also set interim objectives for 2025, including reducing the energy intensity of steel production by 2% and recycling 320 million tonnes of scrap steel, as well as reducing the energy intensity of cement production by 3% (from 2020 levels) (Bloomberg, 2021; EEO, 2021; China Dialogue, 2022; MIIT of China, 2022; MoHURD of China and NDRC, 2022). To achieve a 1.5°C-compatible steel industry, China must retire its emissions-intensive Blast Furnace-Basic Oxygen Furnace (BF-BOF) route and cease building new coal-based steel plants. The resulting capacity gap should be filled through increased scrap recycling and green hydrogen-based direct iron reduction (DRI), with ironmaking prioritizing the use of electric arc furnaces (EAF) powered by clean energy (Climate Action Tracker, 2024). The Special Action Plan for Energy Conservation and Emission Reduction in the Iron and Steel Industry, issued in June 2024, aims to reduce energy consumption per unit of product by more than 1% for the BF-BOF and by more than 2% for EAF by 2025 compared to 2023 levels (NDRC et al. , 2024). The government is taking decisive steps to transition the steel sector to low-carbon production and address overcapacity by indefinitely suspending all new steel plant permits as of August 23, 2024. Earlier in the year, permits were only granted for EAF steelmaking plants (MIIT of China, 2024). By cutting steel output and increasing scrap-based steel production through EAFs, China could reduce CO₂ emissions from the steel industry by 200 Mt by 2025—equivalent to the EU's annual emissions from steelmaking (CREA, 2024). Key emitting sectors, such as cement, steel, and aluminium are likely to be the first targeted in the scope expansion of the country’s ETS (Wang, 2021; Wulandari, 2022). While the inclusion of these sectors was already in the pipeline, the approval of Carbon Border Adjustment Mechanism (CBAM) regulations by Europe (to be officially launched in 2026) has added a sense of urgency. To cover sectors eligible under the CBAM phase 1, cement, aluminium and iron and steel, China announced plans to expand its national ETS to include these industries by the end of 2024 (ChinaNews, 2024).. The MoU between the Chinese and German governments in June 2023 highlighted the focus on industrial emission reduction, especially in the cement, steel, chemical, and pulp and paper industries (German and Chinese Governments, 2023). To fully decarbonise China’s harder-to-abate sectors, the development of CCUS and hydrogen solutions have become priority strategy areas. CCUS will be a critical technology to help China drastically reduce emissions towards carbon neutrality in the long-term and has received increasing national attention in the last two decades, with objectives now focusing mainly on large-scale project demonstrations. As of 2021, CCUS was highlighted in the last three FYPs, the Ministry of Ecology and Environment (MEE) has encouraged provinces to pilot and demonstrate CCUS projects, and 29 provinces have already issued policies and plans related to the technology. China has commissioned three projects in 2023 and now has a project pipeline with the potential to capture around 10 MtCO₂/year (IEA, 2023a). However, the efficacy of CCS has yet to be fully realised in any CCUS project anywhere in the world, with budget blowouts and failure to reach announced sequestration rates (IEEFA, 2022). China published its national hydrogen strategy (2021–2035) in 2022, confirming the technology’s key role in China’s future energy system and mitigation efforts. While hydrogen is mainly produced from coal and gas, the plan targets a modest production of 100,000–200,000 tonnes of renewable-based hydrogen with renewable sources by 2025: this would constitute less than 1% of its production (Yao, 2022). The China Hydrogen Alliance estimates this could reach 100 Mt by 2060, accounting for 20 percent of the country’s final energy consumption (Nakano, 2022). The application of hydrogen in steelmaking decarbonisation has commenced, though it remains largely in the R&amp;D phase. An Italian firm specialising in sustainable metal production has partnered with China's leading steel manufacturers, Hesteel Group and Sinosteel, to establish DRI plants powered by hydrogen-enriched fossil gas, with a combined production capacity of 1.6 Mtpa (Tenova, 2020, 2022, 2024). F-gases China ratified and started enforcing the Kigali Amendment in 2022 (Rudd, 2021). China reported that it halted the new production capacity of five of the 11 HFCs it produces (covering 75% of total HFC production) two years ahead of the freeze requirements (McKenna, 2022). According to our analysis, China would reduce emissions by a modest ~50 MtCO₂e/year by 2030 under the Kigali Amendment’s phase-out schedule, although reductions could increase to almost 300 MtCO₂e/year by 2045.</t>
-  </si>
-  <si>
-    <t>The EU’s industrial emissions, both energy related and from industrial processes, accounted for about 24% of its total GHG emissions in 2021 (Climate Analytics, 2024; UNFCCC, 2023). Industrial emissions have been falling on average about 2.3% per year but this is not fast enough and the EU’s industry will need to accelerate this 1.3 times faster than its current trend to reach 1.5°C compatibility (European Climate Neutrality Observatory, 2024b). The EU has not signed the Beyond Oil and Gas (BOGA) declaration but eight of its member states have. Six member states — Denmark, France, Ireland, Portugal, Spain and Sweden — are core members of the Alliance and have committed to ending oil and fossil gas exploration and development (Beyond Oil and Gas Alliance, 2021). To decarbonise its industries, the EU introduced indicative targets in the revised Renewable Energy Directive (EU 2023/2413) for the share of renewables in industry. Article 22 requires the industry sectors in member states to increase the share of renewable energy by an average annual rate of 1.6% between 2021 and 2030. This annual 1.6% indicative benchmark was watered down by the Commission from the initial 1.9% growth rate it estimated it would need to deliver on the REPowerEU objectives (European Commission, 2022a). The revised Renewable Energy Directive also requires that only 42% of incorporated hydrogen be derived from renewable energy by 2030 and 60% by 2035. This means that the industry will use a mix of renewable and fossil fuel derived hydrogen. This design will allow industries to start their shift to hydrogen but access cheaper fossil fuel derived hydrogen until the green hydrogen is available at scale and affordably. The EU does not have any provisions to fully eliminate fossil fuel derived hydrogen from industry beyond 2035, which risks the long-term dependence on fossil derived hydrogen. Green hydrogen The Commission’s Hydrogen Strategy sets out that installed capacity of electrolysers in the EU should reach 40 GW by 2030, resulting in the production of up to 10 million tonnes of green hydrogen, complemented with similar capacity installed in neighbouring countries (European Commission, 2020). The EU hydrogen policy framework has several key gaps hindering market development and does not go far enough to address issues such as high-cost entry barriers and uncertainties. At present, renewable hydrogen is also much more expensive than fossil fuel-based hydrogen. Financial support is fragmented, with a shortage of targeted funds necessary to meet the 2030 REPowerEU goals. Additionally, the EU lacks a clear definition for low-carbon hydrogen, and is only expected to develop a methodology by 2025 as part of the Delegated Act of the revised Gas Regulation. Developing a net zero technology Industry To tackle replacing industrial technology with cleaner alternatives, the EU has been developing a nexus of polices to facilitate the growth of (1) net zero technology industry and (2) industrial carbon removals, encapsulated by the: Net Zero Industry Act (NZIA) (EU) 2024/1735, and more broadly the Green Industrial Plan Industrial Carbon Management Strategy Carbon Removal Certification Framework (proposal) 2040 climate targets (proposal) In June 2024, the Net Zero Industry Act entered into force (European Parliament &amp; European Council, 2024c). It focuses on 19 net zero technologies. It also includes the objective of developing annual injection capacity for carbon capture and storage of 50 MtCO 2 e by 2030 that should be used to mitigate residual emissions. These capacities should be developed by oil and fossil gas companies proportionally to their current oil and gas production levels. The NZIA will be crucial to operationalising the direction set by the Industrial Carbon Management Strategy (ICMS) (European Commission, 2024d). The ICMS lays out how it plans to scale up industrial carbon removals to deliver the EU’s climate neutrality objective, most notably from bioenergy with carbon capture and storage (BECCs) and direct air carbon capture (DACC). It sets out a target to reach 50 MtCO 2 e in carbon removals annually by 2030. The ICMS is strongly linked to the proposed 2040 targets, which are yet to be adopted. In its impact assessment the Commission envisions it would need about 75 MtCO 2 e of industrial carbon removals from BECCs and DACCs by 2040. Additionally, the Commission will create policy options and support mechanisms for industrial carbon removals, including considerations on whether and how to integrate them into the EU Emissions Trading System (ETS) but this is not expected until the planned revision of the ETS in 2026 (EPG, 2024). In April 2024, the political agreement was reached on the Carbon Removal Certification Framework (CRCF) but is still to be adopted (Carbon Gap, 2024a; European Commission, 2022b). The CRCF seeks to establish a framework to certify the emission removals from carbon farming, carbon storage in products and industrial carbon removals (from technologies like Direct Air Carbon Capture and storage (DACCS) and bioenergy with carbon capture and storage (BECCs). The CRCF is the mechanism to deliver on the goals of the ICMS and lays out the role the CDR will play. The CRCF gives the Commission the ability to assess options for CDR and CCS targets. The CRCF is riddled with concerning elements that could go against climate action. The regulation lacks a distinction between emission reductions and removal, potentially allowing removals to offset emissions that should be reduced. It also risks offsetting and greenwashing through the permitting of sales of carbon credits as offsets in voluntary carbon markets, especially if large emitters are allowed to buy these credits. The 2040 climate target communication keeps the role of CCS in the power sector vague under the proposed 2040 targets. This is worrying as the application of CCS to certain sectors is left open to interpretation. The incoming Commission has the opportunity during the subsequent expansion of the Industrial Carbon Management Strategy and Clean Industry Deal to clearly commit to no CCS in the power sector. Carbon Capture and Storage (CCS) refers to technologies which use engineered methods to capture CO 2 from a source and store it geologically. CCS can be applied to a range of different CO 2 sources in different sectors. CCS technologies are neither commercially viable nor proven at scale, despite large public subsidies for research and development globally. Heavily relying on unproven CCS for power generation simply prolongs the use of fossil fuels, diverting attention and resources away from the necessary and urgent switch to renewable energy generation that drives down actual emissions. The use of CCS should be limited to industrial applications where there are fewer options to reduce process emissions—not to reduce emissions from the electricity sector where renewables are cost-effective mitigation alternatives, not least because CCS doesn't remove 100% of emissions from power plants.</t>
-  </si>
-  <si>
-    <t>The UK’s Industrial Decarbonisation Strategy introduced by the previous government (UK Government, 2021a) aims to reduce industrial emissions by two-thirds below 2018 levels in 2035 and 90% by 2050. While emissions fell 3% in 2022 to 63 MtCO 2 e, they will need to fall much faster, by around 8% per year, to achieve the government’s climate targets (CCC, 2023a). The strategy has a three-pronged approach: switching to low carbon fuels, efficiency gains, and carbon capture and storage (CCS). While some action is beginning to occur on fuel-switching, in particular in the electrification of steel, there remain significant gaps in the policies supporting resource efficiency in the industrial sector (CCC, 2024). Fuel switching In 2023, over 50% of industrial final energy was provided directly by fossil fuels (DESNZ, 2024c). This will need to be reduced substantially on the path to net zero. Two key options are the use of hydrogen, and direct electrification. The Industrial Decarbonisation Strategy sets a target of 50 TWh of fossil fuels to be replaced by low-carbon alternatives by 2035 in the manufacturing sector (UK Government, 2021a). This is roughly a third of industrial fossil consumption in 2022. To support this target, the previous government introduced the Industrial Decarbonisation and Hydrogen Revenue Support (IDHRS) scheme. This is similar to the CfD scheme in the power sector, providing financial support to cover the additional cost of low-carbon hydrogen production. GBP 140m was allocated to support fuel-switching over 2023–2024. This provides a business model to support industrial fuel-switching to hydrogen and is a positive step. There is also a GBP 240m Net Zero Hydrogen Fund (DESNZ, 2023). While these funds are to be welcomed, they are much smaller than the scale of funds being offered in Europe to support hydrogen deployment (Abnett, 2023). Industrial electrification has taken a step forwards in the UK, with the agreement of a deal to transform the Tata steelworks from a coal-fired blast furnace to an electric arc furnace producing recycled steel (H. Thomas &amp; Browne, 2024). In November 2023, a similar decision was announced for the remaining blast furnaces operated by British Steel, although the planned switch date of 2025 may be set back due to grid connection delays (Gill, 2024). This marks a transition away from coal in steelmaking which will reduce emissions. However, there has not yet been sufficient planning on how to ensure a just transition which preserves jobs in local communities dependent on steelmaking. This is a critical gap that must be addressed. There is also a need to drive industrial electrification in a more systematic way, with electricity prices still too high when compared to fossil gas (CCC, 2024). Carbon capture and storage The previous government set an aim of delivering 6 MtCO 2 /yr of industrial CCS by 2030, and 9 MtCO 2 /yr by 2035. This represents around 17% of total abatement in the industrial sector by 2035 (CCC, 2023a). The new government has continued this commitment to CCS, pledging GBP 22 bn of funding to drive CCS projects over the next 25 years (UK Government, 2024). Relying too heavily on CCS to deliver emissions reductions in the industrial sector could be risky, as the majority of previous CCS projects have ended in failure (Abdulla et al., 2020). In many sectors, the role and value of CCS is also being eroded as the cost of renewables declines (Grant, Hawkes, Napp, et al., 2021). CCS should be prioritised for applications where there are few alternatives, such as cement production (E3G, 2023). Fossil fuel supply Achieving the UK’s climate targets will require strong and sustained reductions in oil and gas production, as well as improvements to the emissions intensity of any remaining extraction. Oil and gas demand will need to fall around 30% by 2030 to achieve the UK’s NDC (CCC, 2020). The CCC also suggested that the emissions associated with oil and gas extraction should fall 68% by 2030, through electrification of processes and addressing fugitive emissions (CCC, 2020). The previous UK government moved in the opposite direction, continuing to support new oil and gas extraction in the North Sea, approving the Abigail, Jackdaw and Talbot fields (Oil and Gas Authority, 2023; A. Thomas, 2022; Tidman, 2022). New licensing rounds were held annually (UK Government, 2023a). The incoming government has set a new direction, committing to end licensing for new oil and gas fields (Lempriere, 2024). This is a good start and should be welcomed. However, it does not address the substantial pipeline of projects which have already received exploration licenses and are either waiting for development consent or are already in production. There are thirteen such projects awaiting approval (Dunne, 2024). The new government could strengthen its position on oil and gas by publicly committing to not approve this remaining pipeline of projects, and also set out a clear path to phasing out oil and gas production in the UK in line with the Paris Agreement goals, for example joining the Beyond Oil and Gas Alliance (BOGA).</t>
-  </si>
-  <si>
-    <t>Oil production Oil extraction has been the backbone of the Saudi economy for decades. Saudi Arabia is the world’s second largest oil producer after the United States and is OPEC’s leading oil producer (BP, 2023). It produced approximately 12% of the world’s oil in 2022 and held 17% of proven oil reserves. While the government has taken small steps to diversify the economy, Saudi Arabia remains highly dependent on hydrocarbon revenue. In 2022, Saudi Arabia reported USD 362bn in total crude oil export revenues and an additional USD 45bn in refined petroleum export revenues: several orders of magnitude higher than the oil export revenues from any other country (OEC, 2024). Oil is Saudi’s most exported commodity, accounting for 75% of the total value of exports in 2021 (OPEC, 2023). Over the past two decades oil rents, which are the difference between crude oil market prices and production costs, have consistently contributed at least 20% of Saudi’s annual GDP (World Bank, 2021). This close dependency between Saudi’s GDP growth and the oil market puts the sustainable growth of Saudi’s economy at risk. Recent geopolitical conflicts have once more shown the vulnerability of the global oil market to exogenous shocks. Saudi Arabia does not plan to end investment in new oil production, which is required to hold global warming to 1.5°C (IEA, 2023a). While Aramco recently abandoned its plan to increase oil production capacity to 13 million barrels per day (mb/d) by 2027, this decision appears largely driven by strategic considerations rather than a commitment to phase out fossil fuels. This reversal reflects changes in the global oil market, including slowing demand growth and increased production from non-OPEC countries, particularly the U.S ( FT, 2024 ). The government’s current diversification plans include no scenario with a decline in global oil consumption in the coming decades, which is required to meet the objectives of the Paris Agreement and reach net zero CO 2 emissions by mid-century (IEA, 2023a; IPCC, 2018). Both the “business-as-usual” and the “2030 renewable energy target” scenarios outlined in KAPSARC’s Energy Policy Solutions project hydrocarbon exports to significantly increase until 2050 (KAPSARC, 2021). At COP28, Saudi Aramco signed the Oil and Gas Decarbonisation Charter (OGDC), a new initiative which aims to “accelerate climate action” in the fossil fuel sector. However, the OGDC only addresses a fraction of relevant emissions from oil and gas production. Although most emissions come from fuel combustion, the initiative solely focuses on reducing emissions within the operations of oil and gas companies, such as in drilling and refining processes. Without a commitment to reducing the extraction and burning of fossil fuels, the charter fails to tackle the main driver of climate change. So far, none of the signatories have agreed to cut fossil fuel production. Carbon capture and storage Saudi Arabia is betting on carbon capture and storage (CCS) technologies to reach its climate goals while sustaining its fossil fuel production and exports. As of 2024, it only had one operational CCS plant—which is used for enhanced oil recovery (EOR), rather than reducing emissions from fossil fuels (Global CCS Institute, 2023). The government has a target to capture and store 44 million tonnes of CO 2 annually by 2035. To this end, Saudi Arabia is in the process of building a CCS hub at the industrial complex of Jubail, which it plans to capture CO 2 from fossil gas plants. The hub is expected to be operational from 2027 and the plans are to capture up to nine million tonnes of CO 2 per year from three Aramco fossil gas plants (The CCUS hub, 2023). But given the track record of CCS technology so far, these planned capture rates are questionable. CCS technologies are not commercially viable, nor are they proven at scale, despite large public subsidies for research and development globally. Relying on CCS to the extent Saudi Arabia is planning diverts attention and resources away from cost-effective mitigation options. The use of CCS should be limited to industrial applications where there are fewer options to reduce process emissions—not to reduce emissions from the electricity sector where there are cost-effective mitigation alternatives, not least because CCS does not remove 100% of emissions from power plants. Saudi Arabia is promoting the concept of a Circular Carbon Economy (CCE) to reduce emissions from oil and gas production (Luomi et al., 2021). This, however, only addresses a fraction of relevant emissions as most emissions come from fuel combustion rather than oil and gas extraction and processing. Saudi Arabia’s CCE plans largely rely on the development and deployment of CSS technologies (Kingdom of Saudi Arabia, 2022).</t>
-  </si>
-  <si>
-    <t>In 2021, Singapore’s industrial sector accounted for 44.4% of its primary emissions, plus 16.6% of secondary emissions from electricity use (National Climate Change Secretariat, 2024). Singapore´s mitigation strategy for the industry sector is based on increasing energy and carbon efficiency. The main policies are the Energy Conservation Act from 2013, which mandates monitoring and reporting energy usage and GHG emissions for large energy users; the Energy Efficiency Fund (E2F), which provided grants and tax incentives for energy efficiency investments in industrial processes; and the Energy Efficiency National Partnership Programme (EENP), which is a learning network for companies in the industrial sector to learn about energy efficiency ideas, technologies, practices, and standards (National Environment Agency, 2020). In 2017, the Energy Conservation Act (ECA) was enhanced, requiring, from 2018 onwards, the energy users it covers to have their monitoring plans verified by an independent third party and appoint a GHG manager (National Environment Agency, 2017). From 2021 onwards, these companies must establish a structured energy management system, and periodically assess energy efficiency opportunities at existing industrial facilities. In 2018, minimum energy performance standards were introduced to phase out the least efficient industrial electric motors and expanded to other common industrial equipment and systems thereafter (National Environment Agency, 2018). In the context of Singapore’s 2018 Climate Action Year, over 450 organisations, including industrial manufacturers, made voluntary commitments to improve their carbon footprint or increase awareness on climate change-related issues, such as upgrading existing equipment (e.g. chillers, lightings, appliances) with more energy efficient models, or starting recycling and waste management programmes. Given the voluntary nature of the pledges, and the lack of information to translate these targets into emission reduction targets, we have not included these in our current policy projections. The Sustainable Jurong Island report, which outlines targets and aspirations to decarbonise Singapore’s Energy &amp; Chemical (E&amp;C) hub, is targeting 2 Mt of carbon capture, utilisation and storage (CCUS) by 2030. (Singapore Economic Development Board, 2021) In December 2023 the government signed an agreement with ExxonMobil and Shell to "coordinate the planning and development of a CCS project, capable of capturing and permanently storing at least 2.5 million tons of CO2 a year, by 2030." Storage sites have not yet been selected and no details were included regarding capture facilities or transport infrastructure (Singapore Economic Development Board, 2024). Given the early phase of the consortium development and the track record of CCS across the world to date, including high costs and protracted development times, this is an ambitious target. Other developments on Jurong Island include a 285 MWh battery energy storage system, which surpasses Singapore’s target of 200 MWh energy storage by 2025, and Singapore’s first hydrogen-ready power plant, which will be operational by 2026 and is designed to operate initially on 30% hydrogen gas. A tender to install solar PV on 60 hectares of interim vacant land and the rooftops of five buildings on Jurong Island has also been initiated as part of the SolarRoof and SolarLand programs, following an initial pilot on 3.9 hectares of land (Energy Market Authority, 2023b).</t>
-  </si>
-  <si>
-    <t>Policy and planning documents for the South African industry sector generally address sustainable industrial economic development but barely mention mitigation targets for the industry sector or concrete measures for implementation. The post-2015 draft National Energy Efficiency Strategy proposes industrial sector targets for energy efficiency in 2030; however, there is no indication of implementation. (Department of Energy, 2016). Energy use from the mining and quarrying sector amounted to 185 PJ in 2015 (IEA, 2017). The South African government intends to achieve these targets through implementing several proposed measures such as the National Cleaner Production Centre South Africa (NCPC-SA) that promotes energy efficiency measures, its associated Industrial Energy Efficiency Project (IEE) implemented between 2011–2021 that promoted energy management systems, or the Green Fund South Africa that financially supports green technology research and implementation. However, these measures may only induce small emissions reduction impacts. South Africa is also aiming to develop value chains for renewable energy and storage technologies through the South African Renewable Energy Masterplan (SAREM), released for public comment in July 2023 (The dtic, 2023). The plan particularly aims to take advantage of increasing domestic and international demand for these technologies to drive industrial development and create jobs as part of the just transition. There are no signs of policy-driven emissions reductions in the near future for emissions-intensive subsectors such as steel production and mining, though there has been some interest in hydrogen. The Hydrogen Society Roadmap (2021) and draft Green Hydrogen Commercialisation Strategy (2020) highlight the potential role of and steps to develop green hydrogen for use in steel production, industrial mining, mineral beneficiation, manufacturing, logistics, and other sectors (DSI, 2021; The dtic, 2022). The South African Steel and Metal Fabrication Master Plan 1.0 (2021) mentions hydrogen, along other measures, in consideration of greening the industry (The dtic, 2021). For hydrogen to decarbonise the industry sector, it must be produced using renewable energy. Analysis by the Climate Action Tracker indicates that the steel industry’s emissions intensity would need to be reduced by about 30% in 2030 and by about 90%-100% by 2050 to be compatible with the Paris Agreement.</t>
-  </si>
-  <si>
-    <t>Emissions from manufacturing industries, construction and industrial processes and product use (IPPU), accounted for 23% of Switzerland’s CO 2 emissions in 2022. These levels are almost equal to those in 1990 (Bundesamt für Umwelt BAFU, 2024b). With Switzerland's new Climate Protection Act that passed a referendum in 2023, Switzerland now has emissions reductions targets for the industry sector to reduce emissions by 50% by 2040 and by 90% by 2050 below 1990 levels (Bundesgesetz Über Die Ziele Im Klimaschutz, Die Innovation Und Die Stärkung Der Energiesicherheit (KlG), 2023). Most GHG emission reduction policies and measures affecting Switzerland’s industry sector are implemented under the CO 2 Act and cover CO 2 emissions from fossil fuel use. These include the CO 2 levy on heating and process fuels, the Swiss ETS, and the negotiated reduction commitments. A number of key non-CO 2 emissions are not covered under the Act, and have been targeted separately. For example, a number of provisions relating to substances stable in the atmosphere cover all F-gases and are expected to result in a reduction of roughly 1.1 MtCO 2 e in emissions of such gases in 2020 (Schweizerische Eidgenossenschaft, 2020c). Similar to the EU, Switzerland also uses an ETS to lower emissions from large, energy-intensive entities. The Swiss ETS is much smaller than the European ETS, not only because of the smaller market but also due to the fact that the emissions generated by 54 companies in the power, cement, pharmaceutical, refinery, paper, district heating, and steel sectors covered by the scheme represent only 10% of the country’s emissions. Emissions from the sector were capped in 2013 at 5.63 MtCO 2 , and required to reduce by 1.74% per year in order to reach a target of 4.91 MtCO 2 in 2020 (13% reduction on 2013 levels) (Mission of Switzerland to the European Union, 2017). From 2021, the annual required rate of reduction rose to 2.2% of the 2010 baseline, which applies until 2030 (Federal Office of the Environment, 2020).</t>
-  </si>
-  <si>
-    <t>Türkiye’s industry sector accounts for 25% of total emissions (excl. LULUCF) (Republic of Türkiye Ministry of Energy and Natural Resources, 2023). This share is split between industrial processes (13%) and energy use (12%). The manufacturing industry alone represents over a fifth of Turkish GDP (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024a), so decoupling economic growth from emissions will be critical to Turkish industry on the path to net zero. Cement, iron and steel production account for the majority of process-related emissions (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024a). These industries will be negatively impacted by the EU’s Carbon Adjustment Border Mechanism (CBAM), which will be fully introduced in 2026 (European Commission, 2024). CBAM places a carbon price on goods imported into the EU. Given that the EU represents an important trading partner for Türkiye, decarbonising the industrial sector will be essential to maintaining industrial competitiveness. Türkiye has announced the launch of an Emissions Trading System (ETS) largely modelled on the EU’s ETS (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024a). This is a market mechanism which caps how much GHGs a company can emit, with the cap gradually declining over time. The pilot phase of Türkiye’s ETS will begin in October 2024, with full implementation planned for two years later, in October 2026 (Barut &amp; Kesikli, 2024). Critically, the ETS will also be applied to the shipping sector. By setting a carbon price on emissions from ships entering and exiting Turkish ports, Turkish policy is aligned with EU policy, thus closing potential loopholes which shipping companies could use to avoid carbon prices (Safety4Sea, 2024). The ETS is a central pillar of Türkiye’s climate legislation, and the government has been clear in communicating specific details about the policy (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024b), more so due to its trade implications than climate. Developing clear policies with actionable targets and measures are critical for ministries to successfully reduce emissions. The government’s drafting and communication of the ETS can therefore be followed when developing future climate policies.</t>
-  </si>
-  <si>
-    <t>The industry sector, including oil and gas production, is the largest source of emissions in the UAE, accounting for 46% of the country’s total emissions, or 103 MtCO 2 e. This includes emissions from industrial processes as well as indirect emissions from power and heat generation (Government of the UAE, 2024b). The UAE’s LTS includes a target to reduce industry emissions by 5% below 2019 levels by 2030, and 93% by 2050, while its current policy projections estimate these emissions will rise by 18% above 2019 levels by 2030. The UAE has a series of policies to reduce emissions from its industry sector, mostly focusing on increasing efficiency through adoption of best practices. To reach its target, the UAE plans to adopt a series of policies such as a cap and trade system, contracts for difference, regulated transport and storage for CCS, updated blended cement regulations, updated building codes, hydrogen production incentives and others (Government of the UAE, 2024b). On April 2024, the UAE also ratified the Kigali amendment, committing to reducing HFCs consumption by 87% by 2047 compared to its average consumption in 2024-2026 (IIR, 2024). The UAE plans to reduce its industry emissions through different means. Around 20% of the reductions towards its net zero target will come from fuel substitution and process switches in key industries such as steel and cement (Government of the UAE, 2024b). For example, the UAE’s LTS mentions the switch to concentrated solar power for heat for industrial processes and switching from blast furnaces to hydrogen-powered direct reduced iron processes for steel. However, a large share of the emissions reductions (32%) is expected to come directly from the deployment of CCS and from the decarbonisation of the power sector which will also heavily rely on CCS. Such overreliance on a technology that has not yet been proven at scale can seriously hinder the UAE’s progress towards transitioning its industry sector and can serve as a smokescreen to continue expanding fossil fuel production (Government of the UAE, 2024b). Oil &amp; gas production The UAE is the world’s seventh largest oil producer and 14th largest gas producer (US EIA, 2023a). It is also one of the world’s largest oil exporters. The UAE’s exported emissions from oil and gas are about 2.5 times larger than its domestic emissions (see graph below) (Climate Action Tracker, 2023c). In 2022, oil production reached 4.2 million barrels per day, an increase of 12% compared to the previous year, and surpassed pre-pandemic levels (US EIA, 2023b). Following an OPEC+ decision in October 2022 (Deepthi Nair, 2022), to cut production by twomillion barrels per day (mbpd) in an effort to keep oil prices up the UAE announced it would cut over 140,000 barrels per day from May 2023 until the end of the year (Gulf Today, 2023). However, the government also recently announced it was bringing forward its oil production capacity of five mbpd target (up from 3.8 mbpd currently), from 2030 to 2025, signalling its intent to ramp up production in the short term (Di Paola, 2022). The UAE is also developing oil and gas offshore exploration and production. This is part of its efforts to reach “gas self-sufficiency” (ICLG, 2022). In February 2022, the first offshore fields were discovered, which are estimated to contain between 43 and 57 billion cubic metres of gas (AFP, 2022). During 2022, Abu Dhabi National Oil Company (ADNOC) Drilling was awarded almost USD 6bn in contracts to “maximise value from Abu Dhabi’s offshore oil and gas resources” (World-Energy, 2022). In October 2023, ADNOC awarded contracts worth USD 17 bn for the Hail and Ghasha Offshore Development project. This project aims to produce 1.5 billion standard cubic feet per day (bscfd) of gas before the end of the decade (Reuters, 2023). This is part of a USD 150bn ADNOC plan to increase production of oil and gas. According to the IEA, the development of new fossil fuel infrastructure beyond what was already committed in 2021 is incompatible with reaching net zero by 2050 (IEA, 2021). The UAE’s plans to further develop and invest in new fossil fuel infrastructure are inconsistent with limiting global warming to 1.5°C. These plans are also likely to lock the UAE into a high-emissions trajectory and undermine its transition to renewable energy. Instead of ramping up its gas production towards self-sufficiency, the UAE should set out an ambitious plan to phase-out its dependency on gas for electricity and avoid the risk of stranded assets (CAT, 2022). In October 2023, ADNOC announced plans to double its CCS target from 5 to 10 MtCO 2 e removed annually by 2030 as part of its decarbonisation plan (Energy Voice, 2023). In a sustainable 1.5°C pathway, CCS with fossil fuels does not play a relevant role in energy sector decarbonisation, as renewable energy is much cheaper and has a much lower environmental footprint. The use of CCS needs be limited to industrial applications where it is proven there are no other options to reduce process emissions. Hydrogen During COP26, the UAE unveiled its “Hydrogen Leadership Roadmap”, a strategy aimed at developing the domestic production of green and blue hydrogen aimed at export markets in Asia and Europe. The roadmap already includes seven projects which are either completed or underway (including blue ammonia production). The overarching target of the strategy is to reach a 25% market share in key markets such as India, Japan, Germany and others (H2 World News, 2021). According to the UAE’s 2023 NDC update, several projects are already under way to support the country’s hydrogen ambitions, and a new Hydrogen Strategy is being prepared (Government of the UAE, 2023a). In its updated Energy Strategy 2050, the UAE also includes a target to produce 1.4 Mt of hydrogen annually by 2031. The UAE’s LTS includes additional information on its hydrogen development plans, including production targets of 7.3 Mt by 2040 and 14.9 Mt by 2050. Around half of the hydrogen is expected to come from fossil fuels with CCS (blue hydrogen), with the majority of the second half being green hydrogen and a small share coming from nuclear power (pink hydrogen) (Government of the UAE, 2024b).</t>
-  </si>
-  <si>
-    <t>Direct GHG emissions from industry accounted for 23% of total US emissions in 2023, making it the third largest contributor to US GHG emissions after the transport and electricity sectors. In 2020, emissions from the industrial sector decreased by 6% due the COVID-19 pandemic. In 2021, sectoral emissions increased by 1% as a result of the economy’s recovery. In 2022, emissions remained stable, indicating that the sector’s emissions have not reached pre-pandemic levels again (U.S. Environmental Protection Agency, 2024n). Industrial emissions have remained largely stable over the past decade, even as the US economy has transitioned from a manufacturing to a service-based economy and as industrial processes have experienced efficiency improvements and shifted to less emissions-intensive fuels (U.S. Environmental Protection Agency, 2024n). Under current policies, emissions from the industrial sector are projected to remain stable or minimally decrease as a result of the counteracting forces of renewed growth in domestic manufacturing and strengthen decarbonisation policies under the Inflation Reduction Act (IRA) (King, Kolus, et al., 2024; U.S. Environmental Protection Agency, 2023d). The IRA funds several measures to decarbonise the industrial sector. The act provides USD 5.8bn in funding for the new Advanced Industrial Facilities Deployment Program. In 2024, this programme selected, and began awarding financing to, projects in emissions-intensive industrial facilities (e.g. iron, steel, concrete sectors). The DOE estimates that the programme will reduce 14 MtCO 2 annually (Office of Clean Energy Demonstrations, 2024). The IRA also expands tax credits for carbon capture, utilisation, and sequestration (CCUS) technology, building on the Bipartisan Infrastructure Law’s (BIL) investments in CCUS demonstrations and industrial applications (The White House, 2023b; U.S. Department of Energy, 2022d). Estimates suggest that measures under the IRA for industrial CCUS might reduce up to 240MtCO 2 e/year (U.S. Environmental Protection Agency, 2023d). The IRA includes the Advanced Energy Project Credit, which provides tax credits for industrial and manufacturing facilities that invest in certain clean energy technologies. Eligible facilities either must re-tool with equipment designed to reduce GHG emissions by at least 20%, re-equip, expand, or establish measures for producing and recycling clean energy equipment, or process, refine, and recycle critical materials (The White House, 2023b). A total of USD 10bn in tax credits was allocated in a first round. A second round in 2024 aims to allocate an additional USD 6bn (IRS, 2024; U.S. Department of Energy, 2024g). The US implemented a diverse patchwork of financial incentives to support the research and development of technologies that are key for industrial decarbonisation. However, the government has not introduced instruments to facilitate the commercialisation of many of the technologies needed in hard-to-abate industrial subsectors (System Change Lab, 2024). Unlike the EU, the US has not developed a national emissions trading scheme, which, if designed correctly, could help expediate the commercialisation of key technologies. The challenging economics of many technologies in the industrial sector, such as green hydrogen and CCUS, require clear, robust incentive schemes to de-risk and attract investment (Department of Energy, 2024). Individual products, such as clean and/or green steel, might otherwise still find niche market applications (e.g. via government procurement), but will likely not be sufficiently commercialised to enable a full sector decarbonisation. In March 2023, the US Environmental Protection Agency (EPA) finalised its Good Neighbour Plan, which requires industrial facilities and power plants in 23 states to cut NOx emissions to prevent pollution across state lines. By 2026, the EPA plans to set enforceable NOx emissions control requirements, which will primarily reduce emissions from harmful air pollutants and also reduce CO 2 emissions by 16 MtCO 2 e/year (U.S. Environmental Protection Agency, 2023e). F-gases In December 2020, the US Congress enacted legislation under the American Innovation and Manufacturing (AIM) Act to tackle hydrofluorocarbon emissions (HFC). The act directs the EPA to phase down the production and imports of HFCs by 85% until 2036. It is expected to reduce emissions by 4.7 GtCO 2 e by 2050 via sector-based requirements to transition to non-HFC-emitting alternatives and next-generation technologies (U.S. Environmental Protection Agency, 2021b). In 2024, the US met its HFC phase-down target of reducing HFCs by 40% below 2020 levels (Haroldsen, 2024). The IRA provides an additional USD 38.5m to the EPA to implement the AIM Act (The White House, 2023b). We incorporate the IRA's effects on reducing non-CO 2 emissions into our current policy projections through a review of studies that quantify this impact (see Assumptions section). Hydrogen Hydrogen plays a central role in the Biden Administration’s roadmap for decarbonising hard-to-abate industrial processes and replacing fossil fuel-based feedstock with cleaner alternatives. The IRA established the Hydrogen Production Tax Credit to incentivise domestic production of clean hydrogen and to meet the Biden Administration’s Hydrogen Shot target, which aims to reduce the cost of clean hydrogen by 80% to USD 1 per kilogram through 2030 (The White House, 2023b). Recently, the credit has received criticism for its requirements to minimise emissions from hydrogen production, which certain actors argue are too costly (Pontecorvo, 2024).</t>
-  </si>
-  <si>
     <t>CO 2 emissions from the industry sector (including indirect emissions from electricity use as well as emissions from industrial processes) accounted for 34% of Japan’s total energy-related CO 2 emissions in 2022 (GIO, 2024). Within the industry sector, the iron and steel, chemical and cement industries are the three largest emitters, respectively emitting 39%, 15% and 8% of industrial emissions in 2021. Emissions in the sector have reduced by 20% below 2013 levels (GIO, 2023). A 2023 progress report shows that the industry CO 2 emissions from the member companies of Keidanren, the most influential business association in Japan, including indirect emissions from electricity use in FY2022, was 20.8% lower than in 2013, and 3.7% lower than the previous year (Keidanren, 2024). The overall reduction since 2019 is primarily due the changes in industrial activity levels induced by the COVID-19 pandemic. Following Japan’s economic recovery, emissions from electric use rebounded slightly in FY2021 but remained lower than in FY2019, as the effects of the pandemic continued to linger in key industrial sectors. CO 2 emissions from the industry sector decreased again slightly in 2022 compared to the previous year mainly due to a decrease in iron and steel production (MOE, 2024). The main GHG emissions reduction effort in the industry is Keidanren’s Commitment to a Low-Carbon Society (Keidanren, 2013), a voluntary action plan which has monitoring obligations under the Plan for Global Warming Countermeasures (MOEJ, 2016b). Keidanren has since launched its Challenge Zero Initiative, in collaboration with the Japanese government, inviting companies to submit strategies to decarbonise their activities; a number of actors have already disclosed measures to be implemented, including in the steel and chemical industries (Keidanren, 2020). Over 370 companies from the GX league have publicly announced their 2030 emission reduction targets. Combined, these aim for 40% reduction in 2030 compared to 2013 levels, falling short of the government 46% target (Nikkei, 2024b). Among the industrial sectors that pledged to 2050 net zero goal is the iron and steel sector. The Japanese Iron and Steel Federation (JISF) announced in 2021 that it would aim to reach net zero CO 2 emissions by 2050 (JISF, 2021). JISF aims to cut emissions in the iron and steel industry, which is Japan’s largest CO 2 emitter, by 30% by 2030 compared to 2013 levels. Its stance on climate change seemed to have changed considerably since 2018, when it published a long-term decarbonisation vision that drew global emissions pathways reaching zero in 2100 to achieve the 2°C temperature goal (JISF, 2018). In 2021, CO 2 emissions from JISF members were 16% below 2013 levels. However the majority of this reduction can be attributed to “production fluctuations”, namely decrease in production, rather than the adoption of sector specific mitigation measures (JISF, 2023). Nippon steel, the largest steel-producing company in Japan and the fourth largest in the world, also released a decarbonisation road map in 2021. The company aims to develop and commercialise large electric arc furnaces by 2030 and expand the use of hydrogen in the sector (Argus Media, 2021; Nikkei, 2021). JFE Steel, Japan’s second largest steelmaker, has also announced plans to replace its blast furnace located in Okayama Prefecture with an electric arc furnace by 2027 (Nikkei, 2022c). However, the deployment of electric furnaces remain slow in Japan (Global Energy Monitor, 2023). Other key industry associations have also unveiled new decarbonisation strategies. In 2022, the Japan Cement Association announced that it will aim to cut emissions in the sector by 15% by 2030 compared to 2013 levels (METI, 2022c). The GX Basic Policy set roadmaps covering key sectors of the Japanese economy including the chemical, the iron and steel and the cement industries. These roadmaps introduced several targets, although many were already announced by industry associations in 2022 (METI, 2023d). One new target includes the increase of green steel supply to 10 million tonnes by 2030, although the exact definition of green steel remains unclear. It should however be noted that 10 million tonnes only represented around 1% of Japan annual steel production in 2021 (World Steel Association, 2022). Carbon pricing In December 2022, the Japanese government unveiled a blueprint for the introduction of a carbon pricing scheme, as part of the GX Basic Policy (METI, 2023e). This system will be based on two pillars: A carbon levy targeting power, gas, and oil companies, which will be introduced in 2028 and reviewed upward annually. An emissions trading scheme (ETS), which is being implemented in phases. The ETS was first launched in April 2023 but only among the GX league companies. The scheme was set up on a voluntary basis with GX League companies allowed to set their own emissions caps. Based on the results of this trial, the government aims to expand the scheme to cover more companies in 2026. The scope of the target companies and the exact features of the ETS remain to be determined (MoEJ, 2023). As for the final phase, the government plans to introduce the ETS “fully” in 2033, with a shift to a mandatory scheme that will include trading based on allowances auction. However, it will exclusively target the power sector (Nikkei, 2023), and no other sectors of the Japanese economy. The government plans to use the revenues generated by the carbon pricing scheme to issue more ”Japan Climate Transition Bonds”, the world’s first sovereign transition bonds, through which it hopes to raise JPY 20 tn (METI, 2023d). The first tranche of these bonds was auctioned in February 2024 (MoF, 2024). Details on the overall system have yet to be announced, but the carbon levy is expected to be set at around JPY 1,500 /t-CO 2 , which is seen as too low to be effective (Climate Integrate, 2023). Research shows that with a carbon price set at JPY 3,300/t-CO 2 , new solar PV energy and onshore wind power generation would outcompete coal-fired power generation (Carbon Tracker, 2022). This blueprint constitutes a step in the right direction, as discussions on carbon pricing in Japan have stalled for many years. However, it remains unclear whether the emissions trading scheme being considered for 2026 will still be based on voluntary participation (InfluenceMap, 2023). Additionally, the timeline and the carbon levy currently being considered by the government means the scheme will not help Japan meet its 2030 target. On top of that, the government is considering investing the revenues generated from the “GX Transition bonds” partly in the development of grey hydrogen and grey ammonia, rather than renewable energy (Renewable Energy Institute, 2023c).</t>
   </si>
   <si>
     <t>In 2022, emissions from the transport sector in Argentina represented 16% (~56 MtCO 2 e) of Argentina’s GHG emissions (excluding LULUCF) according to the Fifth BUR, and approximately 32% of energy demand (IEA, 2024b). Argentina has set out policies to reduce emissions in all key areas of the transport sector, but under current policies, emissions in the sector are still expected to rise towards 2030. Electric vehicles In its 2022 climate strategy, the government included several targets related to electric vehicles (EVs). These include: The installation of over 86,000 charging stations and 2,500 fast-charging stations Targets to increase the sales of light- and heavy-duty hybrid and EVs to 100.000 and 150.000 respectively by 2030 Target to replace 100% of public administration vehicles with EVs or hybrid vehicles by 2030 (around 146,000 vehicles) Incentivising the conversion of private vehicles to compressed natural gas (CNG) (Government of Argentina, 2022d). The uptake of EVs remains low in Argentina, but it is now picking up due to incentive policies such as tax breaks. In 2021, the Argentinian Association of Automobile Dealerships reported 5,871 new sales of low-emissions mobility light-duty passenger vehicles, of which 99% were hybrid cars and only 1% plug-in EVs (Bloomberg Linea, 2022). In 2022, sales increased by 33%, reaching 7,849 new sales, of which 97% were hybrid and 3% pure electric (Della Vecchia, 2023). In 2023, sales reached 9601 cars in total, of which 3.7% were pure electric (Inside EVs, 2024). Overall, the low-emissions mobility market remains marginal in Argentina, with total 2023 EV and hybrid sales being under 1% of all vehicle sales (La Nación, 2023). Public transport In its 2022 climate strategy, the government includes measures to support the development of rail infrastructure, including adding 83km of electric train tracks by 2026 (Government of Argentina, 2022d). Since 2008, the government has incentivised the use of public transport in large urban areas through the development of Bus Rapid Transit Systems (BRTS). As of 2020, 18 BRTS were in place, with a goal to reach 20 by 2030 (Government of Argentina, 2022c). Biofuels In its 2022 climate strategy, the government included biofuels targets: to increase bioethanol blending to 15% in 2025, and to meet 20% of total fuel demand with biofuels by 2030. The government also plans to support second generation biofuels and aims for 2 Mt of organic waste to be used for biofuels by 2028 (Government of Argentina, 2022d). This contrasts with its current mandates to reduce biodiesel blending from 10% to 5%, with the option of being further reduced to 3% if biofuel input prices increase so much that they significantly impact final fuel prices for consumers. A recent study has calculated that this reduction can lead to a cumulative increase emissions between 7.9-11.7 MtCO 2 e in the period 2021–2030 compared to the previous 10% mandate (Magnasco &amp; Caratori, 2021). However, a reduction in the production of first-gen biofuels can also have positive effects in land-related emissions, reducing the pressure to expand agricultural lands and demand for the commodities used as feedstock (Rulli et al., 2016). Vehicle efficiency standards and labels In March 2021, the government also introduced a new mandatory light-duty vehicle label to reflect fuel efficiency and emissions in all new vehicles under 3,500 kg.</t>
   </si>
   <si>
+    <t>Transport emissions represented 19% of Australia’s total emissions (excluding LULUCF) in 2023/24 (DCCEEW, 2024i). The sector is projected to become the greatest source of emissions in by 2030 as power sector emissions decline (DCCEEW, 2023b). The government introduced the long-awaited New Vehicle Efficiency Standard (NVES) in 2024, which will apply to new cars sold from 2025. Until this year, Australia was one of the last developed countries, along with Russia, to lack such standards. On average, new cars in Australia consume 40% more fuel than those in the EU and 20% more than in the US (DCCEEW, 2023c). Under the NVES, emissions intensity limits (g CO 2 /km) are imposed on suppliers across the fleet of new vehicles they sell each year, with higher limits allowed for heavier vehicles. There are no restrictions on which cars may be sold, but the sale of emissions intensive cars must be offset by the sale of more fuel-efficient cars or buying credits from other suppliers (DITRDCA, 2024). The emissions intensity targets are set to decline each year leading to a projected reduction in transport emissions by 4% between 2023 and 2030, and a further 15% between 2030 and 2035. During the legislation’s consultation period in early 2024, the government watered down the proposed standard, allowing some four-wheel drives to be counted as light commercial vehicles (LCVs) instead of passenger vehicles (PVs), with the former being subject to higher CO 2 limits. The government also raised the ‘headline target’ for LCVs, which effectively increases the average emissions intensity allowed for LCVs, and increased ‘breakpoints’ for both LCVs and PVs, which gives heavier vehicles greater emissions headroom. Combined, these changes will allow an additional 17 MtCO 2 e to be emitted cumulatively by 2035 — one sixth of the sector’s current annual emissions (DITRDCA, 2024). The National Electric Vehicle Strategy, published in 2023, outlines a roadmap to encourage EV adoption with a focus on cooperation between the government and states. However, it does not include quantified targets for EV adoption beyond state-level targets that now exist for all states and territories, with varying levels of ambition, except the Northern Territory and Tasmania (DCCEEW, 2023c; IEA, 2023a). The government has committed to building a National EV Charging Network, with charging stations on average every 150 kilometres along the country's major highways by 2026 (DCCEEW, 2024f). Australia’s EV uptake remains slow compared to other countries. EVs made up only 8.5% of new car sales in 2023, including battery electric vehicles (BEVs) and plug-in hybrid electric vehicles (PHEVs) (Electric Vehicle Council, 2024). Comparatively, the market share of EVs (BHEVs and PHEVs) reached 22% in the European Union, 38% in China, and 93% in Norway in 2023 (IEA, 2024a). The government projects that battery EV sales will reach 23% of new light duty vehicle sales by 2030, and 47% by 2035 (DCCEEW, 2023b). The anticipated slow electrification of Australia's vehicle fleet is a missed opportunity to leverage the power sector's transition for decarbonising transportation. The government’s current policies do little to address emissions from heavy-duty vehicles, such as trucks which account for more than a fifth of transport emissions (DCCEEW, 2023b), nor do they address the lack of planning for public transportation and modal shifting. Australia has also not set a phase out date for fossil fuel vehicles.</t>
+  </si>
+  <si>
+    <t>Transport makes up just over 50% of Brazil’s energy sector emissions, and emissions have been steadily increasing since 2018, mainly due to increased vehicle ownership (SEEG, 2023a). As part of its energy transition goals, Brazil launched the Fuels of the Future Programme which plans to increase the ethanol blend in gasoline from 22% to 27%, as well as the amount of biodiesel blended into diesel from 14% to 20% by 2030. The programme also looks at reducing aviation emissions by gradually increasing the mix of sustainable fuels and stipulates that airlines must reduce greenhouse gas emissions by 1% in 2027 and by 10% in 2037 (Silva, 2024; Talanoa, 2023). Brazil is currently one of the world’s largest producers and consumers of biofuels. If the bill is approved by the Senate later this year, this programme would boost the ethanol industry in the country. However, it's essential to ensure that biomass used in future energy systems is sustainably sourced. This means preventing upstream emissions from land-use changes, avoiding competition with food crops, protecting biodiversity, and respecting the rights of indigenous peoples in that land (Energy Transitions Commission, 2021). Furthermore, while biofuels may have reduced the emissions intensity of the road transport sector in Brazil, the potential for further reductions in emissions by biofuel blending is limited (ICCT, 2023). Instead, full decarbonisation of the transport sector will require fast uptake of electric vehicles (EVs). Brazil has not set a specific target for electric vehicles and has not joined the COP27’s Accelerating to Zero coalition (A2Z) , which states that 100% of new car and van sales in 2040 should be electric vehicles, 2035 for leading markets. According to the third yearbook on electric mobility, the sale of EVs has grown significantly in recent years. According to the latest estimates, around 2.5% of light-duty vehicles sold in 2022 were electric. The number of EVs sold in 2023 almost doubled compared to the previous year, a positive development that surpassed all projections (Audi, 2024; PNME, 2023). However, despite these positive development, there is still a long way to go. For comparison, the 1.5°C compatible share of EV sales in Brazil would need to be above 45% by 2030 (see figure below). Increasing electrification of the transport sector would also reduce Brazil’s dependency on biofuels, particularly those produced from soy, thereby reducing pressure on Brazilian land for soy farming (PNME, 2023). EV market share</t>
+  </si>
+  <si>
+    <t>Transport is the second largest source of emissions in Canada, after oil and gas, representing just under a quarter of the country’s emissions (Environment and Climate Change Canada, 2024). In its latest projections and progress reports, Canada foresees transport emissions reductions of 19% below 2005 levels by 2030 (Environment and Climate Change Canada, 2023b, 2023a). Canada is taking steps to reduce transport emissions, but not at the speed needed for such a large source of the country’s emissions. A 2022 ‘action plan’ on road transport did little more than rehash existing targets, plans and funding schemes (Transport Canada, 2022a). Electric Vehicles Targets Canada has had EV sales targets for the past several years. By 2035, 100% of new passenger car and light-duty trucks sales need to be electric vehicles, with interim targets of 20% by 2026 and 60% by 2030 (Environment and Climate Change Canada, 2022a). In December 2023, the government adopted the necessary regulations to make these targets legally binding (Government of Canada, 2023g). Plug-in hybrids (PHEVs) are included in the definition of electric vehicles but their contribution to the sales target is capped at 20% from 2028. The sales targets increase in stringency annually, though at a slower pace in earlier years. The GHG impact of the regulations grows over time, but only contributes to minor reductions by 2030 (less than 5 MtCO 2 e). In 2023, ~19% of all passenger car and truck sales were EVs, of which 8% were battery electric (Statistics Canada, 2024). Canada should easily achieve its (fairly low) 2026 interim target of 20%. The CAT has not developed EV benchmarks for Canada; however, our US benchmark suggests that Canada’s targets are not 1.5°C compatible: 95–100% of all US passenger cars and light-duty trucks sold in 2030 should be zero emission vehicles. The government aims to electrify its own light-duty vehicles LDV fleet by 2030 (Natural Resources Canada, 2022a). Medium and heavy-duty vehicles Canada has also set targets for its medium and heavy-duty vehicles (MHDVs) with the goal of achieving a 35% sales target by 2030 and 100% by 2040 for some models (Environment and Climate Change Canada, 2022a). Stakeholder consultation on the regulations to make these targets binding has begun, but the timeline for their adoption is not clear (Government of Canada, 2022g, 2023a). Infrastructure and support programmes The government began supporting the development of EV-related infrastructure and charging networks in 2016 (Natural Resources Canada, 2021b, 2021c, 2023). Canada has about 26,000 chargers at 10,000 locations across the country (Natural Resources Canada, 2024). Analysis suggests that Canada will need between 440,000-470,000 chargers in 2035 to support its 100% sales target (Dunsky Energy + Climate Advisors, 2022). The government missed an opportunity to support residential charging infrastructure by not including them in the most recent building codes, though some municipalities are taking action (Kozelj, 2024). Making buildings EV-charger-ready through minor changes at the time of construction can significantly reduce the costs when the necessary equipment is actually installed (Efficiency Canada &amp; Carleton University, 2022). Since 2019, the federal government has provided rebates for the purchase or lease of EVs and will continue to do so until March 2025 (Environment and Climate Change Canada, 2020a; Transport Canada, 2022b). In July 2022, it launched a four-year, half billion CAD programme to support the purchase of medium and heavy duty electric vehicles (Transport Canada, 2022c). Vehicle emission standards Canadian fuel economy standards for light and heavy-duty vehicles are aligned with federal-level regulations in the US (Environment and Climate Change Canada, 2020a; Government of Canada, 2021h, 2018c). The Biden administration has been working on reversing the Trump era rollbacks, adopting new rules for emissions and fuel standards (see US assessment for details). GHG standards for new trailers have been delayed for several years in response to legal challenges to those standards in the US. Fuel standards In July 2023, the Clean Fuel Regulations finally took effect, though are unlikely to have much of an impact until 2025 (Bakx, 2023; Government of Canada, 2022p). The regulations require producers and importers of gasoline and diesel to reduce the carbon intensity of their fuels from 2016 levels, with increasing annual reductions through to 2030. The regulations create a credit market for compliance, which allows those not subject to the regulations (like EV charging stations or low carbon fuel producers (e.g. biofuels)) to participate. The regulations aim to improve production processes in the oil and gas sector, foster production of low carbon fuels and enable end-use fuel switching in transport. The fuels used by remote communities, and in international shipping , and domestic and international aviation are exempt from the regulation. The renewable fuel content requirements, 2% for diesel and 5% for gasoline, as set out in the Renewable Fuels Regulations, have been incorporated in these new regulations (Government of Canada, 2010). These regulations were first proposed in 2016 as part of the Pan-Canadian Framework (Government of Canada, 2016a). Originally, standards were also supposed to be prepared for gaseous and solid fuels; however, these were delayed due to industry concerns over trade impacts and have since been shelved (Environment and Climate Change Canada, 2020a; Government of Canada, 2017). Aviation Canada lacks effective policies to address its aviation emissions, which stand at 22 MtCO 2 e in 2019. Most of these emissions are not covered by its carbon pricing system, as this pertains to interprovincial travel only, and its clean fuel regulations (see above) do not extend to jet fuel. 70% of Canada’s aviation emissions are from international flights (Government of Canada, 2022b). In 2022, Canada updated its aviation action plan (Government of Canada, 2022b). As part of the plan, the government commits to exploring ways to consistently apply carbon pricing to domestic aviation emissions. The plan charts a pathway to achieving net-zero emissions by 2050, in which a shift to Sustainable Aviation Fuel (SAF) is responsible for close to half of the needed reductions. In combination with increased efficiency in equipment and operations, this would offset the expected growth in air travel and bring emissions back to their 2005 levels (around 12 MtCO 2 e). These residual emissions would then need to be balanced by negative emissions, such as direct air capture. Around 70% of fuel used in 2050 would be SAF with a 90% reduction in lifecycle emissions compared to conventional jet fuel. Lower lifecycle emissions would increase the need for negative emissions outside the sector. Canada does not produce commercially relevant amounts of SAF currently. In 2023, the airline industry produced a SAF roadmap which is considered an integral part of the government’s aviation action plan. The roadmap charts the requirements for this nascent technology to be able to grow to 25% fuel share by 2035. The roadmap assumes around 50% lifecycle emissions savings in SAF in contrast to the 90% reduction in the aviation plan. Notably, the aviation plan’s four emission reduction measures are all targeting emission reductions per flight, rather than reducing the number of flights by making other transport modes more attractive. The plan only mentions a new highspeed rail network to connect the airports, rather than incentives to shift travel to rail connections to central stations in the major cities (Government of Canada, 2022b).</t>
+  </si>
+  <si>
+    <t>The transport sector accounted for a third of Chile’s total final energy consumption (34%) in 2021, almost the same as the industry sector, as well as a third (33%) of its total GHG emissions, considering 99% of the sector’s energy consumption is from imported fossil fuels (IEA, 2023). As with other sectors, Chile has established a number of targets to minimise emissions from the transport sector in its energy strategy (PEN). The most prominent target is that 100% of new light- and medium-duty vehicles sales must be zero emissions vehicles by 2035. In line with this target, at COP26 Chile signed the declaration on accelerating the transition to 100% EVs. However, Chile is not on progress to meet this target: its EV sales have yet to exceed 1% as of 2024. For Chile to achieve its transport electrification ambitions, it needs additional policies to support EV uptake. In December 2017, Chile published its Electromobility Strategy, which sets out a goal and action plan towards achieving a 40% share of electric passenger vehicles as well as a 100% electrified public transport fleet by 2050 (Ministerio de Energía, 2017a). Chile’s Energy Strategy (PEN, or Política Energética Nacional ), published in 2022, updated these targets and made them more ambitious, aiming for 100% zero emission vehicles in public transport and urban public transport by 2040, and 60% of private and commercial vehicles to be zero emissions by 2050 (Ministerio de Energía, 2022c). Other transport goals include a 40% reduction in direct GHG emissions from the use of fuels in the sector (including land, sea, and air transport) by 2050 compared to 2018 (20% by 2040). Chile’s Energy Route 2018–2022 set out a short-term goal of a 10-fold increase in EVs in 2022 (compared to 2017 levels). While this was overachieved by more than double, the target was relative to a very low initial EV stock in 2017 at only 231 cars (Ministerio de Energía, 2021e; IEA, 2024b). Chile is already beginning to implement actions towards achieving these targets. As of April 2024, Chile has reportedly reached over 2,500 electric buses in its public transport system, representing 38% of its total fleet (Carrara, 2024). Electric buses now represent around one-fifth of total bus sales in the country (IEA, 2024c). At the same time, the market share of EVs remains low, and decreased in past year from 0.5% to 0.3% of vehicles sold in 2023, and EVs make up only 0.1% of the total car fleet. EV sales have more than doubled, however, compared to 2019 and increased five-fold in the past six years, indicating a rapid upward trend. Public charging infrastructure is rather limited, with only 1,070 units (up from 660 in 2022) units in 2023 (compared to e.g., 51,000 in Germany) (IEA, 2024b). In addition to promoting renewables in the energy matrix, the Law on Energy Storage and Electromobility (21.505) includes measures to encourage EV uptake. The law includes temporary exemptions or reductions for driving permit fees for electric and hybrid vehicles, thus matching those of ICE vehicles, and enables battery EVs to connect to the grid and store energy (Ministerio de Energía, 2022b). Building on the Electromobility Strategy, in 2023, Chile presented its Roadmap for the Advancement of Electromobility. This plan contains concrete measures to 2026 aimed at accelerating the EV transition and addressing Chile’s current EV infrastructure gap. Its main pillars are building a robust public infrastructure charging network, promoting public transportation and decentralisation in priority regions, and improving EV education and road safety (Gobierno de Chile, 2023b). The Energy Efficiency Law also targets the transport sector. It establishes energy efficiency standards for imported vehicles, which came into effect this year, and government subsidies are offered for electric taxis and home charging points. It aims to ensure interoperability of the EV charging system, facilitates access and connection to the charging network, and allows the Ministry of Transport to establish energy efficiency standards for vehicles (Ministerio de Energía, 2021c). Building on its Green Hydrogen Strategy, the government has also presented its Sustainable Aviation Fuels 2050 Roadmap (SAF 2050). The roadmap sets out a goal of achieving 50% of SAF use in aviation by 2050 by promoting local, decentralised production of new energy sources. including biofuels and green hydrogen (Ministerio de Energía, 2024). Chile’s electromobility targets, initial implemented measures, and the 2035 ban of non-EV sales are a great step in the right direction, especially since they are integrated into new strategies and laws such as the Energy Efficiency Law and Green Hydrogen Strategy. However, additional policies, especially targeting private car ownership, are needed to meet both these targets and global decarbonisation benchmarks, which foresee having only zero emission cars on the road by 2050 to be compatible with limiting temperature to 1.5°C (Climate Action Tracker, 2016). For the development of an integral policy making framework for transport, it is of great importance to consider social and economic consequences of the different policy options. The total emissions reduction potential of transport electrification also significantly depends on the decarbonisation of the electricity supply used to charge vehicles.</t>
+  </si>
+  <si>
+    <t>China is rapidly becoming an EV, BEV and PHEV powerhouse, producing 52% of global sales, with its BYD company now overtaking Tesla as the world's best-selling company. China’s transport sector is a vast consumer of energy with the sector accounting for 14% of final energy consumption and 43% of oil consumption nationally, with petrol cars the largest consumer and source of emissions (IEA, 2023b). The government has signalled its continuing intent to accelerate the transition towards a low-carbon fleet, with sector action critical to meeting economy-wide targets of a 30% share of electricity in final energy consumption in 2025 and peak oil consumption during the 15th FYP period (2026 to 2030) (Government of China, 2021; NDRC and NEA, 2022). China’s uptake of new energy vehicles (NEVs), including battery electric vehicles (BEVs), plug-in hybrid vehicles (PHEVs), and fuel cell electric vehicles (FCEVs), started in the 1990s. The growth in NEV sales has been rapidly increasing due to subsidies dating back to 2009 and, more recently, investment boosts from pandemic recovery packages and strong national policy signals. In 2023, China's NEV production and sales grew by 35.8% and 37.9% year-on-year (Xinhua News Agency, 2024). However, the government has been aiming to decouple the growth of NEVs with direct financial incentives due to accelerating market forces and the growing government costs of the subsidies. NEV subsidies for producers ended in 2022, although tax exemptions for consumers will continue until the end of 2027 (Xinhuanet, 2023). Research suggests the market is reaching maturity, with BEVs achieving price parity with conventional cars soon, even without accounting for fuel savings (Lutsey et al. , 2021). The NEV Industry Development Plan (2021-2035) targeted NEV sales to take 20% of the market share by 2025, but the market share of NEVs has already reached 31.6% in 2023, significantly exceeding the target (Xinhua News Agency, 2024). China further targets an NEV market share target of 40% by 2030 (raised to 50% in select regions with high air pollution) (Government of China, 2021). However, this still falls short of a 1.5°C-compatible transport sector, which requires China to achieve a 100% EV sales share and a 42% EV stock share by 2030. The penetration of NEVs is finally showing a visible reduction in pollutants and emissions, as the transition towards NEVs has shaved approximately 3% off petrol demand growth, and according to Sinopec, would cause China’s petrol demand to peak in 2023 (Myllyvirta and Qin, 2023). Our previous analysis of NEV penetration scenarios in China shows limited domestic mitigation impact as even 100% BEV sales by 2035 would mean negligible GHG emission reductions if not accompanied by rapid decarbonisation of the power sector (Climate Action Tracker, 2021). Even so, China’s rapid development of industrial infrastructure supporting its EV supply chain is critical to global electric mobility transitions: in 2023, Chinese carmakers produced 32% of global EVs, with BYD overtaking Tesla as the world’s best-selling company when accounting for PHEVs as well as BEVs (IEA, 2024) To limit global temperature increase to 1.5°C, China will need to sell the last fossil fuel car by 2040 meaning a NEV market share of 100% (Climate Action Tracker, 2020a). Projections (from 2021) show China only reaching 70% by then, although this is the most rapid trajectory of any of the world’s largest emitters. The government has also been prioritising service and electrification of its public transport systems with the expansion of national high-speed rail and local electric public transport systems highly prominent in its COVID economic stimulus packages and latest FYPs. The 14th FYP for Green Transportation Development contains numerical targets to increase the growth of NEVs in urban public transport (including taxis, buses, delivery trucks, and more), while the government recently launched a pilot programme for cities to procure 80% of new public vehicles as electric from 2023-2035 (around two million vehicles) (MoT of China, 2021; Xue, 2023). Shenzhen, a city home to two pilot programmes for NEVs since 2009, became the first city in the world with an entirely electric public transport system in 2017 (including 16,000 buses and 20,000 taxis) (CGTN, 2023). For intercity transport, the government has looked to expand its massive high-speed rail network. The network consisted of about 38,000 km in 2020 (all built since 2008) and is planning to extend this by another 120,000 km by 2035 (Jones, 2022; O. Wang, 2022). By 2025, the government aims to have the network cover more than 95% of cities with a population greater than half a million (State Council of China, 2022).</t>
+  </si>
+  <si>
+    <t>The transport sector is the largest source of emissions in the UK, representing 29% of emissions in 2023 (DESNZ, 2024b). Central to decarbonising transport is ending the sale of fossil fuel cars and vans by 2030 and fossil fuelled heavy goods vehicles (HGVs) by 2035–40 (Department for Transport, 2021). The policy context that the new UK government has inherited is mixed. On the one hand, the previous government confirmed the zero emissions vehicle (ZEV) mandate in 2023, which sets minimum EV sales targets for each vehicle manufacturer and will be a key delivery mechanism in scaling up EV sales (UK Government, 2023b). At the same time, the government pushed back the date of the sales ban on internal combustion engine cars from 2030 to 2035, sending a very mixed signal to the public and automotive industry. In 2023, the share of electric car sales in the UK failed to grow, flatlining at 16.5% and falling off track for the UK’s transition for the first time (SMMT, 2024). The share of electric van sales is growing much more slowly and is significantly off-track (CCC, 2024). Key actions for the new government should include: Reinstating the 2030 ban on petrol and diesel vehicle sales Taking action to help accelerate EV rollout . This should include removing barriers for the installation of EV chargers and working with major van fleet operators to understand barriers to EV uptake. Aviation In 2022, the UK released its Jet Zero Strategy which aims to reduce emissions from this sector to net zero (Department for Transport, 2022). This aims for domestic aviation to reach net zero emissions by 2040, and total aviation emissions to reach net zero by 2050. However, in this context, net zero does not mean eliminating the negative climate impacts of aviation, but rather allowing for a large-scale growth in emissions that would be compensated for via the UK emissions trading scheme, CORSIA and other offsetting mechanisms outside the aviation sector. The strategy also ignores the non-CO 2 impact of aviation, which represents up to two-thirds of the sector’s overall climate impact (Lee et al., 2021). The UK’s current strategy relies heavily on speculative technological innovation and carbon dioxide removal to enable a ‘net zero’ aviation sector, without addressing the elephant in the room – demand. The previous government committed that sustainable aviation fuel (SAF) would provide 10% of overall fuel use by 2030, rising to 22% by 2040 (UK Department for Transport, 2024). This is five times the level included in the CCC’s Balanced Net Zero Pathway and would require an unprecedented scale-up of SAF production. The new government confirmed this commitment, and introduced a SAF mandate to drive this uptake (Department for Transport, 2024). There will also be a revenue certainty mechanism to provide confidence to investors seeking to build SAF plants to meet UK demand. However, SAF deployment remains very low globally and has consistently failed to meet expectations (Rutherford, 2022). Relying so heavily on this option therefore represents a major delivery risk. The Jet Zero strategy also fails to address demand. The Government states that “the sector can achieve Jet Zero without the government needing to intervene directly to limit aviation growth” (Department for Transport, 2022), and envisages that passenger numbers could rise 70% from 2021 to 2050. This is in contrast to the CCC’s advice, which was that no net expansion in airport capacity should be permitted, and passenger growth should be 25% at most (CCC, 2020). Numerous airports are currently planning expansions or have received approval to expand in the past two years (AEF, 2022) which again could threaten the UK’s ability to achieve its climate targets. As yet, the new government has not provided any clear commitments that it will curb aviation demand, with the chancellor repeatedly mentioning aviation as a key engine of economic growth (Topham, 2024). As a result, in 2050, the Jet Zero strategy expects that aviation will still be emitting around 19 MtCO 2 per year, which will need to be compensated for by CO 2 removal. Given the very limited potential for CO 2 removal and uncertainties in the climate system, CO 2 removal should be reserved to hedge against climate uncertainties and balance out truly hard-to-abate residual emissions (e.g. from agriculture), rather than to facilitate a stark increase in aviation emissions in one of the world’s wealthiest countries. For more information on the need to align aviation and shipping emissions with the Paris Agreement, see the sectoral pages on international aviation and international shipping .</t>
+  </si>
+  <si>
+    <t>The transport sector accounted for 29% of total final energy consumption in 2022 (IEA, 2024). The sector is primarily individual, road-based transport but the Kingdom has sought to expand its public transportation network in recent years. The King Abdulaziz Public Transport project is a major initiative to modernise transportation in the city of Riyadh. The capital is set to become the second city in Saudi Arabia with a metro network after the Makkah metro opened in 2010 (Saudi Gazette, 2020). Following a delay, the Riyadh metro system is set to open to passengers at the end of 2024 (Railway Technology, 2023; The M Metro Rail Guy, 2024). The Saudi government has also taken steps to invest in rail transport; however, it remains unclear whether the new networks will be electric or diesel-powered. In 2010, it launched the Saudi Railway Master Plan, aiming to construct a 9,900-km network by 2040 (Oxford Business Group, 2020). The first phase, running until 2025, includes constructing and upgrading 5,500 km of tracks for freight and passenger transport, including interlinkages to the wider Gulf Cooperation Council (GCC) railway network. The light rail network in the smart city NEOM is complete as of 2024 (Godfrey, 2024). Electric vehicles Saudi Arabia has taken steps to develop its own electric vehicle (EV) industry. As part of its “Vision 2030” strategy, the government aims to produce 50,000 EVs annually by 2030 and for 30% of Riyadh’s vehicles to be electric by 2030 (Kingdom of Saudi Arabia, 2021c). In 2022, Saudi Arabia introduced its first domestic brand of EV called Ceer, through a joint venture between PIF and Taiwanese car manufacturer Foxxconn (Al Arabiya News, 2023a). Manufacturing facilities for Ceer vehicles are under construction and expected to be operational by 2025 (Al Jazeera, 2023). Additionally, in June 2023, Saudi Arabia signed a USD 6 bn deal with Chinese EV manufacturer Human Horizons to collaborate on the development, manufacture, and sale of electric vehicles (Reuters, 2023). To further promote the use of EVs, by 2024 the government had built 2,800 EV charging points,, with plans to set up 30,000 new stations by 2030 (Mobility Foresights, 2024). Despite the progress made, achieving Saudi Arabia’s 2030 EV target will be challenging. The government will need to accelerate the deployment of charging infrastructure and introduce incentives to promote greater EV adoption (Apricum, 2022).</t>
+  </si>
+  <si>
+    <t>Singapore’s transport sector made up 14.2% of total emissions in 2021 (National Climate Change Secretariat, 2024b). Singapore aims to develop a greener and more sustainable land transport sector, reducing peak land transport emissions by 80%, by or around mid-century. The sector’s energy demand and associated emissions are expected to flatten out as a result of measures to promote public transport, modal shifts, and improve the emissions intensity of road transport. The government estimates that implemented measures reduced emissions by 1.67 MtCO 2 e in 2020 (National Environment Agency, 2022). Singapore aims to phase out Internal Combustion Engine (ICE) vehicles by 2040 (National Environment Agency, 2022). However, to be compatible with the 1.5°C long-term temperature goal, the last fossil fuel car should be sold in 2035 at the latest (Climate Action Tracker, 2016). The Vehicle Emissions Scheme (VES) was introduced in 2018, replacing the Carbon Emissions-based Vehicle Scheme (CEVS), which provided rebates for low-emission cars and imposed surcharges on high-emission cars. The VES expanded the range of pollutants covered to include hydrocarbons (HC), carbon monoxide (CO), nitrogen oxides (NO X ), and particulate matter (PM) (National Environment Agency, 2022). Fuel economy labels have been redesigned to include information on each vehicle’s VES band. To further promote the adoption of cleaner vehicles, the VES was enhanced with increased rebates and higher surcharges from January 2021. Starting from 2021 all new and used petrol or diesel vehicles must comply with the Euro VI emission standards (National Environment Agency, 2022). The Singapore Green Plan 2030 includes a strong push to electrify the vehicle fleet, which would help Singapore achieve its vision of 100% cleaner energy vehicles by 2040 (Land Transport Authority, 2021). Singapore has introduced tax incentives to lower the upfront and running costs of electric vehicles (EVs) such as the Electric Vehicle Early Adoption Incentive (EEAI) (National Environment Agency, 2022). As of 2023, less than 2% of the vehicle population were fully electric or plug-in hybrid electric vehicles (PHEVs) (Land Transport Authority, 2023). Under the new VES standards, CO 2 emissions produced by electricity generation from fossil fuels are accounted for by applying an emissions factor to the electricity consumption of EVs and PHEVs (National Climate Change Secretariat, 2018b). Since February 2018, the growth of private vehicles has been effectively capped, when the permissible growth rate of private vehicle population was reduced from 0.25% to 0% (National Environment Agency, 2018). Prospective vehicle owners must bid and pay for a Certificate of Entitlement which allows them to purchase a vehicle and use it for 10 years (National Environment Agency, 2022). Singapore is encouraging active transport and modal shift in its Land Transport Master Plan (LTMP) 2040 by developing infrastructure, creating more urban space for walking and cycling, and expanding the MRT system (Singapore’s metro). The Land Transport Authority (LTA) announced SGD 1bn in funding over the next decade to support Walk, Cycle, Ride journeys. By 2030, it aims to extend the country’s cycling path network to more than 1000 km, compared to 460 km in 2020 (National Environment Agency, 2022). As of 2019, there were cycling networks in nine out of 24 public housing towns and 200 km of sheltered walkways(National Environment Agency, 2018). Singapore plans to increase the length of the rail network from 245 km in 2022 to about 360 km in the early 2030s so that eight in ten households will be within a ten-minute walk of a train station. Singapore is targeting a mass public transport modal share of 75% during the morning and evening peak hours by 2030 (National Environment Agency, 2022). The Land Transport Master Plan sets a goal for all public buses and taxis to run on cleaner energy sources by 2040 (Republic of Singapore, 2019), and the Land Transport Authority (LTA) aims to have half of its public bus fleet be electric by 2030 (Land Transport Guru, 2022). In 2016, Singapore trialled e-buses, and by 2018, 60 trial e-buses were on the roads (Republic of Singapore, 2019). Around 700 electric taxis have been rolled out by the private taxi operators (The Straits Times, 2021, 2022b). We exclude emissions from marine and aviation bunkers when assessing Singapore’s NDC target and current policies. These emissions are more than three times higher than the rest of Singapore's emissions—with the vast majority being related to Singapore’s role as a hub in international shipping (National Environment Agency, 2022).</t>
+  </si>
+  <si>
+    <t>The Department of Transport published the country’s first Green Transport Strategy (GTS) 2018–2050 in 2018 (Department of Transport South Africa, 2018), proposing a list of measures that should be implemented to transition the sector to a low carbon future. Analysis by the Climate Action Tracker indicates that the share of zero emissions fuels (biofuels, electricity and hydrogen) of the total domestic transport sector demand would need to increase to 20% by 2030, 50-60% by 2040, and 80%-90% by 2050 to be compatible with the Paris Agreement. South Africa’s automotive industry contributed to over 4% of GDP in 2021 and is one of the country’s largest manufacturing sectors (NAAMSA, 2023). In 2013, the government adopted South Africa’s Electric Vehicle Industry Roadmap to introduce electric passenger vehicles (EVs) (South African Government, 2013). Three years after the adoption of the roadmap, the first EV was manufactured in South Africa with the production of plug-in hybrids (PHEVs) at Mercedes-Benz’s East London plant (Venter, 2023). Since then, Toyota has also begun manufacturing PHEVs with Ford also announcing it will manufacture PHEVs in South Africa (Agbetiloye, 2023; Venter, 2021). While some progress has been made, the industry is still dominated by fossil fuel-vehicles. This creates an existential challenge for the auto industry as South Africa’s main export destinations, such as the UK and EU, shift towards EVs (NAAMSA, 2023). On the demand-side, the total number of EVs vehicles sold in South Africa remains marginal.. In the first four months of 2023, the sale of battery EVs doubled compared to the previous year, though remained just 0.16% of new vehicle sales (Kuhudzai, 2023a). In the same time period, the sale of plug-in hybrids declined over 20%, though these make up a smaller share than battery EVs. In May 2021, the Government of South Africa released the ‘Auto Green Paper’ for public consultation (Department of Trade Industry &amp; Competition, 2021). The strategy aims to define South Africa’s framework for a comprehensive and long-term automotive industry transformation plan on low-carbon vehicles. No final policy proposal had been approved by Cabinet, as of September 2023. Analysis by the Climate Action Tracker shows that the electric vehicle share in annual vehicle sales in South Africa would need to increase to 50-95% by 2030 and 90-100% by 2040 to be compatible with the Paris Agreement. Bus Rapid Transit Systems (BRT) have initiated the main switch in modal share of passenger transport in urban areas. These have commenced operation or are currently under consideration in public transportation planning in several South African urban areas (Department of Transport, 2017). Initiatives to implement and expand BRT systems are currently taking place in eight cities and municipalities including Cape Town and Johannesburg. However, BRT still faces challenges such as competition with minibus taxis and overreliance on foreign service plans less suitable for South African cities (Hook &amp; Weinstock, 2021).</t>
+  </si>
+  <si>
+    <t>Emissions from the transport sector were responsible for 33% of Switzerland’s total GHG emissions in 2022, almost exclusively from road transport (Bundesamt für Umwelt BAFU, 2024b). Since peaking in 2008, transport emissions have steadily been decreasing and in 2020 they fell below 1990 levels for the first time since 1996, primarily due to lower car travel during the COVID-19 pandemic. Emissions only slightly rebounded in 2021 and even slightly decreased again in 2022, remaining at 7% below 1990 levels. With the adoption of the Climate Protection Act in 2023, Switzerland now has reduction targets for the transport sector to reduce emissions by 57% by 2040 and by 100% by 2050 (below 1990 levels) (Bundesgesetz Über Die Ziele Im Klimaschutz, Die Innovation Und Die Stärkung Der Energiesicherheit (KlG), 2023). Given the very low emissions intensity of Switzerland’s power sector, a shift to electric mobility has an even higher impact on overall emission reductions. In 2023, 30% of all new passenger cars sold in Switzerland were electrically chargeable vehicles, which includes battery-only (21%) and plug-in hybrid (9%) vehicles (European Alternative Fuels Observatory, 2024a). Although the uptake of electric vehicles is accelerating, the share of new sales in Switzerland remains significantly below that of some countries with a comparable level of income (e.g. 60% in Sweden, 55% in Finland, 90% in Norway in 2023), but it is moving faster than the EU27 average, which in 2023 was 23% (European Alternative Fuels Observatory, 2024b). The target of 15% battery electric vehicle sales in 2022, outlined in the Roadmap for Electric Mobility 2022, was met a year early leading to the creation a new Roadmap for Electric Mobility 2025, with 2025 targets of EV market sales shares of 50% and of 20,000 charging stations. Although the EV uptake is expected to take an exponential trajectory to achieve 50%, sales need to more than double within two years (Schweizerische Eidgenossenschaft, 2023)(Bundesamt für Strassen ASTRA, 2023). While still predominantly on road, the share of freight transported by rail – which is electrified to 99.8% in Switzerland – is slowly growing again and reached 38% in 2022. This is higher than even the EU target for 2030, which is 30% and the current EU average was 18% in 2021 (Bundesamt für Strassen BFS, 2023). The inclusion of domestic and international aviation between Switzerland and member states of the European Economic Area (EEA) into Switzerland’s ETS since 1 January 2020 is a significant policy development, with emissions from the sector in the scheme to be capped at 2018 levels (Schweizerische Eidgenossenschaft, 2020c). In addition, from 2020 for new designs, and from 2023 for in-production models, aircraft in Switzerland will be subject to CO 2 emission reduction targets. Switzerland also participates in the carbon offsetting and reduction scheme for international civil aviation (CORSIA), under which emissions are capped at 2019 levels. Despite becoming more stringent in 2024, this scheme has significant shortcomings, meaning it is unlikely to deliver the substantial reductions needed to achieve the ICAO’s aspirational goal of carbon neutral growth from 2020. Within the framework of the new CO 2 Succession Act, the introduction of a sustainable aviation fuel blending mandate is planned, in coordination with the EU’s ReFuel programme from 2025 and it also includes instruments to support the conversion of diesel-powered buses and ships to fossil free alternatives. The CO 2 Succession Act further introduces quantitative emissions reduction targets for the period after 2025 aligned with those of the EU. It also introduces a new penalty for exceedance of emissions limits at CHF 95 to CHF 152 (USD 119 to USD 176) for each gram of CO 2 /km exceeding the individual target (Bundesgesetz Über Die Reduktion Der CO 2 -Emissionen (CO 2 -Gesetz), 2024).</t>
+  </si>
+  <si>
+    <t>Transport emissions account for around 16% of Türkiye’s GHG emissions (excl. LULUCF), or 91 MtCO 2 e (Republic of Türkiye Ministry of Energy and Natural Resources, 2023). The largest share of emissions comes from road transportation, which more than tripled between 1990 and 2021 (Republic of Türkiye Ministry of Energy and Natural Resources, 2023). In line with increasing road transport emissions, the number of vehicles on Turkish roads has almost tripled since 1990 (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024a). Nevertheless, there are 161 motor vehicles per 1000 inhabitants in Türkiye, which is far less than in developed countries (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024a). In the EU, for instance, this figure is 560 per 1000 inhabitants (Eurostat, 2024). Turkish transport policy is therefore at a crossroads. As the economy continues to grow, so too will vehicle ownership. Putting in place incentives and infrastructure designed to increase electric vehicle (EV) uptake will allow Türkiye to expand vehicle ownership sustainably. Türkiye aims to place EVs at the heart of industrial policy through the manufacturing of its first domestically produced EV, the Togg (Republic of Türkiye Ministry of Industry and Technology, 2022). Türkiye adopted the COP26 declaration on accelerating the transition to 100% zero emission cars and vans, but has not introduced policy at national level with a firm commitment to expanding the market share of zero emission vehicles to 100% by 2040. However, Türkiye does aim to increase the market share of EVs to 35% by 2030 (Republic of Türkiye Ministry of Industry and Technology, 2022). Its domestic EV production gives it an advantage in terms of meeting the goals of the COP26 declaration, and Togg sales have already driven a substantial increase in EV sales in Türkiye (Kasapovic &amp; Knowles, 2024). A stronger target in line with its COP26 commitment can allow Türkiye to achieve 100% zero emission sales by 2040. Rolling out EV infrastructure is critical to supporting their uptake. The government aims to establish a fast-charging network by providing grant support to private sector actors (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2023), as well as supporting drivers’ access to public charging stations at a regulated price (Kaya, 2022). However, EV infrastructure is not being rolled out fast enough. There are 12.5 EVs per charging point. In contrast, there are 3-to-1 in the Netherlands and Belgium, and 5-to-6 in Italy (Hürriyet Daily News, 2024). A modal shift towards rail will form an important aspect of reducing emissions in line with 1.5°C. Türkiye aims to increase the share of freight transport by rail to 20.12% by 2035 and the share of passenger transport by rail to 5.31% by 2035, up from 2019 levels of 0.89% and 3.13%, respectively (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2023). Ongoing measures to achieve this include significant investments in modernising its rolling stock and constructing new lines between major cities (Railway Gazette International, 2024; Railway Supply, 2024). Türkiye also aims to become producer of high-speed electric trains which it can use domestically as well as export. Similar to the Togg, Türkiye sees domestic manufacturing of electric trains as a way to blend industrial policy with environmental goals.</t>
+  </si>
+  <si>
+    <t>The transport sector accounted for ~19% of the UAE’s emissions in 2019. The UAE’s 2023 NDC update sets a target to reduce transport emissions by 1% below 2019 levels by 2030. Emissions from the transport sector are expected to be ~42 MtCO 2 e in 2030 under this target, and to reach zero emissions by 2050 (Government of the UAE, 2023a). The UAE has set out some policies to manage transport emissions, including an increase in the fuel and emissions efficiency of its vehicle fleet, as well incentives for the use of public transport, and the uptake of EVs. The revised Energy Strategy 2050 includes new targets for the uptake of EVs, including reaching 691,100 EVs and hybrid vehicles by 2030 and over three million by 2050 as well as increasing the number of EV chargers to 879 by 2030 and 30k by 2050. The emirates of Abu Dhabi and Dubai have also set out a series of urban transport policies, aimed among others at incentivising the uptake of public transport and EVs (Government of the UAE, 2021). For example, in May 2022 the Abu Dhabi government set out a new EV charging station policy, defining standards and requirements in anticipation of growing demand for EVs. In Dubai, the Green Mobility Strategy 2030 includes a target to reach 30% EVs and hybrids in the government vehicle fleet by 2030 (Government of the UAE, 2022). In its LTS, the UAE lists additional policies it proposes to reach its target for the transport sector towards 2050. The key pillars of the UAE’s transport decarbonisation plan are to reduce transportation needs, decarbonise passenger transport, freight transport, and mechanical vehicles (Government of the UAE, 2024b). The first pillar will include the development of mixed-use buildings, improved infrastructure for cycling and walking, incentives for carpooling and increased use of public transport and rail. In total this will contribute 14% of the reductions needed to achieve the UAE’s target. The second pillar includes incentives for the uptake of EVs, the electrification of buses, taxis and motorcycles. In total this will contribute 22% of the emission reductions needed. The decarbonisation of freight transport includes a shift towards more rail use as well as the electrification of heavy-duty trucks. These measures are expected to contribute 27% of the reductions needed. Finally, the electrification of mechanical vehicles is expected to contribute 28% of the reductions (Government of the UAE, 2024b). Additionally, the UAE has set out plans to decarbonise its domestic maritime and aviation sectors, including electrification and use of sustainable fuels.</t>
+  </si>
+  <si>
+    <t>In 2022, the transport sector accounted for 28.5% of total US GHG emissions and, since 2017, has been the largest contributor. Total sector emissions increased by 19.4% between 1990 and 2022 due to increased motorised transport demand: during the same period, the average number of vehicle miles travelled (VMT) per passenger cars and light-duty trucks increased by 46.7%. Road transport is responsible for the vast majority of transport sector emissions in the US: light, medium, and heavy-duty trucks and passenger cars accounted for 79.8% of total sectoral emissions in 2022 (U.S. Environmental Protection Agency, 2024g). The 2021 Bipartisan Infrastructure Law (BIL) includes several components to decarbonise the transport sector, such as investments to improve roads, modernise public transit, and boost the electric vehicle (EV) market (U.S. Senate, 2021). The BIL includes measures to develop EV charging stations (USD 7.5 bn), strengthen the country’s EV battery supply chain (USD 7bn), update and upgrade public transportation (USD 39bn), build out ‘climate-friendly’ passenger and freight railways (USD 66bn), and invest in roads, bridges and other transportation infrastructure projects (USD 110bn), as well as in clean busses and ferries (USD 7.5bn). The Inflation Reduction Act (IRA), alongside significant investments in electrifying light- and heavy-duty vehicles (see below), provides considerable financial support for EV manufacturing and supply chains: the IRA sets aside USD 2bn for the Domestic Manufacturing Conversion Grant Program, which funds the re-tooling of production lines for EVs. The act allocates another USD 3bn for the Advanced Technology Vehicle Manufacturing Loan Program, which has expanded coverage to heavy-duty vehicles, locomotives, maritime vessels, and planes. As a result, plans for 163 new battery and 117 EV manufacturing plants have been announced. If fully realised, these plants would create over 170,000 new jobs in battery and EV manufacturing and account for over 60% of all new jobs created by the IRA (Climate Power, 2024b). By 2030, if all planned manufacturing plants are operationalised, domestic battery manufacturing capacity is estimated to increase by nearly 20 times to approximately 1000 GWh/year relative to 55 GWh/year in 2021 (U.S. Office of Energy Efficiency &amp; Renewable Energy, 2023). The IRA also extends the Advanced Manufacturing Production Credit to spur the domestic production and sale of clean energy components, including certain EV-relevant battery components and critical minerals (The White House, 2023b). Through these measures, the IRA is expected to reduce transport sector emissions by 15%–35% by 2035 relative to 2005 (U.S. Environmental Protection Agency, 2023c). In combination with existing policies and the BIL, the IRA is estimated to reduce overall GHG emissions by 1,150 MtCO 2 e in 2030 in comparison to business-as-usual scenarios; the result is that GHG emissions are forecasted to be 40% lower in 2030 than in 2005 (U.S. Department of Energy, 2022e). In January 2023, the Biden Administration released its National Blueprint for Transportation Decarbonisation to support the 2050 economy-wide net zero target and the 2050 target of 80%–100% emissions reductions in the transport sector. The blueprint's three key strategies align with the Avoid, Shift, and Improve (ASI) framework: the strategy supports community design and land-use planning, expands access to more efficient public and private transport, and facilitates the transition to zero emission vehicles and fuels (U.S. Department of Energy et al., 2023). Passenger transport The modal split for passenger transport has been and continues to be dominated by road transport. In 2022, nearly 70% of all commutes were undertaken by single-occupancy vehicles, while only approximately 9% of commuters carpooled. The share of single-occupancy vehicle commutes decreased by over 10% between 2018 to 2022. During the same period, and likely attributable to the COVID-19 pandemic, the share of the population working from home increased by nearly 10%. In 2022, approximately 6% of commuters used public transport and engaged active mobility (U.S. Bureau of Transportation Statistics, 2022). In March 2024, the US Environmental Protection Agency (EPA) revised its Multi-Pollutant Emissions Standards for passenger cars, light-duty trucks, and medium-duty vehicles. The standards, which will phase in from 2027 through 2032, set fleet-wide CO 2 emissions targets for auto manufacturers. For light-duty vehicles, the fleet-wide average target is 170 CO 2 grams/mile in 2027. By 2032, the average target for light-duty fleets will be reduced to 85 CO 2 grams/mile (U.S. Environmental Protection Agency, 2024i). To meet the 2032 target, the EPA estimates that battery electric vehicles will account for 30–56% of automaker's fleets to meet the average emissions target (U.S. Environmental Protection Agency, 2024j). The resulting emissions reductions are approximated to total 7.2bn tons of CO 2 through 2055 (U.S. Environmental Protection Agency, 2024b). The efforts are somewhat undermined by the fact that medium-duty vehicles—a vehicle segment that includes vans and pickup trucks and represented nearly 20% of the total US light- and medium-duty vehicle fleet in 2021—are subject to a different, less demanding set of emission standards (U.S. Environmental Protection Agency, 2022a). Although the updated standards are the most stringent in US history, the standards are less ambitious than equivalent regulations in the EU and the UK, where the emissions target for 2035 is 0 CO 2 grams/mile for new light-duty vehicles (The International Council on Clean Transportation, 2024). The relative weakness of the US standards may be partially attributable to lobbying efforts from auto manufacturers. The EPA initially proposed more ambitious fleet-wide average targets between 2027 and 2032, but the auto lobby, spearheaded by Toyota's push for more flexibility in achieving the emissions targets, successfully watered down the standards (Tabuchi, 2024). In doing so, auto manufacturers can continue to fulfil their emission reduction targets with ICE-based vehicles, which prolongs the production and profitability of fossil fuel-powered vehicles and obstructs a faster transition towards a decarbonised transport sector. At the state level, stricter, more ambitious EV policy has been implemented. California established a 100% EV sales target for 2035 through its Advanced Clean Cars II regulation in 2023. This regulation has been duplicated and adopted by twelve other states and the District of Columbia (D.C.) (California Air Resources Board, 2024). As a result, over one-third of all light-duty vehicle (LDV) sales in the US are subject to the 2035 100% EV sales target (IEA, 2024b). The combined sales of hybrid, plug-in hybrid, and battery electric vehicles made up 16.3% of all new LDV sales in the US in 2023. Battery electric vehicles accounted for approximately 7% of new car sales in the US in 2023; BEV sales reached a record of 1.1 million in 2023 (U.S. Energy Information Administration, 2024a). The growth in BEV sales is the result of a larger selection and significant price cuts in vehicles: in 2023, 20 new BEV models were introduced, while the average transaction price for BEVs decreased by over 17% between December 2022 and December 2023. In the first quarter of 2024, the gap in average transaction price between BEVs and ICE-based vehicles decreased to a record low of USD 7,000 before any purchase incentives are applied (Doll, 2024; Kelley Blue Book, 2023; U.S. Energy Information Administration, 2024a). This means that, once government incentives are applied, certain BEVs are as or more affordable than their ICE counterparts. Beyond increases in availability and affordability, growing consumer interest and IRA incentives continue to further augmented uptake (Inside EVs, 2023). To reduce emissions from road transport, the government set a goal for 50% of all new vehicles sold in 2030 be battery electric, plug-in hybrid, or fuel cell vehicles (The White House, 2021d). However, this 50% target is not aligned with the Paris Agreement. To be compatible with the PA, research suggests that 95–100% of sales of new LDVs in the US should be zero-emissions by 2030 (Climate Action Tracker, 2020). Even with IRA support, the US government estimates that LDV EV sales will only reach a median of 36% in 2030 (with a range of 15%–54%) (U.S. Environmental Protection Agency, 2023c), which is insufficient to meet the Biden Administration's goal, let alone to meet the 1.5°C compatible benchmark (U.S. Energy Information Administration, 2023a; U.S. Environmental Protection Agency, 2023c). It is important to note that estimates for EV uptake vary substantially. The International Energy Agency’s (IEA) Global EV Outlook 2023 estimates that the US will achieve the EV sales target of 50% by 2030 under the STEPS scenario and the International Council on Clean Transportation anticipates the LDV EV sales share will reach 48%–61% in 2030 (U.S. Environmental Protection Agency, 2023c). At the same time, recent US Energy Information Agency (EIA) calculations only project 13–29% EV sales in 2050 (IEA, 2023a; U.S. Energy Information Administration, 2023i). The US did not sign the 100% EVs declaration at COP26. Signatories agreed that 100% of new car and van sales in 2040 should be electric vehicles (Race to Zero, 2021). Despite the absence of the federal government’s signature, many US subnational and non-state actors, including states, cities, and automakers, signed the declaration (UK COP 26 Presidency, 2021a). In March 2024, the Biden Administration, building on the set of tariffs imposed by the Trump Administration in 2018, increased tariffs on a range of decarbonisation-relevant products and technologies from China. Tariffs on Chinese electric vehicles increased the most: the border tax on EVs will quadruple from 25% to 100% of the import value (Tankersley &amp; Rappeport, 2024). Although politically significant, research indicates that economic impacts will likely be limited (Sherman, 2024). In September 2024, the Biden Adminsitration, citing national security concerns, proposed a ban on all Chinese connected car hardware and software (Shepardson et al., 2024). If finalised, Chinese software would be banned starting in 2026, while hardware would be prohibited beginning in 2030. The IRA accelerates the uptake of electric light-duty vehicles by extending and expanding tax credits for both new and used EVs. From 2023 through 2032, the Clean Vehicle Credit provides up to USD 7,500 for new battery electric, plug-in hybrid and fuel cell EVs that retail under USD 80,000 for vans, SUVs, and pickup trucks and USD 55,000 for all other types of vehicles. To qualify for the full credit, the vehicle and its critical mineral and battery components must meet certain requirements for assembly in and sourcing from North America or trusted trade partners (U.S. Internal Revenue Service, 2024a). The result of the sourcing and manufacturing requirements is that only 22 EV models qualified for the total tax credit out of the 104 EV models for sale in May 2024 (Lambert, 2024). Beyond targeting new EV sales, the US government seeks to leverage the maturing used electric vehicle market, which was made up of approximately 400,000 EVs in 2023 (IEA, 2024b): the Used Clean Vehicles Credit provides up to USD 4,000 to buyers who purchase a used electric vehicle for USD 25,000 or less (U.S. Internal Revenue Service, 2024c). Both the credits for new and used EVs are capped at different income levels to increase the affordability of and access to EVs for individuals and households with lower to middle incomes. Buyers of used EVs can also claim the credit at the time of purchase, which more immediately reduces the purchasing or monthly financing cost. As high costs remain a crucial barrier to EV adoption, reducing costs, particularly for buyers with lower incomes, accelerates and supports a just transition to EVs (Pamidimukkala et al., 2023). The government is on track to achieve its 2030 target for 500,000 publicly accessible recharging points in 2026 (The White House, 2024a). The number of publicly accessible recharging points increased by over 70% to 170,000 stations since 2021 (U.S. Joint Office of Energy and Transportation, 2024).(U.S. Environmental Protection Agency, 2023i) Freight transport Freight transport emissions account for an increasing share of total transport emissions in the US: the share of emissions from freight transport increased from 24% in 1990 to 32% in 2021 (K. Kennedy, 2023). Trucking accounted for 65% of all freight moved by weight and made up roughly 83% of total freight transport emissions in 2021 (U.S. Environmental Protection Agency, 2024f). To mitigate emissions from trucking, the government revised emissions standards for heavy-duty vehicles in 2024 (see below). Shifting freight transport to rail, which only emitted 5.7% of total sectoral emissions in 2021 (U.S. Bureau of Transportation Statistics, 2023) and accounted for the greatest share of long-distance freight volumes across all modes of freight transport, has significant emissions reductions potential (Association of American Railroads, 2021). In March 2024, the EPA adopted an updated set of vehicle emissions standards for heavy-duty trucks, transit, and vocational vehicles. The Greenhouse Gas Emissions Standards for Heavy-Duty Vehicles Phase 3 strengths the existing emissions standards: heavy-duty vocational vehicles need to reduce emissions by up to 60% more under the Phase 3 standards relative to Phase 2. The revised standards will effect HDVs starting in 2027 through 2032. Between 2027 and 2055, the standards are expected to mitigate approximately 1bn tons of CO 2 emissions (U.S. Environmental Protection Agency, 2024e). In comparison, the EU, which also revised its heavy-duty vehicle emissions standards in 2024, sets a more ambitious emissions reductions target for all new HDVs for 2030, which will escalate to a 90% target for 2040. As a first step to mainstream reductions in freight transport emissions, the Biden Administration established a national goal to transition towards a zero-emissions freight sector in April 2024. Although the administration has not indicated an explicit timeline for the zero-emissions target, separate action plans for decarbonising truck, rail, aviation, and marine freight transport are to be developed. Since its adoption in 2022, the IRA has spurred investments and introduced provisions to reduce GHG emissions from heavy-duty transport. Through the IRA, the EPA launched the Clean Heavy-Duty Vehicle Program, which was revised in 2024, to provide USD 1bn in grants to states, municipalities, and Tribes to offset the costs of replacing heavy-duty vehicles with zero-emissions alternatives and installing related infrastructure; at least USD 400m of the total funding will be channelled towards communities suffering from severe air pollution (U.S. Environmental Protection Agency, 2024d). The programme's first funding round of over USD 900m opened in April 2024 (U.S. Environmental Protection Agency, 2024c). The EPA estimates that 70% of the programmes funding will go towards replacing ICE-based school buses (U.S. Environmental Protection Agency, 2024a). An additional USD 3bn is allocated to provide grants to local governments, port authorities, and other relevant actors to purchase and install zero-emission port equipment and technology (The White House, 2023b). The IRA has also introduced the Commercial Clean Vehicles Credit, which defers 30% of the costs of replacing diesel or gas-powered commercial vehicles—ranging from cars to long-haul trucks —with electric vehicles. A credit of up to 15% is also available when replacing a vehicle with a partially electric alternative. The IRA also allocates USD 3bn for electrifying the United States Postal Service fleet (The White House, 2023b). Beyond providing tax credits for buyers, the government is partnering with truck manufacturers to further develop heavy-duty EV technologies. Through the 21st Century Truck Partnership, the Supertruck 3 programme, and the Million Mile Fuel Cell Truck consortium, the US Department of Energy (DOE) is supporting the research and development of next generation of heavy-duty batteries and fuel cells (U.S. Department of Energy, 2022a). The government is also funding commercial EV demonstration projects. In 2023, the DOE awarded over USD 7m to seven projects that will develop a medium- and heavy-duty recharging station corridor across 23 states. In 2024, the government announced that the DOE would fund the research and development of load management strategies to alleviate recharging-related grid capacity challenges. Federal government support for commercial EV uptake has been supplemented by state action. New York and California provide additional purchase incentives of over USD 100,000 on top of the IRA’s mechanism. In response, adoption of heavy-duty EVs seems to be increasing: delivery van fleets are quickly electrifying as Amazon, FedEx, UPS, USPS, and Walmart place major EV orders. Commercial production by Volvo and Freightliner of electric tractor trailers, or 18-wheelers, began in 2023. Although there are promising signs of increasing implementation, only 1.5% of all commercial heavy-duty vehicles in the US were BEVs or PHEVs in September 2023. At the same point in time, the share of BEVs and PHEVs in the HDV fleets in Europe and China amounted to over 7% and 10%, respectively (Soulopoulos, 2023). Aviation The IRA also seeks to encourage the development and adoption of sustainable fuel technologies in the aviation industry. The Sustainable Aviation Fuel Tax Credit incentivises the sale and use of sustainable aviation fuels (SAF) that reduce lifecycle GHG emissions by at least 50% compared to petroleum-based jet fuel. The tax credit, worth USD 1.25 per gallon, is progressive: SAF that reduce emissions by more than 50% are eligible for an additional USD 0.01 per gallon for each extra percent that the reduction exceeds 50% (up to USD 0.50 per gallon) (U.S. Department of Energy, 2022c). The act additionally provides nearly USD 300m in grants to develop and deploy projects related to sustainable aviation fuel and low-emission aviation technologies (The White House, 2023b). Although the US produced nearly 16m gallons of SAF in 2022, these fuels accounted for less than 0.1% of the total fuel used by US airlines in the same year (U.S. Government Accountability Office, 2023). Additionally, analysis suggests that currently available SAF do not reduce emissions across the fuels’ full lifecycles given their emissions and agricultural resource-intensive production methods (Lashof &amp; Denvir, 2024).</t>
+  </si>
+  <si>
     <t>In 2023, the transport sector was responsible for approximately 20% of Germany’s total emissions. According to the government’s targets, transport sector emissions need to be reduced by 44% below 1990 levels. This means that emissions need to fall to 85 MtCO 2 e in 2030. Emissions were still at 146MtCO 2 e in 2023 and 12 MtCO 2 e above national target pathway for 2023. Transport emissions in 2030 are expected to overshoot the target by 26 MtCO 2 e (UBA, 2024d). Actions by the transport ministry The Ministry of Transport has the ignored the government’s own environmental agency and its policy recommendations for reducing emissions in the transport sector (UBA, 2023c). Instead, the ministry weakened the climate law by removing the emergency programme protocol; previously, emergency policy packages needed to be submitted when a given sector overshot its emissions target. Over the past several years, the Ministry of Transport has generally obstructed more climate action than it has supported: It suddenly and prematurely eliminated purchase incentives for light and heavy-duty electric vehicles at the end of 2023 following federal budget cuts (BAFA, 2023). Germany delayed the adoption of the revised CO 2 -standards for cars at the EU level and negotiated for the continued use ICE vehicles powered by CO 2 -neutral e-fuels after 2035 (Packroff, 2023). Germany is lobbying for a similar exception under the new CO 2 -standards for heavy-duty vehicles, which have yet to be adopted (Wacket and Abnett, 2024). The ministry negotiated favourable treatment of 144 freeway projects that will be accelerated. The individual commuter support was increased during the energy crisis, which incentivises longer travel distance between home and workplace and therefore more transport activity. The carbon price increase in the German ETS was temporarily suspended due to the energy crisis in 2022. The transport ministry objects to a speed limit for freeways. According to Federal Environment Agency research, a speed limit on highways of 130, 120 or 100 km/h would result in emissions savings of 1.5, 2 and 4.3 MtCO 2 e/year, respectively, which is equal to 5-14% of emissions from passenger cars and light commercial vehicles on highways. It is important to note that Germany is one of the only countries in the world without freeway speed limits. (UBA, 2023d). Recent policies that support emissions reductions include: Restructuring of the freeway fee for trucks according to CO 2 emissions of the vehicles. The revenue will be used to expand railway infrastructure. Introducing the “Germany ticket,” which costs EUR 49 per month and is valid on all forms of public transport and regional trains. Overall, the direct impact of the ticket on emissions in 2030 is limited. Public transport Support for public transport has somewhat increased, but the government is far from reaching its targets. The government plans to double the volume of rail passenger transport by 2030 compared to today’s level, increase the capacity and attractiveness of public transport, and raise the share of journeys undertaken by bicycle or on foot. However, the government remains vague regarding specific instruments and necessary finance for achieving these goals (BMWK, 2022). In 2021, rail accounted for only 8% of total passenger transport, while cycling and walking make up only 6% (BMWK, 2022). Deutsche Bahn, the national rail company, and the government further plan to invest EUR 86bn into the rail network by 2030. The income generated from the increase in the freeway fee for trucks will be used to cover half of these investments. The source for the remaining half is to be determined. Germany introduced the “Germany ticket” in May 2023. The ticket, costing EUR 49 month, grants access to all means of local public transit, including regional trains, countrywide. By May 2024, approximately 11 million tickets had been issued. Estimates for the ticket’s short-term impact on emissions range from reductions of 4.2MtCO 2 e/y to 22.6MtCO 2 e/y by 2030 (Expertenrat für Klimafragen, 2024). The long-term impact may be more significant, given the single ticket system makes using public transport more accessible. Electrification of road transport Government policies do not appear to be sufficient to achieve the 2030 target of 15 million electric vehicles (Koska and Jansen, 2022). The most recent UBA emissions projection report notes that, given sectoral developments, the target of 15 million electric vehicles will not be achieved. The report assumes only 8 million electric vehicles will be registered in 2030. On 1 January 2024, only 1.4 million battery electric cars were registered in Germany. The share of newly-registered battery- and fuel cell-electric cars in 2023 was nearly 20% (EAFO, 2024). Although the share of electric cars is increasing, both the existing vehicle fleet and new vehicle registrations remain dominated by internal combustion engine (ICE) vehicles. Research also suggests that the 15 million electric vehicle target is itself not sufficient to meet the sectoral emissions target for passenger transport set in the climate law (Koska and Jansen, 2022). To achieve the emissions target, at least 20 million electric vehicles need to be registered in 2030. Additional measures are needed to accelerate electric vehicle uptake, including the introduction of a registration tax for CO 2 -intensive cars, a higher CO 2 -price, or a comprehensive reform of company car taxation. The government eliminated the purchase subsidy for electric cars at the end of 2023. Previously, the financial incentive for newly-purchased BEVs retailing at EUR 45,000 or less was worth up to EUR 6,750 (EUR 4,500 from the government and EUR 2,250 from manufacturers) (ADAC, 2023a). Although the eliminated subsidies have largely been absorbed by auto manufacturers and the German electric vehicle market is relatively mature, registrations of new electric vehicles have slowed since the government incentive’s termination: battery electric vehicles registrations were 14 percent lower in the first quarter of 2024 than in the same period in 2023 (KBA, 2024e); a worrisome outlook given that the German government anticipated new electric vehicle registrations to increase by nearly 40% in 2024 relative to 2023 (UBA, 2024a). Charging infrastructure is expanding, with over 115,000 public charging points in place in November, 2023 (Bundesnetzagentur, 2024); an increase of over 80% since the end of 2021 (BMDV, 2024). The government plans to operationalise one million public charging points for electric vehicles by 2030 (BMDV, 2022). The EU strengthened the CO 2 emissions performance standards in April 2023: by 2035, all new passenger cars must be zero emissions. The German government delayed the adoption of the new CO 2 -standards by negotiating for an exception for e-fuels. This is problematic for several reasons: there are no cars that run exclusively on e-fuels, e-fuels will remain significantly more expensive in comparison to directly using electricity from batteries, and e-fuels are not zero emissions. Vehicles fuelled by e-fuels, as defined by EU’s Renewable Energy Directive methodology, are expected to use six times the electricity and emit 61 gCO 2 e/km in 2035 (Transport &amp; Environment, 2023). The focus on e-fuels therefore only prolongs the production of diesel and petrol cars and hinders the transition towards non-ICE-based vehicles. As the EU worked towards strengthening the CO 2 emission performance standards for heavy-duty vehicles in 2024, Germany again delayed the legislative process by lobbying for an exemption for e-fuels. Carbon price in the German ETS The German government's carbon price on transport fuels remains far too low to meet the target without other supportive measures. The fixed price was set at EUR 25/tCO 2 in 2021 and increased to EUR 30/tCO 2 in 2022. Price increases were suspended due to the energy crisis, but as of 2024 the price was raised to EUR 45/tCO 2 e. From 2026, new allowances will be auctioned in a range of EUR 55 to EUR 65/tCO 2 e (German Government, 2020a). In 2027, the German ETS will be merged into the revised EU ETS for transport and buildings. The impact of the German ETS on GHG emissions in the transport sector is limited, as the carbon price of EUR 45/tCO 2 e translates into a relatively small markup on the petrol price. By 2026, the price will increase to a maximum of EUR 65/tCO 2 e (ICAP, 2022). Whether the price will change the investment behaviour of car owners depends on the price level and its predictability, which has been notably inconsistent in 2023 and 2024. The German Environmental Agency (UBA) estimates that, without any additional measures, an allowance price of at least EUR 350/tCO 2 e would be necessary to reduce emissions to the sectoral target (Harthan and Repenning, 2022). The German government’s own projections report (UBA, 2024c) assumes an increase to EUR 125/tCO 2 e after 2030 and reaching a maximum of EUR 180/tCO 2 e in 2050. All proceeds from the ETS system will be re-invested into climate protection or returned to citizens. In 2022, the combined revenues of the German ETS and the EU ETS totalled more than EUR 13bn and were channelled into the country’s Climate and Transformation Fund (KTF), which functions as the principal source of climate finance economy-wide (UBA, 2023a). Although the government has agreed to return the revenues of the carbon price to consumers, this payback will likely only happen beginning in 2028. Administrative barriers are one issue, while the fact that the revenues are already planned for other purposes through the KTF is another (Pokraka, 2023).</t>
   </si>
   <si>
+    <t>Transport is the only major sector in the EU where emissions have increased over the last 30 years: emissions in 2022 followed an upward trend of 2.7% compared to 2021. It is too early to say whether emissions from the sector have peaked: the economic rebound and trend towards bigger vehicles may undermine the impact of increasing EV sales on emission levels. The EU has introduced several policies and regulations to reduce emissions from the transport sector across all transport modes. These include but are not limited to: Revised Renewable Energy Directive (EU) 2023/2413, through the adoption of sectoral renewable energy targets, Revised Regulation strengthening CO 2 emission performance standards for new cars and vans (EU) 2023/851, which established a ban on the sale of combustion engine cars by 2035. Revised Regulation on the trans-European transport Network (EU) 2024/1679 New EU ETS II which covers road transport emissions from 2027 In 2023, electric vehicle (battery electric and plug-in hybrid) made up 22% of vehicle sales. To be 1.5°C compatible in line with the Paris Agreement, the CAT finds that the EU would need to achieve 95–100% sales of light-duty electric vehicle sales by 2030 (Climate Action Tracker, 2024). This is five years earlier than the EU’s current target of 2035. The EU did not sign the Zero Emissions Vehicle pledge at COP26 and did not include this target in its NDC. In President von der Leyen’s political guidelines for the next four years in office, she hinted that the 2035 ban on the sale of internal combustion engine vehicles might be watered down through the increased use of alternative fuels to achieve the ban (Mathiesen et al., 2024). The ban on fossil fuel car sales has an exemption to allow synthetic e-fuels to continue beyond 2035. Positively, the guidelines also pushes for greater improvements to the EU’s rail network to encourage a stronger modal shift towards rail (von der Leyen, 2024b). In June 2024, the EU adopted the revised Regulation on the trans-European transport Network (TEN-T) (European Parliament &amp; European Council, 2024b). The regulation intends to create the enabling conditions to scale up zero emission transport modes, improving connecting and promoting a modal shift to more share and zero mission transport. While no new transport regulations have been adopted since the last CAT assessment in February 2024, some have been revised or are still pending agreement such as the CO 2 emission standards for heavy-duty vehicle and the Green Freight Package. Gaps still remain for some regulations. For example, the FuelEU Maritime Regulation (EU) 2023/1805 (European Parliament &amp; Council of the European Union, 2023c) and the Alternative Fuel Infrastructure Regulation (EU) 2023/1804 (European Parliament &amp; European Council, 2023) consider LNG a “low carbon fuel” in shipping. As LNG is a fossil fuel, its prolonged or expanded use will make it difficult to achieve future emission reductions given the long lifetime of ships and infrastructure, resulting in stranded assets. To reach full decarbonisation in the transport sector globally by mid-century, the EU would need to increase the share of zero emission fuels (electricity, hydrogen and biofuels) from 7% in 2019 to 55% by 2030. This covers all modes of domestic transport collectively (i.e. road, rail, domestic aviation and maritime travel) (Climate Action Tracker, 2024). Tariffs on Chinese EVs In October 2024, the EU Commission announced new tariffs on battery EVs manufactured in China on the basis that the Chinese government unfairly subsidies its EVs, undercutting European car manufacturers. Individual duties will range between 17.4% to 37.6% depending on the Chinese manufacturer (European Commission, 2024e). To be 1.5°C compatible, the EU needs continued exponential growth in EV sales, needs a lot of them to meet demand, and needs to make it affordable for consumers (Climate Action Tracker, 2024). One of the major barriers to this is affordability. Chinese EV models sold across EU member states are typically cheaper than European manufactured vehicles, which could affect consumer choices.</t>
+  </si>
+  <si>
     <t>Transport is responsible for 12% of India’s energy related CO 2 emissions (IEA, 2023a). In 2022, India's transport sector consumed 16% of total primary energy but only 1.5% of electricity (IEA, 2023c). The transport sector is dominated by fossil fuels (96% in 2021), mostly oil (93%). 1.5°C compatible pathways for India show a share of electricity in transport reaching 5% by 2030 and 25-76% by 2050 (Climate Analytics, 2024). Several national programmes, including the National Urban Transport policy and the Smart Cities Mission, have been established to reduce vehicle traffic and increase transport efficiency. Electric vehicles By 2030, India aims to increase the share of electric vehicle (EV) sales to 30% in private cars, 70% in commercial vehicles, 40% in buses, and 80% in two and three-wheelers (Clean Energy Ministerial, 2019; The Economic Times, 2021). At COP26, India signed the 100% EV declaration with a focus on two and three-wheeler auto-rickshaws. The government plans to mandate all two-wheelers to be electric by 2026, ahead of the timeline set at COP26 (Pnadya, 2022). Total annual EV sales reached 1.7 million vehicles in FY2024, of which 55% were two-wheelers and 32% were three-wheelers (JMK Research &amp; Analytics, 2024). This corresponds to 5% and 79% shares of EVs in total sales of two and three-wheelers respectively, showing there is still a lot of work to do to reach the government’s 80% target for two and three-wheelers by 2030. For passenger cars the sales share is much lower, at &lt;0.5%. Financing and the installation of five million fast chargers are crucial for accelerating the transition to e-mobility. There is a continued focus on expanding the EV charging network, which is expected to create opportunities for small vendors involved in the manufacture, installation, and maintenance of EV charging stations (Indian Express, 2024)​. To be compatible with 1.5°C, the share of total EV sales (including two and three wheelers) needs to be 34% by 2030, and 100% by 2040 from current level of around 1% (Climate Action Tracker, 2020). Back in 2015, the government launched National Electric Bus Programme (NEBP) with the aim to deploy an additional 50,000 new e-buses (UITP, 2022). However, the programme faced obstacles due to the low bankability of electric bus leasing contracts caused by the weak financial condition of Indian State Transport Undertakings (STUs) (IEEFA, 2023d). A recent report by the Ministry of Petroleum and Natural Gas recommends that diesel city buses be prohibited in urban areas as part of a 10-year plan to transition towards cleaner fuel for urban public transport and intercity buses to shift towards all-electric buses with CNG/ LNG as transition fuels (Ministry of Petroleum and Natural Gas, 2023). Budgetary support for urban public electric transport has increased significantly. In the budget of 2024-25, INR1300 crore (USD 155m) has been allocated for the procurement of electric buses, a huge jump from the USD 2.4m in the 2023-24 budget (Climate Group, 2024). The Faster Adoption and Manufacturing of Electric Vehicles in India (FAME) scheme is a key component of India’s EV strategy. It came into effect in April 2019, with financial support of INR 100bn (USD 1.35bn) to provide incentives to purchase electric vehicles and support for establishing the necessary charging infrastructure (Business Today, 2019). The second phase of FAME ended in March 2024 with a total outlay of INR 115 bn (USD 1.4 bn). The next phase - FAME III - is expected to be introduced soon with a smaller allocation of INR 20 bn (USD 240m) to develop electric mobility infrastructure such as charging networks across the country, although there was no mention of it in the 2024-5 budget (Mint, 2024a). The scheme aims to support one million electric two-wheelers, 500,000 electric three-wheelers, 55,000 electric cars, and 7,090 electric buses through subsidies. In 2021, this scheme was extended until 2024, as it had made minimal progress in achieving these sales targets (Chaliawala, 2021). A vast network of EV charging stations is needed to support the rapid uptake of EVs. The 2023-24 budget allocated USD 632m for the FAME programme, about an 80% increase from previous budget allocations, but the 2024-5 budget halved it to USD 318m (IEEFA, 2023h; Economic Times, 2024a). In the 2024-5 budget the government proposed custom duty waivers on 25 critical minerals, which could help lower the cost of EVs and make them more affordable for buyers. Fuel standards India strengthened its fuel/emissions standards in April 2020, when it adopted Bharat Stage VI emissions standard for vehicles (the same as Euro VI standards) (DieselNet, 2021). BS VI is applicable to all vehicles with a Gross Vehicle Weight (GVW) of more than 3,500 kg, including commercial trucks, buses and on-road heavy-duty vehicles such as refuse haulers and cement mixers. The Indian government has advanced different targets and policy frameworks to introduce alternative fuels in the transport sector. Blending of 20% ethanol in petrol is part of such an initiative, for which the target year was slashed to 2025 from the earlier target of 2030 (NITI Aayog, 2021). Similarly, hydrogen fuel cell electric vehicles are seen as a potential solution for long distances for ships and potentially trucks, where electrification is not easily possible (Kukreti, 2021; Ministry of Petroleum and Natural Gas, 2021). Toyota has initiated a pilot project to test its hydrogen fuel cell-powered light vehicle on Indian roads (ET Auto, 2023). In contrast to these steps forward, in its draft LNG policy 2021 the government is developing plans to use LNG in long-haul heavy-duty trucks and other similar vehicles. The government has also launched a voluntary vehicle scrappage policy in April 2022 to phase out old vehicles from Indian roads (Garg, 2022). The 2023-24 budget includes provisions for scrapping of Central and State Government vehicles that are over 15 years old, as well as tax incentives for private individuals who exchange their old vehicles by purchasing new ones (Times of India, 2023). However, the new vehicles to be purchased are mostly fossil fuel-driven, as under the policy there is no requirement to replace them with electric vehicles. Railways and waterways In July 2020, Indian Railways announced plans to achieve net zero emissions by 2030. It also has a goal of mitigating 60 MtCO 2 e by 2030 by implementing a range of measures, such as planting trees on unoccupied railway areas, decreasing water usage, and constructing facilities that convert waste into energy (Bloomberg, 2022). In February 2023, it has achieved 100% electrification of its network (International Railway Journal, 2023). Indian Railways is also planning to increase its use of renewable energy and to install 30 GW of renewable energy capacity by 2030 (Bloomberg, 2022). However, only 245 MW solar capacity installation has been executed on rooftops of various stations and administrative buildings to date. Indian Railways is looking to introduce hydrogen-fuelled trains on its narrow gauge heritage routes from 2024 and has issued tenders for procuring 35 trains powered by green hydrogen (Railway Technology, 2023; The Economic Times, 2023b). Rollout of green hydrogen driven trains in India will still be subject to the cost competitiveness of the fuel (ET EnergyWorld, 2022b). The Maritime India Vision 2030 outlines a target for Indian ports to reduce carbon emissions by 30% of per tonne of cargo handled by 2030 (Ministry of Ports Shipping and Waterways, 2021). In November 2022, the National Centre of Excellence for Green Port &amp; Shipping was launched. It is tasked with providing policy and regulatory support to the Ministry of Ports, Shipping and Waterways to develop a regulatory framework and roadmap to foster carbon neutrality and circular economy in India’s shipping sector (Press Information Bureau, 2022b).</t>
   </si>
   <si>
     <t>The expansion of zero emission fuels in the transport sector is crucial for meeting the 1.5°C temperature limit. Indonesia has strategies to support biofuels and electric vehicles, but current outcomes fall short of national targets. The Ministry of Transport (MOT) published Ministerial Decree No. 8 of 2023 outlining 34 key actions for land, water, and air transport, including public transit improvements and EV infrastructure (Ministry of Transport, 2023). Biofuels Biofuels are key to achieving Indonesia's renewable energy targets. RUEN states that biofuel consumption should reach 13.9 billion litres by 2025, 20.8 billion litres by 2030, and 52.3 billion litres by 2050 (Republic of Indonesia, 2017). The national biofuel mandate is one of the main instruments used to achieve these targets. Biodiesel Indonesia's biodiesel mandate programme is one of the most ambitious globally. Blending levels have progressively increased from 15% (B15) in 2015, 20% (B20) in 2016, 30% (B30) in 2020, to 35% (B35) by 2023 (Coordinating Ministry for Economic Affairs, 2023). The government subsidises the price difference between biodiesel and conventional through palm oil export levies, with total incentives reaching approximately USD 9.3 bn between 2015 and early 2023 (APROBI, 2023; IEA, 2023). Domestic biodiesel sales amounted to 12.2 million kilolitres in 2023 (Jakarta Globe, 2024). Indonesia plans to increase the blending level to 40% (B40) by 2025 and 50% (B50) by 2029, as committed by the new president to reduce oil imports (BioEnergy Times, 2024; S&amp;P Global, 2024). Trials for B40 have shown minimal performance differences, and the state-owned rail operator Kereta Api Indonesia (KAI) currently uses 300 million litres of B35 fuel without issues, and is conducting B40 trials on the Yogyakarta-Jakarta route (MEMR, 2024a; S&amp;P Global, 2024). Trials in the non-automotive sectors will commence soon (S&amp;P Global, 2024). Further advancing biofuel usage, Pertamina and the Bandung Institute of Technology (ITB) developed J2.4 fuel, containing 2.4% palm oil–based bioavtur (bio-jet fuel), with a successful commercial flight test on Garuda Indonesia in October 2023 (MEMR, 2024a). Bioethanol In contrast to biodiesel, bioethanol blending has not been as successful. MEMR Regulation No. 12 of 2015 targeted 5% (E5) blending by 2020 and 20% (E20) by 2025, but these targets have not been met. Only about 500 kilolitres of bioethanol were blended with gasoline between 2012 and 2017, with virtually no blending since 2018 (ERIA, 2024). In June 2023, Indonesia restarted its bioethanol program (MEMR, 2023c). Presidential Regulation No. 40 of 2023 sets goals to achieve self-sufficient sugar production by 2028 and produce 1.2 billion litres of sugarcane-based ethanol by 2030. Pertamina launched "Pertamax Green 95", a gasoline with 5% bioethanol, in July 2023, which has received a positive market response and is currently available at certain gas stations in Surabaya and Jakarta (MEMR, 2024a). The government proposes maintaining 5% bioethanol content in 2024 and increasing it to 10% by 2029 (MEMR, 2024a). However, realistically, a 2% (E2) blending program would require around 700 million litres of bioethanol annually, while the current installed production capacity is only at 45–100 million litres (ERIA, 2024). In addition, concrete measures are needed to bridge the price gap between fuel-grade bioethanol and gasoline. The government is revising mandatory blending policies and exploring incentive funding sources (CNBC Indonesia, 2019; Bisnis.com, 2020; IESR, 2021a). Link to deforestation and food competition Deforestation is a key issue for biofuel development in Indonesia, as palm oil plantations are a main driver for tree-cover loss ( see the Forestry section ). Implementing the B30-B50 programme is estimated to require 11-18 million tonnes of CPO, equivalent to 20.5-22.8 million hectares by 2024, meaning another 4-6 million hectares of land will need to be cleared (IESR, 2021b). This could also cause domestic supply shortages and rising cooking oil prices, similar to the 2021-2022 crisis (Chain Reaction Research, 2022). Palm oil-based biodiesel can reduce 50-85% of GHG emissions compared to fossil fuels without considering land-use change. However, the GHG emissions will be much higher when considering land-use change. First-generation biofuels also compete with food sources, potentially passing oil price volatility to food prices and affecting food security (IESR, 2021a). To address concerns over palm oil-driven deforestation, Presidential Regulation No. 44 of 2020 mandated all oil palm plantations to be certified under the Indonesia Sustainable Palm Oil (ISPO) scheme. However, significant concerns remain around its limited coverage, weak design, and poor transparency (EIA, 2022; Indonesia Information Portal, 2022). Strengthening environmental policies for biofuel development will be key for Indonesia's export market. In June 2023, the European Union introduced the Regulation on deforestation-free products (EUDR), imposing restrictions to ensure consumption in the EU does not drive deforestation (European Commission, 2023). The EU, Indonesia, and Malaysia have agreed on a Joint Task Force to implement the EUDR (European Directorate-General for Environment, 2023). Electric vehicles Indonesia is focusing on electric vehicles (EVs) to address air pollution and meet its NDC targets. The government aims for electric two-wheelers (E2W) to reach 1.8 million by 2025 and 13 million by 2030, while electric four-wheelers (E4W) are targeted to reach 400,000 by 2025 and 2 million by 2030 (Republic of Indonesia, 2022). By April 2024, Indonesia had approximately 133,000 EVs, with E2Ws dominating at 110,000 units and E4Ws comprising 23,000 units (CNN Indonesia, 2024a). The government has issued regulations to boost the domestic EV industry and support infrastructure development, but barriers remain. The high local content requirement (LCR) for domestically manufactured EVs is considered a barrier to industry growth. MOI Regulation No. 27 of 2020 sets a minimum LCR of 35% for two-wheelers and 40% for four-wheelers in 2021. Government plans to increase this to 60% by 2024 could constrain the expansion of Indonesia's domestic EV industry, as domestic battery production is yet to begin (IESR, 2022b). Presidential Regulation No. 79 of 2023 has extended the 40% minimum LCR deadline for EVs from 2023 to 2026 and the 60% minimum LCR deadline from 2024 to 2027. Fiscal and non-fiscal incentives have been introduced to encourage EV adoption, including luxury tax breaks, subsidies, and discounted electricity rates for home charging (AC Ventures and AEML, 2023; The Diplomat, 2024b). In total, the government earmarked USD 455m in subsidies to promote EV purchases (IEA, 2024). However, these measures are still insufficient to make EV purchase prices comparable with conventional vehicles in Indonesia (IESR, 2021c, 2022b). Challenges persist in accelerating EV adoption. Charging infrastructure, while expanding rapidly, remains insufficient to meet growing demand. By September 2023, Indonesia had around 850 fast-charging stations and 1,700 battery exchange units (Kompas, 2023). The availability of charging stations remains a key barrier, contributing to "range anxiety" among consumers (IESR, 2023a, 2024). Moreover, the lack of standardised batteries hinders the widespread adoption of battery-swapping stations (IESR, 2023a). Transport infrastructure &amp; public transit Public transport coverage remains low in most Indonesian cities, with an average modal share of 2-5% (except Jakarta, which has a 10% share) (WRI Indonesia, 2024). In Greater Jakarta, there are four main modes: TransJakarta (Bus Rapid Transit/BRT), the KRL Commuter Line, Mass Rapid Transit (MRT), and Light Rail Transit (LRT). Approximately three million people – around 10% of Greater Jakarta’s population – use these systems daily (Almaputri, 2019), with TransJakarta serving the largest number of users, followed by KRL, MRT, and LRT (ANTARA News, 2022). Plans are underway to extend the MRT, LRT, and KRL networks in Greater Jakarta, and the government is also considering to develop an LRT system in Bali, with an initial underground route linking the airport to city centre (PwC, 2024). With co-financing from Switzerland, Indonesia is advancing Bus Rapid Transit (BRT) systems in six pilot cities: Pekanbaru, Batam, Bandung, Semarang, Makassar, and Surabaya (GIZ, 2023). Of the 17 BRT systems across Indonesia, only four currently operate electric buses (Faqih Rohman and Kairini, 2023). TransJakarta (BRT operator in Jakarta) is leading the electrification of public transport, with 52 electric buses by 2023 and plans to fully electrify its 10,000 bus fleet by 2030 (Ditjen Hubdat, 2022; Semarang Department of Transportation, 2022; Faqih Rohman and Kairini, 2023). However, limited budgets and the higher costs of electric buses (15-35% above diesel alternatives) pose challenges, with substantial government incentives still needed to make EV buses economically viable (IESR, 2024). Electrifying long-haul and intercity buses presents additional hurdles due to limited range, insufficient charging infrastructure, and higher upfront costs. Policy uncertainties also persist, as the government has yet to decide whether to adopt an EV bus strategy for long-distance routes or prioritise fuel quality improvements for conventional vehicles. Bus operators currently maintain Euro 4 standards, awaiting clearer guidance on long-distance travel electrification (IESR, 2024).</t>
   </si>
   <si>
-    <t>Transport emissions represented 19% of Australia’s total emissions (excluding LULUCF) in 2023/24 (DCCEEW, 2024i). The sector is projected to become the greatest source of emissions in by 2030 as power sector emissions decline (DCCEEW, 2023b). The government introduced the long-awaited New Vehicle Efficiency Standard (NVES) in 2024, which will apply to new cars sold from 2025. Until this year, Australia was one of the last developed countries, along with Russia, to lack such standards. On average, new cars in Australia consume 40% more fuel than those in the EU and 20% more than in the US (DCCEEW, 2023c). Under the NVES, emissions intensity limits (g CO 2 /km) are imposed on suppliers across the fleet of new vehicles they sell each year, with higher limits allowed for heavier vehicles. There are no restrictions on which cars may be sold, but the sale of emissions intensive cars must be offset by the sale of more fuel-efficient cars or buying credits from other suppliers (DITRDCA, 2024). The emissions intensity targets are set to decline each year leading to a projected reduction in transport emissions by 4% between 2023 and 2030, and a further 15% between 2030 and 2035. During the legislation’s consultation period in early 2024, the government watered down the proposed standard, allowing some four-wheel drives to be counted as light commercial vehicles (LCVs) instead of passenger vehicles (PVs), with the former being subject to higher CO 2 limits. The government also raised the ‘headline target’ for LCVs, which effectively increases the average emissions intensity allowed for LCVs, and increased ‘breakpoints’ for both LCVs and PVs, which gives heavier vehicles greater emissions headroom. Combined, these changes will allow an additional 17 MtCO 2 e to be emitted cumulatively by 2035 — one sixth of the sector’s current annual emissions (DITRDCA, 2024). The National Electric Vehicle Strategy, published in 2023, outlines a roadmap to encourage EV adoption with a focus on cooperation between the government and states. However, it does not include quantified targets for EV adoption beyond state-level targets that now exist for all states and territories, with varying levels of ambition, except the Northern Territory and Tasmania (DCCEEW, 2023c; IEA, 2023a). The government has committed to building a National EV Charging Network, with charging stations on average every 150 kilometres along the country's major highways by 2026 (DCCEEW, 2024f). Australia’s EV uptake remains slow compared to other countries. EVs made up only 8.5% of new car sales in 2023, including battery electric vehicles (BEVs) and plug-in hybrid electric vehicles (PHEVs) (Electric Vehicle Council, 2024). Comparatively, the market share of EVs (BHEVs and PHEVs) reached 22% in the European Union, 38% in China, and 93% in Norway in 2023 (IEA, 2024a). The government projects that battery EV sales will reach 23% of new light duty vehicle sales by 2030, and 47% by 2035 (DCCEEW, 2023b). The anticipated slow electrification of Australia's vehicle fleet is a missed opportunity to leverage the power sector's transition for decarbonising transportation. The government’s current policies do little to address emissions from heavy-duty vehicles, such as trucks which account for more than a fifth of transport emissions (DCCEEW, 2023b), nor do they address the lack of planning for public transportation and modal shifting. Australia has also not set a phase out date for fossil fuel vehicles.</t>
-  </si>
-  <si>
-    <t>Transport makes up just over 50% of Brazil’s energy sector emissions, and emissions have been steadily increasing since 2018, mainly due to increased vehicle ownership (SEEG, 2023a). As part of its energy transition goals, Brazil launched the Fuels of the Future Programme which plans to increase the ethanol blend in gasoline from 22% to 27%, as well as the amount of biodiesel blended into diesel from 14% to 20% by 2030. The programme also looks at reducing aviation emissions by gradually increasing the mix of sustainable fuels and stipulates that airlines must reduce greenhouse gas emissions by 1% in 2027 and by 10% in 2037 (Silva, 2024; Talanoa, 2023). Brazil is currently one of the world’s largest producers and consumers of biofuels. If the bill is approved by the Senate later this year, this programme would boost the ethanol industry in the country. However, it's essential to ensure that biomass used in future energy systems is sustainably sourced. This means preventing upstream emissions from land-use changes, avoiding competition with food crops, protecting biodiversity, and respecting the rights of indigenous peoples in that land (Energy Transitions Commission, 2021). Furthermore, while biofuels may have reduced the emissions intensity of the road transport sector in Brazil, the potential for further reductions in emissions by biofuel blending is limited (ICCT, 2023). Instead, full decarbonisation of the transport sector will require fast uptake of electric vehicles (EVs). Brazil has not set a specific target for electric vehicles and has not joined the COP27’s Accelerating to Zero coalition (A2Z) , which states that 100% of new car and van sales in 2040 should be electric vehicles, 2035 for leading markets. According to the third yearbook on electric mobility, the sale of EVs has grown significantly in recent years. According to the latest estimates, around 2.5% of light-duty vehicles sold in 2022 were electric. The number of EVs sold in 2023 almost doubled compared to the previous year, a positive development that surpassed all projections (Audi, 2024; PNME, 2023). However, despite these positive development, there is still a long way to go. For comparison, the 1.5°C compatible share of EV sales in Brazil would need to be above 45% by 2030 (see figure below). Increasing electrification of the transport sector would also reduce Brazil’s dependency on biofuels, particularly those produced from soy, thereby reducing pressure on Brazilian land for soy farming (PNME, 2023). EV market share</t>
-  </si>
-  <si>
-    <t>Transport is the second largest source of emissions in Canada, after oil and gas, representing just under a quarter of the country’s emissions (Environment and Climate Change Canada, 2024). In its latest projections and progress reports, Canada foresees transport emissions reductions of 19% below 2005 levels by 2030 (Environment and Climate Change Canada, 2023b, 2023a). Canada is taking steps to reduce transport emissions, but not at the speed needed for such a large source of the country’s emissions. A 2022 ‘action plan’ on road transport did little more than rehash existing targets, plans and funding schemes (Transport Canada, 2022a). Electric Vehicles Targets Canada has had EV sales targets for the past several years. By 2035, 100% of new passenger car and light-duty trucks sales need to be electric vehicles, with interim targets of 20% by 2026 and 60% by 2030 (Environment and Climate Change Canada, 2022a). In December 2023, the government adopted the necessary regulations to make these targets legally binding (Government of Canada, 2023g). Plug-in hybrids (PHEVs) are included in the definition of electric vehicles but their contribution to the sales target is capped at 20% from 2028. The sales targets increase in stringency annually, though at a slower pace in earlier years. The GHG impact of the regulations grows over time, but only contributes to minor reductions by 2030 (less than 5 MtCO 2 e). In 2023, ~19% of all passenger car and truck sales were EVs, of which 8% were battery electric (Statistics Canada, 2024). Canada should easily achieve its (fairly low) 2026 interim target of 20%. The CAT has not developed EV benchmarks for Canada; however, our US benchmark suggests that Canada’s targets are not 1.5°C compatible: 95–100% of all US passenger cars and light-duty trucks sold in 2030 should be zero emission vehicles. The government aims to electrify its own light-duty vehicles LDV fleet by 2030 (Natural Resources Canada, 2022a). Medium and heavy-duty vehicles Canada has also set targets for its medium and heavy-duty vehicles (MHDVs) with the goal of achieving a 35% sales target by 2030 and 100% by 2040 for some models (Environment and Climate Change Canada, 2022a). Stakeholder consultation on the regulations to make these targets binding has begun, but the timeline for their adoption is not clear (Government of Canada, 2022g, 2023a). Infrastructure and support programmes The government began supporting the development of EV-related infrastructure and charging networks in 2016 (Natural Resources Canada, 2021b, 2021c, 2023). Canada has about 26,000 chargers at 10,000 locations across the country (Natural Resources Canada, 2024). Analysis suggests that Canada will need between 440,000-470,000 chargers in 2035 to support its 100% sales target (Dunsky Energy + Climate Advisors, 2022). The government missed an opportunity to support residential charging infrastructure by not including them in the most recent building codes, though some municipalities are taking action (Kozelj, 2024). Making buildings EV-charger-ready through minor changes at the time of construction can significantly reduce the costs when the necessary equipment is actually installed (Efficiency Canada &amp; Carleton University, 2022). Since 2019, the federal government has provided rebates for the purchase or lease of EVs and will continue to do so until March 2025 (Environment and Climate Change Canada, 2020a; Transport Canada, 2022b). In July 2022, it launched a four-year, half billion CAD programme to support the purchase of medium and heavy duty electric vehicles (Transport Canada, 2022c). Vehicle emission standards Canadian fuel economy standards for light and heavy-duty vehicles are aligned with federal-level regulations in the US (Environment and Climate Change Canada, 2020a; Government of Canada, 2021h, 2018c). The Biden administration has been working on reversing the Trump era rollbacks, adopting new rules for emissions and fuel standards (see US assessment for details). GHG standards for new trailers have been delayed for several years in response to legal challenges to those standards in the US. Fuel standards In July 2023, the Clean Fuel Regulations finally took effect, though are unlikely to have much of an impact until 2025 (Bakx, 2023; Government of Canada, 2022p). The regulations require producers and importers of gasoline and diesel to reduce the carbon intensity of their fuels from 2016 levels, with increasing annual reductions through to 2030. The regulations create a credit market for compliance, which allows those not subject to the regulations (like EV charging stations or low carbon fuel producers (e.g. biofuels)) to participate. The regulations aim to improve production processes in the oil and gas sector, foster production of low carbon fuels and enable end-use fuel switching in transport. The fuels used by remote communities, and in international shipping , and domestic and international aviation are exempt from the regulation. The renewable fuel content requirements, 2% for diesel and 5% for gasoline, as set out in the Renewable Fuels Regulations, have been incorporated in these new regulations (Government of Canada, 2010). These regulations were first proposed in 2016 as part of the Pan-Canadian Framework (Government of Canada, 2016a). Originally, standards were also supposed to be prepared for gaseous and solid fuels; however, these were delayed due to industry concerns over trade impacts and have since been shelved (Environment and Climate Change Canada, 2020a; Government of Canada, 2017). Aviation Canada lacks effective policies to address its aviation emissions, which stand at 22 MtCO 2 e in 2019. Most of these emissions are not covered by its carbon pricing system, as this pertains to interprovincial travel only, and its clean fuel regulations (see above) do not extend to jet fuel. 70% of Canada’s aviation emissions are from international flights (Government of Canada, 2022b). In 2022, Canada updated its aviation action plan (Government of Canada, 2022b). As part of the plan, the government commits to exploring ways to consistently apply carbon pricing to domestic aviation emissions. The plan charts a pathway to achieving net-zero emissions by 2050, in which a shift to Sustainable Aviation Fuel (SAF) is responsible for close to half of the needed reductions. In combination with increased efficiency in equipment and operations, this would offset the expected growth in air travel and bring emissions back to their 2005 levels (around 12 MtCO 2 e). These residual emissions would then need to be balanced by negative emissions, such as direct air capture. Around 70% of fuel used in 2050 would be SAF with a 90% reduction in lifecycle emissions compared to conventional jet fuel. Lower lifecycle emissions would increase the need for negative emissions outside the sector. Canada does not produce commercially relevant amounts of SAF currently. In 2023, the airline industry produced a SAF roadmap which is considered an integral part of the government’s aviation action plan. The roadmap charts the requirements for this nascent technology to be able to grow to 25% fuel share by 2035. The roadmap assumes around 50% lifecycle emissions savings in SAF in contrast to the 90% reduction in the aviation plan. Notably, the aviation plan’s four emission reduction measures are all targeting emission reductions per flight, rather than reducing the number of flights by making other transport modes more attractive. The plan only mentions a new highspeed rail network to connect the airports, rather than incentives to shift travel to rail connections to central stations in the major cities (Government of Canada, 2022b).</t>
-  </si>
-  <si>
-    <t>The transport sector accounted for a third of Chile’s total final energy consumption (34%) in 2021, almost the same as the industry sector, as well as a third (33%) of its total GHG emissions, considering 99% of the sector’s energy consumption is from imported fossil fuels (IEA, 2023). As with other sectors, Chile has established a number of targets to minimise emissions from the transport sector in its energy strategy (PEN). The most prominent target is that 100% of new light- and medium-duty vehicles sales must be zero emissions vehicles by 2035. In line with this target, at COP26 Chile signed the declaration on accelerating the transition to 100% EVs. However, Chile is not on progress to meet this target: its EV sales have yet to exceed 1% as of 2024. For Chile to achieve its transport electrification ambitions, it needs additional policies to support EV uptake. In December 2017, Chile published its Electromobility Strategy, which sets out a goal and action plan towards achieving a 40% share of electric passenger vehicles as well as a 100% electrified public transport fleet by 2050 (Ministerio de Energía, 2017a). Chile’s Energy Strategy (PEN, or Política Energética Nacional ), published in 2022, updated these targets and made them more ambitious, aiming for 100% zero emission vehicles in public transport and urban public transport by 2040, and 60% of private and commercial vehicles to be zero emissions by 2050 (Ministerio de Energía, 2022c). Other transport goals include a 40% reduction in direct GHG emissions from the use of fuels in the sector (including land, sea, and air transport) by 2050 compared to 2018 (20% by 2040). Chile’s Energy Route 2018–2022 set out a short-term goal of a 10-fold increase in EVs in 2022 (compared to 2017 levels). While this was overachieved by more than double, the target was relative to a very low initial EV stock in 2017 at only 231 cars (Ministerio de Energía, 2021e; IEA, 2024b). Chile is already beginning to implement actions towards achieving these targets. As of April 2024, Chile has reportedly reached over 2,500 electric buses in its public transport system, representing 38% of its total fleet (Carrara, 2024). Electric buses now represent around one-fifth of total bus sales in the country (IEA, 2024c). At the same time, the market share of EVs remains low, and decreased in past year from 0.5% to 0.3% of vehicles sold in 2023, and EVs make up only 0.1% of the total car fleet. EV sales have more than doubled, however, compared to 2019 and increased five-fold in the past six years, indicating a rapid upward trend. Public charging infrastructure is rather limited, with only 1,070 units (up from 660 in 2022) units in 2023 (compared to e.g., 51,000 in Germany) (IEA, 2024b). In addition to promoting renewables in the energy matrix, the Law on Energy Storage and Electromobility (21.505) includes measures to encourage EV uptake. The law includes temporary exemptions or reductions for driving permit fees for electric and hybrid vehicles, thus matching those of ICE vehicles, and enables battery EVs to connect to the grid and store energy (Ministerio de Energía, 2022b). Building on the Electromobility Strategy, in 2023, Chile presented its Roadmap for the Advancement of Electromobility. This plan contains concrete measures to 2026 aimed at accelerating the EV transition and addressing Chile’s current EV infrastructure gap. Its main pillars are building a robust public infrastructure charging network, promoting public transportation and decentralisation in priority regions, and improving EV education and road safety (Gobierno de Chile, 2023b). The Energy Efficiency Law also targets the transport sector. It establishes energy efficiency standards for imported vehicles, which came into effect this year, and government subsidies are offered for electric taxis and home charging points. It aims to ensure interoperability of the EV charging system, facilitates access and connection to the charging network, and allows the Ministry of Transport to establish energy efficiency standards for vehicles (Ministerio de Energía, 2021c). Building on its Green Hydrogen Strategy, the government has also presented its Sustainable Aviation Fuels 2050 Roadmap (SAF 2050). The roadmap sets out a goal of achieving 50% of SAF use in aviation by 2050 by promoting local, decentralised production of new energy sources. including biofuels and green hydrogen (Ministerio de Energía, 2024). Chile’s electromobility targets, initial implemented measures, and the 2035 ban of non-EV sales are a great step in the right direction, especially since they are integrated into new strategies and laws such as the Energy Efficiency Law and Green Hydrogen Strategy. However, additional policies, especially targeting private car ownership, are needed to meet both these targets and global decarbonisation benchmarks, which foresee having only zero emission cars on the road by 2050 to be compatible with limiting temperature to 1.5°C (Climate Action Tracker, 2016). For the development of an integral policy making framework for transport, it is of great importance to consider social and economic consequences of the different policy options. The total emissions reduction potential of transport electrification also significantly depends on the decarbonisation of the electricity supply used to charge vehicles.</t>
-  </si>
-  <si>
-    <t>China is rapidly becoming an EV, BEV and PHEV powerhouse, producing 52% of global sales, with its BYD company now overtaking Tesla as the world's best-selling company. China’s transport sector is a vast consumer of energy with the sector accounting for 14% of final energy consumption and 43% of oil consumption nationally, with petrol cars the largest consumer and source of emissions (IEA, 2023b). The government has signalled its continuing intent to accelerate the transition towards a low-carbon fleet, with sector action critical to meeting economy-wide targets of a 30% share of electricity in final energy consumption in 2025 and peak oil consumption during the 15th FYP period (2026 to 2030) (Government of China, 2021; NDRC and NEA, 2022). China’s uptake of new energy vehicles (NEVs), including battery electric vehicles (BEVs), plug-in hybrid vehicles (PHEVs), and fuel cell electric vehicles (FCEVs), started in the 1990s. The growth in NEV sales has been rapidly increasing due to subsidies dating back to 2009 and, more recently, investment boosts from pandemic recovery packages and strong national policy signals. In 2023, China's NEV production and sales grew by 35.8% and 37.9% year-on-year (Xinhua News Agency, 2024). However, the government has been aiming to decouple the growth of NEVs with direct financial incentives due to accelerating market forces and the growing government costs of the subsidies. NEV subsidies for producers ended in 2022, although tax exemptions for consumers will continue until the end of 2027 (Xinhuanet, 2023). Research suggests the market is reaching maturity, with BEVs achieving price parity with conventional cars soon, even without accounting for fuel savings (Lutsey et al. , 2021). The NEV Industry Development Plan (2021-2035) targeted NEV sales to take 20% of the market share by 2025, but the market share of NEVs has already reached 31.6% in 2023, significantly exceeding the target (Xinhua News Agency, 2024). China further targets an NEV market share target of 40% by 2030 (raised to 50% in select regions with high air pollution) (Government of China, 2021). However, this still falls short of a 1.5°C-compatible transport sector, which requires China to achieve a 100% EV sales share and a 42% EV stock share by 2030. The penetration of NEVs is finally showing a visible reduction in pollutants and emissions, as the transition towards NEVs has shaved approximately 3% off petrol demand growth, and according to Sinopec, would cause China’s petrol demand to peak in 2023 (Myllyvirta and Qin, 2023). Our previous analysis of NEV penetration scenarios in China shows limited domestic mitigation impact as even 100% BEV sales by 2035 would mean negligible GHG emission reductions if not accompanied by rapid decarbonisation of the power sector (Climate Action Tracker, 2021). Even so, China’s rapid development of industrial infrastructure supporting its EV supply chain is critical to global electric mobility transitions: in 2023, Chinese carmakers produced 32% of global EVs, with BYD overtaking Tesla as the world’s best-selling company when accounting for PHEVs as well as BEVs (IEA, 2024) To limit global temperature increase to 1.5°C, China will need to sell the last fossil fuel car by 2040 meaning a NEV market share of 100% (Climate Action Tracker, 2020a). Projections (from 2021) show China only reaching 70% by then, although this is the most rapid trajectory of any of the world’s largest emitters. The government has also been prioritising service and electrification of its public transport systems with the expansion of national high-speed rail and local electric public transport systems highly prominent in its COVID economic stimulus packages and latest FYPs. The 14th FYP for Green Transportation Development contains numerical targets to increase the growth of NEVs in urban public transport (including taxis, buses, delivery trucks, and more), while the government recently launched a pilot programme for cities to procure 80% of new public vehicles as electric from 2023-2035 (around two million vehicles) (MoT of China, 2021; Xue, 2023). Shenzhen, a city home to two pilot programmes for NEVs since 2009, became the first city in the world with an entirely electric public transport system in 2017 (including 16,000 buses and 20,000 taxis) (CGTN, 2023). For intercity transport, the government has looked to expand its massive high-speed rail network. The network consisted of about 38,000 km in 2020 (all built since 2008) and is planning to extend this by another 120,000 km by 2035 (Jones, 2022; O. Wang, 2022). By 2025, the government aims to have the network cover more than 95% of cities with a population greater than half a million (State Council of China, 2022).</t>
-  </si>
-  <si>
-    <t>Transport is the only major sector in the EU where emissions have increased over the last 30 years: emissions in 2022 followed an upward trend of 2.7% compared to 2021. It is too early to say whether emissions from the sector have peaked: the economic rebound and trend towards bigger vehicles may undermine the impact of increasing EV sales on emission levels. The EU has introduced several policies and regulations to reduce emissions from the transport sector across all transport modes. These include but are not limited to: Revised Renewable Energy Directive (EU) 2023/2413, through the adoption of sectoral renewable energy targets, Revised Regulation strengthening CO 2 emission performance standards for new cars and vans (EU) 2023/851, which established a ban on the sale of combustion engine cars by 2035. Revised Regulation on the trans-European transport Network (EU) 2024/1679 New EU ETS II which covers road transport emissions from 2027 In 2023, electric vehicle (battery electric and plug-in hybrid) made up 22% of vehicle sales. To be 1.5°C compatible in line with the Paris Agreement, the CAT finds that the EU would need to achieve 95–100% sales of light-duty electric vehicle sales by 2030 (Climate Action Tracker, 2024). This is five years earlier than the EU’s current target of 2035. The EU did not sign the Zero Emissions Vehicle pledge at COP26 and did not include this target in its NDC. In President von der Leyen’s political guidelines for the next four years in office, she hinted that the 2035 ban on the sale of internal combustion engine vehicles might be watered down through the increased use of alternative fuels to achieve the ban (Mathiesen et al., 2024). The ban on fossil fuel car sales has an exemption to allow synthetic e-fuels to continue beyond 2035. Positively, the guidelines also pushes for greater improvements to the EU’s rail network to encourage a stronger modal shift towards rail (von der Leyen, 2024b). In June 2024, the EU adopted the revised Regulation on the trans-European transport Network (TEN-T) (European Parliament &amp; European Council, 2024b). The regulation intends to create the enabling conditions to scale up zero emission transport modes, improving connecting and promoting a modal shift to more share and zero mission transport. While no new transport regulations have been adopted since the last CAT assessment in February 2024, some have been revised or are still pending agreement such as the CO 2 emission standards for heavy-duty vehicle and the Green Freight Package. Gaps still remain for some regulations. For example, the FuelEU Maritime Regulation (EU) 2023/1805 (European Parliament &amp; Council of the European Union, 2023c) and the Alternative Fuel Infrastructure Regulation (EU) 2023/1804 (European Parliament &amp; European Council, 2023) consider LNG a “low carbon fuel” in shipping. As LNG is a fossil fuel, its prolonged or expanded use will make it difficult to achieve future emission reductions given the long lifetime of ships and infrastructure, resulting in stranded assets. To reach full decarbonisation in the transport sector globally by mid-century, the EU would need to increase the share of zero emission fuels (electricity, hydrogen and biofuels) from 7% in 2019 to 55% by 2030. This covers all modes of domestic transport collectively (i.e. road, rail, domestic aviation and maritime travel) (Climate Action Tracker, 2024). Tariffs on Chinese EVs In October 2024, the EU Commission announced new tariffs on battery EVs manufactured in China on the basis that the Chinese government unfairly subsidies its EVs, undercutting European car manufacturers. Individual duties will range between 17.4% to 37.6% depending on the Chinese manufacturer (European Commission, 2024e). To be 1.5°C compatible, the EU needs continued exponential growth in EV sales, needs a lot of them to meet demand, and needs to make it affordable for consumers (Climate Action Tracker, 2024). One of the major barriers to this is affordability. Chinese EV models sold across EU member states are typically cheaper than European manufactured vehicles, which could affect consumer choices.</t>
-  </si>
-  <si>
-    <t>The transport sector is the largest source of emissions in the UK, representing 29% of emissions in 2023 (DESNZ, 2024b). Central to decarbonising transport is ending the sale of fossil fuel cars and vans by 2030 and fossil fuelled heavy goods vehicles (HGVs) by 2035–40 (Department for Transport, 2021). The policy context that the new UK government has inherited is mixed. On the one hand, the previous government confirmed the zero emissions vehicle (ZEV) mandate in 2023, which sets minimum EV sales targets for each vehicle manufacturer and will be a key delivery mechanism in scaling up EV sales (UK Government, 2023b). At the same time, the government pushed back the date of the sales ban on internal combustion engine cars from 2030 to 2035, sending a very mixed signal to the public and automotive industry. In 2023, the share of electric car sales in the UK failed to grow, flatlining at 16.5% and falling off track for the UK’s transition for the first time (SMMT, 2024). The share of electric van sales is growing much more slowly and is significantly off-track (CCC, 2024). Key actions for the new government should include: Reinstating the 2030 ban on petrol and diesel vehicle sales Taking action to help accelerate EV rollout . This should include removing barriers for the installation of EV chargers and working with major van fleet operators to understand barriers to EV uptake. Aviation In 2022, the UK released its Jet Zero Strategy which aims to reduce emissions from this sector to net zero (Department for Transport, 2022). This aims for domestic aviation to reach net zero emissions by 2040, and total aviation emissions to reach net zero by 2050. However, in this context, net zero does not mean eliminating the negative climate impacts of aviation, but rather allowing for a large-scale growth in emissions that would be compensated for via the UK emissions trading scheme, CORSIA and other offsetting mechanisms outside the aviation sector. The strategy also ignores the non-CO 2 impact of aviation, which represents up to two-thirds of the sector’s overall climate impact (Lee et al., 2021). The UK’s current strategy relies heavily on speculative technological innovation and carbon dioxide removal to enable a ‘net zero’ aviation sector, without addressing the elephant in the room – demand. The previous government committed that sustainable aviation fuel (SAF) would provide 10% of overall fuel use by 2030, rising to 22% by 2040 (UK Department for Transport, 2024). This is five times the level included in the CCC’s Balanced Net Zero Pathway and would require an unprecedented scale-up of SAF production. The new government confirmed this commitment, and introduced a SAF mandate to drive this uptake (Department for Transport, 2024). There will also be a revenue certainty mechanism to provide confidence to investors seeking to build SAF plants to meet UK demand. However, SAF deployment remains very low globally and has consistently failed to meet expectations (Rutherford, 2022). Relying so heavily on this option therefore represents a major delivery risk. The Jet Zero strategy also fails to address demand. The Government states that “the sector can achieve Jet Zero without the government needing to intervene directly to limit aviation growth” (Department for Transport, 2022), and envisages that passenger numbers could rise 70% from 2021 to 2050. This is in contrast to the CCC’s advice, which was that no net expansion in airport capacity should be permitted, and passenger growth should be 25% at most (CCC, 2020). Numerous airports are currently planning expansions or have received approval to expand in the past two years (AEF, 2022) which again could threaten the UK’s ability to achieve its climate targets. As yet, the new government has not provided any clear commitments that it will curb aviation demand, with the chancellor repeatedly mentioning aviation as a key engine of economic growth (Topham, 2024). As a result, in 2050, the Jet Zero strategy expects that aviation will still be emitting around 19 MtCO 2 per year, which will need to be compensated for by CO 2 removal. Given the very limited potential for CO 2 removal and uncertainties in the climate system, CO 2 removal should be reserved to hedge against climate uncertainties and balance out truly hard-to-abate residual emissions (e.g. from agriculture), rather than to facilitate a stark increase in aviation emissions in one of the world’s wealthiest countries. For more information on the need to align aviation and shipping emissions with the Paris Agreement, see the sectoral pages on international aviation and international shipping .</t>
-  </si>
-  <si>
-    <t>The transport sector accounted for 29% of total final energy consumption in 2022 (IEA, 2024). The sector is primarily individual, road-based transport but the Kingdom has sought to expand its public transportation network in recent years. The King Abdulaziz Public Transport project is a major initiative to modernise transportation in the city of Riyadh. The capital is set to become the second city in Saudi Arabia with a metro network after the Makkah metro opened in 2010 (Saudi Gazette, 2020). Following a delay, the Riyadh metro system is set to open to passengers at the end of 2024 (Railway Technology, 2023; The M Metro Rail Guy, 2024). The Saudi government has also taken steps to invest in rail transport; however, it remains unclear whether the new networks will be electric or diesel-powered. In 2010, it launched the Saudi Railway Master Plan, aiming to construct a 9,900-km network by 2040 (Oxford Business Group, 2020). The first phase, running until 2025, includes constructing and upgrading 5,500 km of tracks for freight and passenger transport, including interlinkages to the wider Gulf Cooperation Council (GCC) railway network. The light rail network in the smart city NEOM is complete as of 2024 (Godfrey, 2024). Electric vehicles Saudi Arabia has taken steps to develop its own electric vehicle (EV) industry. As part of its “Vision 2030” strategy, the government aims to produce 50,000 EVs annually by 2030 and for 30% of Riyadh’s vehicles to be electric by 2030 (Kingdom of Saudi Arabia, 2021c). In 2022, Saudi Arabia introduced its first domestic brand of EV called Ceer, through a joint venture between PIF and Taiwanese car manufacturer Foxxconn (Al Arabiya News, 2023a). Manufacturing facilities for Ceer vehicles are under construction and expected to be operational by 2025 (Al Jazeera, 2023). Additionally, in June 2023, Saudi Arabia signed a USD 6 bn deal with Chinese EV manufacturer Human Horizons to collaborate on the development, manufacture, and sale of electric vehicles (Reuters, 2023). To further promote the use of EVs, by 2024 the government had built 2,800 EV charging points,, with plans to set up 30,000 new stations by 2030 (Mobility Foresights, 2024). Despite the progress made, achieving Saudi Arabia’s 2030 EV target will be challenging. The government will need to accelerate the deployment of charging infrastructure and introduce incentives to promote greater EV adoption (Apricum, 2022).</t>
-  </si>
-  <si>
-    <t>Singapore’s transport sector made up 14.2% of total emissions in 2021 (National Climate Change Secretariat, 2024b). Singapore aims to develop a greener and more sustainable land transport sector, reducing peak land transport emissions by 80%, by or around mid-century. The sector’s energy demand and associated emissions are expected to flatten out as a result of measures to promote public transport, modal shifts, and improve the emissions intensity of road transport. The government estimates that implemented measures reduced emissions by 1.67 MtCO 2 e in 2020 (National Environment Agency, 2022). Singapore aims to phase out Internal Combustion Engine (ICE) vehicles by 2040 (National Environment Agency, 2022). However, to be compatible with the 1.5°C long-term temperature goal, the last fossil fuel car should be sold in 2035 at the latest (Climate Action Tracker, 2016). The Vehicle Emissions Scheme (VES) was introduced in 2018, replacing the Carbon Emissions-based Vehicle Scheme (CEVS), which provided rebates for low-emission cars and imposed surcharges on high-emission cars. The VES expanded the range of pollutants covered to include hydrocarbons (HC), carbon monoxide (CO), nitrogen oxides (NO X ), and particulate matter (PM) (National Environment Agency, 2022). Fuel economy labels have been redesigned to include information on each vehicle’s VES band. To further promote the adoption of cleaner vehicles, the VES was enhanced with increased rebates and higher surcharges from January 2021. Starting from 2021 all new and used petrol or diesel vehicles must comply with the Euro VI emission standards (National Environment Agency, 2022). The Singapore Green Plan 2030 includes a strong push to electrify the vehicle fleet, which would help Singapore achieve its vision of 100% cleaner energy vehicles by 2040 (Land Transport Authority, 2021). Singapore has introduced tax incentives to lower the upfront and running costs of electric vehicles (EVs) such as the Electric Vehicle Early Adoption Incentive (EEAI) (National Environment Agency, 2022). As of 2023, less than 2% of the vehicle population were fully electric or plug-in hybrid electric vehicles (PHEVs) (Land Transport Authority, 2023). Under the new VES standards, CO 2 emissions produced by electricity generation from fossil fuels are accounted for by applying an emissions factor to the electricity consumption of EVs and PHEVs (National Climate Change Secretariat, 2018b). Since February 2018, the growth of private vehicles has been effectively capped, when the permissible growth rate of private vehicle population was reduced from 0.25% to 0% (National Environment Agency, 2018). Prospective vehicle owners must bid and pay for a Certificate of Entitlement which allows them to purchase a vehicle and use it for 10 years (National Environment Agency, 2022). Singapore is encouraging active transport and modal shift in its Land Transport Master Plan (LTMP) 2040 by developing infrastructure, creating more urban space for walking and cycling, and expanding the MRT system (Singapore’s metro). The Land Transport Authority (LTA) announced SGD 1bn in funding over the next decade to support Walk, Cycle, Ride journeys. By 2030, it aims to extend the country’s cycling path network to more than 1000 km, compared to 460 km in 2020 (National Environment Agency, 2022). As of 2019, there were cycling networks in nine out of 24 public housing towns and 200 km of sheltered walkways(National Environment Agency, 2018). Singapore plans to increase the length of the rail network from 245 km in 2022 to about 360 km in the early 2030s so that eight in ten households will be within a ten-minute walk of a train station. Singapore is targeting a mass public transport modal share of 75% during the morning and evening peak hours by 2030 (National Environment Agency, 2022). The Land Transport Master Plan sets a goal for all public buses and taxis to run on cleaner energy sources by 2040 (Republic of Singapore, 2019), and the Land Transport Authority (LTA) aims to have half of its public bus fleet be electric by 2030 (Land Transport Guru, 2022). In 2016, Singapore trialled e-buses, and by 2018, 60 trial e-buses were on the roads (Republic of Singapore, 2019). Around 700 electric taxis have been rolled out by the private taxi operators (The Straits Times, 2021, 2022b). We exclude emissions from marine and aviation bunkers when assessing Singapore’s NDC target and current policies. These emissions are more than three times higher than the rest of Singapore's emissions—with the vast majority being related to Singapore’s role as a hub in international shipping (National Environment Agency, 2022).</t>
-  </si>
-  <si>
-    <t>The Department of Transport published the country’s first Green Transport Strategy (GTS) 2018–2050 in 2018 (Department of Transport South Africa, 2018), proposing a list of measures that should be implemented to transition the sector to a low carbon future. Analysis by the Climate Action Tracker indicates that the share of zero emissions fuels (biofuels, electricity and hydrogen) of the total domestic transport sector demand would need to increase to 20% by 2030, 50-60% by 2040, and 80%-90% by 2050 to be compatible with the Paris Agreement. South Africa’s automotive industry contributed to over 4% of GDP in 2021 and is one of the country’s largest manufacturing sectors (NAAMSA, 2023). In 2013, the government adopted South Africa’s Electric Vehicle Industry Roadmap to introduce electric passenger vehicles (EVs) (South African Government, 2013). Three years after the adoption of the roadmap, the first EV was manufactured in South Africa with the production of plug-in hybrids (PHEVs) at Mercedes-Benz’s East London plant (Venter, 2023). Since then, Toyota has also begun manufacturing PHEVs with Ford also announcing it will manufacture PHEVs in South Africa (Agbetiloye, 2023; Venter, 2021). While some progress has been made, the industry is still dominated by fossil fuel-vehicles. This creates an existential challenge for the auto industry as South Africa’s main export destinations, such as the UK and EU, shift towards EVs (NAAMSA, 2023). On the demand-side, the total number of EVs vehicles sold in South Africa remains marginal.. In the first four months of 2023, the sale of battery EVs doubled compared to the previous year, though remained just 0.16% of new vehicle sales (Kuhudzai, 2023a). In the same time period, the sale of plug-in hybrids declined over 20%, though these make up a smaller share than battery EVs. In May 2021, the Government of South Africa released the ‘Auto Green Paper’ for public consultation (Department of Trade Industry &amp; Competition, 2021). The strategy aims to define South Africa’s framework for a comprehensive and long-term automotive industry transformation plan on low-carbon vehicles. No final policy proposal had been approved by Cabinet, as of September 2023. Analysis by the Climate Action Tracker shows that the electric vehicle share in annual vehicle sales in South Africa would need to increase to 50-95% by 2030 and 90-100% by 2040 to be compatible with the Paris Agreement. Bus Rapid Transit Systems (BRT) have initiated the main switch in modal share of passenger transport in urban areas. These have commenced operation or are currently under consideration in public transportation planning in several South African urban areas (Department of Transport, 2017). Initiatives to implement and expand BRT systems are currently taking place in eight cities and municipalities including Cape Town and Johannesburg. However, BRT still faces challenges such as competition with minibus taxis and overreliance on foreign service plans less suitable for South African cities (Hook &amp; Weinstock, 2021).</t>
-  </si>
-  <si>
-    <t>Emissions from the transport sector were responsible for 33% of Switzerland’s total GHG emissions in 2022, almost exclusively from road transport (Bundesamt für Umwelt BAFU, 2024b). Since peaking in 2008, transport emissions have steadily been decreasing and in 2020 they fell below 1990 levels for the first time since 1996, primarily due to lower car travel during the COVID-19 pandemic. Emissions only slightly rebounded in 2021 and even slightly decreased again in 2022, remaining at 7% below 1990 levels. With the adoption of the Climate Protection Act in 2023, Switzerland now has reduction targets for the transport sector to reduce emissions by 57% by 2040 and by 100% by 2050 (below 1990 levels) (Bundesgesetz Über Die Ziele Im Klimaschutz, Die Innovation Und Die Stärkung Der Energiesicherheit (KlG), 2023). Given the very low emissions intensity of Switzerland’s power sector, a shift to electric mobility has an even higher impact on overall emission reductions. In 2023, 30% of all new passenger cars sold in Switzerland were electrically chargeable vehicles, which includes battery-only (21%) and plug-in hybrid (9%) vehicles (European Alternative Fuels Observatory, 2024a). Although the uptake of electric vehicles is accelerating, the share of new sales in Switzerland remains significantly below that of some countries with a comparable level of income (e.g. 60% in Sweden, 55% in Finland, 90% in Norway in 2023), but it is moving faster than the EU27 average, which in 2023 was 23% (European Alternative Fuels Observatory, 2024b). The target of 15% battery electric vehicle sales in 2022, outlined in the Roadmap for Electric Mobility 2022, was met a year early leading to the creation a new Roadmap for Electric Mobility 2025, with 2025 targets of EV market sales shares of 50% and of 20,000 charging stations. Although the EV uptake is expected to take an exponential trajectory to achieve 50%, sales need to more than double within two years (Schweizerische Eidgenossenschaft, 2023)(Bundesamt für Strassen ASTRA, 2023). While still predominantly on road, the share of freight transported by rail – which is electrified to 99.8% in Switzerland – is slowly growing again and reached 38% in 2022. This is higher than even the EU target for 2030, which is 30% and the current EU average was 18% in 2021 (Bundesamt für Strassen BFS, 2023). The inclusion of domestic and international aviation between Switzerland and member states of the European Economic Area (EEA) into Switzerland’s ETS since 1 January 2020 is a significant policy development, with emissions from the sector in the scheme to be capped at 2018 levels (Schweizerische Eidgenossenschaft, 2020c). In addition, from 2020 for new designs, and from 2023 for in-production models, aircraft in Switzerland will be subject to CO 2 emission reduction targets. Switzerland also participates in the carbon offsetting and reduction scheme for international civil aviation (CORSIA), under which emissions are capped at 2019 levels. Despite becoming more stringent in 2024, this scheme has significant shortcomings, meaning it is unlikely to deliver the substantial reductions needed to achieve the ICAO’s aspirational goal of carbon neutral growth from 2020. Within the framework of the new CO 2 Succession Act, the introduction of a sustainable aviation fuel blending mandate is planned, in coordination with the EU’s ReFuel programme from 2025 and it also includes instruments to support the conversion of diesel-powered buses and ships to fossil free alternatives. The CO 2 Succession Act further introduces quantitative emissions reduction targets for the period after 2025 aligned with those of the EU. It also introduces a new penalty for exceedance of emissions limits at CHF 95 to CHF 152 (USD 119 to USD 176) for each gram of CO 2 /km exceeding the individual target (Bundesgesetz Über Die Reduktion Der CO 2 -Emissionen (CO 2 -Gesetz), 2024).</t>
-  </si>
-  <si>
-    <t>Transport emissions account for around 16% of Türkiye’s GHG emissions (excl. LULUCF), or 91 MtCO 2 e (Republic of Türkiye Ministry of Energy and Natural Resources, 2023). The largest share of emissions comes from road transportation, which more than tripled between 1990 and 2021 (Republic of Türkiye Ministry of Energy and Natural Resources, 2023). In line with increasing road transport emissions, the number of vehicles on Turkish roads has almost tripled since 1990 (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024a). Nevertheless, there are 161 motor vehicles per 1000 inhabitants in Türkiye, which is far less than in developed countries (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2024a). In the EU, for instance, this figure is 560 per 1000 inhabitants (Eurostat, 2024). Turkish transport policy is therefore at a crossroads. As the economy continues to grow, so too will vehicle ownership. Putting in place incentives and infrastructure designed to increase electric vehicle (EV) uptake will allow Türkiye to expand vehicle ownership sustainably. Türkiye aims to place EVs at the heart of industrial policy through the manufacturing of its first domestically produced EV, the Togg (Republic of Türkiye Ministry of Industry and Technology, 2022). Türkiye adopted the COP26 declaration on accelerating the transition to 100% zero emission cars and vans, but has not introduced policy at national level with a firm commitment to expanding the market share of zero emission vehicles to 100% by 2040. However, Türkiye does aim to increase the market share of EVs to 35% by 2030 (Republic of Türkiye Ministry of Industry and Technology, 2022). Its domestic EV production gives it an advantage in terms of meeting the goals of the COP26 declaration, and Togg sales have already driven a substantial increase in EV sales in Türkiye (Kasapovic &amp; Knowles, 2024). A stronger target in line with its COP26 commitment can allow Türkiye to achieve 100% zero emission sales by 2040. Rolling out EV infrastructure is critical to supporting their uptake. The government aims to establish a fast-charging network by providing grant support to private sector actors (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2023), as well as supporting drivers’ access to public charging stations at a regulated price (Kaya, 2022). However, EV infrastructure is not being rolled out fast enough. There are 12.5 EVs per charging point. In contrast, there are 3-to-1 in the Netherlands and Belgium, and 5-to-6 in Italy (Hürriyet Daily News, 2024). A modal shift towards rail will form an important aspect of reducing emissions in line with 1.5°C. Türkiye aims to increase the share of freight transport by rail to 20.12% by 2035 and the share of passenger transport by rail to 5.31% by 2035, up from 2019 levels of 0.89% and 3.13%, respectively (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2023). Ongoing measures to achieve this include significant investments in modernising its rolling stock and constructing new lines between major cities (Railway Gazette International, 2024; Railway Supply, 2024). Türkiye also aims to become producer of high-speed electric trains which it can use domestically as well as export. Similar to the Togg, Türkiye sees domestic manufacturing of electric trains as a way to blend industrial policy with environmental goals.</t>
-  </si>
-  <si>
-    <t>The transport sector accounted for ~19% of the UAE’s emissions in 2019. The UAE’s 2023 NDC update sets a target to reduce transport emissions by 1% below 2019 levels by 2030. Emissions from the transport sector are expected to be ~42 MtCO 2 e in 2030 under this target, and to reach zero emissions by 2050 (Government of the UAE, 2023a). The UAE has set out some policies to manage transport emissions, including an increase in the fuel and emissions efficiency of its vehicle fleet, as well incentives for the use of public transport, and the uptake of EVs. The revised Energy Strategy 2050 includes new targets for the uptake of EVs, including reaching 691,100 EVs and hybrid vehicles by 2030 and over three million by 2050 as well as increasing the number of EV chargers to 879 by 2030 and 30k by 2050. The emirates of Abu Dhabi and Dubai have also set out a series of urban transport policies, aimed among others at incentivising the uptake of public transport and EVs (Government of the UAE, 2021). For example, in May 2022 the Abu Dhabi government set out a new EV charging station policy, defining standards and requirements in anticipation of growing demand for EVs. In Dubai, the Green Mobility Strategy 2030 includes a target to reach 30% EVs and hybrids in the government vehicle fleet by 2030 (Government of the UAE, 2022). In its LTS, the UAE lists additional policies it proposes to reach its target for the transport sector towards 2050. The key pillars of the UAE’s transport decarbonisation plan are to reduce transportation needs, decarbonise passenger transport, freight transport, and mechanical vehicles (Government of the UAE, 2024b). The first pillar will include the development of mixed-use buildings, improved infrastructure for cycling and walking, incentives for carpooling and increased use of public transport and rail. In total this will contribute 14% of the reductions needed to achieve the UAE’s target. The second pillar includes incentives for the uptake of EVs, the electrification of buses, taxis and motorcycles. In total this will contribute 22% of the emission reductions needed. The decarbonisation of freight transport includes a shift towards more rail use as well as the electrification of heavy-duty trucks. These measures are expected to contribute 27% of the reductions needed. Finally, the electrification of mechanical vehicles is expected to contribute 28% of the reductions (Government of the UAE, 2024b). Additionally, the UAE has set out plans to decarbonise its domestic maritime and aviation sectors, including electrification and use of sustainable fuels.</t>
-  </si>
-  <si>
-    <t>In 2022, the transport sector accounted for 28.5% of total US GHG emissions and, since 2017, has been the largest contributor. Total sector emissions increased by 19.4% between 1990 and 2022 due to increased motorised transport demand: during the same period, the average number of vehicle miles travelled (VMT) per passenger cars and light-duty trucks increased by 46.7%. Road transport is responsible for the vast majority of transport sector emissions in the US: light, medium, and heavy-duty trucks and passenger cars accounted for 79.8% of total sectoral emissions in 2022 (U.S. Environmental Protection Agency, 2024g). The 2021 Bipartisan Infrastructure Law (BIL) includes several components to decarbonise the transport sector, such as investments to improve roads, modernise public transit, and boost the electric vehicle (EV) market (U.S. Senate, 2021). The BIL includes measures to develop EV charging stations (USD 7.5 bn), strengthen the country’s EV battery supply chain (USD 7bn), update and upgrade public transportation (USD 39bn), build out ‘climate-friendly’ passenger and freight railways (USD 66bn), and invest in roads, bridges and other transportation infrastructure projects (USD 110bn), as well as in clean busses and ferries (USD 7.5bn). The Inflation Reduction Act (IRA), alongside significant investments in electrifying light- and heavy-duty vehicles (see below), provides considerable financial support for EV manufacturing and supply chains: the IRA sets aside USD 2bn for the Domestic Manufacturing Conversion Grant Program, which funds the re-tooling of production lines for EVs. The act allocates another USD 3bn for the Advanced Technology Vehicle Manufacturing Loan Program, which has expanded coverage to heavy-duty vehicles, locomotives, maritime vessels, and planes. As a result, plans for 163 new battery and 117 EV manufacturing plants have been announced. If fully realised, these plants would create over 170,000 new jobs in battery and EV manufacturing and account for over 60% of all new jobs created by the IRA (Climate Power, 2024b). By 2030, if all planned manufacturing plants are operationalised, domestic battery manufacturing capacity is estimated to increase by nearly 20 times to approximately 1000 GWh/year relative to 55 GWh/year in 2021 (U.S. Office of Energy Efficiency &amp; Renewable Energy, 2023). The IRA also extends the Advanced Manufacturing Production Credit to spur the domestic production and sale of clean energy components, including certain EV-relevant battery components and critical minerals (The White House, 2023b). Through these measures, the IRA is expected to reduce transport sector emissions by 15%–35% by 2035 relative to 2005 (U.S. Environmental Protection Agency, 2023c). In combination with existing policies and the BIL, the IRA is estimated to reduce overall GHG emissions by 1,150 MtCO 2 e in 2030 in comparison to business-as-usual scenarios; the result is that GHG emissions are forecasted to be 40% lower in 2030 than in 2005 (U.S. Department of Energy, 2022e). In January 2023, the Biden Administration released its National Blueprint for Transportation Decarbonisation to support the 2050 economy-wide net zero target and the 2050 target of 80%–100% emissions reductions in the transport sector. The blueprint's three key strategies align with the Avoid, Shift, and Improve (ASI) framework: the strategy supports community design and land-use planning, expands access to more efficient public and private transport, and facilitates the transition to zero emission vehicles and fuels (U.S. Department of Energy et al., 2023). Passenger transport The modal split for passenger transport has been and continues to be dominated by road transport. In 2022, nearly 70% of all commutes were undertaken by single-occupancy vehicles, while only approximately 9% of commuters carpooled. The share of single-occupancy vehicle commutes decreased by over 10% between 2018 to 2022. During the same period, and likely attributable to the COVID-19 pandemic, the share of the population working from home increased by nearly 10%. In 2022, approximately 6% of commuters used public transport and engaged active mobility (U.S. Bureau of Transportation Statistics, 2022). In March 2024, the US Environmental Protection Agency (EPA) revised its Multi-Pollutant Emissions Standards for passenger cars, light-duty trucks, and medium-duty vehicles. The standards, which will phase in from 2027 through 2032, set fleet-wide CO 2 emissions targets for auto manufacturers. For light-duty vehicles, the fleet-wide average target is 170 CO 2 grams/mile in 2027. By 2032, the average target for light-duty fleets will be reduced to 85 CO 2 grams/mile (U.S. Environmental Protection Agency, 2024i). To meet the 2032 target, the EPA estimates that battery electric vehicles will account for 30–56% of automaker's fleets to meet the average emissions target (U.S. Environmental Protection Agency, 2024j). The resulting emissions reductions are approximated to total 7.2bn tons of CO 2 through 2055 (U.S. Environmental Protection Agency, 2024b). The efforts are somewhat undermined by the fact that medium-duty vehicles—a vehicle segment that includes vans and pickup trucks and represented nearly 20% of the total US light- and medium-duty vehicle fleet in 2021—are subject to a different, less demanding set of emission standards (U.S. Environmental Protection Agency, 2022a). Although the updated standards are the most stringent in US history, the standards are less ambitious than equivalent regulations in the EU and the UK, where the emissions target for 2035 is 0 CO 2 grams/mile for new light-duty vehicles (The International Council on Clean Transportation, 2024). The relative weakness of the US standards may be partially attributable to lobbying efforts from auto manufacturers. The EPA initially proposed more ambitious fleet-wide average targets between 2027 and 2032, but the auto lobby, spearheaded by Toyota's push for more flexibility in achieving the emissions targets, successfully watered down the standards (Tabuchi, 2024). In doing so, auto manufacturers can continue to fulfil their emission reduction targets with ICE-based vehicles, which prolongs the production and profitability of fossil fuel-powered vehicles and obstructs a faster transition towards a decarbonised transport sector. At the state level, stricter, more ambitious EV policy has been implemented. California established a 100% EV sales target for 2035 through its Advanced Clean Cars II regulation in 2023. This regulation has been duplicated and adopted by twelve other states and the District of Columbia (D.C.) (California Air Resources Board, 2024). As a result, over one-third of all light-duty vehicle (LDV) sales in the US are subject to the 2035 100% EV sales target (IEA, 2024b). The combined sales of hybrid, plug-in hybrid, and battery electric vehicles made up 16.3% of all new LDV sales in the US in 2023. Battery electric vehicles accounted for approximately 7% of new car sales in the US in 2023; BEV sales reached a record of 1.1 million in 2023 (U.S. Energy Information Administration, 2024a). The growth in BEV sales is the result of a larger selection and significant price cuts in vehicles: in 2023, 20 new BEV models were introduced, while the average transaction price for BEVs decreased by over 17% between December 2022 and December 2023. In the first quarter of 2024, the gap in average transaction price between BEVs and ICE-based vehicles decreased to a record low of USD 7,000 before any purchase incentives are applied (Doll, 2024; Kelley Blue Book, 2023; U.S. Energy Information Administration, 2024a). This means that, once government incentives are applied, certain BEVs are as or more affordable than their ICE counterparts. Beyond increases in availability and affordability, growing consumer interest and IRA incentives continue to further augmented uptake (Inside EVs, 2023). To reduce emissions from road transport, the government set a goal for 50% of all new vehicles sold in 2030 be battery electric, plug-in hybrid, or fuel cell vehicles (The White House, 2021d). However, this 50% target is not aligned with the Paris Agreement. To be compatible with the PA, research suggests that 95–100% of sales of new LDVs in the US should be zero-emissions by 2030 (Climate Action Tracker, 2020). Even with IRA support, the US government estimates that LDV EV sales will only reach a median of 36% in 2030 (with a range of 15%–54%) (U.S. Environmental Protection Agency, 2023c), which is insufficient to meet the Biden Administration's goal, let alone to meet the 1.5°C compatible benchmark (U.S. Energy Information Administration, 2023a; U.S. Environmental Protection Agency, 2023c). It is important to note that estimates for EV uptake vary substantially. The International Energy Agency’s (IEA) Global EV Outlook 2023 estimates that the US will achieve the EV sales target of 50% by 2030 under the STEPS scenario and the International Council on Clean Transportation anticipates the LDV EV sales share will reach 48%–61% in 2030 (U.S. Environmental Protection Agency, 2023c). At the same time, recent US Energy Information Agency (EIA) calculations only project 13–29% EV sales in 2050 (IEA, 2023a; U.S. Energy Information Administration, 2023i). The US did not sign the 100% EVs declaration at COP26. Signatories agreed that 100% of new car and van sales in 2040 should be electric vehicles (Race to Zero, 2021). Despite the absence of the federal government’s signature, many US subnational and non-state actors, including states, cities, and automakers, signed the declaration (UK COP 26 Presidency, 2021a). In March 2024, the Biden Administration, building on the set of tariffs imposed by the Trump Administration in 2018, increased tariffs on a range of decarbonisation-relevant products and technologies from China. Tariffs on Chinese electric vehicles increased the most: the border tax on EVs will quadruple from 25% to 100% of the import value (Tankersley &amp; Rappeport, 2024). Although politically significant, research indicates that economic impacts will likely be limited (Sherman, 2024). In September 2024, the Biden Adminsitration, citing national security concerns, proposed a ban on all Chinese connected car hardware and software (Shepardson et al., 2024). If finalised, Chinese software would be banned starting in 2026, while hardware would be prohibited beginning in 2030. The IRA accelerates the uptake of electric light-duty vehicles by extending and expanding tax credits for both new and used EVs. From 2023 through 2032, the Clean Vehicle Credit provides up to USD 7,500 for new battery electric, plug-in hybrid and fuel cell EVs that retail under USD 80,000 for vans, SUVs, and pickup trucks and USD 55,000 for all other types of vehicles. To qualify for the full credit, the vehicle and its critical mineral and battery components must meet certain requirements for assembly in and sourcing from North America or trusted trade partners (U.S. Internal Revenue Service, 2024a). The result of the sourcing and manufacturing requirements is that only 22 EV models qualified for the total tax credit out of the 104 EV models for sale in May 2024 (Lambert, 2024). Beyond targeting new EV sales, the US government seeks to leverage the maturing used electric vehicle market, which was made up of approximately 400,000 EVs in 2023 (IEA, 2024b): the Used Clean Vehicles Credit provides up to USD 4,000 to buyers who purchase a used electric vehicle for USD 25,000 or less (U.S. Internal Revenue Service, 2024c). Both the credits for new and used EVs are capped at different income levels to increase the affordability of and access to EVs for individuals and households with lower to middle incomes. Buyers of used EVs can also claim the credit at the time of purchase, which more immediately reduces the purchasing or monthly financing cost. As high costs remain a crucial barrier to EV adoption, reducing costs, particularly for buyers with lower incomes, accelerates and supports a just transition to EVs (Pamidimukkala et al., 2023). The government is on track to achieve its 2030 target for 500,000 publicly accessible recharging points in 2026 (The White House, 2024a). The number of publicly accessible recharging points increased by over 70% to 170,000 stations since 2021 (U.S. Joint Office of Energy and Transportation, 2024).(U.S. Environmental Protection Agency, 2023i) Freight transport Freight transport emissions account for an increasing share of total transport emissions in the US: the share of emissions from freight transport increased from 24% in 1990 to 32% in 2021 (K. Kennedy, 2023). Trucking accounted for 65% of all freight moved by weight and made up roughly 83% of total freight transport emissions in 2021 (U.S. Environmental Protection Agency, 2024f). To mitigate emissions from trucking, the government revised emissions standards for heavy-duty vehicles in 2024 (see below). Shifting freight transport to rail, which only emitted 5.7% of total sectoral emissions in 2021 (U.S. Bureau of Transportation Statistics, 2023) and accounted for the greatest share of long-distance freight volumes across all modes of freight transport, has significant emissions reductions potential (Association of American Railroads, 2021). In March 2024, the EPA adopted an updated set of vehicle emissions standards for heavy-duty trucks, transit, and vocational vehicles. The Greenhouse Gas Emissions Standards for Heavy-Duty Vehicles Phase 3 strengths the existing emissions standards: heavy-duty vocational vehicles need to reduce emissions by up to 60% more under the Phase 3 standards relative to Phase 2. The revised standards will effect HDVs starting in 2027 through 2032. Between 2027 and 2055, the standards are expected to mitigate approximately 1bn tons of CO 2 emissions (U.S. Environmental Protection Agency, 2024e). In comparison, the EU, which also revised its heavy-duty vehicle emissions standards in 2024, sets a more ambitious emissions reductions target for all new HDVs for 2030, which will escalate to a 90% target for 2040. As a first step to mainstream reductions in freight transport emissions, the Biden Administration established a national goal to transition towards a zero-emissions freight sector in April 2024. Although the administration has not indicated an explicit timeline for the zero-emissions target, separate action plans for decarbonising truck, rail, aviation, and marine freight transport are to be developed. Since its adoption in 2022, the IRA has spurred investments and introduced provisions to reduce GHG emissions from heavy-duty transport. Through the IRA, the EPA launched the Clean Heavy-Duty Vehicle Program, which was revised in 2024, to provide USD 1bn in grants to states, municipalities, and Tribes to offset the costs of replacing heavy-duty vehicles with zero-emissions alternatives and installing related infrastructure; at least USD 400m of the total funding will be channelled towards communities suffering from severe air pollution (U.S. Environmental Protection Agency, 2024d). The programme's first funding round of over USD 900m opened in April 2024 (U.S. Environmental Protection Agency, 2024c). The EPA estimates that 70% of the programmes funding will go towards replacing ICE-based school buses (U.S. Environmental Protection Agency, 2024a). An additional USD 3bn is allocated to provide grants to local governments, port authorities, and other relevant actors to purchase and install zero-emission port equipment and technology (The White House, 2023b). The IRA has also introduced the Commercial Clean Vehicles Credit, which defers 30% of the costs of replacing diesel or gas-powered commercial vehicles—ranging from cars to long-haul trucks —with electric vehicles. A credit of up to 15% is also available when replacing a vehicle with a partially electric alternative. The IRA also allocates USD 3bn for electrifying the United States Postal Service fleet (The White House, 2023b). Beyond providing tax credits for buyers, the government is partnering with truck manufacturers to further develop heavy-duty EV technologies. Through the 21st Century Truck Partnership, the Supertruck 3 programme, and the Million Mile Fuel Cell Truck consortium, the US Department of Energy (DOE) is supporting the research and development of next generation of heavy-duty batteries and fuel cells (U.S. Department of Energy, 2022a). The government is also funding commercial EV demonstration projects. In 2023, the DOE awarded over USD 7m to seven projects that will develop a medium- and heavy-duty recharging station corridor across 23 states. In 2024, the government announced that the DOE would fund the research and development of load management strategies to alleviate recharging-related grid capacity challenges. Federal government support for commercial EV uptake has been supplemented by state action. New York and California provide additional purchase incentives of over USD 100,000 on top of the IRA’s mechanism. In response, adoption of heavy-duty EVs seems to be increasing: delivery van fleets are quickly electrifying as Amazon, FedEx, UPS, USPS, and Walmart place major EV orders. Commercial production by Volvo and Freightliner of electric tractor trailers, or 18-wheelers, began in 2023. Although there are promising signs of increasing implementation, only 1.5% of all commercial heavy-duty vehicles in the US were BEVs or PHEVs in September 2023. At the same point in time, the share of BEVs and PHEVs in the HDV fleets in Europe and China amounted to over 7% and 10%, respectively (Soulopoulos, 2023). Aviation The IRA also seeks to encourage the development and adoption of sustainable fuel technologies in the aviation industry. The Sustainable Aviation Fuel Tax Credit incentivises the sale and use of sustainable aviation fuels (SAF) that reduce lifecycle GHG emissions by at least 50% compared to petroleum-based jet fuel. The tax credit, worth USD 1.25 per gallon, is progressive: SAF that reduce emissions by more than 50% are eligible for an additional USD 0.01 per gallon for each extra percent that the reduction exceeds 50% (up to USD 0.50 per gallon) (U.S. Department of Energy, 2022c). The act additionally provides nearly USD 300m in grants to develop and deploy projects related to sustainable aviation fuel and low-emission aviation technologies (The White House, 2023b). Although the US produced nearly 16m gallons of SAF in 2022, these fuels accounted for less than 0.1% of the total fuel used by US airlines in the same year (U.S. Government Accountability Office, 2023). Additionally, analysis suggests that currently available SAF do not reduce emissions across the fuels’ full lifecycles given their emissions and agricultural resource-intensive production methods (Lashof &amp; Denvir, 2024).</t>
-  </si>
-  <si>
     <t>CO 2 emissions from the transport sector accounted for 18.5% of Japan’s total energy-related CO 2 emissions in 2022 (GIO, 2024). Regarding vehicle decarbonisation, the government currently aims for 100% of “electrified vehicles” – a category that includes non-plug-in hybrids (HVs) and plug-in hybrid vehicles (PHV) – in the sale of passenger vehicles by, latest, 2035 (METI, 2020), replacing the previous target of reaching 50-70% of ‘new generation’ vehicles (including hybrids, plug-in hybrids, battery electric vehicles, fuel cell electric vehicles, as well as ‘clean diesel’ vehicles and gas-powered vehicles) in the share of sales by 2030 (METI, 2018b). This policy, which still allows for non-plug-in HVs to be sold in 2035, could be further strengthened to become consistent with the 1.5°C-compatible benchmark to phase out all fossil-fuel passenger (ICE) cars from new sales by 2035 (Kuramochi et al., 2018). Japan’s commitment to transition away from ICE vehicles could further impact the global car manufacturing sector. Given the importance of the industry at both the national and international level, it could define a globally ambitious and innovative strategy favouring the development and deployment of zero-emission vehicles. Additional pressure from investors has also started to impact car manufacturers’ strategies; Toyota for example, aims to launch 10 new EV models by 2026 and recently unveiled plans to build a battery plant in Fukuoka (Nikkei, 2024c; Nikkei Asia, 2023b). Honda aims to release 30 EV models by 2030 (Nikkei, 2022b). Nissan has also announced the launch of 16 EV models by 2026 and aims to achieve EV and ICE vehicle cost parity by 2030 (Nissan Motor Corporation, 2024). However, despite these announcements, Japanese car manufacturers are still falling behind in the global race towards EVs. In 2020, Japanese cars only accounted for less than 5% of EVs sold worldwide (The New York Times, 2021). While EV sales in Japan increased by 50% in 2023 compared to the previous year, they only accounted for 2% of all new passenger car sales (Nikkei Asia, 2024). Despite the mounting pressure to speed up electrification of the transport industry, Japanese carmakers are moving cautiously compared to their counterparts. Many in the industry remain wary about making the shift to electric vehicles and would rather keep investing in internal combustion engine manufacture. For example, Toyota has recently announced that, while it will continue to ramp up its EV production capacity, hybrid vehicles will remain an important pillar of the company’s strategy (Reuters, 2023b). More recently, Toyota’s chairman, who retains significant power within the company, has renewed his scepticism towards EVs. He has openly doubted that the car industry would fully shift to EV, predicting they would capture 30% of the market at most (Bloomberg, 2024). The GX Basic Policy did not set a more ambitious target for EVs. However, as part of the strategy, Japan plans to install 150,000 EV charging stations and 1000 hydrogen stations by 2030 (METI, 2023d), a positive development considering Japan is also lagging behind on EV infrastructure.</t>
   </si>
   <si>
     <t>In 2020, emissions from the buildings sector in Argentina represented 8% (~27 MtCO 2 eq) of Argentina’s GHG emissions (excluding LULUCF), according to its fifth BUR. They grew by 60% between 1990 and 2018, mostly through increases in electricity and heat demand from the residential buildings sector. In 2020, the sector was responsible for 47% of power demand, 23% of gas demand and 27% of total energy demand in Argentina (Government of Argentina, 2023a). In 2017, the government adopted Law 27,424 to promote the use of renewables in the building sector. This law encourages self-consumption of electricity through the introduction of net-metering (Government of Argentina, 2017). Argentina’s 2022 climate strategy also includes targets for solar water heating in residential housing, as well as the for installation of four million square metres of solar panels in businesses by 2030 (Government of Argentina, 2022d). In 2018, the government adopted an energy efficiency labelling scheme for residential housing, aiming at improving access to information for consumers and incentivise efficiency improvements. Until 2022, this system was run by provinces, with slightly different standards being applied. Starting in 2023 the programme is handled by the national government, with the overarching aim of reaching six million households by 2030 (Government of Argentina, 2023e). In its 2022 climate strategy, the government also lists several measures aimed at reducing energy consumption from household appliances. These measures include credit lines to upgrade fridges, heat pumps, lighting, and others. It also includes quantitative targets for specific appliances, such as 9.6 million fridges replaced by 2030, and 7.8 million heat pumps installed (Government of Argentina, 2022d).</t>
   </si>
   <si>
+    <t>The buildings sector accounted for 20% of Australia’s total final energy consumption, and 3% of total emissions excluding LULUCF in 2023 (DCCEEW, 2023b, 2024a). Emissions from the sector are expected to decline just 7% by 2030 and 12% by 2035. Energy efficiency measures in buildings and for appliances are essential to decarbonise. The IEA notes that while there has been progress in energy efficiency for commercial buildings, the residential sector is still lagging (IEA, 2023b). Jurisdictions have not fully implemented the latest 2022 National Construction code (Climate Change Authority, 2024a). The Energy Savings Package, announced in the 2023/24 federal budget, allocates AUD 1.7bn to improve energy efficiency and help households and businesses save on energy costs, including energy efficient renovations and energy efficiency improvements for social housing (DCCEEW, 2024g). Fossil gas accounted for 30% of final energy consumption in residential buildings in 2023, and 16% in commercial buildings (DCCEEW, 2024a). The government refused a call from the Climate Change Authority in 2023 to phase out new and existing gas connections for residential and small commercial buildings (Climate Change Authority, 2023).</t>
+  </si>
+  <si>
+    <t>A little over a tenth of Canada’s emissions are from the buildings sector (excluding electricity) (Environment and Climate Change Canada, 2024). Under the climate plan, the government hopes to cut emissions from the sector by 37% below 2005 levels, by 2030, yet emissions have stagnated since 2005 and the last progress report’s NDC-compatible scenario shows 25% of reductions (Environment and Climate Change Canada, 2022a, 2023b, 2023a). Provinces, and not the federal government, have jurisdiction over building regulations; however, there is much the federal government can still do to provide direction and support. The federal government has been active in four key areas under the 2016 Pan Canadian Framework (Government of Canada, 2016b): 1) Creation of a ‘net-zero energy ready’ building code for new buildings, 2) programmes to encourage retrofits and fuel switch in existing buildings, 3) energy efficiency labelling, and 4) standards and renovation programmes in Indigenous communities. Building on this framework, the government held a consultation in 2022 on a new Green Buildings Strategy aligned with the overall 2030 Emissions Reduction Plan (Government of Canada, 2021j; Natural Resources Canada, 2022b). The three main goals under the strategy are 1) all new buildings to be net-zero carbon ready by 2032 latest, 2) deep retrofit rate to increase to 3–5% per year by 2025, 3) transitioning from fossil-fuel based to electric water and space heating systems. The Strategy was scheduled for release in 2023 but appears to be delayed. The new building codes were adopted in 2022, after a two year delay (but are referred to as the ‘2020’ codes) (National Research Council Canada, 2020, 2022a, 2022b). They adopted a tiered system for the first time, which includes a ‘net zero energy ready’ level. (‘Net zero energy ready’ means that the building is efficient enough that a renewable energy system, once added, would be able to provide all of the building’s energy needs). The aim is to move to progressively more stringent tiers so that by 2030 all new buildings are net zero energy ready. Provinces have agreed to implement this code by 2024 and subsequent updates with a year and a half from publication (Efficiency Canada &amp; Carleton University, 2022). While the codes are heading in the right direction, they are missing key elements: there are no GHG emission requirements, nor provisions to support renewable or EV readiness, though GHG emissions will be addressed in the next update cycle (Efficiency Canada &amp; Carleton University, 2022; Natural Resources Canada, 2022b). As 80% of the buildings stock that will exist in 2030 has already been built (Environment and Climate Change Canada, 2022a), accelerating energy-efficient renovations and retrofits is crucial to decarbonising the sector. Canada has several programmes which support its goal of a 3–5% deep retrofit rate, including CAD 200m for a Deep Retrofit Accelerator Initiative for large buildings (Natural Resources Canada, n.d.), but additional measures are likely needed to achieve this goal. While we have not undertaken this analysis for Canada, the CAT estimates the USA and the EU would need to renovate at least 3.5% of the existing buildings stock per year to be compatible with the 1.5°C temperature limit. The government has also been slowly updating its energy efficiency regulations for a number of residential and commercial products (water heaters, furnaces, etc) and is planning a further round of revisions (Government of Canada, 2022l, 2019c, 2019b). Often the regulatory updates seek to align with existing standards in the USA. As part of the Green Buildings Strategy, it will adopt regulations to prohibit the installation of new oil or fossil gas heating systems and will develop incentives to accelerate heat pump adoption.</t>
+  </si>
+  <si>
+    <t>Buildings consumed almost a quarter of the country's total energy in 2021, with a significant share of this used for heating, and were responsible for approximately 7% of Chile’s total GHG emissions (excl. LULUCF) in the same year (Comisión Nacional de Energía, 2021; Ministerio de Energía, 2022c; IEA, 2024a). It is therefore not surprising that the buildings sector is a central part of the Chile’s cross-sectoral Energy Efficiency Law. The law establishes that residential buildings, public buildings, commercial buildings, and office buildings must have an energy rating to be commercialised (i.e. put on the market): this is applicable to construction and real estate companies as well as housing and urban planning services. As with appliances such as refrigerators, the energy efficiency label allows people to have better information when renting or buying homes. The label must be included in all sales advertising by companies (Ministerio de Energía, 2021d). This provision builds upon the existing Calificación Energética de Viviendas (CEV), established in 2011, and is also integrated into voluntary national building sustainability certifications (Ministerio de Energía, 2021b). The Energy Efficiency Law also states that companies with high energy consumption (over 50 tcal) must annually report their energy consumption and energy intensity. It also introduces an Energy Management System (EMS), covering at least 80% of total energy consumption that includes an energy efficiency action plan, goals, and performance indicators. In 2023, the list of companies that must apply these regulations was published (Ministerio de Energía, 2023b). As with other sectors, Chile’s energy strategy (PEN) also established a number of targets to minimise emissions from the buildings sector, including: a requirement that 10% of existing homes have a specific standard for thermal regulation by 2050, which should point towards net zero energy buildings; that 100% of new public buildings are "zero net energy consuming" by 2030, considering optimal energy performance of heating, hot water, cooling and lighting systems; that 100% of new residential and non-residential buildings are “zero net energy consumption” by 2050 (Ministerio de Energía, 2022c). Even prior to the updated PEN and the Energy Efficiency Law, Chile has been pursuing strategies for the buildings sector such as the National Strategy for Sustainable Construction (ENCS), its main objectives being to incorporate sustainability criteria into buildings and infrastructure, reduce the sector’s energy consumption, reduce GHG emissions, and promote renewable energy use in construction (Ministerio de Vivienda y Urbanismo, 2013). In addition to being revalidated, the ENCS is currently in the process of being updated to respond to new national and international commitments, and better account for the impacts of climate change (Ministerio de Vivienda y Urbanismo, 2024). Chile has also implemented different financial incentives and support programmes to improve building energy efficiency. For instance, under Law no. 20.571/2016, Chile aims to incentivise the use of solar heating through tax cuts for developers who implement this technology (Ministerio de Energía, 2017b). In 2023, the energy and housing ministries introduced subsidies for families to implement solar heating, photovoltaic systems, thermal insulation, and to replace wood-burning heaters (Ministerio de Energía, 2023a).</t>
+  </si>
+  <si>
+    <t>China’s buildings accounted for about 22% of the country’s final energy consumption in 2022, with almost 40% of the energy consumed coming from electricity (IEA, 2023b). China constructs the most buildings globally, having, on average, constructed around four billion square metres of new floor space annually over the last decade (despite a slowdown since 2020) (National Bureau of Statistics, 2021). China’s continuing urbanisation trend is expected to come with a large increase in energy consumption and embodied emissions from the construction sector: the efficiency with which new floor space is built will impact China’s ability to meet headline energy intensity reduction goals in the economy (-13.5% from 2021 to 2025), while the production processes for carbon-intensive construction materials, such as steel and cement, are vital to China’s carbon peaking goals. The 14th FYP for Building Energy Efficiency and Green Building and Implementation Plan for Carbon Peaking in Urban and Rural Construction outlines the government’s main targets for 2025, including setting energy consumption caps in building operations and increasing energy efficiency of new public and residential buildings by 20% and 30% (MoHURD of China, 2022; MoHURD of China and NDRC, 2022). The 14th FYP and implementation plan also contain indicators for increasing solar and geothermal applications to new buildings by 2025, aims to have 55% of the energy consumed in urban buildings from electricity (fossil fuel sources supplied a third of energy consumption in buildings and half of all space heating in 2021), and raises the proportion of energy from renewable electricity to 8% (from 6% in the 13th FYP). The document further sets indicators for renovating 350 million m2 of existing buildings with efficiency measures and constructing 50 million m2 of ultra-low or zero-energy consumption buildings. Retrofits of buildings are paramount in China’s bid for energy efficiency in the sector, as the average age of the building stock is young at 15 years, meaning almost half of the existing floor space could still exist by 2050 (IEA, 2021a). China launched its Near Zero-emission Buildings Standard (NZEB) in 2019 to provide an appendage to the “Green Building Evaluation Standard” and the ongoing development of green buildings, defined as buildings that save energy, land, water, materials and are ecologically unharmful (MoHURD of China, 2019; Cao et al. , 2022). More than 2.5 billion m2 of urban and commercial floor space has already been green-building certified since 2018, whereas almost 10 million m2 of NZEB projects have either been in construction or completed by 2020 (Zhang and Fu, 2021; Zhang et al. , 2021). For compatibility with the Paris Agreement temperature goals, China’s emissions intensity in residential and commercial buildings needs to be reduced by at least 65% in 2030, 90% in 2040, and 95–100% in 2050 below 2015 levels, while energy intensity needs to be reduced by at least 20% in 2030, 35–40% in 2040, and 45–50% in 2050 compared to 2015 levels. China will also need to achieve renovation rates of 2.5% per year until 2030 and 3.5% until 2040 to achieve a Paris-compatible buildings sector by 2050 (Climate Action Tracker, 2020b).</t>
+  </si>
+  <si>
+    <t>Buildings were responsible for 20% of UK emissions in 2023 (DESNZ, 2024b). Emissions fell strongly in 2023 by 7.2% relative to 2022, due to reductions in gas demand (CCC, 2024). However, it remains unclear whether this was due to gas prices (which remain above the levels seen before the fossil gas energy crisis) or due to other drivers. Importantly, key indicators for tracking buildings decarbonisation, including the rate of heat pump installations and the rate of energy efficiency installations, are lagging far behind the level needed. The number of heat pumps installed in 2023 increased only 4% from 2022 (CCC, 2024). The growth rate should be nearer 40–50% per year, if the number of annual installations is to reach 600,000–900,000 by 2030. Meanwhile the number of energy efficiency installations driven by government schemes fell in 2023, moving significantly off-track. This suggests that, without government action, the emissions reductions seen in 2023 will not be sustained into the future. Priority actions for the new government should include: Introducing a comprehensive programme for decarbonising public sector buildings . Public buildings such as schools, hospitals and administrative buildings represent a low-hanging fruit which could deliver substantial emissions reductions quickly. Removing planning barriers to heat pumps . The previous Government proposed such changes which would make it easier to install heat pumps (DLUHC, 2024). The new government should implement these changes immediately. Re-introducing obligations for landlords to improve the energy efficiency of rented homes. The new government has committed to do this in its manifesto – it must now turn this ambition into action. Removing the exemption of 20% of houses from the fossil-fuel boiler installation phase-out . The previous government introduced this exemption, suggesting that it would save money. However, maintaining the gas distribution network for such a small set of households would likely increase, not reduce costs.</t>
+  </si>
+  <si>
+    <t>In Saudi Arabia, per capita emissions in the buildings sector remain above regional and world average, despite a slow decline in recent years (Climate Transparency, 2022). In 2012, the Saudi Energy Efficiency Center (SEEC) launched the Saudi Energy Efficiency Program (SEEP), which targets key sectors of the country’s economy (Kingdom of Saudi Arabia, 2022). Through this program, SEEC has introduced a series of measures in the building sector, including mandatory labelling for insulation materials and air conditioners (Acs). SEEC has also developed guidelines designed to optimise energy consumption in buildings, with a focus on Acs, washing machines, refrigerators, lighting, and heaters. Since their introduction, these standards and guidelines have been further refined and continue to be enforced. Saudi Arabia is taking steps to improve energy efficiency in buildings. Through the national Energy Services Company, TARSHID, the government aims to renovate numerous government buildings, public schools, hospitals, and mosques throughout the country (Kingdom of Saudi Arabia, 2021b). Efforts are also underway to develop and implement an Energy Use Intensity (EUI) ecosystem (Saudi Arabia, 2024).</t>
+  </si>
+  <si>
+    <t>As of 2021, Singapore´s buildings sector accounted for 0.9% of emissions, from energy combustion related to commercial and residential sub sectors and their cooking and hot water systems (National Climate Change Secretariat, 2024b). Emissions from electricity use, such as for air conditioning or appliance use, is not accounted for in primary emissions from the buildings sector but made up a further 12.6% of national emissions (within electricity). The government’s mitigation strategy for the sector is based on increasing energy efficiency. The main policy for the sector is the Green Mark Scheme, which encourages developers and owners to build and maintain greener buildings and requires the achievement of a 28% energy efficiency improvement from 2005 building codes for new and existing buildings undergoing major retrofitting works (with a gross floor area of 2,000 m 2 or more). The Green Building Masterplan, first rolled out in 2006 with several subsequent updates, contains several initiatives aimed at increasing energy efficiency and reducing energy demand in buildings (APEC, 2022). In 2018, the Building Control Act launched the Super Low Energy (SLE) Building programme to encourage firms to go beyond the existing Green Mark Platinum standards and push the envelope of environmental sustainability in Singapore. The fourth edition of Singapore’s Green Building Masterplan (SGBMP), launched in 2021, aims to deliver against three key targets dubbed “80-80-80 in 2030”- greening 80% of Singapore’s buildings, 80% of new developments to be Super Low Energy (SLE) buildings from 2030 and achieving 80% improvement in energy efficiency for best-in-class green buildings by 2030 (Building and Construction Authority, 2023; SG Green Plan, 2021). As of end 2022, 55% of Singapore’s buildings by floor area had been “greened” (Building and Construction Authority, 2023). Since 2013, the Building Control Act has required all existing buildings with a gross floor area of 15,000 m 2 or more to achieve the minimum Green Mark standard after retrofitting. Audits are conducted every three years and companies have to submit energy consumption and energy-related building data (National Climate Change Secretariat, 2018a). Singapore has adopted a Mandatory Energy Labelling Scheme (MELS), which encourages households to buy energy-efficient appliances, and Mandatory Energy Performance Standards (MEPS), to ensure energy inefficient appliances are discontinued (Republic of Singapore, 2019).</t>
+  </si>
+  <si>
+    <t>South Africa has implemented several building regulations and codes on energy efficiency and usage in buildings for new buildings and major refurbishments of old buildings (Sustainable Energy Africa, 2017). The draft Post-2015 National Energy Efficiency Strategy foresees reductions of the final energy consumption by 33% in the residential sector and 37% in the public and commercial sector by 2030, compared to the 2015 baseline (Department of Energy, 2016). Direct and indirect building emissions per capita in South Africa are increasing (Climate Transparency, 2022). The move away from biomass use for cooking and heating towards the use of more modern appliances that require electricity, which, in turn, is largely generated by fossil fuels, might significantly increase indirect emissions without a rapid shift to renewables in the power sector. Analysis by the Climate Action Tracker suggests that the buildings emissions intensity would need to decline by 50% for residential buildings by 2030 in comparison to 2015 values, 90% by 2040, and 100% by 2050 to be compatible with the Paris Agreement. Although retrofitting rates in the residential and commercial buildings sector are still comparatively low, green retrofitting of existing buildings is expected to be the largest sector of the green building industry in South Africa within the next three years (World Green Building Council, 2016). It is expected that the proportion of green buildings in South African building activity will increase over the next years due to cheaper operations costs and higher returns on investments compared to conventional buildings (GBCSA, 2017; World Green Building Council, 2016). The trend towards more energy efficient buildings has been accelerating. A pending regulation on stricter building and appliances standards and certifications could potentially further stimulate this trend (Sustainable Energy Africa, 2017). The government released a regulation for mandatory energy performance certificates in 2020 (Department of Mineral Resources and Energy, 2020). The regulation applies to four different classes of larger-scale buildings with a requirement that all buildings must to be compliant until the end of 2022 (Smith, 2021).</t>
+  </si>
+  <si>
+    <t>In 2022, the buildings sector, including commercial and residential, was responsible for roughly 23% of Switzerland’s total GHG emissions (excl. LULUCF), a decrease from 1990 levels when they represented around 30% of the country’s emissions. The warm winter of 2022 and subsequent lower demand for emissions intensive heating, contributed to this low number, which – in absolute terms – fell below 10 MtCO 2 e for the first time, a reduction equivalent to 44% below 1990 levels (Bundesamt für Umwelt BAFU, 2024b). While missed in 2020, for the first time the achieved emission reduction in 2022 was larger than the goal of a 40% reduction in emissions below 1990 levels by 2020 that was adopted in the 2012 CO 2 Regulation (Der Bundesrat, 2012). With the adoption of the Climate Protection Act, Switzerland now has targets for the buildings sector to reduce emissions by 82% by 2040 and by 100% by 2050 (below 1990 levels) (Bundesgesetz Über Die Ziele Im Klimaschutz, Die Innovation Und Die Stärkung Der Energiesicherheit (KlG), 2023). Within this same Climate Protection Act, a programme to replace fossil-fuelled heating systems with renewable energy sources is prominently featured. The programme receives an annual budget of CHF 200 million (USD 230 million), partly cross-subsidised by the CO 2 levy, for 10 years by the Federal Government. Subsidy details and minimum requirements will be defined by the Federal Council (Bundesgesetz Über Die Ziele Im Klimaschutz, Die Innovation Und Die Stärkung Der Energiesicherheit (KlG), 2023). The focus on heating systems is important, as seen by the impacts that a warmer winter have on overall emissions, and previous efforts have already shown positive results. While 37% of homes were still heated by oil heating systems in 2023, this number has decreased from 59% in 1990. Unfortunately, a substantial share of this reduction has been taken up by other fossil fuels, namely gas (17% in 2023, up from 9% in 1990). The share of buildings with gas heating, however, has dropped for the first time in 2023. Heat pumps are on the rise and already the main heating source in new buildings, accounting for 21% of homes in 2023 (up from only 4.1% in 2000 and 17% in 2021). In new buildings built between 2011 and 2023, 73% were equipped with heat pumps while fossil fuels like heating oil (just over 1%) and natural gas (10%) are in clear decline. Besides these traditional energy carriers, district heating is also playing an increasingly important role, accounting for 7% of new buildings and accounting for a total of 3.8% of total buildings in 2023 (Bundesamt für Statistik BFS, 2024). In Switzerland, regulations and bans on specific heating systems are usually made on the Cantonal level. The installation of new direct resistance heating – with few exceptions –­­­­­ ­is now banned in all cantons. In some Cantons, such as Zurich, a phase out for such heating systems is even planned for 2030 (buildigo, 2024). The Conference of Cantonal Energy Directors (EnDK), has proposed to the Cantons to ban installations of new oil and gas heating systems by 2030 (with few expectations) (Häne, 2023). The Canton of Zurich already has a law in place that bans the installation of fossil heaters to replace older heating systems (Kanton Zürich, 2024). Switzerland has several energy efficiency labels for buildings, the so called “Minergie” standards. There are three major categories: Minergie houses should not consume more than 55 kWh/m2 for new single houses and 90 kWh/m2 for renovations. For Minergie-P the standards are 50 kWh/m2 and 80 kWh/m2 respectively. For Minergie-A the standards are 35 kWh/m2 and heating should be zero or below zero. By May 2023, there were over 55,000 Minergie-certified buildings in Switzerland (Minergie, 2022). These are only certifications and not mandatory standards. Public referenda at the local level to mandate that all new buildings have certain Minergie standards have so far failed to pass.</t>
+  </si>
+  <si>
+    <t>The buildings sector accounted for ~28% of the UAE’s emissions in 2019. The UAE’s 2023 NDC update sets a target to reduce building emissions by 56% below 2019 levels by 2030, while its LTS targets a 98% reduction below 2019 levels by 2050 (Government of the UAE, 2024b). Emissions from the building sector are expected to be 27 MtCO 2 e in 2030 under the NDC from 2023, while under current policies they are expected to be 35 MtCO 2 e (Government of the UAE, 2023a, 2024b). As part of its Energy Strategy 2050, the UAE set out a target of reducing energy consumption by 40%. Several policies are in place to support this target in the buildings sector, including the National Water and Energy Demand Side Management Programme and a federal government building retrofit programme, aiming at 2000 retrofits by 2050. Some Emirates have also produced their own plans and policies to reduce energy consumption from the buildings sector, including Dubai’s plan to retrofit 30,000 buildings by 2030 (Government of the UAE, 2022). The majority of the emissions reductions in the building sector towards the UAE’s NDC target are expected to come from energy efficiency measures including more efficient heating and cooling, as well as demand side management initiatives. The emissions reductions necessary to reach the LTS target of 1 MtCO 2 e in 2050 will come almost entirely from reducing power and heat emissions (Government of the UAE, 2024b).</t>
+  </si>
+  <si>
+    <t>In 2022, direct GHG emissions from buildings accounted for 13.5% percent of total US GHG emissions; 7.3% of the sector’s emissions came from commercial buildings and 6.2% from residential buildings. When accounting for indirect, electricity-related emissions, the buildings sector made up almost one-third (31.1%) of the country’s total GHG emissions in 2022. Since 2005, total emissions—the combination of direct and indirect emissions—from residential and commercial buildings have decreased by approximately 25%. However, direct emissions from buildings have remained nearly constant since 2005 (U.S. Environmental Protection Agency, 2024g). The Biden Administration aims to reduce emissions from buildings by 65% in 2035 and by 90% in 2050 compared to 2005 emissions levels. However, to be 1.5°C compatible, the CAT estimates that emissions from buildings in the US should already be 60% lower in residential buildings and 70% lower in commercial buildings by 2030 compared to 2015 levels (Climate Action Tracker, 2021a, 2021b). Achieving these levels of emissions reductions requires the complete phase-out of new fossil fuel-based energy supply installations in buildings and the rapid retrofitting of the existing housing stock to improve energy efficiency. Building codes Developing and implementing building codes is largely the responsibility of state and local authorities. The federal government’s ability to regulate emissions from buildings is limited; the federal government can directly regulate federal buildings and, otherwise, can only provide financial support and technical guidance for state and local governments. In April 2024, the US Department of Energy (DOE) released a national strategy to guide the decarbonisation of the building sector by 2050, which emphasises the federal government’s role in coordinating and supporting subnational governments in reaching this target (U.S. Department of Energy, 2024a). The strategy outlines key actions, performance targets, and barriers to increase building energy efficiency, accelerate on-site emissions reductions, transform the grid edge, and minimise embodied lifecycle emissions. The Bipartisan Infrastructure Law (BIL) includes USD 225m for state and local implementation of energy codes. Albeit limited in comparison with other funding allocations under the BIL, these resources have largely gone towards the Resilient and Efficient Codes Implementation programme to support energy code adoption, enforcement, training, and technical assistance at the subnational level. In 2022, the DOE released a new building energy code for federal buildings that aims to improve energy efficiency (The White House, 2022b). The Biden Administration’s National Initiative to Advance Building Codes unlocked USD 1bn in IRA grants to further support state and local governments in the adoption of the latest building codes and energy efficiency standards. The initiative aims to provide technical and financial support to state and local governments to modernise building codes in underserved communities, to enhance resilience to increasingly severe weather impacts, to increase household savings on utility bills, and, in turn, to further reduce residential GHG emissions. In June 2024, the DOE released its National Definition for a Zero Emissions Building (U.S. Department of Energy, 2024e). According to the definition, a net zero energy building (nZEB) must be highly energy efficient, cannot emit greenhouse gases on-site, and is powered entirely by clean energy. It is important to note that this definition is not a binding, regulatory standard. Instead, the definition is intended to support and guide public and private sectors in decarbonising new and existing commercial and residential buildings. At the state level, only California and Massachusetts have set targets for nZEBs in their building codes (Massachusetts State, 2022; State of California Public Utilities Commission, 2021). Due to its limited jurisdiction regarding building codes, the federal government has only set a net zero target for federal buildings (see federal buildings section below). In contrast, the EU, which is similarly legally constrained in implementing building codes, requires Member States to set domestic regulations for all new buildings to be zero emissions by 2030 and for the entire building stock to be zero emissions by 2050. Given that the average lifetime of residential buildings is over 60 years (Aktas &amp; Bilec, 2012), renovating and converting existing buildings into nZEBs is key to mitigating emissions from the sector. To encourage net zero renovations, the federal government provides financial incentives. However, the government does not clearly define or provide guidance on the process of converting buildings to net zero structures. In comparison, the EU provides a step-by-step, long-term guide for deep, net zero renovations through its Building Renovation Passport; the guidelines make the renovation process more accessible to homeowners and, in turn, expediate the transition to nZEBs (European Commision, 2024). As it stands, the decarbonisation of buildings in the US will mainly rely on financial incentives for energy efficiency improvements, which, as a result, may have to rely heavily on the electrification of buildings and put more pressure on the power sector. Modelling work by the US Environmental Protection Agency (EPA) hints at the building sector’s dependency on electrification for decarbonisation: under the IRA, total emissions from buildings will decrease significantly by 2035 as the share of electricity in final energy consumption is expected to increase by nearly 5% between 2025 and 2035 (in contrast, to an increase of only 2% in the absence of the IRA) (U.S. Environmental Protection Agency, 2023a). At the same time, direct emissions from fuel combustion will likely remain stable; indicating that reductions in total emissions seem to be driven by a decrease in indirect, end-use electricity emissions (U.S. Environmental Protection Agency, 2023c). Support for energy efficiency and RE measures Through the BIL, the government allocated USD 3bn to support energy efficiency and electrification upgrades in homes (U.S. Department of Energy, 2022g). The 2022 IRA builds on the BIL by unlocking nearly USD 9bn for states and Tribes to support consumer home energy rebate programmes; specifically, for programmes related to retrofitting buildings and purchasing high-efficiency electronic appliances in lower-income communities (The White House, 2023b). The incentives aim to simultaneously reduce energy costs for homeowners and emissions from residential buildings. Via IRA funding, households that retrofit their homes and reduce energy use by at least 35% are eligible for a tax rebate worth USD 4,000. Multifamily structures can qualify for up to USD 400,000. To further incentivise home energy improvements, the government provides tax rebates for energy efficiency upgrades, such as for installing heat pumps, insulation, doors, and windows, and for investing in residential clean energy, including rooftop solar, wind, geothermal, and battery storage (U.S. Internal Revenue Service, 2024b). Beyond supporting residential building upgrades, the IRA targets energy use in commercial buildings by providing tax deductions for buildings that increase their energy efficiency by at least 25% (The White House, 2023b). The BIL introduced the Energy Efficiency Revolving Loan Fund Capitalization Grant Program (RLF), which channels USD 250m to states to establish revolving loan funds. With these funds, states can provide loans, grants, and technical assistance for energy upgrades and retrofits in commercial and residential buildings (U.S. Department of Energy, 2022b, 2024d). Embodied life-cycle carbon emissions of construction and building materials are a significant contributor to GHG emissions: embodied carbon is estimated to make up approximately 14% of building emissions (U.S. Department of Energy, 2024a) and as much as 6% of total national emissions (Huynh et al., 2023). However, there is a lack of standardised, high-quality data on embodied emissions and the federal government does not publicly release data on such emissions. Nevertheless, the government, under the IRA, has taken steps to reduce embodied emissions in buildings. In 2023, the IRA allocates USD 100m to develop standardised labels for lower-embodied carbon building materials, as well as USD 2.15bn for 150 construction projects that employ types of asphalt, concrete, glass, and steel with low embodied carbon (Chase, 2024). Energy efficiency standards Energy efficiency standards for consumer products and appliances in the US are generally ambitious; a 2023 review of the stringency of minimum energy performance standards determined that the federal government’s energy standards for electric motors, refrigerators, and water heaters meet or exceed international best practice (Mavandad &amp; Malinowski, 2023). The EPA’s voluntary energy efficiency labelling programme, ENERGY STAR, supports the government’s efficiency standards. The programme labels efficient products, as well as residential, commercial, and industrial buildings and, in 2020, is estimated to have reduced emissions by 400 MtCO 2 e, which is equivalent to a 5% reduction in total national emissions (ENERGY STAR, 2023). In 2022, the Biden Administration took over 100 actions to strengthen energy efficiency standards for a broad range of products, including household products and appliances, as well as commercial and industrial equipment. The updated standards will reduce GHG emissions by an estimated 2.4 GtCO 2 e over the next 30 years, or around 80 MtCO 2 e/year (The White House, 2022c). In 2023 and 2024, the DOE finalised new standards for refrigerators and freezers, air conditioners and cleaners, and clothes washers and dryers. In combination, these new standards are expected to reduce emissions by an average of 19.9 MtCO 2 e/year over the next 30 years (U.S. Department of Energy, 2023b, 2023a, 2024c). In total, the revised standards for these products will reduce household and business energy costs by USD 8.7bn per year. Federal buildings The federal government is the largest energy consumer in the US and federal buildings are a principal source of the government’s emissions (Council on Environmental Quality, 2024). In April 2024, the DOE amended its energy performance standards for the new construction and renovation of federal buildings (U.S. Department of Energy, 2024b). The revised standards explicitly require federal buildings to reduce the use of fossil fuels. According to the standards, federal agencies must reduce their fossil fuel use in new construction and major renovation projects by 90% between FY2025 and FY2029. The standards mandate that the on-site use of fossil fuels is eliminated by 2030 (U.S. Department of Energy, 2024f). In 2021, President Biden established through Executive Order numerous targets for federal operations and procurement, including reaching net zero emissions in the federal buildings portfolio by 2045 and reducing federal buildings emissions by 50% by 2032 (The White House, 2021c). In 2022, the Biden Administration issued implementing instructions on the Executive Order, which detailed the agency planning, reporting requirements, and accountability mechanism to achieve such targets (The White House Council on Environmental Quality, 2022).</t>
+  </si>
+  <si>
     <t>The buildings sector in Germany emitted 102 MtCO 2 e in 2023, about 15% of Germany’s total emissions. Emissions for 2023 reached a new record low, driven by gas-saving efforts following the suspension of imports from Russia and relatively mild temperatures, and were in line with the sectoral target. Over the years, emissions from this sector have declined, but this has slowed in the last decade. By 2030, the climate change law foresees a limit of 67 MtCO 2 e for buildings, which the UBA forecasts will be slightly exceeded by 1 MtCO 2 e (UBA, 2024c). A Climate Action Tracker report stresses the importance of a comprehensive approach to increasing efficiency and speeding up decarbonisation, particularly in the buildings sector (Climate Action Tracker, 2022). The government coalition agreed on a 65% renewable requirement for new heating systems from 2024, and producing 50% of all heat in a GHG-neutral manner by 2030, which would speed up the decarbonisation of the sector. By 2045, all heating systems would need to fully run on GHG-neutral energy (Federal Ministry of Economics and Climate Protection (BMWK), 2023). A draft law to implement this principle for new heating systems received significant opposition. Subsequently, the government released a watered-down version, which delayed the start of implementation for some regions from 2024 to 2028, and introduced more exceptions and relaxed the use of wood heating. The legislative process for this version faced initial delays due to procedural questions raised by the federal court. Eventually, the law was passed in September 2023. While the proposed law did not specify particular technologies, it effectively aimed to promote the adoption of heat pumps, replacing traditional gas and oil boilers. The law did include some exceptions. While the law's provision for new buildings in new residential areas to meet a 65% renewable energy target for heating systems by 2024 seems like a positive step towards decarbonisation, the option for owners of existing buildings to delay compliance until a municipal heating plan is available raises concerns. This delay could potentially slow down the transition to renewable heating systems, allowing more new fossil fuel-based systems to be installed. The law mandates that municipal heat planning should be completed nationwide by mid-2028. After this point, it will generally not be permissible for heating systems in both new and existing buildings to exclusively rely on fossil fuels for heating systems. Financial support programmes offering up to 70% assistance for transitioning to renewable heating systems are also available (Bundesamt für Wirtschaft und Ausfuhrkontrolle, 2024). In November 2023, the Bundestag passed the Heat Planning and Decarbonisation of Heating Networks Act, which came into effect in 2024. The legislation requires federal states to develop heating plans for municipalities within their jurisdiction to achieve a greenhouse gas-neutral heat supply by 2045. Plans must be implemented by 2026 for municipalities with populations exceeding 100,000, and by 2028 for those with populations below 100,000. These plans are intended to encourage sustainable and climate-neutral heating solutions. By 2030, half of grid-based heat production is expected to be climate-neutral, and by 2040, 80% of heat is aimed to be sourced from renewable energy or waste heat. (BMWSB, 2023). The recent approval of the EU Building Directive compromise is a positive step, yet the goals for reducing energy consumption could be more ambitious. The directive aims for an average reduction of 16% by 2030 and 20-22% by 2035. However, it falls short of the originally proposed stringent standards; notable is the absence of mandatory renovation requirements (Tagesschau, 2024a). Another concern is the approach to green hydrogen, which the law seems to assume will be available for the buildings sector. Green hydrogen is a very expensive source of energy, meaning its use should be limited to applications without alternatives (NewClimate Institute, 2023). A clear direction for this energy source in the law would provide more certainty to the planning communities and the industry providing the required expertise and technologies. Germany’s national emissions trading scheme “Brennstoffemissionshandelsgesetz – BEHG” covers all non-ETS sectors, incl. the buildings sector. Companies selling fossil fuels have to purchase certificates for the carbon content of those fuels, and pass on the additional financial burden to the end consumers through an increased price. The scheme started in 2021 with an initial price of EUR 25 per tonne of CO 2 . It was meant to increase annually, but in 2022 the government postponed the increase because of the high energy prices driven by the illegal invasion of Russia in Ukraine. As of 2024, it is raised to EUR 45 per tonne of CO 2 . An increasing carbon price will mean that running fossil-based heating systems will cost more over time. This trend is foreseeable to informed building owners, but it can be assumed that most owners will lack knowledge and opt for a system with lower investment costs and a technology they are familiar with, unless they are required to deviate from this by law. In the absence of a clear ban of new fossil heating systems, there is a risk that high prices for fuel will burden many house owners and tenants in the future.</t>
   </si>
   <si>
+    <t>In 2021, buildings accounted for 13% of the EU’s total GHG emissions (Climate Analytics, 2024), consuming 40% of the EU’s final energy consumption. The buildings sector has traditionally been heavily reliant on fossil gas and oil. High energy prices triggered by Russia’s illegal invasion of Ukraine is having some impact on consumer behaviour and spurring policy action in the sector. GHG emissions in buildings have been steadily falling since 1990, but not fast enough (European Climate Neutrality Observatory, 2024a). The main legislation driving the decarbonisation of the EU’s building sector fall under: Revised Renewable Energy Directive (EU) 2023/2413 Revised Energy Efficiency Directive (EU) 2023/1791 Revised Energy Performance of Buildings Directive (EU) 2024/1275 New EU ETS II which covers buildings sector The revised Renewable Energy Directive sets an EU wide target to achieve 49% share of renewables in the final energy consumption in buildings by 2030 (European Parliament &amp; Council of the European Union, 2023a). The revised Energy Efficiency Directive sets a binding target to reduce the final energy consumption by 11.7% relative to the 2020 or a target of 763 Mtoe of final energy consumption by 2030 across all sectors (European Parliament, 2023). The EED lacks robust measures specifically targeting the building sector, focusing instead on general improvements in energy efficiency and renovation rates linked to the Energy Performance of Buildings Directive. As of early 2024, no updated NECP submissions from member states fully comply with EED requirements, revealing a concerning lack of commitment. Furthermore, only twelve member states recognise the broader renovation obligation for public buildings (Chapelot et al., 2024), highlighting significant implementation gaps that undermine the EU's climate ambitions. According to the reform of the EU ETS agreed in early 2023, the buildings sector will be covered by a new emissions trading scheme (EU ETS II) from 2027 onward. The requirement to purchase emission allowances to cover the sale of fossil fuels used in the transport and building sectors will further increase the incentive for home insulation and installation of clean sources of heating. The revised Energy Performance of Buildings Directive (EPBD), adopted in 2024, includes several important measures aimed at achieving a zero emission building sectors by 2050. One of the most significant changes is the mandate that all new buildings must meet "zero emission" standards by 2030. While a step in the right direction, the proposal was watered down from the EU Commission's initial plan, which called for binding EU-level minimum energy performance standards. While the EPBD targets a 3.5% annual renovation rate by 2030, which aligns with 1.5°C compatible benchmarks, the EU’s current renovation rate stands at only around 1% annually (Climate Action Tracker, 2020; European Climate Neutrality Observatory, 2024b). The Directive also targets the renovation of 15% of the EU's building stock by 2030, but this is widely regarded as insufficient to meet climate goals (European Climate Neutrality Observatory, 2024a). The table below provides a summary of the main targets set out in the EPBD (BPIE, 2024). The revised EPBD missed an opportunity to fully address the issue of locking in fossil fuel heating systems, by introducing an ambiguous ban on fossil fuel boilers by 2040, while it did ban member states from subsiding the installation of fossil fuel boilers from 2025. The 2040 ban leaves the member state to decide whether or not they wish to include this in their national phase-out plans (Verplancke et al., 2024). The implementation timeline of the revised EPBD is too slow. Key milestones, such as mandatory solar installations for new public and commercial buildings by 2027 and minimum energy performance standards for existing buildings by 2033, push essential changes far into the future. This drawn-out schedule is seen as inadequate to meet the urgent decarbonisation goals needed to address the climate crisis. To reach full decarbonisation in the buildings sector globally by mid-century, the EU would need to reduce the emission intensity (kgCO2/m2) in residential buildings and commercial buildings by 60% and 75% respectively by 2030, compared to 2015 levels. In energy saving terms, the EU would need to reduce the energy intensity (kWh/m2) by 30% and 25%, respectively, by 2030.</t>
+  </si>
+  <si>
     <t>Per capita building-related emissions in India were nearly four times lower than the G20 average in 2021, reflecting low energy consumption due to lack of access to modern appliances (CTR, 2022). Energy consumption in residential buildings is expected to rise by more than eight times by 2050, hence it is of vital importance for India to develop energy-efficiency strategies focused on the residential sector (Climate Analytics, 2021). In the last few years, space cooling has become a major source of energy demand from the urban building sector as summer temperatures increase. It has been projected that by 2050, 45% of India's peak electricity demand could come from space cooling (CEEW, 2022). Governmental initiatives like the Energy Conservation Building Code (ECBC), voluntary initiatives on green building guidelines and a push for the adoption of thermal performance standards in building design and construction materials, can help reduce the internal heat load and lower space cooling requirements (BEE, 2021). The Energy Conservation Act 2022 amendment has expanded the scope for the buildings sector as it now includes offices and residential buildings with a minimum connected load of 100 kW. The amendment of Energy Conservation Act has changed ECBC to “Energy Conservation and Sustainable Building Code”, which specifies norms and standards for energy efficiency, use of renewable energy and other sustainability-related requirements for different types of buildings. Energy Efficiency Services Limited (EESL), an initiative of the Ministry of Power, is implementing the Buildings Energy Efficiency Programme to retrofit commercial buildings in India with energy efficiency devices. This programme has delivered an estimated cumulative energy savings of 790 GWh since 2009 with avoided peak demand of 75.64 MW, cumulative emissions reduction of 0.57 MtCO 2 and an estimated cumulative monetary savings of INR 6 bn (USD 72 mn) in electricity bills since its inception in 2009 (EESL, 2022).</t>
   </si>
   <si>
     <t>Energy efficiency The growing middle class in Indonesia keeps the building sector a critical part of the country’s energy demand landscape. To address this, the Indonesian government has implemented policies to promote energy efficiency. The 2014 National Energy Policy (KEN) targets a 15% reduction in building sector energy consumption by 2025 compared to business-as-usual (ASEAN Centre for Energy and GIZ, 2018). The National Energy General Plan (RUEN) supports this goal through four initiatives: developing Energy Service Companies (ESCOs), implementing energy audits, incentivising industrial machinery upgrades, and raising public awareness (MEMR, 2022c). In 2022, MEMR published a roadmap for energy efficiency and low-carbon buildings, outlining short, medium, and long-term priorities. Short-term actions include enforcing building codes, establishing Minimum Energy Performance Standards (MEPS), and promoting green certifications and Net Zero Energy Buildings (MEMR, 2022c). Early actions have focused on the adoption of Ministerial Regulation No. 14 of 2021 and implementing Ministerial Decisions for appliances like air conditioners, fans, refrigerators, and rice cookers to align with international standards (IESR, 2022c). The Government Regulation No. 33 of 2023 on Energy Conservation mandates local administrations to include energy efficiency in budgets and enforce conservation in public buildings. The regulation sets stricter consumption thresholds, requiring large energy users across transportation, industry, and buildings sectors consuming over 500 tonnes of oil equivalent to adopt energy management practices (The Jakarta Post, 2024e). Green building Although still in its early stages, Indonesia is progressing in green buildings through regulation and certification efforts. Government Regulations No. 16 and No. 21 of 2021 set standards for green building performance, covering new and existing buildings and green areas. Projects meeting these standards are eligible for certification by the Green Building Council Indonesia (GBCI). A key initiative in green building is the Indonesia Green Affordable Housing Programme (IGAHP), launched by the Ministry of Public Works and Housing (PUPR: Kementerian Pekerjaan Umum dan Perumahan Rakyat). The programme aims to build 100,000 green affordable housing units by 2024, build and retrofit one million units by 2030 (with a potential emissions reduction of 19-36 MtCO 2 ), and achieve 100% net-zero housing by 2050 (PUPR, 2023). Challenges remain, particularly in the residential sector, which accounts for 83% of building energy demand and has limited adoption of green building standards. Government Regulation No. 16 of 2021 mandates compliance only for large buildings (over 5,000 m²), and current regulations lack details for city-level implementation and renewable energy integration, which is essential for achieving net-zero carbon buildings (Climate Policy Initiative, 2024). Smaller budget allocation, coupled with low public awareness and the complexity of energy audits, continue to hinder progress in energy efficiency initiatives (The Jakarta Post, 2024e). Future trend: data centres Indonesia’s digital economy has driven demand for green data centres. In June 2022, the country opened its first solar-powered data centre in Bekasi (30 MW capacity) (DCI Indonesia, 2023). Currently, there are 35 centres operating in Greater Jakarta by the end of 2023 (Business Indonesia, 2024). The government is also developing four national data centres, including Nongsa Digital Park in the Riau Islands, expected to reach a capacity of 221 MW by 2025 (The Jakarta Post, 2023; Indonesia Investment Authority, 2024).</t>
   </si>
   <si>
-    <t>The buildings sector accounted for 20% of Australia’s total final energy consumption, and 3% of total emissions excluding LULUCF in 2023 (DCCEEW, 2023b, 2024a). Emissions from the sector are expected to decline just 7% by 2030 and 12% by 2035. Energy efficiency measures in buildings and for appliances are essential to decarbonise. The IEA notes that while there has been progress in energy efficiency for commercial buildings, the residential sector is still lagging (IEA, 2023b). Jurisdictions have not fully implemented the latest 2022 National Construction code (Climate Change Authority, 2024a). The Energy Savings Package, announced in the 2023/24 federal budget, allocates AUD 1.7bn to improve energy efficiency and help households and businesses save on energy costs, including energy efficient renovations and energy efficiency improvements for social housing (DCCEEW, 2024g). Fossil gas accounted for 30% of final energy consumption in residential buildings in 2023, and 16% in commercial buildings (DCCEEW, 2024a). The government refused a call from the Climate Change Authority in 2023 to phase out new and existing gas connections for residential and small commercial buildings (Climate Change Authority, 2023).</t>
-  </si>
-  <si>
-    <t>A little over a tenth of Canada’s emissions are from the buildings sector (excluding electricity) (Environment and Climate Change Canada, 2024). Under the climate plan, the government hopes to cut emissions from the sector by 37% below 2005 levels, by 2030, yet emissions have stagnated since 2005 and the last progress report’s NDC-compatible scenario shows 25% of reductions (Environment and Climate Change Canada, 2022a, 2023b, 2023a). Provinces, and not the federal government, have jurisdiction over building regulations; however, there is much the federal government can still do to provide direction and support. The federal government has been active in four key areas under the 2016 Pan Canadian Framework (Government of Canada, 2016b): 1) Creation of a ‘net-zero energy ready’ building code for new buildings, 2) programmes to encourage retrofits and fuel switch in existing buildings, 3) energy efficiency labelling, and 4) standards and renovation programmes in Indigenous communities. Building on this framework, the government held a consultation in 2022 on a new Green Buildings Strategy aligned with the overall 2030 Emissions Reduction Plan (Government of Canada, 2021j; Natural Resources Canada, 2022b). The three main goals under the strategy are 1) all new buildings to be net-zero carbon ready by 2032 latest, 2) deep retrofit rate to increase to 3–5% per year by 2025, 3) transitioning from fossil-fuel based to electric water and space heating systems. The Strategy was scheduled for release in 2023 but appears to be delayed. The new building codes were adopted in 2022, after a two year delay (but are referred to as the ‘2020’ codes) (National Research Council Canada, 2020, 2022a, 2022b). They adopted a tiered system for the first time, which includes a ‘net zero energy ready’ level. (‘Net zero energy ready’ means that the building is efficient enough that a renewable energy system, once added, would be able to provide all of the building’s energy needs). The aim is to move to progressively more stringent tiers so that by 2030 all new buildings are net zero energy ready. Provinces have agreed to implement this code by 2024 and subsequent updates with a year and a half from publication (Efficiency Canada &amp; Carleton University, 2022). While the codes are heading in the right direction, they are missing key elements: there are no GHG emission requirements, nor provisions to support renewable or EV readiness, though GHG emissions will be addressed in the next update cycle (Efficiency Canada &amp; Carleton University, 2022; Natural Resources Canada, 2022b). As 80% of the buildings stock that will exist in 2030 has already been built (Environment and Climate Change Canada, 2022a), accelerating energy-efficient renovations and retrofits is crucial to decarbonising the sector. Canada has several programmes which support its goal of a 3–5% deep retrofit rate, including CAD 200m for a Deep Retrofit Accelerator Initiative for large buildings (Natural Resources Canada, n.d.), but additional measures are likely needed to achieve this goal. While we have not undertaken this analysis for Canada, the CAT estimates the USA and the EU would need to renovate at least 3.5% of the existing buildings stock per year to be compatible with the 1.5°C temperature limit. The government has also been slowly updating its energy efficiency regulations for a number of residential and commercial products (water heaters, furnaces, etc) and is planning a further round of revisions (Government of Canada, 2022l, 2019c, 2019b). Often the regulatory updates seek to align with existing standards in the USA. As part of the Green Buildings Strategy, it will adopt regulations to prohibit the installation of new oil or fossil gas heating systems and will develop incentives to accelerate heat pump adoption.</t>
-  </si>
-  <si>
-    <t>Buildings consumed almost a quarter of the country's total energy in 2021, with a significant share of this used for heating, and were responsible for approximately 7% of Chile’s total GHG emissions (excl. LULUCF) in the same year (Comisión Nacional de Energía, 2021; Ministerio de Energía, 2022c; IEA, 2024a). It is therefore not surprising that the buildings sector is a central part of the Chile’s cross-sectoral Energy Efficiency Law. The law establishes that residential buildings, public buildings, commercial buildings, and office buildings must have an energy rating to be commercialised (i.e. put on the market): this is applicable to construction and real estate companies as well as housing and urban planning services. As with appliances such as refrigerators, the energy efficiency label allows people to have better information when renting or buying homes. The label must be included in all sales advertising by companies (Ministerio de Energía, 2021d). This provision builds upon the existing Calificación Energética de Viviendas (CEV), established in 2011, and is also integrated into voluntary national building sustainability certifications (Ministerio de Energía, 2021b). The Energy Efficiency Law also states that companies with high energy consumption (over 50 tcal) must annually report their energy consumption and energy intensity. It also introduces an Energy Management System (EMS), covering at least 80% of total energy consumption that includes an energy efficiency action plan, goals, and performance indicators. In 2023, the list of companies that must apply these regulations was published (Ministerio de Energía, 2023b). As with other sectors, Chile’s energy strategy (PEN) also established a number of targets to minimise emissions from the buildings sector, including: a requirement that 10% of existing homes have a specific standard for thermal regulation by 2050, which should point towards net zero energy buildings; that 100% of new public buildings are "zero net energy consuming" by 2030, considering optimal energy performance of heating, hot water, cooling and lighting systems; that 100% of new residential and non-residential buildings are “zero net energy consumption” by 2050 (Ministerio de Energía, 2022c). Even prior to the updated PEN and the Energy Efficiency Law, Chile has been pursuing strategies for the buildings sector such as the National Strategy for Sustainable Construction (ENCS), its main objectives being to incorporate sustainability criteria into buildings and infrastructure, reduce the sector’s energy consumption, reduce GHG emissions, and promote renewable energy use in construction (Ministerio de Vivienda y Urbanismo, 2013). In addition to being revalidated, the ENCS is currently in the process of being updated to respond to new national and international commitments, and better account for the impacts of climate change (Ministerio de Vivienda y Urbanismo, 2024). Chile has also implemented different financial incentives and support programmes to improve building energy efficiency. For instance, under Law no. 20.571/2016, Chile aims to incentivise the use of solar heating through tax cuts for developers who implement this technology (Ministerio de Energía, 2017b). In 2023, the energy and housing ministries introduced subsidies for families to implement solar heating, photovoltaic systems, thermal insulation, and to replace wood-burning heaters (Ministerio de Energía, 2023a).</t>
-  </si>
-  <si>
-    <t>China’s buildings accounted for about 22% of the country’s final energy consumption in 2022, with almost 40% of the energy consumed coming from electricity (IEA, 2023b). China constructs the most buildings globally, having, on average, constructed around four billion square metres of new floor space annually over the last decade (despite a slowdown since 2020) (National Bureau of Statistics, 2021). China’s continuing urbanisation trend is expected to come with a large increase in energy consumption and embodied emissions from the construction sector: the efficiency with which new floor space is built will impact China’s ability to meet headline energy intensity reduction goals in the economy (-13.5% from 2021 to 2025), while the production processes for carbon-intensive construction materials, such as steel and cement, are vital to China’s carbon peaking goals. The 14th FYP for Building Energy Efficiency and Green Building and Implementation Plan for Carbon Peaking in Urban and Rural Construction outlines the government’s main targets for 2025, including setting energy consumption caps in building operations and increasing energy efficiency of new public and residential buildings by 20% and 30% (MoHURD of China, 2022; MoHURD of China and NDRC, 2022). The 14th FYP and implementation plan also contain indicators for increasing solar and geothermal applications to new buildings by 2025, aims to have 55% of the energy consumed in urban buildings from electricity (fossil fuel sources supplied a third of energy consumption in buildings and half of all space heating in 2021), and raises the proportion of energy from renewable electricity to 8% (from 6% in the 13th FYP). The document further sets indicators for renovating 350 million m2 of existing buildings with efficiency measures and constructing 50 million m2 of ultra-low or zero-energy consumption buildings. Retrofits of buildings are paramount in China’s bid for energy efficiency in the sector, as the average age of the building stock is young at 15 years, meaning almost half of the existing floor space could still exist by 2050 (IEA, 2021a). China launched its Near Zero-emission Buildings Standard (NZEB) in 2019 to provide an appendage to the “Green Building Evaluation Standard” and the ongoing development of green buildings, defined as buildings that save energy, land, water, materials and are ecologically unharmful (MoHURD of China, 2019; Cao et al. , 2022). More than 2.5 billion m2 of urban and commercial floor space has already been green-building certified since 2018, whereas almost 10 million m2 of NZEB projects have either been in construction or completed by 2020 (Zhang and Fu, 2021; Zhang et al. , 2021). For compatibility with the Paris Agreement temperature goals, China’s emissions intensity in residential and commercial buildings needs to be reduced by at least 65% in 2030, 90% in 2040, and 95–100% in 2050 below 2015 levels, while energy intensity needs to be reduced by at least 20% in 2030, 35–40% in 2040, and 45–50% in 2050 compared to 2015 levels. China will also need to achieve renovation rates of 2.5% per year until 2030 and 3.5% until 2040 to achieve a Paris-compatible buildings sector by 2050 (Climate Action Tracker, 2020b).</t>
-  </si>
-  <si>
-    <t>In 2021, buildings accounted for 13% of the EU’s total GHG emissions (Climate Analytics, 2024), consuming 40% of the EU’s final energy consumption. The buildings sector has traditionally been heavily reliant on fossil gas and oil. High energy prices triggered by Russia’s illegal invasion of Ukraine is having some impact on consumer behaviour and spurring policy action in the sector. GHG emissions in buildings have been steadily falling since 1990, but not fast enough (European Climate Neutrality Observatory, 2024a). The main legislation driving the decarbonisation of the EU’s building sector fall under: Revised Renewable Energy Directive (EU) 2023/2413 Revised Energy Efficiency Directive (EU) 2023/1791 Revised Energy Performance of Buildings Directive (EU) 2024/1275 New EU ETS II which covers buildings sector The revised Renewable Energy Directive sets an EU wide target to achieve 49% share of renewables in the final energy consumption in buildings by 2030 (European Parliament &amp; Council of the European Union, 2023a). The revised Energy Efficiency Directive sets a binding target to reduce the final energy consumption by 11.7% relative to the 2020 or a target of 763 Mtoe of final energy consumption by 2030 across all sectors (European Parliament, 2023). The EED lacks robust measures specifically targeting the building sector, focusing instead on general improvements in energy efficiency and renovation rates linked to the Energy Performance of Buildings Directive. As of early 2024, no updated NECP submissions from member states fully comply with EED requirements, revealing a concerning lack of commitment. Furthermore, only twelve member states recognise the broader renovation obligation for public buildings (Chapelot et al., 2024), highlighting significant implementation gaps that undermine the EU's climate ambitions. According to the reform of the EU ETS agreed in early 2023, the buildings sector will be covered by a new emissions trading scheme (EU ETS II) from 2027 onward. The requirement to purchase emission allowances to cover the sale of fossil fuels used in the transport and building sectors will further increase the incentive for home insulation and installation of clean sources of heating. The revised Energy Performance of Buildings Directive (EPBD), adopted in 2024, includes several important measures aimed at achieving a zero emission building sectors by 2050. One of the most significant changes is the mandate that all new buildings must meet "zero emission" standards by 2030. While a step in the right direction, the proposal was watered down from the EU Commission's initial plan, which called for binding EU-level minimum energy performance standards. While the EPBD targets a 3.5% annual renovation rate by 2030, which aligns with 1.5°C compatible benchmarks, the EU’s current renovation rate stands at only around 1% annually (Climate Action Tracker, 2020; European Climate Neutrality Observatory, 2024b). The Directive also targets the renovation of 15% of the EU's building stock by 2030, but this is widely regarded as insufficient to meet climate goals (European Climate Neutrality Observatory, 2024a). The table below provides a summary of the main targets set out in the EPBD (BPIE, 2024). The revised EPBD missed an opportunity to fully address the issue of locking in fossil fuel heating systems, by introducing an ambiguous ban on fossil fuel boilers by 2040, while it did ban member states from subsiding the installation of fossil fuel boilers from 2025. The 2040 ban leaves the member state to decide whether or not they wish to include this in their national phase-out plans (Verplancke et al., 2024). The implementation timeline of the revised EPBD is too slow. Key milestones, such as mandatory solar installations for new public and commercial buildings by 2027 and minimum energy performance standards for existing buildings by 2033, push essential changes far into the future. This drawn-out schedule is seen as inadequate to meet the urgent decarbonisation goals needed to address the climate crisis. To reach full decarbonisation in the buildings sector globally by mid-century, the EU would need to reduce the emission intensity (kgCO2/m2) in residential buildings and commercial buildings by 60% and 75% respectively by 2030, compared to 2015 levels. In energy saving terms, the EU would need to reduce the energy intensity (kWh/m2) by 30% and 25%, respectively, by 2030.</t>
-  </si>
-  <si>
-    <t>Buildings were responsible for 20% of UK emissions in 2023 (DESNZ, 2024b). Emissions fell strongly in 2023 by 7.2% relative to 2022, due to reductions in gas demand (CCC, 2024). However, it remains unclear whether this was due to gas prices (which remain above the levels seen before the fossil gas energy crisis) or due to other drivers. Importantly, key indicators for tracking buildings decarbonisation, including the rate of heat pump installations and the rate of energy efficiency installations, are lagging far behind the level needed. The number of heat pumps installed in 2023 increased only 4% from 2022 (CCC, 2024). The growth rate should be nearer 40–50% per year, if the number of annual installations is to reach 600,000–900,000 by 2030. Meanwhile the number of energy efficiency installations driven by government schemes fell in 2023, moving significantly off-track. This suggests that, without government action, the emissions reductions seen in 2023 will not be sustained into the future. Priority actions for the new government should include: Introducing a comprehensive programme for decarbonising public sector buildings . Public buildings such as schools, hospitals and administrative buildings represent a low-hanging fruit which could deliver substantial emissions reductions quickly. Removing planning barriers to heat pumps . The previous Government proposed such changes which would make it easier to install heat pumps (DLUHC, 2024). The new government should implement these changes immediately. Re-introducing obligations for landlords to improve the energy efficiency of rented homes. The new government has committed to do this in its manifesto – it must now turn this ambition into action. Removing the exemption of 20% of houses from the fossil-fuel boiler installation phase-out . The previous government introduced this exemption, suggesting that it would save money. However, maintaining the gas distribution network for such a small set of households would likely increase, not reduce costs.</t>
-  </si>
-  <si>
-    <t>In Saudi Arabia, per capita emissions in the buildings sector remain above regional and world average, despite a slow decline in recent years (Climate Transparency, 2022). In 2012, the Saudi Energy Efficiency Center (SEEC) launched the Saudi Energy Efficiency Program (SEEP), which targets key sectors of the country’s economy (Kingdom of Saudi Arabia, 2022). Through this program, SEEC has introduced a series of measures in the building sector, including mandatory labelling for insulation materials and air conditioners (Acs). SEEC has also developed guidelines designed to optimise energy consumption in buildings, with a focus on Acs, washing machines, refrigerators, lighting, and heaters. Since their introduction, these standards and guidelines have been further refined and continue to be enforced. Saudi Arabia is taking steps to improve energy efficiency in buildings. Through the national Energy Services Company, TARSHID, the government aims to renovate numerous government buildings, public schools, hospitals, and mosques throughout the country (Kingdom of Saudi Arabia, 2021b). Efforts are also underway to develop and implement an Energy Use Intensity (EUI) ecosystem (Saudi Arabia, 2024).</t>
-  </si>
-  <si>
-    <t>As of 2021, Singapore´s buildings sector accounted for 0.9% of emissions, from energy combustion related to commercial and residential sub sectors and their cooking and hot water systems (National Climate Change Secretariat, 2024b). Emissions from electricity use, such as for air conditioning or appliance use, is not accounted for in primary emissions from the buildings sector but made up a further 12.6% of national emissions (within electricity). The government’s mitigation strategy for the sector is based on increasing energy efficiency. The main policy for the sector is the Green Mark Scheme, which encourages developers and owners to build and maintain greener buildings and requires the achievement of a 28% energy efficiency improvement from 2005 building codes for new and existing buildings undergoing major retrofitting works (with a gross floor area of 2,000 m 2 or more). The Green Building Masterplan, first rolled out in 2006 with several subsequent updates, contains several initiatives aimed at increasing energy efficiency and reducing energy demand in buildings (APEC, 2022). In 2018, the Building Control Act launched the Super Low Energy (SLE) Building programme to encourage firms to go beyond the existing Green Mark Platinum standards and push the envelope of environmental sustainability in Singapore. The fourth edition of Singapore’s Green Building Masterplan (SGBMP), launched in 2021, aims to deliver against three key targets dubbed “80-80-80 in 2030”- greening 80% of Singapore’s buildings, 80% of new developments to be Super Low Energy (SLE) buildings from 2030 and achieving 80% improvement in energy efficiency for best-in-class green buildings by 2030 (Building and Construction Authority, 2023; SG Green Plan, 2021). As of end 2022, 55% of Singapore’s buildings by floor area had been “greened” (Building and Construction Authority, 2023). Since 2013, the Building Control Act has required all existing buildings with a gross floor area of 15,000 m 2 or more to achieve the minimum Green Mark standard after retrofitting. Audits are conducted every three years and companies have to submit energy consumption and energy-related building data (National Climate Change Secretariat, 2018a). Singapore has adopted a Mandatory Energy Labelling Scheme (MELS), which encourages households to buy energy-efficient appliances, and Mandatory Energy Performance Standards (MEPS), to ensure energy inefficient appliances are discontinued (Republic of Singapore, 2019).</t>
-  </si>
-  <si>
-    <t>South Africa has implemented several building regulations and codes on energy efficiency and usage in buildings for new buildings and major refurbishments of old buildings (Sustainable Energy Africa, 2017). The draft Post-2015 National Energy Efficiency Strategy foresees reductions of the final energy consumption by 33% in the residential sector and 37% in the public and commercial sector by 2030, compared to the 2015 baseline (Department of Energy, 2016). Direct and indirect building emissions per capita in South Africa are increasing (Climate Transparency, 2022). The move away from biomass use for cooking and heating towards the use of more modern appliances that require electricity, which, in turn, is largely generated by fossil fuels, might significantly increase indirect emissions without a rapid shift to renewables in the power sector. Analysis by the Climate Action Tracker suggests that the buildings emissions intensity would need to decline by 50% for residential buildings by 2030 in comparison to 2015 values, 90% by 2040, and 100% by 2050 to be compatible with the Paris Agreement. Although retrofitting rates in the residential and commercial buildings sector are still comparatively low, green retrofitting of existing buildings is expected to be the largest sector of the green building industry in South Africa within the next three years (World Green Building Council, 2016). It is expected that the proportion of green buildings in South African building activity will increase over the next years due to cheaper operations costs and higher returns on investments compared to conventional buildings (GBCSA, 2017; World Green Building Council, 2016). The trend towards more energy efficient buildings has been accelerating. A pending regulation on stricter building and appliances standards and certifications could potentially further stimulate this trend (Sustainable Energy Africa, 2017). The government released a regulation for mandatory energy performance certificates in 2020 (Department of Mineral Resources and Energy, 2020). The regulation applies to four different classes of larger-scale buildings with a requirement that all buildings must to be compliant until the end of 2022 (Smith, 2021).</t>
-  </si>
-  <si>
-    <t>In 2022, the buildings sector, including commercial and residential, was responsible for roughly 23% of Switzerland’s total GHG emissions (excl. LULUCF), a decrease from 1990 levels when they represented around 30% of the country’s emissions. The warm winter of 2022 and subsequent lower demand for emissions intensive heating, contributed to this low number, which – in absolute terms – fell below 10 MtCO 2 e for the first time, a reduction equivalent to 44% below 1990 levels (Bundesamt für Umwelt BAFU, 2024b). While missed in 2020, for the first time the achieved emission reduction in 2022 was larger than the goal of a 40% reduction in emissions below 1990 levels by 2020 that was adopted in the 2012 CO 2 Regulation (Der Bundesrat, 2012). With the adoption of the Climate Protection Act, Switzerland now has targets for the buildings sector to reduce emissions by 82% by 2040 and by 100% by 2050 (below 1990 levels) (Bundesgesetz Über Die Ziele Im Klimaschutz, Die Innovation Und Die Stärkung Der Energiesicherheit (KlG), 2023). Within this same Climate Protection Act, a programme to replace fossil-fuelled heating systems with renewable energy sources is prominently featured. The programme receives an annual budget of CHF 200 million (USD 230 million), partly cross-subsidised by the CO 2 levy, for 10 years by the Federal Government. Subsidy details and minimum requirements will be defined by the Federal Council (Bundesgesetz Über Die Ziele Im Klimaschutz, Die Innovation Und Die Stärkung Der Energiesicherheit (KlG), 2023). The focus on heating systems is important, as seen by the impacts that a warmer winter have on overall emissions, and previous efforts have already shown positive results. While 37% of homes were still heated by oil heating systems in 2023, this number has decreased from 59% in 1990. Unfortunately, a substantial share of this reduction has been taken up by other fossil fuels, namely gas (17% in 2023, up from 9% in 1990). The share of buildings with gas heating, however, has dropped for the first time in 2023. Heat pumps are on the rise and already the main heating source in new buildings, accounting for 21% of homes in 2023 (up from only 4.1% in 2000 and 17% in 2021). In new buildings built between 2011 and 2023, 73% were equipped with heat pumps while fossil fuels like heating oil (just over 1%) and natural gas (10%) are in clear decline. Besides these traditional energy carriers, district heating is also playing an increasingly important role, accounting for 7% of new buildings and accounting for a total of 3.8% of total buildings in 2023 (Bundesamt für Statistik BFS, 2024). In Switzerland, regulations and bans on specific heating systems are usually made on the Cantonal level. The installation of new direct resistance heating – with few exceptions –­­­­­ ­is now banned in all cantons. In some Cantons, such as Zurich, a phase out for such heating systems is even planned for 2030 (buildigo, 2024). The Conference of Cantonal Energy Directors (EnDK), has proposed to the Cantons to ban installations of new oil and gas heating systems by 2030 (with few expectations) (Häne, 2023). The Canton of Zurich already has a law in place that bans the installation of fossil heaters to replace older heating systems (Kanton Zürich, 2024). Switzerland has several energy efficiency labels for buildings, the so called “Minergie” standards. There are three major categories: Minergie houses should not consume more than 55 kWh/m2 for new single houses and 90 kWh/m2 for renovations. For Minergie-P the standards are 50 kWh/m2 and 80 kWh/m2 respectively. For Minergie-A the standards are 35 kWh/m2 and heating should be zero or below zero. By May 2023, there were over 55,000 Minergie-certified buildings in Switzerland (Minergie, 2022). These are only certifications and not mandatory standards. Public referenda at the local level to mandate that all new buildings have certain Minergie standards have so far failed to pass.</t>
-  </si>
-  <si>
-    <t>The buildings sector accounted for ~28% of the UAE’s emissions in 2019. The UAE’s 2023 NDC update sets a target to reduce building emissions by 56% below 2019 levels by 2030, while its LTS targets a 98% reduction below 2019 levels by 2050 (Government of the UAE, 2024b). Emissions from the building sector are expected to be 27 MtCO 2 e in 2030 under the NDC from 2023, while under current policies they are expected to be 35 MtCO 2 e (Government of the UAE, 2023a, 2024b). As part of its Energy Strategy 2050, the UAE set out a target of reducing energy consumption by 40%. Several policies are in place to support this target in the buildings sector, including the National Water and Energy Demand Side Management Programme and a federal government building retrofit programme, aiming at 2000 retrofits by 2050. Some Emirates have also produced their own plans and policies to reduce energy consumption from the buildings sector, including Dubai’s plan to retrofit 30,000 buildings by 2030 (Government of the UAE, 2022). The majority of the emissions reductions in the building sector towards the UAE’s NDC target are expected to come from energy efficiency measures including more efficient heating and cooling, as well as demand side management initiatives. The emissions reductions necessary to reach the LTS target of 1 MtCO 2 e in 2050 will come almost entirely from reducing power and heat emissions (Government of the UAE, 2024b).</t>
-  </si>
-  <si>
-    <t>In 2022, direct GHG emissions from buildings accounted for 13.5% percent of total US GHG emissions; 7.3% of the sector’s emissions came from commercial buildings and 6.2% from residential buildings. When accounting for indirect, electricity-related emissions, the buildings sector made up almost one-third (31.1%) of the country’s total GHG emissions in 2022. Since 2005, total emissions—the combination of direct and indirect emissions—from residential and commercial buildings have decreased by approximately 25%. However, direct emissions from buildings have remained nearly constant since 2005 (U.S. Environmental Protection Agency, 2024g). The Biden Administration aims to reduce emissions from buildings by 65% in 2035 and by 90% in 2050 compared to 2005 emissions levels. However, to be 1.5°C compatible, the CAT estimates that emissions from buildings in the US should already be 60% lower in residential buildings and 70% lower in commercial buildings by 2030 compared to 2015 levels (Climate Action Tracker, 2021a, 2021b). Achieving these levels of emissions reductions requires the complete phase-out of new fossil fuel-based energy supply installations in buildings and the rapid retrofitting of the existing housing stock to improve energy efficiency. Building codes Developing and implementing building codes is largely the responsibility of state and local authorities. The federal government’s ability to regulate emissions from buildings is limited; the federal government can directly regulate federal buildings and, otherwise, can only provide financial support and technical guidance for state and local governments. In April 2024, the US Department of Energy (DOE) released a national strategy to guide the decarbonisation of the building sector by 2050, which emphasises the federal government’s role in coordinating and supporting subnational governments in reaching this target (U.S. Department of Energy, 2024a). The strategy outlines key actions, performance targets, and barriers to increase building energy efficiency, accelerate on-site emissions reductions, transform the grid edge, and minimise embodied lifecycle emissions. The Bipartisan Infrastructure Law (BIL) includes USD 225m for state and local implementation of energy codes. Albeit limited in comparison with other funding allocations under the BIL, these resources have largely gone towards the Resilient and Efficient Codes Implementation programme to support energy code adoption, enforcement, training, and technical assistance at the subnational level. In 2022, the DOE released a new building energy code for federal buildings that aims to improve energy efficiency (The White House, 2022b). The Biden Administration’s National Initiative to Advance Building Codes unlocked USD 1bn in IRA grants to further support state and local governments in the adoption of the latest building codes and energy efficiency standards. The initiative aims to provide technical and financial support to state and local governments to modernise building codes in underserved communities, to enhance resilience to increasingly severe weather impacts, to increase household savings on utility bills, and, in turn, to further reduce residential GHG emissions. In June 2024, the DOE released its National Definition for a Zero Emissions Building (U.S. Department of Energy, 2024e). According to the definition, a net zero energy building (nZEB) must be highly energy efficient, cannot emit greenhouse gases on-site, and is powered entirely by clean energy. It is important to note that this definition is not a binding, regulatory standard. Instead, the definition is intended to support and guide public and private sectors in decarbonising new and existing commercial and residential buildings. At the state level, only California and Massachusetts have set targets for nZEBs in their building codes (Massachusetts State, 2022; State of California Public Utilities Commission, 2021). Due to its limited jurisdiction regarding building codes, the federal government has only set a net zero target for federal buildings (see federal buildings section below). In contrast, the EU, which is similarly legally constrained in implementing building codes, requires Member States to set domestic regulations for all new buildings to be zero emissions by 2030 and for the entire building stock to be zero emissions by 2050. Given that the average lifetime of residential buildings is over 60 years (Aktas &amp; Bilec, 2012), renovating and converting existing buildings into nZEBs is key to mitigating emissions from the sector. To encourage net zero renovations, the federal government provides financial incentives. However, the government does not clearly define or provide guidance on the process of converting buildings to net zero structures. In comparison, the EU provides a step-by-step, long-term guide for deep, net zero renovations through its Building Renovation Passport; the guidelines make the renovation process more accessible to homeowners and, in turn, expediate the transition to nZEBs (European Commision, 2024). As it stands, the decarbonisation of buildings in the US will mainly rely on financial incentives for energy efficiency improvements, which, as a result, may have to rely heavily on the electrification of buildings and put more pressure on the power sector. Modelling work by the US Environmental Protection Agency (EPA) hints at the building sector’s dependency on electrification for decarbonisation: under the IRA, total emissions from buildings will decrease significantly by 2035 as the share of electricity in final energy consumption is expected to increase by nearly 5% between 2025 and 2035 (in contrast, to an increase of only 2% in the absence of the IRA) (U.S. Environmental Protection Agency, 2023a). At the same time, direct emissions from fuel combustion will likely remain stable; indicating that reductions in total emissions seem to be driven by a decrease in indirect, end-use electricity emissions (U.S. Environmental Protection Agency, 2023c). Support for energy efficiency and RE measures Through the BIL, the government allocated USD 3bn to support energy efficiency and electrification upgrades in homes (U.S. Department of Energy, 2022g). The 2022 IRA builds on the BIL by unlocking nearly USD 9bn for states and Tribes to support consumer home energy rebate programmes; specifically, for programmes related to retrofitting buildings and purchasing high-efficiency electronic appliances in lower-income communities (The White House, 2023b). The incentives aim to simultaneously reduce energy costs for homeowners and emissions from residential buildings. Via IRA funding, households that retrofit their homes and reduce energy use by at least 35% are eligible for a tax rebate worth USD 4,000. Multifamily structures can qualify for up to USD 400,000. To further incentivise home energy improvements, the government provides tax rebates for energy efficiency upgrades, such as for installing heat pumps, insulation, doors, and windows, and for investing in residential clean energy, including rooftop solar, wind, geothermal, and battery storage (U.S. Internal Revenue Service, 2024b). Beyond supporting residential building upgrades, the IRA targets energy use in commercial buildings by providing tax deductions for buildings that increase their energy efficiency by at least 25% (The White House, 2023b). The BIL introduced the Energy Efficiency Revolving Loan Fund Capitalization Grant Program (RLF), which channels USD 250m to states to establish revolving loan funds. With these funds, states can provide loans, grants, and technical assistance for energy upgrades and retrofits in commercial and residential buildings (U.S. Department of Energy, 2022b, 2024d). Embodied life-cycle carbon emissions of construction and building materials are a significant contributor to GHG emissions: embodied carbon is estimated to make up approximately 14% of building emissions (U.S. Department of Energy, 2024a) and as much as 6% of total national emissions (Huynh et al., 2023). However, there is a lack of standardised, high-quality data on embodied emissions and the federal government does not publicly release data on such emissions. Nevertheless, the government, under the IRA, has taken steps to reduce embodied emissions in buildings. In 2023, the IRA allocates USD 100m to develop standardised labels for lower-embodied carbon building materials, as well as USD 2.15bn for 150 construction projects that employ types of asphalt, concrete, glass, and steel with low embodied carbon (Chase, 2024). Energy efficiency standards Energy efficiency standards for consumer products and appliances in the US are generally ambitious; a 2023 review of the stringency of minimum energy performance standards determined that the federal government’s energy standards for electric motors, refrigerators, and water heaters meet or exceed international best practice (Mavandad &amp; Malinowski, 2023). The EPA’s voluntary energy efficiency labelling programme, ENERGY STAR, supports the government’s efficiency standards. The programme labels efficient products, as well as residential, commercial, and industrial buildings and, in 2020, is estimated to have reduced emissions by 400 MtCO 2 e, which is equivalent to a 5% reduction in total national emissions (ENERGY STAR, 2023). In 2022, the Biden Administration took over 100 actions to strengthen energy efficiency standards for a broad range of products, including household products and appliances, as well as commercial and industrial equipment. The updated standards will reduce GHG emissions by an estimated 2.4 GtCO 2 e over the next 30 years, or around 80 MtCO 2 e/year (The White House, 2022c). In 2023 and 2024, the DOE finalised new standards for refrigerators and freezers, air conditioners and cleaners, and clothes washers and dryers. In combination, these new standards are expected to reduce emissions by an average of 19.9 MtCO 2 e/year over the next 30 years (U.S. Department of Energy, 2023b, 2023a, 2024c). In total, the revised standards for these products will reduce household and business energy costs by USD 8.7bn per year. Federal buildings The federal government is the largest energy consumer in the US and federal buildings are a principal source of the government’s emissions (Council on Environmental Quality, 2024). In April 2024, the DOE amended its energy performance standards for the new construction and renovation of federal buildings (U.S. Department of Energy, 2024b). The revised standards explicitly require federal buildings to reduce the use of fossil fuels. According to the standards, federal agencies must reduce their fossil fuel use in new construction and major renovation projects by 90% between FY2025 and FY2029. The standards mandate that the on-site use of fossil fuels is eliminated by 2030 (U.S. Department of Energy, 2024f). In 2021, President Biden established through Executive Order numerous targets for federal operations and procurement, including reaching net zero emissions in the federal buildings portfolio by 2045 and reducing federal buildings emissions by 50% by 2032 (The White House, 2021c). In 2022, the Biden Administration issued implementing instructions on the Executive Order, which detailed the agency planning, reporting requirements, and accountability mechanism to achieve such targets (The White House Council on Environmental Quality, 2022).</t>
-  </si>
-  <si>
     <t>CO 2 emissions (including indirect emissions from electricity use) from the commercial and residential building sectors together accounted for 32% of Japan’s total energy-related CO 2 emissions in 2021 (GIO, 2023). Compared to 1990, the emissions in these two sectors have increased by 42% and 19%, respectively (GIO, 2023). Although these significant increases are partially attributable to the increased electricity CO 2 -intensity post-Fukushima, there’s an urgent need for strengthened action on the demand side in the buildings sector. An important recent development is the revised Building Energy Conservation Act, which entered into force in June 2022 mandating all new houses and buildings from 2025 to comply with upgraded energy efficiency standards. This is a significant step forward from the current regulation which is only applicable to buildings larger than 300 m2. To also support decarbonising existing houses and buildings, several measures have been introduced, including financial support for household renovations to improve energy efficiency, as well as promoting the use of renewable energy in buildings. Japan aims to achieve on stock average net-zero energy consumption for newly constructed buildings (ZEBs) and houses (ZEHs) by 2030 as well as all buildings and houses by 2050 (MLIT, 2022). This is a step change as in 2020, only 0.42% of newly built buildings was ZEBs, and 24% of newly built houses was ZEHs (METI, 2022f; METI &amp; MOEJ, 2022). For comparison: the EU requires all new buildings to be near zero energy as of 2022. The GX Basic Policy sets the objective to invest at least JPY 14 tn in the building sector over the next ten years (METI, 2023d). In December 2022, the Tokyo Metropolitan Government also adopted the “Renewable Energy Installation Standards”, a regulation requiring construction companies to install rooftop solar panels on new buildings (including residential properties) of up to 2,000 m2, from 2025 (The Japan Times, 2022c). This new policy exclusively targets companies whose building projects total at least 20,000 m2 or more per year, so around 50 companies. The Tokyo Metropolitan Government will set up thresholds per district, ranging from 30%, to 70 -85% of new buildings. The city will also provide subsidies to encourage the installation of solar panels on existing buildings, which are currently excluded from the regulation (Tokyo Metropolitan Government, 2022). The “Renewable Energy Installation Standards“ is expected to be impactful, as half of existing buildings will be replaced with new ones before 2050.</t>
   </si>
   <si>
     <t>Agricultural emissions in Argentina were 102 MtCO 2 e in 2022, accounting for roughly one third of Argentina’s total emissions (excl. LULUCF), and 7% of total energy demand (Government of Argentina, 2024a). Emissions from this sector have increased by 13% over the last 10 years due to growing agricultural and livestock production. The agricultural sector is a major economic powerhouse of the country, especially for its export market. Key commodities produced in Argentina are soybeans, wheat, maize, and cattle. In total, agricultural commodities represented 71% of Argentinian exports in 2020, and USD 38.6 billion in value. In 2022-2023 the sector was hard hit by droughts, costing the country an estimated 3% of its GDP (Reuters, 2024). Despite the high emissions in the sector, Argentina’s national action plan for agriculture and climate change only includes three concrete measures planned for the agriculture, livestock and forestry sectors up to 2030, including afforestation (area from 1.38 million to 2 million hectares between 2018 and 2030), crop rotation (increasing the area under cereals such as wheat and maize and decreasing the area under oilseeds such as soybeans and sunflower) and biomass utilisation for energy generation, particularly for off-grid use (Secretaria de Ambiente y Desarrollo Sustentable, 2019). As part of its 2022 climate strategy, the Argentinian government has set out some additional livestock-related measures. These include a 5% increase in the GHG-efficiency of livestock until 2030 (without a clear baseline), and the promotion of silvopastoral systems through REDD+ payments. However, it remains unlikely that these measures will significantly bring down livestock-related emissions (Government of Argentina, 2022d). A recent study analyses the potential of supply-side mitigation options to reduce emissions in the agriculture and land use sector including feed optimisation, livestock health monitoring, the use of cover crops and crop rotation, synthetic fertiliser management and the use of silvopastoral systems. It found that the combined technical mitigation potential for these measures was around 28.1 MtCO 2 e, or around 14% below the reference scenario in 2030. The gap to the sectoral net zero scenario, that is the amount that Argentina would need to further reduce its emissions to be on track to a net zero AFOLU sector, was of around 103 MtCO 2 e in 2030 (Gonzales-Zuñiga et al., 2022). This shows the need for transformation in the sector: even when implementing best practices and increasing the efficiency of agricultural production, the sectoral gap to a 1.5˚C compatible emissions pathway is very large. Argentina will need a deeper transformation of its wider food system if it is to keep its emissions in line with limiting warming to 1.5˚C.</t>
   </si>
   <si>
+    <t>Agriculture accounted for 16% of Australia’s total emissions excluding LULUCF in 2024 (DCCEEW, 2024i). Emissions from the sector are expected to remain stable until 2035, falling just 3% below 2023 levels (DCCEEW, 2023b). Emissions in the agriculture sector are mainly derived from enteric fermentation (digestive processes of animals), which accounted for 69% of the sector’s emissions in 2022/23 (DCCEEW, 2023b). Emissions from beef account for over half of agricultural emissions at 52% in 2023. This share is expected to remain steady, accounting for 53% of agricultural emissions in 2035 (DCCEEW, 2023b). Application from lime, urea and fertilisers are other sources of emissions from the sector. The government has allocated an additional AUD 30.8m to the Carbon Farming Outreach Program, aimed at supporting farmers and land managers to reduce emissions and store carbon (Department of Climate Change, 2023c). At COP28, Australia signed the Emirates Declaration on Sustainable Agriculture, Resilient Food Systems and Climate Action to foster adaptation and resilience in the sector (COP28, 2023b).</t>
+  </si>
+  <si>
+    <t>Agriculture is the second biggest contributor to Brazil’s GHG emissions after the land use sector (LULUCF), with emissions consistently growing over the years and reaching its highest reported levels in 2022 at just over 600 MtCO 2 e. Excluding LULUCF emissions, agriculture and livestock represent just over half of the country’s emissions. Almost 75% of the sector’s emissions are methane and nitrous oxide from livestock alone (SEEG, 2023a). If the indirect emissions of the agriculture sector (mostly related to deforestation resulting from the expansion of agricultural land) were considered, the sector would be by far the single largest emissions source in Brazil. However, there are limited policies in place to reduce agricultural emissions. Brazil’s main policy instrument of agricultural activity is the Agricultural Plan (Plano Safra) which aims to facilitate sustainable development by providing credit lines tailored to support crop production and product marketing (CPI, 2023). The Plano Safra for 2023/2024, with a record allocation of BRL 435bn for agricultural financing, designates only 0.5% of this sum for low-carbon measures in the sector (Talanoa, 2023). Furthermore, the new Safra Plan 24/25, unveiled in the first half of 2024, has a 16.5% increase in investment credit lines. This the largest increase in public resources the Safra Plan has received so far (Government of Brazil, 2024). Renovagro, formerly known as ABC+ Plan, supports low-carbon agriculture by financing practices such as land restoration, integrated crop-livestock-forest systems, the production of bio-fertilisers, and others. The ABC+ Plan aims to prevent over one billion tonnes of carbon emissions between 2021-2030, primarily through restoring degraded pastures and planting forests. The Brazilian agricultural sector is heavily dependent on fertilisers. In November 2023, the government approved the revised National Fertiliser Plan 2050 aiming to reduce the country’s dependence on fertiliser imports — currently at 87% of total demand — and meet 45% to 50% of the demand domestically by 2050. The plan outlines strategies such as reactivating idle factories, incentivising new industrial plants, and investing in sustainable nutrient production to achieve the goal. Historically, there is a strong relationship between agriculture expansion and deforestation emissions in Brazil. Forest land is consistently lost to make room for agriculture and cattle ranching. The expansion of soybean plantations became a direct driver of deforestation as it became more financially attractive than cattle ranching (Ionova, 2021). Forests are either directly converted to soybean farms, or soybeans are planted on old pasture, driving deforestation for more pastureland (Kimbrough, 2021). However, expanding the agriculture frontier through deforestation is unnecessary to increase productivity. Brazil has considerable potential to add value and productivity to already available but currently underutilised land by investing in more sustainable and efficient agriculture methods (Observatório do Clima, 2019; Stabile et al., 2020).</t>
+  </si>
+  <si>
+    <t>Agriculture was responsible for around 8% of Canada’s total emissions in 2022 (Environment and Climate Change Canada, 2024). The sector is projected to contribute around 4% of the emissions reductions in its latest 2030 climate plan. While the sector is responsible for 27% of the country’s methane emissions, it will contribute only about 1% of the reductions under Canada’s methane plan. Policy action is a mix of cross-cutting measures, individual targets and programmes and funding initiatives . In 2020 Canada announced a voluntary target of reducing emissions from fertiliser use by 30% below 2020 levels by 2030, a key source of N 2 O emissions (Environment and Climate Change Canada, 2020a). Direct emissions from synthetic nitrogen fertiliser have increased substantially since 2005. The government concluded consultations on the approaches to achieve the target in August 2022, but has not yet announced the next steps (Government of Canada, 2022c, 2022m, 2022n). Some agricultural activities will be eligible for the federal government’s GHG offset system , established in June 2022. Credits generated under the system can be used to reduce the compliance costs of industrial facilities covered by the government’s carbon pricing system (OBPS). Protocols for projects related to livestock feed management and enhancing soil organic carbon are currently being developed and ones for manure management and anaerobic digestions are planned (Environment and Climate Change Canada, 2022d; Government of Canada, 2022c). Health Canada for the first time did not include a meat category, instead choosing to focus on “protein foods” (Government of Canada, 2019a; Health Canada, 2019). It also recommends choosing plant-based protein more often than other sources. Reducing emissions from agriculture , including through shifting the system to a more plant-based diet, will be key to meeting the Paris Agreement’s temperature goal.</t>
+  </si>
+  <si>
+    <t>Agriculture was responsible for 12% of UK emissions in 2022 (DESNZ, 2024a). There has been essentially no progress made in agricultural decarbonisation over the past decade, with emissions in 2022 at the same level as in 2012. In many places, the existing policy portfolio for agricultural decarbonisation is “too little, too late”. There is still no ban on the use of peat in gardening products, and plans to introduce methane-supressing feed products by 2030 are too late. Key actions for the new government include: Introducing policies to hedge against the risk of delivery failure . The existing approach to agricultural decarbonisation has relied heavily on measures which are technological and voluntary in nature: this is a significant delivery risk. Productivity improvements on their own will not necessarily reduce emissions, with a risk that farmers simply increase herd numbers instead of freeing up land. Policies need to be developed to address these risks. Introducing measures to address dietary change and food waste prevention . The existing Government Food Strategy does not introduce measures to support and accelerate dietary shifts, despite the clear health benefits of doing so, and the evidence of consumer appetite for reduced meat consumption (Stewart et al., 2021; UK Government, 2022). The Food Strategy also only addressed food waste from large businesses, despite the majority of food waste occurring at the household, farm and supply-chain stages.</t>
+  </si>
+  <si>
+    <t>In 2020, agriculture accounted for nearly 10% of South Africa’s emissions, with the majority coming from livestock. Emissions from agriculture have remained fairly constant since 2000. There is a limited number of policies in South Africa’s agricultural and forestry sector targeted at climate change mitigation. The National Climate Change Response Policy, the country’s core climate policy published in 2011, names climate smart agriculture (CSA) as a practice “that lowers agricultural emissions, is more resilient to climate changes, and boosts agricultural production” (Government of South Africa, 2011). A number of CSA activities are already in place in South Africa (Nciizah &amp; Wakindiki, 2015), but their expected or actual mitigation impacts are not reported. In 2018, the Department of Agriculture, Forestry and Fisheries has published two draft agricultural policies for public comment: the draft Conservation Agriculture Policy and the draft Climate Smart Agriculture Strategic Framework (DAFF, 2018b, 2018a). Final versions of the policies do not seem to have been published.</t>
+  </si>
+  <si>
+    <t>Emissions from the agriculture sector in 2022 constituted around 16% of total emissions (excluding LULUCF), representing a roughly constant share of total emissions as they have been decreasing at around the same pace as overall emissions (Bundesamt für Umwelt BAFU, 2024b). In 2023, Switzerland released its new Climate Strategy for Agriculture 2050 , replacing the 2011 Climate Strategy for Agriculture with a more ambitious, comprehensive approach based on recent sustainable development and agricultural policy framework serving as a guideline for reducing greenhouse gas emissions and adapting to climate change in the agricultural sector, with a focus on enhancing food security. The strategy sets three primary goals: adapting agricultural production to local climate conditions with at least 50% self-sufficiency rates, reducing the per capita ecological footprint of diets by two-thirds from 2020 levels, and cutting agricultural greenhouse gas emissions by 40% compared to 1990 (this shows an increase in ambitious from a previous one third increase) (Bundesamt für Landwirtschaft BLW; et al., 2023). The strategy includes some measures to achieve these targets, but the plan to make the reduction target mandatory by including it in the third CO 2 Act was dropped after the rejection of the act by the Swiss electorate. Swiss agricultural policy reform faced a significant delay with the suspension of AP22+, the successor of the Agricultural Policy 2014-2017 and 2018-2021. Switzerland’s AP 14-17 and AP 18-21 contained the abolition of unspecific direct payments (livestock subsidies, general acreage payments), additional funds for environmentally friendly production systems, and for the efficient use of resources (e.g., increase in nutrient efficiency and ecological set-aside areas, reduction of ammonia emissions) (Schweizerische Eidgenossenschaft, 2020c). In 2020 and 2021, Parliament halted further policy development until the Federal Council could submit a detailed report on the future direction of agricultural policy. This June 2022 report aimed to provide a long-term vision, addressing unresolved issues from previous policies and the need for more sustainable agricultural practices. Following this, work on AP30+ began, with the Federal Council scheduled to review and discuss proposals in 2026, with hopes of finally implementing a sustainable and cohesive agricultural policy framework (Der Bundesrat, 2022). Switzerland’s unique direct democratic system, which allows citizens to propose constitutional amendments via initiatives, has not been effective in advancing agricultural policy reform. Despite efforts – such as the 2021 initiatives on clean drinking water and pesticide reduction, both rejected by 61% of voters, and the 2024 biodiversity initiative, rejected with 63% – all three proposals were blocked at the ballot, largely due to the strong influence of the farming lobby (Müller, 2021; Rigendinger, 2024)</t>
+  </si>
+  <si>
+    <t>Greenhouse gas emissions from the agriculture sector made up 9% of US emissions in 2022. Between 1990 and 2022, agriculture emissions increased by 8%, primarily from the growth of the livestock sector and the intensification of farming practices. Nitrous oxide emissions from soils made up half of agricultural emissions. Enteric fermentation and manure management from livestock represented other significant emissions sources. Agricultural emissions decreased in 2022 compared to the previous year. However, this decrease was not the result of new policy, but is rather attributable to the decline in herd size—the smallest since the 1960s—due to drought conditions (U.S. Environmental Protection Agency, 2024h). The Inflation Reduction Act (IRA) allocates USD 19.5bn for mitigation activities in the agriculture sector. The act mainly boosts the funding of existing conservation programmes, such as the Environmental Quality Incentives Program (EQIP) and the Conservation Stewardship Program (CSP) (Monke et al., 2022). Both programmes offer financial and technical support to farmers to implement climate-friendly practices, including nutrient management, cover crops, low or no-tillage, and agroforestry. Historically, farmers have struggled to access funding under such programmes due to high demand and limited institutional capacity. These barriers could potentially be addressed by better distributing programme spending (e.g. by capping funds per farm), limiting the funding that goes to ineffective conservation practices, and increasing agency resources (Happ, 2023; Tham, 2023). However, the efficacy of existing programmes to address on-farm emissions has come into question. Between 2019 and 2020, only one-fifth of total EQIP spending reportedly went towards the implementation of agricultural practices that directly reduce GHG emissions (Schechinger, 2022). While programmes like EQIP and CSP are now bolstered by IRA funding, they still face structural issues that may impede climate mitigation. In 2024, 15 new practices were added to the 'climate-smart' category under the EQIP, but many of the new measures do not have proven climate benefits. A significant portion of EQIP funding goes towards manure management practices, including biodigesters that convert manure into biogas, which can be sold for profit and, therefore, may incentivise farmers to maintain or increase their herd sizes (Happ, 2024; Schechinger, 2024). The IRA has also funded several programmes to support renewable energy use in the agriculture sector, including loans and grants for farmers who implement energy efficient equipment or underutilised renewable energy technologies (The White House, 2023b). However, certain provisions of these programmes could lead to perverse incentives. For instance, the Rural Energy for America Program (REAP) subsidises biogas production. However, in combination with existing state subsidies for cattle farmers to produce biomass, REAP’s subsidies could lead to intensified livestock production (Sainato, 2022). The Farm Bill is a policy that heavily influences farmers’ decisions on what food to produce and how to produce it. The 2018 bill expired last year, but was temporarily extended through FY2024. Its official renewal was pushed to 2024 since Congress could not come to an agreement on the contents of the new bill. In 2024, the Republican-led House Committee on Agriculture released a draft bill that could deter climate progress in the agriculture sector. The bill would reallocate up to USD 14.4bn from the IRA that is specifically meant for climate-friendly farming practices to cover all conservation practices. The bill would also reinstate the requirement that 50% of EQIP funds are channelled to livestock operations (House Committee on Agriculture, 2024). However, the fate of the Farm Bill and its contents remain unclear as it has yet to arrive on the House floor. There are still considerable policy gaps in addressing agricultural emissions. Beyond the structural issues of existing programmes (i.e. EQIP, CSP), the US lacks regulations or plans for addressing emissions from animal production. There are no incentives for reducing the volume of animal agriculture or for promoting plant-based foods and crops (CBD, 2020). Instead, Concentrated Animal Feeding Operations (CAFOs), which are detrimental to animal and environmental welfare, continue to be subsidised by the government (Happ, 2024). The government also lacks policies on the demand-side. The US has one of the highest rates of meat and dairy consumption in the world, but food consumption patterns have not been addressed by the government. Historically, the meat industry has lobbied against key demand-side policies, such as changes to dietary guidelines, which constitute the basis of federal nutrition programmes and policy (Bottemiller Evich, 2016; Sebastian, 2024). Without a shift in diets, related emissions may increase by 9% in the US as a result of population growth (Heller et al., 2020). The volume of food waste in the US is very high. Approximately one-third of available food is lost or wasted. Surplus, wasted food results in significant embodied emissions across the supply chain, and has been estimated to account for 6% of the country’s total GHG emissions (Harwood et al., 2023). The US Environmental Protection Agency (EPA) has set a goal to halve food loss and waste by 2030. However, the target puts little focus on food losses, which occur during the production and processing stages, due to a lack of data (U.S. Environmental Protection Agency, 2024o). The US is not on track to reach this target due to insufficient federal and state-level policies. Interventions to prevent food waste, such as policies on date labels, are insufficient. At the subnational level, some states hinder the recycling of food waste through bans on diverting food waste streams towards animal feed (ReFED, 2024).</t>
+  </si>
+  <si>
     <t>The agricultural sector in Germany emitted 59 MtCO 2 e in 2023, about 8% of Germany’s total emissions. Over the last two decades, emissions in the sector slightly declined, but at a slower rate than most other sectors. The largest source, with about half of the sector’s emissions, is methane released through enteric fermentation of livestock, followed by nitrous oxide emissions from agricultural lands. In 2023, emissions from the agricultural sector remained below the sectoral limit set by the climate change law. For 2030, the climate change law foresees a limit of 57 MtCO 2 e/yr for agriculture, which the UBA forecasts will be almost met with implemented measures (UBA, 2024c). Emissions in the agriculture sector need to reduce significantly so that Germany can reach climate neutrality by 2045. So far, policies are not in place and agreement with farmers is urgently needed, as they recently have been a stumbling block to new policies. Meat consumption in 2023 decreased by 4% relative to 2022, which was also reflected in reduced production (BMEL, 2024). The level of meat consumption is still clearly above world average and beyond a level that constitutes a healthy diet (Climate Action Tracker, 2018). While demand for meat products is down, plant-based products saw an increasingly strong pick up by German citizens in 2023. Another factor for decreased meat consumption in recent years might be increased food prices as a result of the energy crisis. To decrease the burden of inflation on poorer households and steer nutrition in a healthier and more environmentally sustainable direction, the German Minister for Agriculture proposed waiving the value added tax on plant-based products in early 2023. At the moment, all food products, including meat and dairy products, are taxed at a reduced rate of 7% (as opposed to 19% for other goods and drinks). This measure would need to be implemented by the Ministry of Finance, who has not yet picked up this proposal.</t>
   </si>
   <si>
+    <t>Agriculture accounts for 11% of the EU’s total GHG emissions in 2021 (UNFCCC, 2023). The EU agricultural sector generates about 60% of its emissions from methane, nearly all of which come from livestock, primarily through enteric fermentation and manure management (Eurostat, 2022). Despite this, methane reduction efforts remain insufficient. While the EU is a co-initiator of the Global Methane Pledge, aiming to cut global methane emissions by 30% below 2020 levels by 2030, only 11 member states have committed to reducing methane from livestock, covering less than 3% of the EU’s livestock units. Leaked reports indicate the EU is not on track to meet its methane reduction target, signifying the need for stronger measures (Ainger, 2022; Changing Markets, 2022). Previous Common Agricultural Policy (CAP) efforts from 2014–2020 had limited success in cutting emissions, focusing instead on increasing CO 2 removals (European Union, 2022). Early 2024 saw widespread protests by farmers against the climate and nature regulations under the Green Deal reach a fever-pitch across many member states, particularly around cutting subsidies for fossil fuels and pesticides (Dwyer, 2024). This prompted the EU to backtrack on some of its initiatives to cut emissions from agriculture under the proposed 2040 target, including on introducing sectoral targets for the first time. The Commission also rapidly passed a new regulation (EU 2024/1468) to limit some of the environmental requirements for farmers under the CAP (2023-2027), which weakened its environmental impact (European Parliament &amp; European Council, 2024a). The European Court of Auditors (ECA) criticised the 2023–2027 CAP strategic plans for falling short of the EU’s climate and environmental ambitions. Despite being more ambitious than previous plans, the new CAP still lacks alignment with the European Green Deal targets. The ECA recommended that the Commission promote more environmental best practices, estimate CAP’s contribution to the Green Deal, and improve its monitoring of climate and environmental outcomes (ECA, 2024). Key to the EU achieving its 2040 targets would be the introduction of an emission reductions target for the agricultural sector combined with a levy on agricultural emission. In June 2024, Denmark took a first step in this direction by becoming the first country to introduce an agricultural carbon tax and is pushing for this to be applied at an EU level (Mooney et al., 2024) . The influence of farmer protests were significant enough to mark a shift in the EU’s tone on regulating farmers. Critically, the EU will need to find alternative pathways in supporting farmers as they transition to decarbonise and adapt to climate impacts but continuing with exemptions risks failing to deliver on net zero by 2050.</t>
+  </si>
+  <si>
     <t>Agriculture is the second highest emitting sector in India after energy, contributing around 14% of total emissions (excluding LULUCF) (Gütschow &amp; Pflüger, 2023). Given that well over half of India’s population generates an income from agriculture, this sector is particularly important. It is also intricately linked to the power sector, as electricity is used for water pumping in modern irrigation. The heavily-subsidised power supply to agriculture has contributed to the use of inefficient pumps and a resulting excessive use of both water and power (Sagebiel et al., 2015). Demand Side Management (DSM) has been recognised as one of the major interventions to achieve energy efficiency in India’s agricultural sector (MoEFCC, 2021). In 2023, the Bureau of Energy Efficiency (BEE) launched Agricultural Demand Side Management (AgDSM) to reduce overall power consumption, improve efficiencies of ground water extraction, and reduce the subsidy burden on power utilities (BEE, 2023). The PM-KUSUM (Pradhan Mantri Kisan Urja Suraksha evam Utthan Mahabhiyan) scheme aims at setting up 10 GW of decentralised grid-connected solar capacity in barren land, along with 17.5 million solar pumps to reduce the use of diesel in agricultural activity (MNRE, 2020). The government has extended PM-KUSUM scheme until March 2026, as its implementation was significantly affected by the pandemic (The Economic Times, 2023d). India is the second largest emitter of nitrous oxide (N 2 O) after China, contributing around 11% of global nitrous oxide in 2020, mostly due to the use of nitrogen-based fertilisers. The government has implemented measures to reduce N2O emissions associated with fertiliser (urea) use and has programmes in place to assist farmers in reducing emissions and building resiliency (Department of Fertilizers, 2022).</t>
   </si>
   <si>
     <t>Over the past two decades, Indonesia's agriculture sector has seen a declining trend in emissions intensity. Key mitigation areas identified in Indonesia's LTS include rice cultivation, livestock, and fertilisers (Government of Indonesia, 2021). Main mitigation measures include adopting low-emission rice varieties, water-saving paddy cultivation, utilising livestock waste for biogas, improving livestock feed, and expanding the use of organic fertilisers. In response to food security concerns and reducing reliance on imported crops  —  especially in the aftermath of the COVID-19 pandemic  —  former President Joko Widodo launched the Food Estate Programmes as part of the 2020–2024 National Strategic Projects (MoEF, 2020). The government aims to enhance food self-sufficiency and stimulate economic growth by developing large-scale agricultural estates across several provinces, including Central Kalimantan, North Sumatra, with plans for South Sumatra, Papua, and East Nusa Tenggara (Environmental Paper Network et al. , 2021; Tempo, 2021; USDA, 2021). However, these initiatives have failed to enhance food security, instead posing significant environmental and social risks. Past projects resulted in environmental disasters rather than improved food security. The new food estates are expected to span over 5.7 million hectares, exceeding the land area of Croatia (Siborutorop, 2023). Conversion for these estates can occur in Convertible Production Forests (HPK) if certain criteria are met, but critics highlight vague language that could permit the conversion of protected forests (USDA, 2021). The Central Kalimantan project plans to convert 770,000 hectares for rice and cassava cultivation. This area overlaps with regions affected by the failed 1996 Mega Rice Project under President Soeharto, which led to massive peat fires due to peatland clearing and draining (Environmental Paper Network et al. , 2021). Similarly, the Papua project plans to convert two million hectares for sugarcane, mirroring the environmentally damaging Merauke Integrated Food and Energy Estate (MIFEE) launched in 2010 under former President Susilo Bambang Yudhoyono (GRAIN, 2015; Mongabay, 2024a). Indonesia’s forests are among the most biodiverse ecosystems on Earth. Converting these habitats threatens species like Sumatran tigers and orangutans, pushing them closer to extinction (Environmental Paper Network et al. , 2021). To make matters worse, these programmes also have devastating impacts on indigenous communities who depend on forests for their livelihood, leading to displacement and land grabbing without their free, prior, and informed consent (FPIC) or fair compensation (Green Network, 2024; Mongabay, 2024b). The government violated laws designed to protect indigenous land rights, such as Indonesia’s 2013 Constitutional Court ruling that recognised indigenous communities rights to their customary forests (Environmental Paper Network et al. , 2021). The initiatives neglect core issues like food distribution inefficiencies and access to affordable, nutritious food. High logistics costs and infrastructural deficiencies hinder food access, especially in remote areas, driving up prices and exacerbating malnutrition and poverty (WRI Indonesia, 2021). The food estate projects also struggle due to insufficient planning, unsuitable soil conditions, neglect of scientific and local knowledge, and inadequate infrastructure (The Jakarta Post, 2022; Mongabay, 2023). To improve food resilience, Indonesia should move diversify its agriculture to include a wider array of nutritious crops, invest in sustainable practices, and improve its food supply chain and infrastructure (WRI Indonesia, 2021).</t>
   </si>
   <si>
-    <t>Agriculture accounted for 16% of Australia’s total emissions excluding LULUCF in 2024 (DCCEEW, 2024i). Emissions from the sector are expected to remain stable until 2035, falling just 3% below 2023 levels (DCCEEW, 2023b). Emissions in the agriculture sector are mainly derived from enteric fermentation (digestive processes of animals), which accounted for 69% of the sector’s emissions in 2022/23 (DCCEEW, 2023b). Emissions from beef account for over half of agricultural emissions at 52% in 2023. This share is expected to remain steady, accounting for 53% of agricultural emissions in 2035 (DCCEEW, 2023b). Application from lime, urea and fertilisers are other sources of emissions from the sector. The government has allocated an additional AUD 30.8m to the Carbon Farming Outreach Program, aimed at supporting farmers and land managers to reduce emissions and store carbon (Department of Climate Change, 2023c). At COP28, Australia signed the Emirates Declaration on Sustainable Agriculture, Resilient Food Systems and Climate Action to foster adaptation and resilience in the sector (COP28, 2023b).</t>
-  </si>
-  <si>
-    <t>Agriculture is the second biggest contributor to Brazil’s GHG emissions after the land use sector (LULUCF), with emissions consistently growing over the years and reaching its highest reported levels in 2022 at just over 600 MtCO 2 e. Excluding LULUCF emissions, agriculture and livestock represent just over half of the country’s emissions. Almost 75% of the sector’s emissions are methane and nitrous oxide from livestock alone (SEEG, 2023a). If the indirect emissions of the agriculture sector (mostly related to deforestation resulting from the expansion of agricultural land) were considered, the sector would be by far the single largest emissions source in Brazil. However, there are limited policies in place to reduce agricultural emissions. Brazil’s main policy instrument of agricultural activity is the Agricultural Plan (Plano Safra) which aims to facilitate sustainable development by providing credit lines tailored to support crop production and product marketing (CPI, 2023). The Plano Safra for 2023/2024, with a record allocation of BRL 435bn for agricultural financing, designates only 0.5% of this sum for low-carbon measures in the sector (Talanoa, 2023). Furthermore, the new Safra Plan 24/25, unveiled in the first half of 2024, has a 16.5% increase in investment credit lines. This the largest increase in public resources the Safra Plan has received so far (Government of Brazil, 2024). Renovagro, formerly known as ABC+ Plan, supports low-carbon agriculture by financing practices such as land restoration, integrated crop-livestock-forest systems, the production of bio-fertilisers, and others. The ABC+ Plan aims to prevent over one billion tonnes of carbon emissions between 2021-2030, primarily through restoring degraded pastures and planting forests. The Brazilian agricultural sector is heavily dependent on fertilisers. In November 2023, the government approved the revised National Fertiliser Plan 2050 aiming to reduce the country’s dependence on fertiliser imports — currently at 87% of total demand — and meet 45% to 50% of the demand domestically by 2050. The plan outlines strategies such as reactivating idle factories, incentivising new industrial plants, and investing in sustainable nutrient production to achieve the goal. Historically, there is a strong relationship between agriculture expansion and deforestation emissions in Brazil. Forest land is consistently lost to make room for agriculture and cattle ranching. The expansion of soybean plantations became a direct driver of deforestation as it became more financially attractive than cattle ranching (Ionova, 2021). Forests are either directly converted to soybean farms, or soybeans are planted on old pasture, driving deforestation for more pastureland (Kimbrough, 2021). However, expanding the agriculture frontier through deforestation is unnecessary to increase productivity. Brazil has considerable potential to add value and productivity to already available but currently underutilised land by investing in more sustainable and efficient agriculture methods (Observatório do Clima, 2019; Stabile et al., 2020).</t>
-  </si>
-  <si>
-    <t>Agriculture was responsible for around 8% of Canada’s total emissions in 2022 (Environment and Climate Change Canada, 2024). The sector is projected to contribute around 4% of the emissions reductions in its latest 2030 climate plan. While the sector is responsible for 27% of the country’s methane emissions, it will contribute only about 1% of the reductions under Canada’s methane plan. Policy action is a mix of cross-cutting measures, individual targets and programmes and funding initiatives . In 2020 Canada announced a voluntary target of reducing emissions from fertiliser use by 30% below 2020 levels by 2030, a key source of N 2 O emissions (Environment and Climate Change Canada, 2020a). Direct emissions from synthetic nitrogen fertiliser have increased substantially since 2005. The government concluded consultations on the approaches to achieve the target in August 2022, but has not yet announced the next steps (Government of Canada, 2022c, 2022m, 2022n). Some agricultural activities will be eligible for the federal government’s GHG offset system , established in June 2022. Credits generated under the system can be used to reduce the compliance costs of industrial facilities covered by the government’s carbon pricing system (OBPS). Protocols for projects related to livestock feed management and enhancing soil organic carbon are currently being developed and ones for manure management and anaerobic digestions are planned (Environment and Climate Change Canada, 2022d; Government of Canada, 2022c). Health Canada for the first time did not include a meat category, instead choosing to focus on “protein foods” (Government of Canada, 2019a; Health Canada, 2019). It also recommends choosing plant-based protein more often than other sources. Reducing emissions from agriculture , including through shifting the system to a more plant-based diet, will be key to meeting the Paris Agreement’s temperature goal.</t>
-  </si>
-  <si>
-    <t>Agriculture accounts for 11% of the EU’s total GHG emissions in 2021 (UNFCCC, 2023). The EU agricultural sector generates about 60% of its emissions from methane, nearly all of which come from livestock, primarily through enteric fermentation and manure management (Eurostat, 2022). Despite this, methane reduction efforts remain insufficient. While the EU is a co-initiator of the Global Methane Pledge, aiming to cut global methane emissions by 30% below 2020 levels by 2030, only 11 member states have committed to reducing methane from livestock, covering less than 3% of the EU’s livestock units. Leaked reports indicate the EU is not on track to meet its methane reduction target, signifying the need for stronger measures (Ainger, 2022; Changing Markets, 2022). Previous Common Agricultural Policy (CAP) efforts from 2014–2020 had limited success in cutting emissions, focusing instead on increasing CO 2 removals (European Union, 2022). Early 2024 saw widespread protests by farmers against the climate and nature regulations under the Green Deal reach a fever-pitch across many member states, particularly around cutting subsidies for fossil fuels and pesticides (Dwyer, 2024). This prompted the EU to backtrack on some of its initiatives to cut emissions from agriculture under the proposed 2040 target, including on introducing sectoral targets for the first time. The Commission also rapidly passed a new regulation (EU 2024/1468) to limit some of the environmental requirements for farmers under the CAP (2023-2027), which weakened its environmental impact (European Parliament &amp; European Council, 2024a). The European Court of Auditors (ECA) criticised the 2023–2027 CAP strategic plans for falling short of the EU’s climate and environmental ambitions. Despite being more ambitious than previous plans, the new CAP still lacks alignment with the European Green Deal targets. The ECA recommended that the Commission promote more environmental best practices, estimate CAP’s contribution to the Green Deal, and improve its monitoring of climate and environmental outcomes (ECA, 2024). Key to the EU achieving its 2040 targets would be the introduction of an emission reductions target for the agricultural sector combined with a levy on agricultural emission. In June 2024, Denmark took a first step in this direction by becoming the first country to introduce an agricultural carbon tax and is pushing for this to be applied at an EU level (Mooney et al., 2024) . The influence of farmer protests were significant enough to mark a shift in the EU’s tone on regulating farmers. Critically, the EU will need to find alternative pathways in supporting farmers as they transition to decarbonise and adapt to climate impacts but continuing with exemptions risks failing to deliver on net zero by 2050.</t>
-  </si>
-  <si>
-    <t>Agriculture was responsible for 12% of UK emissions in 2022 (DESNZ, 2024a). There has been essentially no progress made in agricultural decarbonisation over the past decade, with emissions in 2022 at the same level as in 2012. In many places, the existing policy portfolio for agricultural decarbonisation is “too little, too late”. There is still no ban on the use of peat in gardening products, and plans to introduce methane-supressing feed products by 2030 are too late. Key actions for the new government include: Introducing policies to hedge against the risk of delivery failure . The existing approach to agricultural decarbonisation has relied heavily on measures which are technological and voluntary in nature: this is a significant delivery risk. Productivity improvements on their own will not necessarily reduce emissions, with a risk that farmers simply increase herd numbers instead of freeing up land. Policies need to be developed to address these risks. Introducing measures to address dietary change and food waste prevention . The existing Government Food Strategy does not introduce measures to support and accelerate dietary shifts, despite the clear health benefits of doing so, and the evidence of consumer appetite for reduced meat consumption (Stewart et al., 2021; UK Government, 2022). The Food Strategy also only addressed food waste from large businesses, despite the majority of food waste occurring at the household, farm and supply-chain stages.</t>
-  </si>
-  <si>
-    <t>In 2020, agriculture accounted for nearly 10% of South Africa’s emissions, with the majority coming from livestock. Emissions from agriculture have remained fairly constant since 2000. There is a limited number of policies in South Africa’s agricultural and forestry sector targeted at climate change mitigation. The National Climate Change Response Policy, the country’s core climate policy published in 2011, names climate smart agriculture (CSA) as a practice “that lowers agricultural emissions, is more resilient to climate changes, and boosts agricultural production” (Government of South Africa, 2011). A number of CSA activities are already in place in South Africa (Nciizah &amp; Wakindiki, 2015), but their expected or actual mitigation impacts are not reported. In 2018, the Department of Agriculture, Forestry and Fisheries has published two draft agricultural policies for public comment: the draft Conservation Agriculture Policy and the draft Climate Smart Agriculture Strategic Framework (DAFF, 2018b, 2018a). Final versions of the policies do not seem to have been published.</t>
-  </si>
-  <si>
-    <t>Emissions from the agriculture sector in 2022 constituted around 16% of total emissions (excluding LULUCF), representing a roughly constant share of total emissions as they have been decreasing at around the same pace as overall emissions (Bundesamt für Umwelt BAFU, 2024b). In 2023, Switzerland released its new Climate Strategy for Agriculture 2050 , replacing the 2011 Climate Strategy for Agriculture with a more ambitious, comprehensive approach based on recent sustainable development and agricultural policy framework serving as a guideline for reducing greenhouse gas emissions and adapting to climate change in the agricultural sector, with a focus on enhancing food security. The strategy sets three primary goals: adapting agricultural production to local climate conditions with at least 50% self-sufficiency rates, reducing the per capita ecological footprint of diets by two-thirds from 2020 levels, and cutting agricultural greenhouse gas emissions by 40% compared to 1990 (this shows an increase in ambitious from a previous one third increase) (Bundesamt für Landwirtschaft BLW; et al., 2023). The strategy includes some measures to achieve these targets, but the plan to make the reduction target mandatory by including it in the third CO 2 Act was dropped after the rejection of the act by the Swiss electorate. Swiss agricultural policy reform faced a significant delay with the suspension of AP22+, the successor of the Agricultural Policy 2014-2017 and 2018-2021. Switzerland’s AP 14-17 and AP 18-21 contained the abolition of unspecific direct payments (livestock subsidies, general acreage payments), additional funds for environmentally friendly production systems, and for the efficient use of resources (e.g., increase in nutrient efficiency and ecological set-aside areas, reduction of ammonia emissions) (Schweizerische Eidgenossenschaft, 2020c). In 2020 and 2021, Parliament halted further policy development until the Federal Council could submit a detailed report on the future direction of agricultural policy. This June 2022 report aimed to provide a long-term vision, addressing unresolved issues from previous policies and the need for more sustainable agricultural practices. Following this, work on AP30+ began, with the Federal Council scheduled to review and discuss proposals in 2026, with hopes of finally implementing a sustainable and cohesive agricultural policy framework (Der Bundesrat, 2022). Switzerland’s unique direct democratic system, which allows citizens to propose constitutional amendments via initiatives, has not been effective in advancing agricultural policy reform. Despite efforts – such as the 2021 initiatives on clean drinking water and pesticide reduction, both rejected by 61% of voters, and the 2024 biodiversity initiative, rejected with 63% – all three proposals were blocked at the ballot, largely due to the strong influence of the farming lobby (Müller, 2021; Rigendinger, 2024)</t>
-  </si>
-  <si>
-    <t>Greenhouse gas emissions from the agriculture sector made up 9% of US emissions in 2022. Between 1990 and 2022, agriculture emissions increased by 8%, primarily from the growth of the livestock sector and the intensification of farming practices. Nitrous oxide emissions from soils made up half of agricultural emissions. Enteric fermentation and manure management from livestock represented other significant emissions sources. Agricultural emissions decreased in 2022 compared to the previous year. However, this decrease was not the result of new policy, but is rather attributable to the decline in herd size—the smallest since the 1960s—due to drought conditions (U.S. Environmental Protection Agency, 2024h). The Inflation Reduction Act (IRA) allocates USD 19.5bn for mitigation activities in the agriculture sector. The act mainly boosts the funding of existing conservation programmes, such as the Environmental Quality Incentives Program (EQIP) and the Conservation Stewardship Program (CSP) (Monke et al., 2022). Both programmes offer financial and technical support to farmers to implement climate-friendly practices, including nutrient management, cover crops, low or no-tillage, and agroforestry. Historically, farmers have struggled to access funding under such programmes due to high demand and limited institutional capacity. These barriers could potentially be addressed by better distributing programme spending (e.g. by capping funds per farm), limiting the funding that goes to ineffective conservation practices, and increasing agency resources (Happ, 2023; Tham, 2023). However, the efficacy of existing programmes to address on-farm emissions has come into question. Between 2019 and 2020, only one-fifth of total EQIP spending reportedly went towards the implementation of agricultural practices that directly reduce GHG emissions (Schechinger, 2022). While programmes like EQIP and CSP are now bolstered by IRA funding, they still face structural issues that may impede climate mitigation. In 2024, 15 new practices were added to the 'climate-smart' category under the EQIP, but many of the new measures do not have proven climate benefits. A significant portion of EQIP funding goes towards manure management practices, including biodigesters that convert manure into biogas, which can be sold for profit and, therefore, may incentivise farmers to maintain or increase their herd sizes (Happ, 2024; Schechinger, 2024). The IRA has also funded several programmes to support renewable energy use in the agriculture sector, including loans and grants for farmers who implement energy efficient equipment or underutilised renewable energy technologies (The White House, 2023b). However, certain provisions of these programmes could lead to perverse incentives. For instance, the Rural Energy for America Program (REAP) subsidises biogas production. However, in combination with existing state subsidies for cattle farmers to produce biomass, REAP’s subsidies could lead to intensified livestock production (Sainato, 2022). The Farm Bill is a policy that heavily influences farmers’ decisions on what food to produce and how to produce it. The 2018 bill expired last year, but was temporarily extended through FY2024. Its official renewal was pushed to 2024 since Congress could not come to an agreement on the contents of the new bill. In 2024, the Republican-led House Committee on Agriculture released a draft bill that could deter climate progress in the agriculture sector. The bill would reallocate up to USD 14.4bn from the IRA that is specifically meant for climate-friendly farming practices to cover all conservation practices. The bill would also reinstate the requirement that 50% of EQIP funds are channelled to livestock operations (House Committee on Agriculture, 2024). However, the fate of the Farm Bill and its contents remain unclear as it has yet to arrive on the House floor. There are still considerable policy gaps in addressing agricultural emissions. Beyond the structural issues of existing programmes (i.e. EQIP, CSP), the US lacks regulations or plans for addressing emissions from animal production. There are no incentives for reducing the volume of animal agriculture or for promoting plant-based foods and crops (CBD, 2020). Instead, Concentrated Animal Feeding Operations (CAFOs), which are detrimental to animal and environmental welfare, continue to be subsidised by the government (Happ, 2024). The government also lacks policies on the demand-side. The US has one of the highest rates of meat and dairy consumption in the world, but food consumption patterns have not been addressed by the government. Historically, the meat industry has lobbied against key demand-side policies, such as changes to dietary guidelines, which constitute the basis of federal nutrition programmes and policy (Bottemiller Evich, 2016; Sebastian, 2024). Without a shift in diets, related emissions may increase by 9% in the US as a result of population growth (Heller et al., 2020). The volume of food waste in the US is very high. Approximately one-third of available food is lost or wasted. Surplus, wasted food results in significant embodied emissions across the supply chain, and has been estimated to account for 6% of the country’s total GHG emissions (Harwood et al., 2023). The US Environmental Protection Agency (EPA) has set a goal to halve food loss and waste by 2030. However, the target puts little focus on food losses, which occur during the production and processing stages, due to a lack of data (U.S. Environmental Protection Agency, 2024o). The US is not on track to reach this target due to insufficient federal and state-level policies. Interventions to prevent food waste, such as policies on date labels, are insufficient. At the subnational level, some states hinder the recycling of food waste through bans on diverting food waste streams towards animal feed (ReFED, 2024).</t>
-  </si>
-  <si>
     <t>Argentina’s average share of emissions from Land Use, Land-Use Change and Forestry (LULUCF) over the past 20 years is more than 20% of the country’s total emissions. Between 2014 and 2019, however, emissions from LULUCF started falling up to as low as to 3% of total emissions, only to bounce back to 22% in 2020. This indicates that Argentina’s recent approach to curbing land use emissions might be working and would need to be maintained, updated, and reinforced. Argentina signed the Glasgow declaration on forests and land use during COP26. LULUCF emissions in Argentina were around 51 MtCO 2 e in 2022 according to its first BTR (Government of Argentina, 2024a), accounting for ~20% of national GHG emissions. LULUCF emissions were exceptionally high in 2020 but have otherwise been on a downward trend partially thanks to the implementation of the 2007 Native Forests Law (Law 26.331). They decreased by 41% in 2020 compared to 2007 levels but remain a significant source of emissions in Argentina. Argentina has around 54 million hectares of native forests, as well as 1.3 million hectares of cultivated forests. According to its fourth BUR, in 2018 some 187,000 hectares were lost due to the expansion of agricultural land, to forest fires, and the overexploitation of forest resources (Government of Argentina, 2022c). The government acknowledges that some of this land clearing is illegal, and that better enforcement of forestry regulations is needed. According to the Forest Declaration Assessment, deforestation in Argentina remains at high levels with 140,000 ha lost in 2023 (The forest declaration Assessment, 2024). The Native Forests Law aims at slowing the reduction of Argentina’s native forest surface, focused on achieving net-zero deforestation. The law set minimum budgets to be spent on forest protection and established a capacity building scheme and requirements for provinces to comprehensively monitor and track forest areas. It also established the National Fund for Enriching and Conserving Native Forests that disburses funds to provinces that protect native forests ( Law 26331 , 2007). As early as the late 1990s, Argentina implemented Law 25.080 to promote investments in afforestation and prevent forest degradation ( Ley 25.080 , 1999). According to Argentina’s fourth BUR, this law, amended by Law 26.432 in 2008, has contributed to a total of 1.3 million hectares of forest area, with a target of 1.6 million in 2030 (Government of Argentina, 2022c). However, independent sources claim that the programme has been de-funded and ecosystem services payments have been greatly decreased in real terms, and its effectiveness to continue to support afforestation and preservation is at risk (Escobar, 2021). Alongside the implementation of its PANByCC, Argentina launched its ForestAr 2030 initiative, which aims to develop a broad stakeholder dialogue and strategy to conserve natural forests and to deliver on the country’s commitment to reducing climate change while achieving other sustainable development benefits. In the context of this initiative, the government created the National Plan for the Restoration of Native Forests through Resolution 267/2019, which seeks to restore 20 million ha of native forest per year by 2030 ( Resolución 267/2019 , 2019). Recent studies show that for Argentina’s AFOLU sector to get close to carbon neutrality, the LULUCF sector would need to become a net emissions sink as fast as possible, and reach around -71 to -138 MtCO 2 e per year just to neutralise emissions from agriculture by 2050 (Frank et al., 2023; Keesler &amp; Blanco, 2024). To achieve this, Argentina would need to set out stronger forestry policies, including ambitious targets and well-designed implementation and enforcement mechanisms, as well as improved coordination with subnational governments.</t>
   </si>
   <si>
     <t>Between 1990 and 2022, Argentina’s waste emissions more than doubled, accounting for 7% (23.3 MtCO 2 e) of Argentina’s total GHG emissions in 2020. Waste production is in the order of 1kg per person per day in Argentina (Government of Argentina, 2022c). A recent study has also shown that Argentina was home to around 100 super emitter events from waste sites in and around Buenos Aires between 2019 and 2023, reaching up to 230 tonnes of methane per hour (The Guardian, 2024). In 2021, the Environment Ministry released Resolution 290/2021 establishing the National Programme to Strengthen the Circular Economy. This policy aims at improving waste collection and treatment systems, reducing waste and increasing recycling rates. According to Argentina’s Fourth BUR, there has been progress on segmented waste collection and treatment. Big urban centres have also implemented systems to capture and store or destroy methane from waste, while in the rest of the country, solid urban waste is still disposed of in open landfills without sanitary treatment. Argentina’s 2022 climate strategy also includes measures and targets for the waste sector. In particular, it aims at eradicating open landfills by 2030, and to reduce food loss by 10-30% and waste by 5-10% by 2025 below 2015 levels. These targets are also part of Argentina’s National Plan for Food Loss and Waste Reduction (Government of Argentina, 2022d).</t>
   </si>
   <si>
+    <t>The waste sector accounted for 3% of total emissions excluding LULUCF in 2024 (DCCEEW, 2024i). Emissions from the sector are expected to remain stable until 2035, falling just 1% (DCCEEW, 2023b). Emissions are mainly due to methane related to landfill, wastewater treatment, waste incineration and treatment of solid waste. The National Waste Policy published in 2019, and subsequent Annexure published in 2022, do not focus on reducing emissions from this sector (Department of Climate Change, 2022). It includes a target of reducing total waste generated in Australia by 10% per person by 2030.</t>
+  </si>
+  <si>
+    <t>Waste sector emissions accounted for around 3% of Canada’s total emissions in 2022, but 18% of the country’s methane emissions (Environment and Climate Change Canada, 2024). Municipal landfills are the primary source of emissions. Efforts to reduce methane emissions to date have only been able to balance out the increased waste generated from a growing population and thus current methane levels from landfills are at about the same level as 20 years ago (Environment and Climate Change Canada, 2022d). Canada anticipates cutting methane emissions from the waste sector by 45% between 2020 and 2030 (Environment and Climate Change Canada, 2022d). The government issued draft new regulations for consultation in 2023; final regulations are expected in 2024 (Environment and Climate Change Canada, 2022b; Government of Canada, 2023d). In June 2022, the government finalised the details around generating offset credits from landfill methane recovery and destruction projects (Government of Canada, 2022j). These credits can be used to reduce the compliance costs of industrial facilities covered by the government’s carbon pricing system (OBPS). The Food Waste Reduction Challenge (discussed in the agriculture section) will also contribute to avoiding emissions in the sector.</t>
+  </si>
+  <si>
+    <t>Singapore recovers heat from the incineration of waste to produce electricity. In 2020, waste to energy provided about 2.3% of Singapore’s total electricity generated (National Environment Agency, 2022). Yet, the waste sector just accounts for 0.6% of Singapore’s total emissions (National Environment Agency, 2018). To raise awareness of waste issues and the need to recycle resources Singapore declared 2019 as “Year Towards Zero Waste“ (Ministry of the Environment and Water Resources, 2019a). In the same year, the government launched the Zero Waste Masterplan detailing strategies to reduce waste sent to Semakau Landfill by 30% by 2030, extending the landfill’s lifespan beyond 2035 and reducing incineration emissions (Ministry of the Environment and Water Resources, 2019b). The government also introduced the Resource Sustainability Act 2019 to enforce mandatory packaging data reporting by 2020, Extended Producer Responsibilities for e-waste by 2021 and mandatory food waste segregation for treatment from 2024, and Extended Producer Responsibility for packaging, including plastics by 2025 (Ministry of the Environment and Water Resources, 2019b). The government aims to increase the waste recycling rate from 52% in 2022 to 70% by 2030 (National Environment Agency, 2022).</t>
+  </si>
+  <si>
+    <t>Emissions from the waste sector in Switzerland made up roughly 3% of total GHG emissions (excluding LULUCF) in 2022 and registered an absolute decrease of almost 50% since 1990 (Bundesamt für Umwelt BAFU, 2024b). Since 2000, the disposal of untreated municipal waste into landfill has been prohibited, with an increase in the capacity of waste incineration plants implemented to accommodate this ban (Schweizerische Eidgenossenschaft, 2020c). These incineration plants have substantially reduced methane emissions from Swiss landfills and produce roughly 2% of Switzerland’s total energy consumption.</t>
+  </si>
+  <si>
+    <t>According to the UAE’s latest National Communication to the UNFCCC, the waste sector accounted for 6% of the country’s emissions in 2021 (Government of the UAE, 2024a). The UAE’s LTS sets a target for waste emissions, which are set to increase by 8% above 2019 levels by 2030 and should decrease by 75% below 2019 levels in 2050. Emissions from the waste sector are expected to reach 14 MtCO 2 e in 2030, up from 13 MtCO 2 e in 2019 (Government of the UAE, 2023a). This includes emissions from landfills as well as emissions stemming from energy used to transport and treat waste. In January 2021, the UAE launched its Circular Economy Policy 2031, establishing a Circular Economy Council, tasked with supervising the implementation of waste reduction policies that also target the manufacturing sector. In May 2022, the Sharjah Waste-to-Energy plant was launched, with a capacity of 30 MW. A further 200 MW plant is planned in Dubai and a 70 MW plant in Abu Dhabi, both expected to be operational in 2024 (Government of the UAE, 2023a; Sharma, 2022). However, the UAE’s Circular Economy Policy has no concrete waste or emissions reduction targets. We were not able to check whether its previous target of diverting 75% of its waste from landfills by 2021 (Government of the UAE, 2019) has been achieved. The UAE’s LTS includes a target of diverting 80% of its waste by 2031 and 90% by 2035. It also plans to capture the remaining methane produced in its landfills and retrofitting its waste-to-energy plants with CCS. Under its net zero scenario, the UAE expects waste to contribute around 3 MtCO 2 e by 2050.</t>
+  </si>
+  <si>
+    <t>The waste sector made up only 2.7% of national emissions in 2021 but contributed to 17% of anthropogenic methane emissions (U.S. Environmental Protection Agency, 2023f). Therefore, addressing methane emissions from landfills is a key pillar of the US Methane Emissions Reduction Action Plan. In 2021, the Biden Administration finalised emissions standards to ensure that large municipal landfills significantly reduce their methane emissions, and the US Environmental Protection Agency (EPA) has developed a Landfill Methane Outreach Program to support methane collection and distribution at smaller, unregulated landfills (The White House, 2021b). The IRA has not led to significant policies or programmes in the waste sector, aside from some funding to improve methane monitoring and to develop a better method to measure fugitive methane sources (e.g. landfills) (The White House, 2023b). Recently, the EPA has been sued by environmental groups for failing to update its landfill emissions accounting methodology, which it has not revised since 1998. The current emissions factors reportedly underestimate the emissions released from landfills from several pollutants, including nitrogen oxide, by as much as 25%. As a result of the lawsuit, the EPA has agreed to evaluate whether methodology needs updating and to suggest new emissions factors in case updating is required (Quinn, 2023).</t>
+  </si>
+  <si>
     <t>In 1990 the German waste sector emitted 38 MtCO 2 e (3% of total emissions). By 2021, emissions were at just 4 MtCO 2 e - a decrease of 89% and contributing only about 1% of total emissions (UBA, 2023b). This reduction was mainly achieved by ending the disposal of untreated residential waste and the increased utilisation of energy and materials from waste (Umweltbundesamt, 2017). Since 2005, landfilling of biodegradable waste has been prohibited in Germany. From 2024, CO 2 emissions from waste incineration are part of the emissions trading scheme for fuels (BEHG).</t>
   </si>
   <si>
-    <t>The waste sector accounted for 3% of total emissions excluding LULUCF in 2024 (DCCEEW, 2024i). Emissions from the sector are expected to remain stable until 2035, falling just 1% (DCCEEW, 2023b). Emissions are mainly due to methane related to landfill, wastewater treatment, waste incineration and treatment of solid waste. The National Waste Policy published in 2019, and subsequent Annexure published in 2022, do not focus on reducing emissions from this sector (Department of Climate Change, 2022). It includes a target of reducing total waste generated in Australia by 10% per person by 2030.</t>
-  </si>
-  <si>
-    <t>Waste sector emissions accounted for around 3% of Canada’s total emissions in 2022, but 18% of the country’s methane emissions (Environment and Climate Change Canada, 2024). Municipal landfills are the primary source of emissions. Efforts to reduce methane emissions to date have only been able to balance out the increased waste generated from a growing population and thus current methane levels from landfills are at about the same level as 20 years ago (Environment and Climate Change Canada, 2022d). Canada anticipates cutting methane emissions from the waste sector by 45% between 2020 and 2030 (Environment and Climate Change Canada, 2022d). The government issued draft new regulations for consultation in 2023; final regulations are expected in 2024 (Environment and Climate Change Canada, 2022b; Government of Canada, 2023d). In June 2022, the government finalised the details around generating offset credits from landfill methane recovery and destruction projects (Government of Canada, 2022j). These credits can be used to reduce the compliance costs of industrial facilities covered by the government’s carbon pricing system (OBPS). The Food Waste Reduction Challenge (discussed in the agriculture section) will also contribute to avoiding emissions in the sector.</t>
-  </si>
-  <si>
     <t>Waste sector emissions have continuously fallen since the mid-90s, dropping by 40% between 1990 and 2021 (European Environment Agency, 2023a). Regulation of waste sector emissions is covered by the Effort Sharing Regulation (ESR), along with those from transport, buildings, and agriculture. Combined, emissions from these sectors needs to decrease by 40% below 2005 levels by 2030 (European Parliament &amp; Council of the European Union, 2023e). As of 2024, the European Parliament has voted to strengthen the proposed Extended Producer Responsibility (EPR) scheme for textiles. The European Parliament's approval of Extended Producer Responsibility (EPR) for textiles is seen as a step forward, but it lacks specific waste prevention targets and effective management strategies. Meanwhile, the EU Council has prioritised textile reforms, neglecting critical food waste reduction measures. This approach is viewed as insufficiently ambitious, highlighting the need for stronger commitments to ensure both textile and food waste are managed effectively for sustainable outcomes (Zero Waste Europe, 2024) . The current design may not adequately incentivise producers to improve product design for longevity and recyclability, with some suggesting that the focus remains too heavily on waste management rather than preventing waste generation.</t>
   </si>
   <si>
-    <t>Singapore recovers heat from the incineration of waste to produce electricity. In 2020, waste to energy provided about 2.3% of Singapore’s total electricity generated (National Environment Agency, 2022). Yet, the waste sector just accounts for 0.6% of Singapore’s total emissions (National Environment Agency, 2018). To raise awareness of waste issues and the need to recycle resources Singapore declared 2019 as “Year Towards Zero Waste“ (Ministry of the Environment and Water Resources, 2019a). In the same year, the government launched the Zero Waste Masterplan detailing strategies to reduce waste sent to Semakau Landfill by 30% by 2030, extending the landfill’s lifespan beyond 2035 and reducing incineration emissions (Ministry of the Environment and Water Resources, 2019b). The government also introduced the Resource Sustainability Act 2019 to enforce mandatory packaging data reporting by 2020, Extended Producer Responsibilities for e-waste by 2021 and mandatory food waste segregation for treatment from 2024, and Extended Producer Responsibility for packaging, including plastics by 2025 (Ministry of the Environment and Water Resources, 2019b). The government aims to increase the waste recycling rate from 52% in 2022 to 70% by 2030 (National Environment Agency, 2022).</t>
-  </si>
-  <si>
-    <t>Emissions from the waste sector in Switzerland made up roughly 3% of total GHG emissions (excluding LULUCF) in 2022 and registered an absolute decrease of almost 50% since 1990 (Bundesamt für Umwelt BAFU, 2024b). Since 2000, the disposal of untreated municipal waste into landfill has been prohibited, with an increase in the capacity of waste incineration plants implemented to accommodate this ban (Schweizerische Eidgenossenschaft, 2020c). These incineration plants have substantially reduced methane emissions from Swiss landfills and produce roughly 2% of Switzerland’s total energy consumption.</t>
-  </si>
-  <si>
-    <t>According to the UAE’s latest National Communication to the UNFCCC, the waste sector accounted for 6% of the country’s emissions in 2021 (Government of the UAE, 2024a). The UAE’s LTS sets a target for waste emissions, which are set to increase by 8% above 2019 levels by 2030 and should decrease by 75% below 2019 levels in 2050. Emissions from the waste sector are expected to reach 14 MtCO 2 e in 2030, up from 13 MtCO 2 e in 2019 (Government of the UAE, 2023a). This includes emissions from landfills as well as emissions stemming from energy used to transport and treat waste. In January 2021, the UAE launched its Circular Economy Policy 2031, establishing a Circular Economy Council, tasked with supervising the implementation of waste reduction policies that also target the manufacturing sector. In May 2022, the Sharjah Waste-to-Energy plant was launched, with a capacity of 30 MW. A further 200 MW plant is planned in Dubai and a 70 MW plant in Abu Dhabi, both expected to be operational in 2024 (Government of the UAE, 2023a; Sharma, 2022). However, the UAE’s Circular Economy Policy has no concrete waste or emissions reduction targets. We were not able to check whether its previous target of diverting 75% of its waste from landfills by 2021 (Government of the UAE, 2019) has been achieved. The UAE’s LTS includes a target of diverting 80% of its waste by 2031 and 90% by 2035. It also plans to capture the remaining methane produced in its landfills and retrofitting its waste-to-energy plants with CCS. Under its net zero scenario, the UAE expects waste to contribute around 3 MtCO 2 e by 2050.</t>
-  </si>
-  <si>
-    <t>The waste sector made up only 2.7% of national emissions in 2021 but contributed to 17% of anthropogenic methane emissions (U.S. Environmental Protection Agency, 2023f). Therefore, addressing methane emissions from landfills is a key pillar of the US Methane Emissions Reduction Action Plan. In 2021, the Biden Administration finalised emissions standards to ensure that large municipal landfills significantly reduce their methane emissions, and the US Environmental Protection Agency (EPA) has developed a Landfill Methane Outreach Program to support methane collection and distribution at smaller, unregulated landfills (The White House, 2021b). The IRA has not led to significant policies or programmes in the waste sector, aside from some funding to improve methane monitoring and to develop a better method to measure fugitive methane sources (e.g. landfills) (The White House, 2023b). Recently, the EPA has been sued by environmental groups for failing to update its landfill emissions accounting methodology, which it has not revised since 1998. The current emissions factors reportedly underestimate the emissions released from landfills from several pollutants, including nitrogen oxide, by as much as 25%. As a result of the lawsuit, the EPA has agreed to evaluate whether methodology needs updating and to suggest new emissions factors in case updating is required (Quinn, 2023).</t>
-  </si>
-  <si>
     <t>While Argentina’s carbon emissions have almost doubled since 1990, its methane emissions have only increased moderately, reaching roughly 12% above 1990 levels in 2020 (Government of Argentina, 2023a). Nevertheless, methane still accounts for 29% of all national GHG emissions in terms of global warming potential, above the global average of around 20% (Global Methane Initiative, 2022). In 2023, Argentina ranked 13th worldwide in terms of methane emissions, with most emissions coming from the agriculture sector (IEA, 2024c). While methane is covered in Argentina’s NDC target, the NDC contains no specific targets nor actions aimed at reducing methane emissions. Current methane emissions are 100.7 MtCO 2 e (in AR4 GWP), with two thirds related to livestock. Argentina is one of the 95 countries that signed the methane pledge. Meeting the 30% methane reduction target would mean a 28.5 MtCO 2 e reduction by 2030.</t>
   </si>
   <si>
@@ -452,34 +451,22 @@
     <t>Methane is a major contributor to emissions in China, accounting for 12.6% of total GHG emissions (excl. LULUCF) in 2018, according to China’s most recent national inventory. Our estimates indicate that methane emissions have surpassed 1.4 GtCO₂e per year since 2020. The primary sources of emissions are coal mine fugitives (~40%), agriculture, including livestock and rice cultivation (~42%), and waste and waste water (~10%) (Government of China, 2023; Patel, 2023). Methane is not included in China's 2030 carbon peaking target (which only covers CO₂) but is included in the 2060 carbon neutral goal. China’s updated NDC does not have explicit reduction targets for non-CO₂ gases, including methane, though Measure 13 outlines the goal to accelerate control of these gases and phase out HFC gases under the Kigali Amendment (see section on F-gases above). The long-awaited Methane Action Plan was published in November 2023 (State Council of China, 2023a).While the plan sets basic directions to control methane emissions across sectors as well as setting short-term targets on such measures as the utilisation of manure in livestock and, domestic waste recycling, and harmless disposal of sludge, it does not specify any quantitative emission reduction targets or commitments. A notable emphasis within the action plan is the prioritisation of establishing a methane measurement, reporting, and verification system, despite the absence of a firm commitment or a defined timeline. China has not adopted the Global Methane Pledge (launched at COP26), in which signatories agreed to cut emissions in all sectors by 30% globally over the next decade.</t>
   </si>
   <si>
+    <t>14% of the UK’s total emissions in 2022 came from methane (DESNZ, 2024a), with 80% of these emissions coming from agriculture and waste. The UK is also a signatory to the Global Methane Pledge, which sets a target of reducing methane emissions by 30% over 2020–2030. However, to date methane emission reductions are not happening fast enough in the UK. On average, methane emissions fell 0.9 MtCO 2 e/yr over 2015–2022. This would need to double to over 1.9 Mt CO 2 e/yr to reach the current 2030 targets. Key actions for the government to take include: Publishing plans to capture methane emissions from landfill sites, as well as improving the monitoring of landfill emissions. Develop plans to reduce methane emissions from agriculture . This should include accelerating the deployment of methane-supressing feed products within the industry, as well as promoting measures to cut demand for meat and dairy. Track, monitor and transparently report on the UK’s progress towards the Global Methane Pledge.</t>
+  </si>
+  <si>
+    <t>In 2022, the methane sector accounted for 10% of total GHGs, the majority coming from the waste and energy sectors (Gütschow et al., 2024). At COP26, Saudi Arabia signed the Global Methane Pledge, in which signatories agreed to cut methane emissions in all sectors by 30% globally over the next decade. While its 2021 NDC does not have explicit emission reduction targets for non-CO 2 gases, it includes several measures to manage methane emissions, such as the objective to achieve zero flaring in the oil and gas industry (Kingdom of Saudi Arabia, 2021b). However, Saudi Arabia is still planning to ramp-up its oil production capacity towards the end of the decade, making it in practice difficult to reduce its methane emissions.</t>
+  </si>
+  <si>
+    <t>Methane is responsible for around 16% of Turkiye’s emissions and comes predominantly from agriculture and waste (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2023). Türkiye has not signed the global methane pledge .</t>
+  </si>
+  <si>
+    <t>The UAE signed the methane pledge at COP26, in which signatories agreed to cut methane emissions in all sectors by 30% globally over the next decade. According to the UAE’s latest inventory, methane represented ~7% of total GHG emissions in 2021, mostly stemming from upstream fossil fuel production and waste (Government of the UAE, 2024a). The UAE already includes methane in its NDC and has some policies in place designed to reduce both energy and waste-related methane emissions.</t>
+  </si>
+  <si>
+    <t>Methane is an important source of GHG emissions in the US, representing 15% of total GHG emissions in 2022, which are split between the oil and gas industry (37%), agriculture (36%), waste (19%), and land use, land-use change and forestry (LULUCF) (8%) sectors (U.S. Environmental Protection Agency, 2024o). Alongside the EU, the US spearheaded the launch of the Global Methane Pledge. The Biden Administration released its Methane Emissions Reduction Action Plan in 2021. The plan seeks to reduce emissions from all major sources through regulations, financial incentives, and public-private partnerships. The plan also includes USD 20bn in new investments targeted at reducing methane emissions (The White House, 2022a). The IRA provided USD 1.5bn for the Methane Emissions Reduction Fund, which aims to monitor and reduce emissions from petroleum and natural gas systems through financial and technical assistance, but also potentially locks in new “brown” infrastructure. It also established a ‘waste emissions charge’ per ton of methane emissions to oil and gas facilities that exceed emissions thresholds (The White House, 2023b).</t>
+  </si>
+  <si>
     <t>In 2022, methane emissions accounted for 11% of the EU’s total GHG emissions. The majority of these emissions came from the agricultural sector, followed by waste management and energy. Methane emissions have fallen about 60% since 1990 (UNFCCC, 2024). The EU signed the methane pledge at COP26 in 2021. Methane is covered in the overall scope of the EU’s latest NDC from 2023 but is also specifically mentioned in the context of mitigating methane emissions from maritime transport under the revised EU ETS. In 2020, the EU released its methane reduction strategy laying out its intention to cut emissions from energy, agriculture, and waste. As part of the strategy, in 2024, the EU adopted the regulation on methane emission reduction in the energy sector (EU) 2024/1787 (European Parliament &amp; European Council, 2024d), covering emissions from oil and fossil gas exploration, production, transmission, distribution, coal mining and imports of fossil fuels. The regulation introduces new measures to measure, report and verify (MRV) methane emissions, methane abatement measures and a ban on routine venting and flaring. While a step in the right direction, the regulation does not go far enough – starting with the lack of an overarching methane reduction target and prolonged implementation timeline, which does not reflect the urgency and pace needed. In addition, many exemptions and loopholes diminish the regulation's effectiveness. The regulation excludes the petrochemical sector and LNG consumption. Methane intensive LNG can be expected to grow considerably, given the signal that other EU polices are pushing. For example, the FuelEU Maritime for LNG fuel in shipping, as well as the build up of LNG infrastructure over the past few years following the shift away from imported Russian gas (Climate Action Network Europe, 2023). A recent study finds that LNG as a fuel has an emission footprint 33% greater than that of coal due to the associated methane leakage (Howarth, 2024). Additionally, despite representing the largest source of methane, the agricultural sector is not included. Instead, it is counted under the overall GHG emission reduction target for member states under the Revised Effort Sharing Directive.</t>
-  </si>
-  <si>
-    <t>14% of the UK’s total emissions in 2022 came from methane (DESNZ, 2024a), with 80% of these emissions coming from agriculture and waste. The UK is also a signatory to the Global Methane Pledge, which sets a target of reducing methane emissions by 30% over 2020–2030. However, to date methane emission reductions are not happening fast enough in the UK. On average, methane emissions fell 0.9 MtCO 2 e/yr over 2015–2022. This would need to double to over 1.9 Mt CO 2 e/yr to reach the current 2030 targets. Key actions for the government to take include: Publishing plans to capture methane emissions from landfill sites, as well as improving the monitoring of landfill emissions. Develop plans to reduce methane emissions from agriculture . This should include accelerating the deployment of methane-supressing feed products within the industry, as well as promoting measures to cut demand for meat and dairy. Track, monitor and transparently report on the UK’s progress towards the Global Methane Pledge.</t>
-  </si>
-  <si>
-    <t>In 2022, the methane sector accounted for 10% of total GHGs, the majority coming from the waste and energy sectors (Gütschow et al., 2024). At COP26, Saudi Arabia signed the Global Methane Pledge, in which signatories agreed to cut methane emissions in all sectors by 30% globally over the next decade. While its 2021 NDC does not have explicit emission reduction targets for non-CO 2 gases, it includes several measures to manage methane emissions, such as the objective to achieve zero flaring in the oil and gas industry (Kingdom of Saudi Arabia, 2021b). However, Saudi Arabia is still planning to ramp-up its oil production capacity towards the end of the decade, making it in practice difficult to reduce its methane emissions.</t>
-  </si>
-  <si>
-    <t>Methane is responsible for around 16% of Turkiye’s emissions and comes predominantly from agriculture and waste (Republic of Türkiye Ministry of Environment Urbanisation and Climate Change, 2023). Türkiye has not signed the global methane pledge .</t>
-  </si>
-  <si>
-    <t>The UAE signed the methane pledge at COP26, in which signatories agreed to cut methane emissions in all sectors by 30% globally over the next decade. According to the UAE’s latest inventory, methane represented ~7% of total GHG emissions in 2021, mostly stemming from upstream fossil fuel production and waste (Government of the UAE, 2024a). The UAE already includes methane in its NDC and has some policies in place designed to reduce both energy and waste-related methane emissions.</t>
-  </si>
-  <si>
-    <t>Methane is an important source of GHG emissions in the US, representing 15% of total GHG emissions in 2022, which are split between the oil and gas industry (37%), agriculture (36%), waste (19%), and land use, land-use change and forestry (LULUCF) (8%) sectors (U.S. Environmental Protection Agency, 2024o). Alongside the EU, the US spearheaded the launch of the Global Methane Pledge. The Biden Administration released its Methane Emissions Reduction Action Plan in 2021. The plan seeks to reduce emissions from all major sources through regulations, financial incentives, and public-private partnerships. The plan also includes USD 20bn in new investments targeted at reducing methane emissions (The White House, 2022a). The IRA provided USD 1.5bn for the Methane Emissions Reduction Fund, which aims to monitor and reduce emissions from petroleum and natural gas systems through financial and technical assistance, but also potentially locks in new “brown” infrastructure. It also established a ‘waste emissions charge’ per ton of methane emissions to oil and gas facilities that exceed emissions thresholds (The White House, 2023b).</t>
-  </si>
-  <si>
-    <t>According to the targets anchored in the climate law, the energy sector (electricity and heat supply) will have to limit its GHG emissions to 108 MtCO 2 e by 2030, a reduction of 62% below 1990 levels. In 2023, total emissions from the energy supply sector stood at 205 MtCO 2 e, a decrease of 51 MtCO 2 e compared to the previous year. Renewable energy covers half of gross electricity consumption for the first time, and coal-fired power generation declined as electricity demand decreased (Expertenrat für Klimafragen, 2024). Despite these positive developments, the sluggish expansion of wind energy and the extensive new investments in gas infrastructure pose a risk to Germany's ability to achieve its longer-term targets for 2030 and 2045. A slow and gradual coal phase-out by 2038 puts pressure on global emissions budgets, which require a coal phase-out by 2030 (CAT, 2023). The government intends to phase out coal by 2030, with phase outs already negotiated for the western coal mines and is attempting to do the same in Eastern Germany. With the policies currently adopted, Germany could exceed its 2030 power sector target. However, the official projections from the UBA report assumes that the renewable electric capacity increases as in the government's original plans from early 2022. For solar energy, this has been the case. For wind energy, implementation has once again fallen behind in 2023. The price for CO 2 emission allowances in the EU Emissions Trading System (EU ETS), has recently fallen steadily from a level of EUR 100/tCO 2 in February 2023 to a low of EUR 52/tCO 2 in April 2024, and is currently between EUR 60-75/tCO 2 [1] . With the reform of the EU ETS, it was expected that these prices would increase further. Higher prices make coal very unattractive compared to renewables. [1] Carbon Price Tracker | Ember (ember-climate.org) Renewables Accelerating renewable energy expansion is a priority of the German government and has been approached in a very comprehensive manner through increased targets and planned legislative measures that aim at overcoming very specific challenges for renewables in Germany. The Renewable Energy Law (EEG) and the wind energy offshore law (WindSeeG) were revised in 2023, determining that renewable energy installations are of public interest so they can be prioritised over other issues, and give particular support for rooftop solar PV, increase the focus on participatory models for citizens, support storage, and redirect biogas towards flexible power generation (BMWK, 2023f, 2023d). Electricity generation from renewables stands at 60% January to July 2024 (Fraunhofer ISE, 2024c). The German government aims to raise the share of electricity generated from renewable energy to 80% of gross electricity consumption by 2030 (BMWK, 2022) while increasing overall electricity use to further electrify the transport, buildings and industry sectors. This goal is not yet fully aligned with the Paris Agreement but is getting close: studies suggest the share of renewable electricity in total generation needs to reach 85-100% by 2030 to be compatible with a 1.5°C pathway (Climate Action Tracker, 2023). The government is aiming for capacity additions for solar PV and onshore and offshore wind to a total of 360 GW cumulative installed capacity by 2030 (30GW offshore wind, 115 GW onshore wind, 215 GW solar PV)(Federal Ministry of Economics and Climate Protection, 2022), more than twice the current capacity of 161 GW (Fraunhofer ISE, 2024a). Solar capacity additions are ramping up at record levels, with the addition of 15 GW in 2023 alone, showing the effect of government policies. If the trend of the first six months continues, Germany will build an additional 15.2 GW of new solar capacity in 2024 (Fraunhofer ISE, 2024b). The government’s plan is to annually expand solar capacity by 22 GW each year by 2028 (Wirth, 2023), the realisation of which appears to be within reach if the pace of massive expansion continues. The installed capacity of solar energy increased by around 130% between 2012 and 2022 (IEA, 2024). According to the government's targets on wind energy, an expansion of 14 GW would be required for 2023 and 2024. This would meet the 2024 EEG onshore wind target of 69GW and, assuming linear interpolation, the offshore wind target of 30GW installed capacity by 2030. In 2023 and 2024 so far, wind energy has only been expanded by 4.5 GW (Fraunhofer ISE, 2024b). Onshore wind capacity expansion remains below its all-time high of 5.5 GW in 2017. In 2023, only an additional 3 GW were newly built (Deutsche WindGuard GmbH, 2024), half of the planned 6 GW (BMWK, 2022). This needs to be ramped up to 16 GW annually by 2029 to meet the government's target, five times faster than in 2023. The government's own projections report assumes the expansion targets for wind are met, which we judge as optimistic. For our analysis, we use a range for wind expansion between fully meeting the target and only adding half the capacity each year. Bundesnetzagentur (2024b) As part of its National Hydrogen Strategy (German Government, 2020b), the government is providing EUR 11bn to support projects (BMWK, 2023a). The first auction of “Carbon Contracts for Difference” (CCfDs), through which the additional costs of companies compared to conventional production are compensated, was launched mid-March 2024 (BMWK, 2024b). The strategy was updated in June 2023, doubling the previous goal for electrolyser capacity from 5 GW to 10 GW in 2030 (BMWK, 2023c). The strategy also includes support for several projects to import green hydrogen to Germany from Australia, Morocco, Brazil and South Africa, and the development of an auction model for green hydrogen. Importing green hydrogen from distant countries such as Australia and South Africa calls into question its sustainability due to the significant emissions generated during transport. The hydrogen strategy explicitly includes hydrogen from fossil gas for an interim period. Coal phase-out The share of coal in the electricity system has been halved over the last five years, but still stands at 21% for January to July 2024, of which three-quarters are from lignite, the most emissions-intense form of coal (Fraunhofer ISE, 2024d). Roughly one third of CO 2 emissions from coal-fired electricity generation in Europe are from Germany (IEA, 2021). In July 2020, the previous government adopted a coal exit law stipulating the last coal-fired power plant will be closed by 2038. The compromise was found only by compensating the affected regions (with EUR 40bn) and the affected companies operating the coal-fired power plants (with an additional EUR 4.35bn) (Agora Energiewende, 2019; Bundesministerium für Wirtschaft und Energie, 2019). In November 2020, the European Commission approved its proposed competitive coal phase-out tender mechanism under the coal exit law (European Commission, 2021). In the first auction rounds between September 2020 and March 2022, the Federal Network Agency awarded bids for a combined capacity of around 9.7 GW (Bundesnetzagentur, 2022). The operators received up to EUR 165,000 for each MW of installed capacity to be phased out by the end of 2022 at the latest and, in 2021, a total of 5.8 GW coal capacity was retired (Bundesnetzagentur, 2021, 2022; Global Energy Monitor et al. , 2022). A total of 15 lignite and hard coal-fired power plants in Germany were shut down by April 2024. This included seven lignite-fired power plant units with a capacity of around 3.1 gigawatts, which the German government had originally planned to shut down earlier. Due to energy-saving measures for natural gas during the energy crisis, the shutdown date for two of these units was postponed and the remaining five units were taken out of security standby (MDR, 2024; Zeit, 2024). According to the coalition agreement, the government wants to phase out coal by 2030. However, there is no consensus on this among the federal states, and a legally required evaluation of the feasibility of the coal phase-out by 2030 by the federal government has not yet taken place. While the energy company RWE and the state of North Rhine-Westphalia agreed on a coal phase-out by 2030, the eastern German states recently emphasised their rejection of a phase-out of coal mining in the region by 2030 (Tagesschau, 2024b). First attempts to move the coal phase-out to an earlier date have likely led to more greenhouse gas emissions according to our analysis: in early 2022, the largest coal operator in west Germany, RWE, and the state government of that region struck a deal under which the coal phase-out would be moved forward from 2038 to 2030 at the expense of moving the shut-down of some capacity originally scheduled for a 2022 closure back to 2024, in an attempt to save gas. For RWE, this is probably a good deal because it will lead to more operating hours before 2030 than originally planned. After 2030 it would likely not have been viable to operate the coal-fired power plants anyway, because of the high carbon price expected from the revised EU ETS. This deal saved several villages from destruction. However, it did not save the iconic village of Lützerath as it was argued the lignite underneath the village was needed for energy security in Germany (RWE Power AG, 2023). This was contested by scientific groups (Oei et al. , 2023), heavily criticised by civil society, and led to major protests. Fossil gas Fossil gas is currently providing 13% of Germany's electricity. Only 13% of gas is used in the electricity sector: most is used in industry and for heating (BDEW, 2024). If renewables are expanded as planned and coal is phased out, the existing gas-fired power plants could provide the remaining electricity, if they run on a higher load. This is, however, unlikely, as with the large share of variable renewables, the flexibility of other sources in the system will need to increase and will need to cover peaks in demand, rather than running long hours. Building new gas peaker plants is expensive. While power plants that operate as combined heat and power (CHP) generation are more efficient, they are much less flexible, with only a limited ability to react to variations in the grid. The German government should carefully consider which combination of storage capacity, grid investments, demand management, and additional gas peaker plants is most (cost) efficient when moving to a high share of renewable energy. The stakeholder consultation process “Platform for a climate neutral electricity system” (BMWK, 2023e) is working to fill the current gap of an overall plan. In its new strategy in February 2024, the government agreed to support four new gas-powered stations that would initially run on fossil gas, but would need to move to hydrogen between 2035 and 2040 (BMWK, 2024a). With this strategy, the government takes a transitional approach without a fully comprehensive plan. As a reaction to the Russian invasion of Ukraine and the need to reduce dependency energy imports from Russia, the German government is pursuing partnerships with other potential suppliers. These include Qatar, the US and Senegal (Tagesschau, 2022). Such long-term partnerships not only risk a lock-in of the German economy into the unsustainable use of a fossil fuel, but also threatens the necessary transition in the partner countries and raises questions around international justice and geopolitical risks. Nuclear In April 2023, the last nuclear power plant was disconnected from the German grid. Due to the gas crisis, the end date was postponed from 31 December 2022 to 15 April 2023. The shutdown provides investment certainty for renewables and paves the way to a truly sustainable electricity system. In 2024, one year after the last nuclear power plants were shut down, the feared impact on electricity prices proved unfounded. The remaining share of nuclear energy amounted to 3.6 % of electricity consumption in 2023 and came from imports from neighbouring countries such as France. Meanwhile, renewable energy like solar and wind, are progressively fulfilling the demand. (Agora Energiewende, 2024).</t>
-  </si>
-  <si>
-    <t>Electricity generation is responsible for less than 10% of Canada’s emissions. Its share of the country’s emissions has been falling since 2015 as Canada shifts away from coal (Environment and Climate Change Canada, 2023b). The government has committed to achieving a net zero emissions grid by 2035 (Liberal Party of Canada, 2021a). Draft regulations were issued in August 2023, but will not be adopted until 2024 (Government of Canada, 2023a). To be 1.5°C compatible , Canada would need to phase out all fossil fuels in the power sector by 2030 (Climate Action Tracker, 2023a). The CAT does not see a role for CCS in the power sector, given its high cost, low technological maturity and residual emissions (Climate Action Tracker, 2023b). Coal power phase out – almost, but not quite Canada co-founded the Powering Past Coal Alliance in 2017 to help accelerate the rapid phase-out of “unabated” coal-fired electricity. It has had a regulatory system in place since 2018 to phase out “unabated” coal power by 2030 and is on track to achieve this phase-out. However, this regulation still allows plants which emit up to 420 gCO 2 /kWh, i.e. roughly half the emissions intensity of conventional coal power (Government of Canada, 2018d). Currently only three of its ten provinces still generate power from coal (Natural Resources Canada, 2023b). Alberta (Severson-Baker, 2024). While these developments are positive, they fall short of the 1.5°C benchmark. The CAT does not see a role for coal power with CCS for three main reasons: CCS does not remove 100% of emissions from power plants Heavily relying on unproven CCS for power generation simply prolongs the use of fossil fuels, diverting attention and resources away from the necessary and urgent switch to renewable energy generation that drives down actual emissions. The use of CCS should be limited to industrial applications where there are fewer options to reduce process emissions—not to reduce emissions from the electricity sector where renewables are cost-effective mitigation alternatives Since 2014, Canada has had one coal-fired power plant equipped with CCS in operation (Saskatchewan’s Boundary Dam), but it has been plagued with technical and operational problems and has still not met its annual CO 2 capture target (Rives, 2022; SaskPower, 2022b, 2022a; Schlissel, 2021; Taylor, 2019). Fossil gas power phase-out To achieve its goal of a (net) zero emissions grid, the government proposed new Clean Electricity Regulations in 2023 to streamline and strengthen emissions performance standards for all fossil-generated electricity above 25 MW capacity (Government of Canada, 2022g, 2023a, 2018e). These regulations will replace the coal and fossil gas regulations when they come into force in 2035. They will apply different rules to older plants (in operation before 2021) and newer plants (commissioned in or after 2021). For newer plants, any emissions that occur after 2035 would need to be offset or will be subject to the federal carbon price (which will be a minimum of CAD 170/tCO 2 e by that time). Exemptions will apply in cases of emergencies, when fossil gas without CCS may be used, and for remote northern communities (where much of the power is diesel generated). For older facilities, only emissions that exceed the sector benchmark of 370 gCO 2 /kWh need to be offset. The regulations may also provide flexibility for newer fossil gas units built prior to 2025, which would be allowed to continue to operate ‘for a short prescribed period’ after 2035 (Government of Canada, 2022j). Cascade Power, a 900 MW fossil gas plant, due to start operation in 2024 could fall under such exception (Cascade Power, 2021). SaskPower is also building new fossil gas plants to come online in 2024–2026 (SaskPower, 2022a). While the commitment to decarbonise its power sector by 2035 is a positive step, the extent to which Canada continues to build and rely on fossil gas is concerning, especially given that the cost of fossil gas is expected to increase further, while renewable electricity generation continues to get cheaper. Renewables Two-thirds of Canada’s electricity is already renewable, due to a long legacy of hydropower that still supplies 60% of demand. Solar and wind power are increasing fast, having grown from 2% to 7% market share in the last decade. Another 15% is nuclear power, leaving less than 20% to be supplied from fossil sources (IEA, 2023). Despite this strong starting position for achieving an early carbon-free grid, under current policy, Canada is expected to use gas for power generation beyond 2030, betting on CCS to deliver on its promise of a net-zero emissions grid by 2035. Canada has several funding programmes for ‘clean electricity’ projects, including renewables, nuclear and CCS-projects as well as programmes to fund storage and grid strengthening (Environment and Climate Change Canada, 2022a). Hydrogen Canada released its Hydrogen Strategy in 2020 (Natural Resources Canada, 2020). It sees the shift to hydrogen as a key contributor in meeting both its 2030 NDC and net zero goals. The Strategy estimates that Canada could reduce emissions by 22–45 MtCO 2 e by 2030, representing 15% of total reductions, by supplying 6% of final demand, primarily in the transport and industry sectors. By 2050 it foresees savings of 90–190 MtCO 2 e through the use of hydrogen representing 26% of total reductions, by supplying 30% of final demand. The Strategy is not limited to green hydrogen (produced with renewable energy only), but includes hydrogen produced from fossil fuels with CCUS. In contrast, Canada’s latest climate plan only includes a 15 MtCO 2 e reduction from hydrogen use by 2030. As much of the hydrogen would be produced using fossil gas, an additional 30 MtCO 2 e of CCUS capacity would be needed to capture the associated emissions (Office of the Auditor General of Canada, 2022b). For comparison, Canada’s only commercial CCS abated coal-fired power plant in operation was designed to capture 1 MtCO 2 e and has not yet achieved this target (see above for details). Canada’s Commissioner for the Environment and Sustainable Development has heavily criticised the estimates in the Hydrogen Strategy, finding the underlying assumptions on policy implementation and price development ‘unrealistic’ (Commissioner of the Environment and Sustainable Development, 2022b; Office of the Auditor General of Canada, 2022b). One example is the assumption that a blending level of 7.3% can be achieved in the medium term: In the absence of blending obligations for 2030 a carbon price of at least CAD 500/tCO 2 , rather than the anticipated CAD 170/tCO 2 , would be required to achieve this. Russia’s illegal invasion of Ukraine has reinforced the need for securing green hydrogen production and supply. In August 2022, Canada and Germany established a Hydrogen Alliance through which Canada would aim to start exporting hydrogen to Germany in 2025 (Government of Canada &amp; Government of the Federal Republic of Germany, 2022).</t>
-  </si>
-  <si>
-    <t>Switzerland has the third lowest carbon intensity of electricity generation (41g CO 2 ) in the world ( Carbon Intensity of Electricity Generation, 1990 to 2023 , 2024), owing to its historically highly decarbonised power system. In 2023, over 95% of electricity in Switzerland was generated from zero carbon sources, mainly from hydro (56%, mostly hydro) and nuclear (33%) (IEA, 2024). The Swiss power sector has been included in the ETS since 1 January 2020, but this only affects a small number of operators given the sector’s highly decarbonised nature. The Energy Strategy 2050 became the key framework in the energy sector when it replaced the previous Energy law. The energy strategy withstood a public referendum in 2017 and contains a package of measures aiming at increasing energy efficiency, reduction of CO 2 emissions, and steadily replacing nuclear energy with renewables (Bundesamt für Energie, 2018a). To execute the strategy, Switzerland revised its Energy Act (EnG) and set targets for the expansion of electricity production from renewable energy for 2020 and 2035. Switzerland exceeded the 2020 target for non-hydro renewables, but electricity generation from non-hydro renewables must increase by 450 GWh annually to meet the 2035 target of 11.4 TWh (Bundesamt für Energie, 2021). While it is good that Switzerland has such targets, they should not be absolute but rather as a share of total, as this better reflects the increase in energy demand due to end-use electrification. The Act also prohibits the construction of new nuclear power plants and states that nuclear energy shall steadily be replaced by renewables. The first of Switzerland's five nuclear power plants was shut down in December 2019. There is no schedule for the other four; they will likely continue running until at least 2030. In August 2024, however, the Environment Minister opened a discussion to amend the Act to again allow the construction of new nuclear plants. While this argument is based around “technology openness”, experts warn this is a derailing tactic to divert the conversation away from implementing the necessary wind and solar expansions (Sarah Schmalz, 2024). The Act also includes a goal for decreasing per capita electricity consumption, and introduced some changes to feed-in tariffs for renewables, including shortening the period during which new installations receive the tariffs from 20 to 15 years (Die Bundesversammlung der Schweizerischen Eidgenossenschaf, 2018; VSE, 2019). In June 2021, the Federal Act on a Secure Electricity Supply with Renewable Energies was launched to set out the necessary amendments to the Energy Act and the Electricity Supply Act to be aligned with the energy strategy 2050, and after several iterations it withstood a public referendum in June 2024 and now is enacted. It includes renewable installation targets for 2035 and 2050 of substantial scale: generation of non-hydro renewable generation needs to grow to 35 TWh in 2035 and 45 TWh in 2050 (from 4.6 TWh in 2023) while hydropower generation not go below 37.6 TWh in 2035 and 39.2 TWh in 2050. The Act further includes demand targets to enforce improvements in energy efficiency and includes electricity import thresholds. It also includes specific market-oriented support mechanisms such as the introduction of competitive tenders and investment contributions, phase-out of feed-in tariffs and expansion of market premiums. Another central part is the a mandatory construction of rooftop PV for new buildings, but this was weakened to only include buildings with a chargeable building area (roofs or facade) of over 300m2.(Bundesgesetz Über Eine Sichere Stromversorgung Mit Erneuerbaren Energien, 2024; IEA, 2024). For energy security reasons, Switzerland is highly dependent on traded electricity with its neighbouring countries. Since 2007, non-EU member Switzerland has been negotiating with the EU to form an agreement to better integrate its own market with the EU electricity market. When negotiations on institutional bilateral agreements between Switzerland and the EU were abruptly terminated in 2021 (based on non-energy/climate related issues), discussions on Switzerland’s access to the European electricity market were also put on hold. As a result, Swissgrid, the Swiss grid company, has had to negotiate technical, private-law agreements with European transmission system operators.</t>
-  </si>
-  <si>
-    <t>Electricity supply contributed to 25% of total US GHG emissions in 2022 (excluding emissions from land use, land use change and forestry, or LULUCF) (U.S. Environmental Protection Agency, 2024k). Total annual emissions in the power sector have declined steadily since 2010, mainly driven by a shift from coal to lower or non-emitting generation sources, such as fossil gas and renewables. Electricity production from renewables overtook production from coal and nuclear power for the first time in 2022, making renewables the country’s second largest source of electricity generation after fossil gas (U.S. Energy Information Administration, 2023j). Preliminary figures for 2023 suggest that coal is now becoming the least relevant generation source in the US, when all types of renewables are counted together (Rhodium Group, 2024) Following a drop in CO 2 emissions during the COVID-19 pandemic, emissions in the power sector returned to pre-pandemic levels as the economy recovered, but began dropping again in 2023. In 2021, electricity generation and emissions from coal-fired power plants increased for the first time since 2014 by 16% and 15%, respectively (U.S. Environmental Protection Agency, 2023f). The marked increase in coal-fired generation in 2021, and its sustained elevated level in 2022, can be mainly attributed to the significantly higher and more volatile prices of fossil gas as a consequence of the 2021 energy crisis, which rendered coal more competitive (U.S. Energy Information Administration, 2021b, 2023n). In 2023, gas generation rebounded and replaced coal generation, which led to emissions reductions in the sector. Although renewables contributed to sectoral emissions reductions, fossil gas had more than double the growth rate of renewable generation. The Biden Administration announced a target for the US' electricity system to become carbon-free by 2035. The CAT estimates that the full decarbonisation of the US power sector by 2035 would reduce total economy-wide emissions by about 25% below 2005 levels by 2030. The goal of a carbon-free power supply by 2035 is aligned with the Paris Agreement, based on the CAT’s primary global least-cost based benchmarks (Climate Action Tracker, 2023b). The target also meets the IEA’s suggested net zero target year for advanced economies (IEA, 2021). If accompanied by ambitious electrification targets in other sectors, such as 100% electric vehicle (EV) sales by 2030 or the full electrification of building heating, the US would be on track to meet the target of 50%–52% emissions reductions below 2005 levels (Climate Action Tracker, 2021b). However, emissions in the power sector must reduce more rapidly to reach the US economy-wide target. In 2021, total emissions from electricity generation had decreased by 36% compared to 2005 levels. With the introduction of the IRA, emissions from electricity generation are projected to further decrease by 67%–87% compared to 2005 levels by 2035 (U.S. Environmental Protection Agency, 2023b). More recent analysis, which takes into account the recent EPA regulations in the power sector, suggests that emissions might be even further reduced to 90% below 2005 levels by 2035 (King, Kolus, et al., 2024). Nevertheless, there remains a gap between the projections and target, highlighting the need for additional, more ambitious policies and actions. Renewable energy status and outlook In 2022, electricity generation from renewable sources surpassed generation from coal and nuclear power for the first time, becoming the second largest source of electricity generation after fossil gas (U.S. Energy Information Administration, 2023j). Increasingly cost-competitive renewables, in combination with the IRA and state-level renewable portfolio standards (RPS), are expected to continue driving the growth of renewables in the electricity sector, further displacing nuclear and fossil fuel-fired power plants. In 2023, renewables generated approximately 22% of total US electricity, with wind (10%), hydropower (6%), and solar (3%) representing the greatest shares. In 2022, solar and wind capacity increased by 5% above 2021 levels, growing to more than 238 GW. Nearly 75% of added generation capacity in 2022 were renewables. The installed capacity of solar increased by roughly 20 GW in 2023 and is projected to increase by 36 GW in 2024. The annual expansion of wind capacity lags behind solar; wind capacity only grew by 6 GW in 2023 and is forecast to increase by 7 GW in 2024 (U.S. Energy Information Administration, 2024e). Modelling of the IRA’s impact on renewables suggests an average capacity deployment of 54 GW/year, driven mainly by the expansion of wind and solar (U.S. Environmental Protection Agency, 2023c). However, according to scenarios that model a 100% clean energy power sector by 2035, annual additions in renewable energy capacity need to increase significantly. To achieve 100% renewable energy generation by 2035, the installed capacity of wind would need to grow by 70–145 GW/year between 2025 and 2035. During the same period, the installed capacity of solar would need to increase by 43–90 GW/year (Denholm et al., 2022). The clean energy project pipeline, that is emerging as a result of the IRA, shows promising growth, having reached 309 GW of announced clean energy capacity (Cleanpower, 2024). The growth in clean energy projects is also reflected in the total project capacity seeking transmission access: in total, 1,480 GW of clean electricity generation are seeking transmission access, of which solar alone accounts for 1,086 GW (WRI, 2024). Historically only about 14% of announced capacity gets interconnected, but the number of new projects that were announced after the passage of the IRA (e.g. more than 500 GW of solar) reflect increased developer interest and may result in a higher interconnection rate. However, major challenges for the deployment of renewables persist; complex permitting processes, higher interest rates and costs, and supply chain issues will need to be overcome to ensure project implementation (WRI, 2024). The IRA is strengthening value chains in the medium to long term in the US by incentivising domestic manufacturing (see above), but current supply chain issues remain. While issues plaguing the solar supply chain have largely been resolved, other decarbonisation-critical equipment, such as transformers, are subject to enduring supply chain issues, resulting in long lead times (WRI, 2024). Heightened interest rates have increased project costs, especially for renewables with high upfront costs, and have elevated prices for power purchase agreement (PPA). In turn, higher PPA prices have reduced clean energy purchases by corporates (WRI, 2024). To address risks that lead to and are associated with higher interest rates, the IRA allocates USD 3.6bn for clean energy loans to enable USD 40bn in loan guarantees, particularly targeting new technologies (Harper et al., 2023). Other instruments, such as contracts for difference, which the EU recommends to its Member States in its market design directive (European Commission, 2023), could help minimise risks and thus financing costs, especially for offshore wind (Beiter et al., 2024). Expanding transmission lines is a major enabler for the deployment of renewables, especially wind and solar, and is essential for their overtaking of fossil gas as the primary source of electricity generation. The historical pace of grid extension of about 1% per year needs to increase to 2.3% per year to reach the full reduction potential of the IRA; a net zero pathway would require an even faster expansion (Jenkins et al., 2022). Currently, only 10% of the necessary investment in transmission infrastructure is planned (WRI, 2024). This low level of investment is especially alarming given that transmission projects in the US take an average of 10 years to build (WRI, 2023). Although state governments are primarily responsible for maintaining and upgrading grid infrastructure, federal agencies are implementing several measures to augment investment. For instance, the US Department of Energy (DOE) introduced the Coordinated Interagency Authorizations and Permits programme (CITAP), which streamlines the permitting process for transmission facilities. The DOE also unlocked additional targeted funding to expand transmission capacity (S&amp;P Global, 2024) and is in the process of developing auxiliary measures (WRI, 2024). Another challenge for the power sector is the growing demand for electricity. The growth in demand is not only driven by the electrification needs of a decarbonised future, but also by the emergence of large-scale data centres, the increase in manufacturing facilities, the enhanced demand for building cooling and heating, and the introduction of hydrogen fuel plants. For example, electricity demand from data centres, which currently account for around 4% of electricity demand, is expected to grow to between 4.6%–9.1% of electricity demand by 2030 (EPRI, 2024). Permitting and siting are major barriers for the buildout of renewable energy capacity. Current project build times average four years. The IRA includes USD 1bn to support the Biden Administration's Permitting Action Plan, which seeks to accelerate the federal permitting and environmental review process for transmission lines and clean energy productions. The federal government is also working to address issues related to project siting. The government set a target to double clean energy permits on public lands in order to reach 25 GW of renewable energy generation by 2025. This goal was reached at the end of 2023, with a total of 29 GW worth of allocated permits. A further 32 GW are currently under consideration by the government (Reuters, 2024). Given that permitting and siting processes are largely controlled by subnational jurisdictions, action at the state level is key. California and Massachusetts have implemented promising approaches for streamlining the permitting process for clean energy projects that could be replicated by other states (WRI, 2023). The US Department of the Interior (DOI) announced a plan to deploy 30 GW of offshore wind by 2030 and unlocked USD 3bn in federal loans for offshore wind and transmission projects. By the end of FY2023, the Bureau of Ocean Energy Management aims to approve a cumulative 14.8 GW in offshore wind energy capacity to support the 2030 target (U.S. Department of the Interior, 2023a). However, estimates suggest that only 14.5 GW will come online by 2030, which means the government will fall significantly short of its 30 GW target. Approximately 11 GW of planned offshore capacity have been cancelled or are being renegotiated (Canary Media, 2023). A diverse set of drivers have been responsible for the growth of renewable energy in the US. At the subnational level, renewable portfolio standards (RPS) and clean energy standards (CES) have been major drivers. In total, 32 states and the District of Columbia (D.C.), accounting for 58% of US electricity sales, have enacted RPS or CES legislation. Of these, 15 states and D.C. have signed 100% clean electricity goals into legislation, while seven states have enacted such a target through state-level executive orders (U.S. Energy Information Administration, 2023c). In the past, roughly half of the growth in renewable generation capacity could be associated with these standards. In recent years, however, these standards have contributed less; with current RPS or CES legislation alone the share of non-hydro RE will only increase to 28% by 2050, well below what is needed (see below). Voluntary utility procurements, net metered PV/onsite production, and corporate PPAs have become drivers for the development of renewable energy sources (Barbose, 2023). However, these drivers are constrained by high interest rates. To ensure that sufficient renewable generation capacity is built, states could increase the ambition of their RPS or CES legislation, while states without such standards could introduce them. At the federal level, tax credits for the production and investment in clean energy support the buildout of renewables . The Biden Administration modified and extended the current Production Tax Credit and Investment Tax Credit through 2024. After 2024, the credits transition towards technology-neutral, emissions-based credits in the form of the Clean Electricity Production Tax Credit and the Clean Energy Investment Tax Credit. Importantly, the current tax credit applies to all projects that commence construction by 2032, providing additional investor certainty (Harper et al., 2023). Both credits incentivise investment in disadvantaged communities and provide additional bonuses to wind and solar projects in low-income neighbourhoods (The White House, 2023c). The direct impact of these credits is uncertain and difficult to assess as they overlap, complement, and engage with other incentive schemes and market dynamics. An EPA review of scenarios estimating the IRA’s impact, which this assessment uses for the current policy projections scenario , shows that the implementation of the IRA could lead to emission reductions of between 49%–83% in the power sector by 2030 below 2005 levels (U.S. Environmental Protection Agency, 2023d). The modelling projects that the share of renewables in total electricity generation will increase significantly, reaching 28%–60% in 2030 and amounting to up to 85% in 2035 (U.S. Environmental Protection Agency, 2023d). However, these penetration levels are insufficient to meet the Biden Administration’s 2035 goal of a carbon-free power sector. In order to be aligned with a Paris Agreement-compatible, least-cost pathway, the CAT estimates that 68%–86% of the electricity generated by 2030 should come from renewable sources (Climate Action Tracker, 2023b). Storage and flexibility With an increasing share of variable renewable energy in the US electricity generation mix, there is an increasing need for supply and demand-side flexibility. Storage needs will increase as gas-fired power plants, currently providing flexibility services, are phased out. To decarbonise the power sector by 2035, approximately 120–350 GW of diurnal storage and up to 680 GW of seasonal storage is required (in a scenario that does not include carbon capture and storage (CCS)) (Harper et al., 2023). The need for utility storage and demand flexibility is also directly linked to the buildout of the transmission grid which, as highlighted above, is happening far too slowly. Building out storage capacity can reduce the need for transmission expansion and vice versa. The IRA has spurred a significant increase in utility-scale diurnal storage projects, as evidenced by the number of storage projects awaiting interconnection. Since August 2022, more than 540 GW of storage has requested interconnection. Approximately half of that storage capacity is combined with a generation technology, mainly solar. In total, around 514 GW of storage is planned to come online before the end of 2026. Historically, only 11% of planned storage capacity has materialised. However, the operationalisation rate might increase given that the IRA makes available the Production Tax Credits and Investment Tax Credits for standalone storage projects. In the current storage project pipeline, battery storage dominates. The number of other storage technologies in the pipeline, notably those better suited for seasonal storage, has also increased. In contrast to supply flexibility, demand flexibility remains underdeveloped in the US. Demand flexibility can play an important role, as transmission projects are developing too slowly, and storage projects incur additional resource use. Economic analyses suggest that large-scale demand flexibility deployment can reduce the costs of grid extension and ancillary services by approximately USD 13bn/year, while simultaneously contributing to the integration of renewables (Bronski et al., 2015). States are beginning to recognise the importance of demand flexibility: state level institutions, such as the California Utility Commission, are starting processes to enable “widespread demand flexibility” (California Public Utilities Commission, 2022). Nevertheless, demand flexibility continues to be largely underfunded. Seasonal storage, or long-duration storage, is underdeveloped, but will likely be critical to decarbonising the power sector by 2035. Unlike for short-term, diurnal storage, where batteries have emerged as a promising, increasingly cost-competitive technology, seasonal storage is much less mature and requires significant investments in research and development. The DOE is beginning to support seasonal storage projects; it is providing a USD 504.4m loan guarantee for a hydrogen storage capacity in Utah and introduced the Long Duration Storage Shot that aims to decrease costs for seasonal storage by 90% within the coming decade (U.S. Department of Energy, 2023c). However, the government’s efforts must be intensified to deploy the technology at the scale and pace to achieve sectoral decarbonisation. Fossil fuel phase-out The US government has not set a fossil fuel phase-out target for coal or fossil gas. It did not support the coal phase-out initiative at COP26, but has taken an important step since the last CAT assessment by becoming a signatory to the Powering Past Coal Alliance. Several states have committed to phasing out coal, but states with a major share of coal generation generally have not. The federal government also recently reframed its position on phasing out fossil fuels: since May 2024, the US refers to a “a fully or predominantly decarbonized power sector by 2035" after initially calling for a “carbon pollution free” electricity sector by 2035. Such reformulation opens the door for use of abated coal (e.g. with carbon capture and storage), as well as the use of coal in sectors that are not directly related to electricity generation (GEM Wiki, 2024). In 2023, the share of coal generation continued to decline at an even faster pace than in 2022. In 2022, approximately 20% of total US electricity generation was derived from coal. This dropped to 16% in 2023, a decrease driven by the continued buildout of fossil gas generation and the growth of renewable sources. Elevated fossil gas prices induced a temporary increase in coal-fired generation in 2021, which did not last, as gas prices returned to 2020 levels in 2023 (U.S. Energy Information Administration, 2024c). As a result, the capacity factor of coal-fired power plants reduced from 48% to 42% (Inside Climate News, 2024); a trend that reflects the worsening economics of coal but one that could be reversed in future if coal-fired power plants are not shut down. Approximately 30% of the US coal-fired generating capacity has been retired since 2010: no new coal-fired capacity has been installed since 2013, and more coal power plants are due to be decommissioned in the near future (U.S. Energy Information Administration, 2021a, 2023g, 2023k). However, the retirement of coal generation capacity has slowed in recent years and is expected to continue to slow in 2024. Although the US Energy Information Administration (EIA) expected 8.9 GW of coal-fired power plants to retire in 2023 (U.S. Energy Information Administration, 2023g), only 5 GW actually retired (Ember, 2024). For 2024, only 2.3 GW of coal-fired power plants are set to retire (U.S. Energy Information Administration, 2024d). In comparison, annual coal retirements averaged 11 GW between 2015 and 2020 (U.S. Energy Information Administration, 2023g). The EIA’s Annual Energy Outlook 2023, used as one of the reference scenarios for this assessment’s current policy projections , suggests that no new coal-fired capacity will be added in the US. In the reference case, coal-fired capacity is projected to decline by 64% to 73 GW by 2050 (U.S. Energy Information Administration, 2023h). This means that a full phase-out of coal power by 2035 requires additional policy action to accelerate and reinforce market forces that, as evidenced by the last decade, are pushing coal out of the mix. According to the CAT, the US needs to phase out all coal-fired power generation by 2030 to be aligned with the Paris Agreement (Climate Action Tracker, 2023b). In April 2024, the EPA finalised its new Greenhouse Gas Standards for Fossil-Fuel Fired Power Plants, which targets existing coal-fired power plants and new gas-fired power plants. The standards cover GHG emissions, waste water, mercury, and toxic metals. The standards set the most stringent emissions limits for both plant types in US history and mandate that all coal-fired power plants reduce or capture nearly all of their CO 2 emissions by 2040 (U.S. Environmental Protection Agency, 2024m). The regulation exempts coal-fired plants that are set to retire before 2032, while relaxing the standards for those retiring between 2032 and 2039; these plants need to reduce emissions by only 16%. Coal plants that operate beyond 2039 will be required to reduce their emissions intensity by implementing CCS technology to capture 90% of CO 2 emissions by 2032. These requirements are expected to accelerate coal plant retirements before the 2040 deadline, resulting in an additional 22 GW of coal-fired capacity going offline between 2023 and 2035 (U.S. Environmental Protection Agency, 2024m). The EPA’s emissions standards for fossil gas distinguish between baseload and peak power plants: the standards only apply to baseload plants larger than 300MW. Plants covered by the regulation have the option to capture 90% of emitted CO 2 using CCS by 2035 or transition to 96% hydrogen fuel use by 2038. These standards are projected to reduce fossil gas emissions by approximately 200–400 MtCO 2 e by the mid-2040s. The combined cumulative reductions for both coal and fossil gas are forecasted to amount to 600 MtCO 2 e by 2050 (U.S. Environmental Protection Agency, 2023h). While setting emissions limits for power plants is a step in the right direction, the regulation’s impact remains uncertain as smaller baseload plants and peak power plants are not covered. Carbon capture and storage (CCS) The new EPA standards aim to reduce the environmental impact of fossil fuel-fired power plants and explicitly allows for CCS, signalling that the government considers CCS a viable solution for emissions reductions in the mid to long term (Parenteau, 2024). However, CCS has yet to be proven commercially viable at scale, and it remains unclear whether the technology will have demonstrated commercial viability by 2040. Given the high cost of CCS applications for fossil fuel-fired power plants (Clarke et al., 2022), the CAT estimates that most fossil fuel-fired power plants that are subject to the proposed regulations will already cease operations by 2040. If instead CCS does get deployed at scale, the widespread adoption of CCS could lead to significant additional emissions since current CCS technology only captures 90% of power plant emissions. Legal challenges In the past, the EPA has met numerous legal challenges in its efforts to regulate GHG emissions from fossil fuel-fired power plants; notable are two failed attempts during the Obama and Trump Administrations. Most recently, in June 2022, the US Supreme Court ruled to limit the EPA’s ability to regulate carbon emissions from power plants (West Virginia v. EPA, 2022). The decision sets a worrying precedent for future climate action. However, experts suggest the design of the EPA’s most recent standards explicitly considers the weaknesses of previously proposed regulations and, therefore, gives the standards a better chance against legal challenges (Parenteau, 2024). In parallel, the government passed stricter standards for power plants whose pollution crosses state lines (U.S. Environmental Protection Agency, 2023e). The EPA has also proposed stronger limits for mercury and water pollution from coal-fired power plants. These rules do not target pollution that directly contributes to global warming, but, nevertheless, limit the operation of coal-fired power plants and, in doing so, could indirectly accelerate their phase-out (U.S. Environmental Protection Agency, 2023g, 2023j). Unlike coal generation, oil and fossil gas generation increased significantly in 2023. More than 10GW of fossil gas-fired power plants were added in 2023, the highest increase since 2003 (Global Energy Monitor, 2024). Generation from fossil gas grew more than twice as fast as generation from renewables in 2023 (Rhodium Group, 2024). Studies suggest that lifetime use for fossil gas-fired plants breaks even after 9–17 years of operation under current regimes. The longevity of gas-fired power plants severely hampers the phase-out of fossil gas and, as a result, either jeopardises the sector’s 2035 decarbonisation target or invites the widespread deployment of CCS if the gas-fired fleet remains in operation or is expanded (Global Energy Monitor, 2024). Oil and fossil gas extraction The US became the world’s largest producer of crude oil in 2018 (U.S. Energy Information Administration, 2018), reaching its highest levels of oil and gas production and exports in 2023. US crude oil exports reached a high of 4.1 million barrels per day in 2023, corresponding to a 13% increase compared to previous record export level in 2022 (U.S. Energy Information Administration, 2024b). Increasing exports were driven by increased crude oil production, several releases from the US Strategic Petroleum Reserve (SPR), and increased demand in Europe for an alternative to Russian crude oil (U.S. Energy Information Administration, 2023l). Exports of petroleum products similarly increased: more petroleum products were exported—nearly six million barrels per day—in the first half of 2023 than in the first half of any prior year. Since 2020, growth in propane exports has driven growth in overall petroleum product exports; approximately 1.5 million barrels were exported per day in the first half of 2023 (U.S. Energy Information Administration, 2023e). The US is also the largest producer of fossil gas. Liquified natural gas (LNG) exports continue to increase year after year. In the first half of 2022, the US became the world’s largest LNG exporter. By the first half of 2023, LNG exports had further increased by 4% (U.S. Energy Information Administration, 2023d). This trend is expected to continue into the future as the US is planning to increase its LNG export capacity by more than 40% by 2026, compared to 2022 (U.S. Energy Information Administration, 2023m). The growth in exports is mainly driven by strong LNG demand from Europe, as well as by expanded and reopened LNG capacity. In 2022, US LNG exports to Europe increased by 141% compared to 2021 levels (U.S. Energy Information Administration, 2023b). Outside of Europe, interest in and demand for US LNG is also growing. In Mexico, new LNG terminals, as well as an expanding pipeline network, are contributing to growth in LNG imports from the US. In Asia, imports from the US continue to increase; Japan, China, and India increased imports in 2023 relative to 2022, while the Philippines and Vietnam imported LNG from the US for the first time in 2023 (Zaretskaya, 2024). In January 2024, the Biden Administration took a step towards addressing the climate impacts of US fossil fuel exports by issuing a temporary pause on the development of new LNG export terminals (Daly, 2024). The administration cited outdated project evaluation criteria, which inadequately capture the financial and environmental cost of new LNG infrastructure, as cause for the moratorium. As of October 2024, the pause remains in place. It is important to note that the pause does not impact operational, as well as approved, LNG terminals and, as a result, does not immediately impact the US supply of LNG to Europe and Asia (The White House, 2024b). Although a step in the right direction, the US should take stronger, more consistent action to phase out fossil fuel production and exportation. As the world’s largest fossil fuel producer and LNG exporter, as well as one of the largest GHG emitters and richest countries in the world, the US has a responsibility and is well-positioned to phase out fossil fuels. On the international stage, the US has signalled support for a reduction in fossil fuel production: at COP26, the US pledged to end international public support for the unabated fossil fuel energy sector by the end of 2022 (UK COP 26 Presidency, 2021b), and at COP27, the US supported language on a “fossil fuel phasedown." However, as evidenced by ever increasing domestic oil and gas exploitation, the government has contradicted itself on this issue (CAT, 2023). Record levels of fossil fuel production translate to record profits for oil and gas corporations. An analysis of five major fossil fuel corporations revealed that this set of companies earned USD 152bn in profit between 2017 and 2020 (Climate Power, 2024a). More recent data for 2021 through 2023 show that profits for the top ten largest oil and gas corporations by value tripled to USD 313bn under the Biden Administration in comparison to reported profits from 2017 through 2019 (McCormick &amp; Smyth, 2024). The EIA’s Annual Energy Outlook 2023 , included in the range of our current policy scenario projections , projects US fossil gas production to increase by 15% and LNG exports to increase by 152% between 2022 and 2050 (U.S. Energy Information Administration, 2023a). This increase is due to the expected increase in domestic and foreign demand for fossil gas and a continued increase in LNG capacity (U.S. Energy Information Administration, 2023m). The US has one of the largest expansion plans for oil and gas projects in the world. The country accounts for over one-third of planned global expansion in oil and gas extraction between 2023 and 2050. With 22 oil and gas mega-project plans in place, the US accounts for more than one-fifth of potential emissions from major carbon emitting energy projects in the world. Together, these 22 mega-projects have the potential to emit nearly 143 GtCO 2 e in their lifetime, which is almost four times more than the entire world emits each year (Kühne et al., 2022). Expansion of oil and gas projects is driven by planned increases in fracking and LNG extraction (Ioualalen &amp; Trout, 2023). In 2022, subsidies for fossil fuels, as defined as budgetary transfers, tax expenditures, and general supply- and demand-side financial support, reached their highest level since 2010: subsidies amounted to USD 14bn in 2022 (Fossil Fuel Subsidy Tracker, 2022). Fossil fuel subsidies have and will continue to spur the expansion of fossil fuel projects. Research indicates that two of the largest and longest standing subsidies—the ‘expensing of intangible drilling costs’ (IDC) subsidy and the ‘percentage depletion’ subsidy—increased the expected value of new oil and gas projects by upwards of USD 20bn over the past two decades (Erickson, 2021). Additionally, the Inflation Reduction Act (IRA), which incentivises the build out of renewable energy, simultaneously enables the expansion of oil and gas production by mandating new leases on public lands for fossil fuel projects (see below on new auctions and project approvals) (Ioualalen &amp; Trout, 2023). To keep 1.5°C of warming within reach, GHG emissions must be halved globally by 2030 and no new oil and gas should be developed (IEA, 2023b; IPCC, 2022). Therefore, the planned investment in and development of new oil and gas infrastructure in the US obstructs progress towards the global 1.5°C temperature target, as well as the country’s 2030 climate target and 2050 net zero target, and will likely lead to significant stranded assets in a Paris Agreement-compatible future. New fossil fuel auctions and project approvals Beyond the IRA’s incentives for clean energy production and investment, the act also provides notable concessions to the fossil fuel industry. The act offers these compromises under the pretence of allowing domestic oil and gas companies to transition away from fossil fuels at a reasonable pace. The IRA requires the federal government to offer an annual minimum area of specified public lands for oil and gas drilling. While the act does increase the royalty rates paid by companies for extracting fossil fuels on public lands, it also requires the prioritisation of oil and gas auctions over renewable energy on federal lands and offshore developments. These provisions not only contradict President Biden’s promise to end new federal fossil fuel leasing of public</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1021,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>137</v>
@@ -1042,7 +1029,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>138</v>
@@ -1050,7 +1037,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>139</v>
@@ -1058,7 +1045,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>140</v>
@@ -1066,7 +1053,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>141</v>
@@ -1074,7 +1061,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>142</v>
@@ -1082,7 +1069,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>143</v>
@@ -1098,7 +1085,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>145</v>
@@ -1106,7 +1093,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>146</v>
@@ -1114,63 +1101,10 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>147</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1414,7 +1348,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
@@ -1422,7 +1356,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -1430,7 +1364,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
@@ -1752,7 +1686,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>99</v>
@@ -1760,7 +1694,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>100</v>
@@ -1768,7 +1702,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>101</v>
@@ -1816,7 +1750,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>107</v>
@@ -1824,7 +1758,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>108</v>
@@ -1832,7 +1766,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>109</v>
@@ -1840,7 +1774,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>110</v>
@@ -1925,7 +1859,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>118</v>
@@ -1933,7 +1867,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>119</v>
@@ -1941,7 +1875,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>120</v>
@@ -1949,7 +1883,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>121</v>
@@ -1957,7 +1891,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>122</v>
@@ -1965,7 +1899,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>123</v>
@@ -1973,7 +1907,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>124</v>
@@ -2055,7 +1989,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>129</v>
@@ -2063,7 +1997,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>130</v>
@@ -2071,7 +2005,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>131</v>
@@ -2087,7 +2021,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>133</v>
@@ -2095,7 +2029,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>134</v>
@@ -2103,7 +2037,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>135</v>

</xml_diff>